<commit_message>
complete 1st iteration for DAC SSP assumption tests
</commit_message>
<xml_diff>
--- a/tutorial/dac_scenarios/SSPs/get_report_output.xlsx
+++ b/tutorial/dac_scenarios/SSPs/get_report_output.xlsx
@@ -501,43 +501,43 @@
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>0.06084682314476883</v>
+        <v>0.05509565926446665</v>
       </c>
       <c r="E2" t="n">
-        <v>0.2000423735851388</v>
+        <v>0.1590496842950373</v>
       </c>
       <c r="F2" t="n">
-        <v>0.5184715086001087</v>
+        <v>0.3551892616106319</v>
       </c>
       <c r="G2" t="n">
-        <v>1.246922336989336</v>
+        <v>0.7252637611620123</v>
       </c>
       <c r="H2" t="n">
-        <v>2.91335467948213</v>
+        <v>1.423517204411967</v>
       </c>
       <c r="I2" t="n">
-        <v>6.725549880421919</v>
+        <v>2.740975909622556</v>
       </c>
       <c r="J2" t="n">
-        <v>15.44647534465582</v>
+        <v>5.226745878556069</v>
       </c>
       <c r="K2" t="n">
-        <v>35.39680237249901</v>
+        <v>9.916875682255711</v>
       </c>
       <c r="L2" t="n">
-        <v>165.6438979927685</v>
+        <v>32.10231912905679</v>
       </c>
       <c r="M2" t="n">
-        <v>598.4913607737827</v>
+        <v>103.5979519695401</v>
       </c>
       <c r="N2" t="n">
-        <v>1803.267092494695</v>
+        <v>334.0024299110544</v>
       </c>
       <c r="O2" t="n">
-        <v>2109.127358184067</v>
+        <v>1029.011522827042</v>
       </c>
       <c r="P2" t="n">
-        <v>3145.665178795743</v>
+        <v>2245.440310793185</v>
       </c>
     </row>
     <row r="3">
@@ -553,43 +553,43 @@
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>0.004104809516001037</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>0.78459371558944</v>
       </c>
       <c r="F3" t="n">
-        <v>0.3430635898450779</v>
+        <v>2.257213598193661</v>
       </c>
       <c r="G3" t="n">
-        <v>1.642745768184947</v>
+        <v>5.035740367461045</v>
       </c>
       <c r="H3" t="n">
-        <v>4.61594908203964</v>
+        <v>10.27824123189513</v>
       </c>
       <c r="I3" t="n">
-        <v>11.41756419444205</v>
+        <v>20.16974762930833</v>
       </c>
       <c r="J3" t="n">
-        <v>26.97720248815939</v>
+        <v>38.83295844036233</v>
       </c>
       <c r="K3" t="n">
-        <v>62.57203398485105</v>
+        <v>74.0465471278178</v>
       </c>
       <c r="L3" t="n">
-        <v>196.2768863297713</v>
+        <v>240.6531204788015</v>
       </c>
       <c r="M3" t="n">
-        <v>575.4532606166779</v>
+        <v>718.1352612365251</v>
       </c>
       <c r="N3" t="n">
-        <v>1626.545148460347</v>
+        <v>2053.267228922684</v>
       </c>
       <c r="O3" t="n">
-        <v>1595.461506701585</v>
+        <v>1980.885760245286</v>
       </c>
       <c r="P3" t="n">
-        <v>1571.999142657128</v>
+        <v>1945.473080744267</v>
       </c>
     </row>
     <row r="4">
@@ -605,43 +605,43 @@
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>0.009015186007274745</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>0.09965326578959403</v>
       </c>
       <c r="F4" t="n">
-        <v>0.01966915236542421</v>
+        <v>0.270668429964076</v>
       </c>
       <c r="G4" t="n">
-        <v>0.1362661498479518</v>
+        <v>0.593338398788041</v>
       </c>
       <c r="H4" t="n">
-        <v>0.4029979594226343</v>
+        <v>1.202149373437236</v>
       </c>
       <c r="I4" t="n">
-        <v>1.013183982863299</v>
+        <v>2.35084878356274</v>
       </c>
       <c r="J4" t="n">
-        <v>2.409069174794571</v>
+        <v>4.518205138436267</v>
       </c>
       <c r="K4" t="n">
-        <v>5.602350230407735</v>
+        <v>8.607554821742397</v>
       </c>
       <c r="L4" t="n">
-        <v>26.46276654732008</v>
+        <v>27.95476705007753</v>
       </c>
       <c r="M4" t="n">
-        <v>82.91189107016777</v>
+        <v>90.30381070479915</v>
       </c>
       <c r="N4" t="n">
-        <v>186.4985544973277</v>
+        <v>205.1557064711814</v>
       </c>
       <c r="O4" t="n">
-        <v>179.4831619841654</v>
+        <v>204.145423337349</v>
       </c>
       <c r="P4" t="n">
-        <v>171.0853707586831</v>
+        <v>187.8022346280416</v>
       </c>
     </row>
     <row r="5">
@@ -657,43 +657,43 @@
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>0.1432487140876133</v>
       </c>
       <c r="E5" t="n">
-        <v>0.02740309748548211</v>
+        <v>0.413529179167097</v>
       </c>
       <c r="F5" t="n">
-        <v>0.2208901278542154</v>
+        <v>0.9234920801876429</v>
       </c>
       <c r="G5" t="n">
-        <v>0.6635185561481562</v>
+        <v>1.885685779021232</v>
       </c>
       <c r="H5" t="n">
-        <v>1.676092500564971</v>
+        <v>3.701144731471113</v>
       </c>
       <c r="I5" t="n">
-        <v>3.992495893053223</v>
+        <v>7.126537365018643</v>
       </c>
       <c r="J5" t="n">
-        <v>9.291590054340805</v>
+        <v>13.58953928424577</v>
       </c>
       <c r="K5" t="n">
-        <v>21.41400319760102</v>
+        <v>25.78387677386484</v>
       </c>
       <c r="L5" t="n">
-        <v>100.5751397846501</v>
+        <v>83.46602973554762</v>
       </c>
       <c r="M5" t="n">
-        <v>338.5858444109535</v>
+        <v>269.3546751208041</v>
       </c>
       <c r="N5" t="n">
-        <v>993.1578194869988</v>
+        <v>831.994569387629</v>
       </c>
       <c r="O5" t="n">
-        <v>1112.081051459048</v>
+        <v>956.9022213283326</v>
       </c>
       <c r="P5" t="n">
-        <v>1131.314382278719</v>
+        <v>948.7330248519417</v>
       </c>
     </row>
     <row r="6">
@@ -709,43 +709,43 @@
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>0.2479304666900999</v>
       </c>
       <c r="E6" t="n">
-        <v>0.1063917866573306</v>
+        <v>0.7157235793276679</v>
       </c>
       <c r="F6" t="n">
-        <v>0.517196677990502</v>
+        <v>1.598351677247844</v>
       </c>
       <c r="G6" t="n">
-        <v>1.456969866093804</v>
+        <v>3.263686925229055</v>
       </c>
       <c r="H6" t="n">
-        <v>3.606831427409955</v>
+        <v>6.405827419853852</v>
       </c>
       <c r="I6" t="n">
-        <v>8.524938042212286</v>
+        <v>12.3343915933015</v>
       </c>
       <c r="J6" t="n">
-        <v>19.77578931086541</v>
+        <v>23.52035645350231</v>
       </c>
       <c r="K6" t="n">
-        <v>45.51367264352295</v>
+        <v>44.62594057015069</v>
       </c>
       <c r="L6" t="n">
-        <v>151.8949556371067</v>
+        <v>144.4604360807555</v>
       </c>
       <c r="M6" t="n">
-        <v>447.795271233757</v>
+        <v>423.0826413460287</v>
       </c>
       <c r="N6" t="n">
-        <v>1138.072187794401</v>
+        <v>1144.801603134423</v>
       </c>
       <c r="O6" t="n">
-        <v>1845.737684631774</v>
+        <v>1855.969581856064</v>
       </c>
       <c r="P6" t="n">
-        <v>2040.126490912864</v>
+        <v>2044.372998097139</v>
       </c>
     </row>
     <row r="7">
@@ -761,43 +761,43 @@
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>0.1483010940000269</v>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>0.4671384943679568</v>
       </c>
       <c r="F7" t="n">
-        <v>0.1352070942251958</v>
+        <v>1.068718211191602</v>
       </c>
       <c r="G7" t="n">
-        <v>0.516184186716673</v>
+        <v>2.203773745065594</v>
       </c>
       <c r="H7" t="n">
-        <v>1.38772214636251</v>
+        <v>4.345386949347978</v>
       </c>
       <c r="I7" t="n">
-        <v>3.381486154944262</v>
+        <v>8.386164673326569</v>
       </c>
       <c r="J7" t="n">
-        <v>7.942497959331208</v>
+        <v>16.01026998886734</v>
       </c>
       <c r="K7" t="n">
-        <v>18.3764453022542</v>
+        <v>30.39536756984104</v>
       </c>
       <c r="L7" t="n">
-        <v>86.52280531913098</v>
+        <v>98.44225321602769</v>
       </c>
       <c r="M7" t="n">
-        <v>276.7867714264312</v>
+        <v>295.3257782175849</v>
       </c>
       <c r="N7" t="n">
-        <v>797.7019499216424</v>
+        <v>841.252875733017</v>
       </c>
       <c r="O7" t="n">
-        <v>1525.206197649374</v>
+        <v>1562.985222812144</v>
       </c>
       <c r="P7" t="n">
-        <v>1143.595999210851</v>
+        <v>1159.921971891186</v>
       </c>
     </row>
     <row r="8">
@@ -813,43 +813,43 @@
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>0.3751426068560831</v>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>1.512212530611525</v>
       </c>
       <c r="F8" t="n">
-        <v>0.4848376942079122</v>
+        <v>3.657626468725813</v>
       </c>
       <c r="G8" t="n">
-        <v>1.997497114644295</v>
+        <v>7.705575385229749</v>
       </c>
       <c r="H8" t="n">
-        <v>5.457915420387105</v>
+        <v>15.3432112463204</v>
       </c>
       <c r="I8" t="n">
-        <v>13.3741024278137</v>
+        <v>29.75383814647366</v>
       </c>
       <c r="J8" t="n">
-        <v>31.48347857824931</v>
+        <v>56.9436873920184</v>
       </c>
       <c r="K8" t="n">
-        <v>72.91118919831163</v>
+        <v>108.2452655341592</v>
       </c>
       <c r="L8" t="n">
-        <v>317.3798140302949</v>
+        <v>350.9350926234887</v>
       </c>
       <c r="M8" t="n">
-        <v>999.1320312291289</v>
+        <v>1107.344721722338</v>
       </c>
       <c r="N8" t="n">
-        <v>2848.860244056852</v>
+        <v>3192.581387894855</v>
       </c>
       <c r="O8" t="n">
-        <v>2566.178944712152</v>
+        <v>2812.087068324503</v>
       </c>
       <c r="P8" t="n">
-        <v>2430.97773345117</v>
+        <v>2685.878947992658</v>
       </c>
     </row>
     <row r="9">
@@ -868,40 +868,40 @@
         <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>0</v>
+        <v>0.1040981152614237</v>
       </c>
       <c r="F9" t="n">
-        <v>0</v>
+        <v>0.40577495075238</v>
       </c>
       <c r="G9" t="n">
-        <v>0.1548655538486071</v>
+        <v>0.9749762585584173</v>
       </c>
       <c r="H9" t="n">
-        <v>0.5854943699744066</v>
+        <v>2.048940483490814</v>
       </c>
       <c r="I9" t="n">
-        <v>1.57061753661041</v>
+        <v>4.075287121520113</v>
       </c>
       <c r="J9" t="n">
-        <v>3.824223466129637</v>
+        <v>7.898580860854038</v>
       </c>
       <c r="K9" t="n">
-        <v>8.979659717727591</v>
+        <v>15.11233922918836</v>
       </c>
       <c r="L9" t="n">
-        <v>42.6712713510577</v>
+        <v>49.24813039342792</v>
       </c>
       <c r="M9" t="n">
-        <v>136.8844870578804</v>
+        <v>159.0331579901501</v>
       </c>
       <c r="N9" t="n">
-        <v>406.7284208074865</v>
+        <v>450.4093979121987</v>
       </c>
       <c r="O9" t="n">
-        <v>431.3567274439047</v>
+        <v>483.1112423043464</v>
       </c>
       <c r="P9" t="n">
-        <v>468.6521909901581</v>
+        <v>525.3853716355027</v>
       </c>
     </row>
     <row r="10">
@@ -917,43 +917,43 @@
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>0</v>
+        <v>0.1011555095085142</v>
       </c>
       <c r="E10" t="n">
-        <v>0</v>
+        <v>0.4387898285311529</v>
       </c>
       <c r="F10" t="n">
-        <v>0.2481342040361893</v>
+        <v>1.075835412873501</v>
       </c>
       <c r="G10" t="n">
-        <v>0.8414521245050525</v>
+        <v>2.277807646338527</v>
       </c>
       <c r="H10" t="n">
-        <v>2.198749190439042</v>
+        <v>4.545678714799618</v>
       </c>
       <c r="I10" t="n">
-        <v>5.303754553730939</v>
+        <v>8.824678711609867</v>
       </c>
       <c r="J10" t="n">
-        <v>12.40688514175531</v>
+        <v>16.89825980152898</v>
       </c>
       <c r="K10" t="n">
-        <v>28.65628192123014</v>
+        <v>32.13142448114791</v>
       </c>
       <c r="L10" t="n">
-        <v>98.5694897895854</v>
+        <v>104.1951451497482</v>
       </c>
       <c r="M10" t="n">
-        <v>281.224839675843</v>
+        <v>306.7799637721929</v>
       </c>
       <c r="N10" t="n">
-        <v>787.0700502847226</v>
+        <v>878.9882653749007</v>
       </c>
       <c r="O10" t="n">
-        <v>660.0695857972041</v>
+        <v>735.6361924730203</v>
       </c>
       <c r="P10" t="n">
-        <v>582.2679910810317</v>
+        <v>640.0245012053052</v>
       </c>
     </row>
     <row r="11">
@@ -978,34 +978,34 @@
         <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>0</v>
+        <v>0.7334876076449184</v>
       </c>
       <c r="H11" t="n">
-        <v>0.6151326922629877</v>
+        <v>2.160787024931722</v>
       </c>
       <c r="I11" t="n">
-        <v>2.265141589553876</v>
+        <v>4.853803522629633</v>
       </c>
       <c r="J11" t="n">
-        <v>6.03976588084128</v>
+        <v>9.934964328159353</v>
       </c>
       <c r="K11" t="n">
-        <v>14.67474267628163</v>
+        <v>19.52205566373853</v>
       </c>
       <c r="L11" t="n">
-        <v>48.48416106569995</v>
+        <v>64.94047214352705</v>
       </c>
       <c r="M11" t="n">
-        <v>146.3536778286008</v>
+        <v>200.3241927329644</v>
       </c>
       <c r="N11" t="n">
-        <v>410.3330147680788</v>
+        <v>562.4956870568271</v>
       </c>
       <c r="O11" t="n">
-        <v>412.473144990007</v>
+        <v>548.4265248585019</v>
       </c>
       <c r="P11" t="n">
-        <v>410.9430474577998</v>
+        <v>544.5031877639265</v>
       </c>
     </row>
     <row r="12">
@@ -1021,43 +1021,43 @@
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>0.09142294107691123</v>
+        <v>0.1542678459405066</v>
       </c>
       <c r="E12" t="n">
-        <v>0.3795137674518616</v>
+        <v>0.4453391160261043</v>
       </c>
       <c r="F12" t="n">
-        <v>1.03856150538672</v>
+        <v>0.9945299325097688</v>
       </c>
       <c r="G12" t="n">
-        <v>2.546224648786345</v>
+        <v>2.030738531253633</v>
       </c>
       <c r="H12" t="n">
-        <v>5.995213277574135</v>
+        <v>3.985848172353506</v>
       </c>
       <c r="I12" t="n">
-        <v>13.88525331309844</v>
+        <v>7.674732546943149</v>
       </c>
       <c r="J12" t="n">
-        <v>31.93481463741522</v>
+        <v>14.66140288272231</v>
       </c>
       <c r="K12" t="n">
-        <v>63.15142106292861</v>
+        <v>27.76725191031598</v>
       </c>
       <c r="L12" t="n">
-        <v>191.1842042735653</v>
+        <v>89.88649356135896</v>
       </c>
       <c r="M12" t="n">
-        <v>462.808219637898</v>
+        <v>290.0742655147121</v>
       </c>
       <c r="N12" t="n">
-        <v>1011.266944619012</v>
+        <v>860.2163140250913</v>
       </c>
       <c r="O12" t="n">
-        <v>800.1667464948351</v>
+        <v>719.2381301111308</v>
       </c>
       <c r="P12" t="n">
-        <v>786.2009261776279</v>
+        <v>738.4008963942065</v>
       </c>
     </row>
     <row r="13">
@@ -1076,40 +1076,40 @@
         <v>0</v>
       </c>
       <c r="E13" t="n">
-        <v>0</v>
+        <v>0.2772013713479323</v>
       </c>
       <c r="F13" t="n">
-        <v>0</v>
+        <v>1.123563894555395</v>
       </c>
       <c r="G13" t="n">
-        <v>0.6632303722779802</v>
+        <v>2.720473562159445</v>
       </c>
       <c r="H13" t="n">
-        <v>2.180461872078013</v>
+        <v>5.733509249069449</v>
       </c>
       <c r="I13" t="n">
-        <v>5.651339443741183</v>
+        <v>11.41847956064264</v>
       </c>
       <c r="J13" t="n">
-        <v>13.59145347318375</v>
+        <v>22.14483357758193</v>
       </c>
       <c r="K13" t="n">
-        <v>31.75556600635521</v>
+        <v>42.38322783313097</v>
       </c>
       <c r="L13" t="n">
-        <v>114.7606369257039</v>
+        <v>138.1534845638089</v>
       </c>
       <c r="M13" t="n">
-        <v>313.2249811389905</v>
+        <v>381.1883384749701</v>
       </c>
       <c r="N13" t="n">
-        <v>707.3091414948265</v>
+        <v>857.6817300466716</v>
       </c>
       <c r="O13" t="n">
-        <v>811.0123715603531</v>
+        <v>938.9952609647501</v>
       </c>
       <c r="P13" t="n">
-        <v>911.6257361672576</v>
+        <v>1019.016489319038</v>
       </c>
     </row>
     <row r="14">
@@ -1125,43 +1125,43 @@
         <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>0.1522697642216801</v>
+        <v>1.238261891870587</v>
       </c>
       <c r="E14" t="n">
-        <v>0.713351025179813</v>
+        <v>5.417328880314932</v>
       </c>
       <c r="F14" t="n">
-        <v>3.526031554511345</v>
+        <v>13.73096391781231</v>
       </c>
       <c r="G14" t="n">
-        <v>11.86587667804315</v>
+        <v>30.15054796791167</v>
       </c>
       <c r="H14" t="n">
-        <v>31.63591461799753</v>
+        <v>61.17424180138279</v>
       </c>
       <c r="I14" t="n">
-        <v>77.10542701248559</v>
+        <v>119.7094855639594</v>
       </c>
       <c r="J14" t="n">
-        <v>181.1232455097217</v>
+        <v>230.1798040268351</v>
       </c>
       <c r="K14" t="n">
-        <v>409.0041683139708</v>
+        <v>438.5377271973533</v>
       </c>
       <c r="L14" t="n">
-        <v>1540.426029046655</v>
+        <v>1424.437744125627</v>
       </c>
       <c r="M14" t="n">
-        <v>4659.652636100112</v>
+        <v>4344.544758802609</v>
       </c>
       <c r="N14" t="n">
-        <v>12716.81056868639</v>
+        <v>12212.84719587053</v>
       </c>
       <c r="O14" t="n">
-        <v>14048.35448160847</v>
+        <v>13827.39415144247</v>
       </c>
       <c r="P14" t="n">
-        <v>14794.45418993903</v>
+        <v>14684.9530153164</v>
       </c>
     </row>
   </sheetData>
@@ -1248,43 +1248,43 @@
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>0.01216936462895377</v>
+        <v>0.01101913185289333</v>
       </c>
       <c r="E2" t="n">
-        <v>0.02783911008807399</v>
+        <v>0.02079080500611413</v>
       </c>
       <c r="F2" t="n">
-        <v>0.06368582700299399</v>
+        <v>0.03922791546311893</v>
       </c>
       <c r="G2" t="n">
-        <v>0.1456901656778454</v>
+        <v>0.07401489991027609</v>
       </c>
       <c r="H2" t="n">
-        <v>0.3332864684985589</v>
+        <v>0.139650688649991</v>
       </c>
       <c r="I2" t="n">
-        <v>0.7746084048169116</v>
+        <v>0.274510872895011</v>
       </c>
       <c r="J2" t="n">
-        <v>1.772024202934854</v>
+        <v>0.5179447987928169</v>
       </c>
       <c r="K2" t="n">
-        <v>4.053751232571633</v>
+        <v>1.015187933466584</v>
       </c>
       <c r="L2" t="n">
-        <v>13.18087626199051</v>
+        <v>2.271497438165975</v>
       </c>
       <c r="M2" t="n">
-        <v>44.5766563261198</v>
+        <v>7.451217592356535</v>
       </c>
       <c r="N2" t="n">
-        <v>129.1596147923544</v>
+        <v>24.81327667966593</v>
       </c>
       <c r="O2" t="n">
-        <v>59.46479286299235</v>
+        <v>74.36226680686001</v>
       </c>
       <c r="P2" t="n">
-        <v>190.5219176204048</v>
+        <v>137.7751259326255</v>
       </c>
     </row>
     <row r="3">
@@ -1300,43 +1300,43 @@
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>0.0008209619032002075</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>0.1560977812146878</v>
       </c>
       <c r="F3" t="n">
-        <v>0.06861271796901558</v>
+        <v>0.2945239765208442</v>
       </c>
       <c r="G3" t="n">
-        <v>0.2599364356679738</v>
+        <v>0.5557053538534771</v>
       </c>
       <c r="H3" t="n">
-        <v>0.5946406627709387</v>
+        <v>1.048500172886818</v>
       </c>
       <c r="I3" t="n">
-        <v>1.360323022480481</v>
+        <v>1.97912224138584</v>
       </c>
       <c r="J3" t="n">
-        <v>3.111927658743469</v>
+        <v>3.888739943425488</v>
       </c>
       <c r="K3" t="n">
-        <v>7.187579017307349</v>
+        <v>7.33724171401194</v>
       </c>
       <c r="L3" t="n">
-        <v>13.64911361801874</v>
+        <v>17.20063505524681</v>
       </c>
       <c r="M3" t="n">
-        <v>39.5244410203095</v>
+        <v>49.97208522554337</v>
       </c>
       <c r="N3" t="n">
-        <v>116.3055170167159</v>
+        <v>146.7543201391017</v>
       </c>
       <c r="O3" t="n">
-        <v>23.47841314328787</v>
+        <v>26.34821327265524</v>
       </c>
       <c r="P3" t="n">
-        <v>75.56874261406705</v>
+        <v>94.82193473222063</v>
       </c>
     </row>
     <row r="4">
@@ -1352,43 +1352,43 @@
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>0.001803037201454949</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>0.01812761595646386</v>
       </c>
       <c r="F4" t="n">
-        <v>0.003933830473084841</v>
+        <v>0.0342030328348964</v>
       </c>
       <c r="G4" t="n">
-        <v>0.02331939949650552</v>
+        <v>0.06453399376479298</v>
       </c>
       <c r="H4" t="n">
-        <v>0.0533463619149365</v>
+        <v>0.1217621949298391</v>
       </c>
       <c r="I4" t="n">
-        <v>0.1220372046881329</v>
+        <v>0.2315429192265556</v>
       </c>
       <c r="J4" t="n">
-        <v>0.2791770383862544</v>
+        <v>0.4515988869311694</v>
       </c>
       <c r="K4" t="n">
-        <v>0.6425900415957178</v>
+        <v>0.8520729694961222</v>
       </c>
       <c r="L4" t="n">
-        <v>2.111037921918221</v>
+        <v>1.99742876844837</v>
       </c>
       <c r="M4" t="n">
-        <v>5.789061904704134</v>
+        <v>6.494016095550691</v>
       </c>
       <c r="N4" t="n">
-        <v>11.80527458406953</v>
+        <v>13.02284016734327</v>
       </c>
       <c r="O4" t="n">
-        <v>3.248510661994942</v>
+        <v>4.144694118616285</v>
       </c>
       <c r="P4" t="n">
-        <v>7.957389121838602</v>
+        <v>8.124109260516244</v>
       </c>
     </row>
     <row r="5">
@@ -1404,43 +1404,43 @@
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>0.02864974281752266</v>
       </c>
       <c r="E5" t="n">
-        <v>0.005480619497096422</v>
+        <v>0.05405609301589675</v>
       </c>
       <c r="F5" t="n">
-        <v>0.03869740607374666</v>
+        <v>0.1019925802041092</v>
       </c>
       <c r="G5" t="n">
-        <v>0.08852568565878818</v>
+        <v>0.1924387397667178</v>
       </c>
       <c r="H5" t="n">
-        <v>0.2025147888833631</v>
+        <v>0.3630917904899764</v>
       </c>
       <c r="I5" t="n">
-        <v>0.4632806784976503</v>
+        <v>0.7137282695270286</v>
       </c>
       <c r="J5" t="n">
-        <v>1.065299451754613</v>
+        <v>1.346656476861323</v>
       </c>
       <c r="K5" t="n">
-        <v>2.46318003472579</v>
+        <v>2.540860078127922</v>
       </c>
       <c r="L5" t="n">
-        <v>8.011005198755146</v>
+        <v>5.955207613674132</v>
       </c>
       <c r="M5" t="n">
-        <v>24.34966436203866</v>
+        <v>19.37316574012699</v>
       </c>
       <c r="N5" t="n">
-        <v>70.96061498728365</v>
+        <v>60.84868739179885</v>
       </c>
       <c r="O5" t="n">
-        <v>28.07265797760181</v>
+        <v>25.15495187097093</v>
       </c>
       <c r="P5" t="n">
-        <v>49.57847275662824</v>
+        <v>39.29400691832382</v>
       </c>
     </row>
     <row r="6">
@@ -1456,43 +1456,43 @@
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>0.04958609333801998</v>
       </c>
       <c r="E6" t="n">
-        <v>0.02127835733146612</v>
+        <v>0.09355862252751362</v>
       </c>
       <c r="F6" t="n">
-        <v>0.08216097826663429</v>
+        <v>0.1765256195840351</v>
       </c>
       <c r="G6" t="n">
-        <v>0.1879546376206603</v>
+        <v>0.3330670495962424</v>
       </c>
       <c r="H6" t="n">
-        <v>0.4299723122632303</v>
+        <v>0.6284280989249593</v>
       </c>
       <c r="I6" t="n">
-        <v>0.9836213229604662</v>
+        <v>1.235298928027549</v>
       </c>
       <c r="J6" t="n">
-        <v>2.271448611062092</v>
+        <v>2.330751594567675</v>
       </c>
       <c r="K6" t="n">
-        <v>5.229737644798142</v>
+        <v>4.397642442913712</v>
       </c>
       <c r="L6" t="n">
-        <v>10.83959869623452</v>
+        <v>10.30709010058985</v>
       </c>
       <c r="M6" t="n">
-        <v>30.75719745197659</v>
+        <v>29.21966491391426</v>
       </c>
       <c r="N6" t="n">
-        <v>77.63022197934622</v>
+        <v>80.10695034923313</v>
       </c>
       <c r="O6" t="n">
-        <v>91.60031010304989</v>
+        <v>90.93915608027595</v>
       </c>
       <c r="P6" t="n">
-        <v>73.59842335364365</v>
+        <v>73.46513192919078</v>
       </c>
     </row>
     <row r="7">
@@ -1508,40 +1508,40 @@
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>0.02966021880000538</v>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>0.06376748007358599</v>
       </c>
       <c r="F7" t="n">
-        <v>0.02704141884503916</v>
+        <v>0.120315943364729</v>
       </c>
       <c r="G7" t="n">
-        <v>0.07619541849829545</v>
+        <v>0.2270111067747985</v>
       </c>
       <c r="H7" t="n">
-        <v>0.1743075919291674</v>
+        <v>0.4283226408564767</v>
       </c>
       <c r="I7" t="n">
-        <v>0.3987528017163504</v>
+        <v>0.8378157635957237</v>
       </c>
       <c r="J7" t="n">
-        <v>0.9122023608773893</v>
+        <v>1.588588543181739</v>
       </c>
       <c r="K7" t="n">
-        <v>2.113830887429639</v>
+        <v>2.997335459559469</v>
       </c>
       <c r="L7" t="n">
-        <v>6.896310608919118</v>
+        <v>7.025274778220184</v>
       </c>
       <c r="M7" t="n">
-        <v>19.49740049978983</v>
+        <v>20.61148817796314</v>
       </c>
       <c r="N7" t="n">
-        <v>56.82463918791484</v>
+        <v>60.00116200622848</v>
       </c>
       <c r="O7" t="n">
-        <v>85.94728032712766</v>
+        <v>85.99161618600436</v>
       </c>
       <c r="P7" t="n">
         <v>0</v>
@@ -1560,43 +1560,43 @@
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>0.07502852137121663</v>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>0.2274139847510885</v>
       </c>
       <c r="F8" t="n">
-        <v>0.09696753884158243</v>
+        <v>0.4290827876228576</v>
       </c>
       <c r="G8" t="n">
-        <v>0.3025318840872766</v>
+        <v>0.8095897833007872</v>
       </c>
       <c r="H8" t="n">
-        <v>0.6920836611485619</v>
+        <v>1.527527172218131</v>
       </c>
       <c r="I8" t="n">
-        <v>1.583237401485319</v>
+        <v>2.957153901401869</v>
       </c>
       <c r="J8" t="n">
-        <v>3.621875230087122</v>
+        <v>5.665383833860036</v>
       </c>
       <c r="K8" t="n">
-        <v>8.382509662854048</v>
+        <v>10.68939841605102</v>
       </c>
       <c r="L8" t="n">
-        <v>24.77114934052911</v>
+        <v>25.05565939363787</v>
       </c>
       <c r="M8" t="n">
-        <v>70.04533014343498</v>
+        <v>78.91776761210542</v>
       </c>
       <c r="N8" t="n">
-        <v>202.4551195919857</v>
+        <v>227.8125414805612</v>
       </c>
       <c r="O8" t="n">
-        <v>19.14010980751206</v>
+        <v>13.93728154583635</v>
       </c>
       <c r="P8" t="n">
-        <v>122.7301037416121</v>
+        <v>140.7443425131489</v>
       </c>
     </row>
     <row r="9">
@@ -1615,40 +1615,40 @@
         <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>0</v>
+        <v>0.02081962305228474</v>
       </c>
       <c r="F9" t="n">
-        <v>0</v>
+        <v>0.06033536709819126</v>
       </c>
       <c r="G9" t="n">
-        <v>0.03097311076972141</v>
+        <v>0.1138402615612075</v>
       </c>
       <c r="H9" t="n">
-        <v>0.08612576322515991</v>
+        <v>0.2147928449864793</v>
       </c>
       <c r="I9" t="n">
-        <v>0.1970246333272007</v>
+        <v>0.4052693276058599</v>
       </c>
       <c r="J9" t="n">
-        <v>0.4507211859038455</v>
+        <v>0.7854783709190696</v>
       </c>
       <c r="K9" t="n">
-        <v>1.031087250319591</v>
+        <v>1.503087040765057</v>
       </c>
       <c r="L9" t="n">
-        <v>3.406179159524162</v>
+        <v>3.52419745845118</v>
       </c>
       <c r="M9" t="n">
-        <v>9.654045624628123</v>
+        <v>11.43120522745154</v>
       </c>
       <c r="N9" t="n">
-        <v>29.31570687635845</v>
+        <v>31.84763583454274</v>
       </c>
       <c r="O9" t="n">
-        <v>8.99294305571795</v>
+        <v>10.74788578216613</v>
       </c>
       <c r="P9" t="n">
-        <v>23.21442260511864</v>
+        <v>25.86683346411277</v>
       </c>
     </row>
     <row r="10">
@@ -1664,43 +1664,43 @@
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>0</v>
+        <v>0.02023110190170283</v>
       </c>
       <c r="E10" t="n">
-        <v>0</v>
+        <v>0.06752686380452776</v>
       </c>
       <c r="F10" t="n">
-        <v>0.04962684080723786</v>
+        <v>0.1274091168684697</v>
       </c>
       <c r="G10" t="n">
-        <v>0.1186635840937726</v>
+        <v>0.2403944466930051</v>
       </c>
       <c r="H10" t="n">
-        <v>0.2714594131867978</v>
+        <v>0.4535742136922183</v>
       </c>
       <c r="I10" t="n">
-        <v>0.6210010726583794</v>
+        <v>0.8760311012637527</v>
       </c>
       <c r="J10" t="n">
-        <v>1.420626117604874</v>
+        <v>1.682243081788349</v>
       </c>
       <c r="K10" t="n">
-        <v>3.299506196702204</v>
+        <v>3.174042052792257</v>
       </c>
       <c r="L10" t="n">
-        <v>7.118517432179113</v>
+        <v>7.439962843629591</v>
       </c>
       <c r="M10" t="n">
-        <v>18.99905690765286</v>
+        <v>21.23045173674648</v>
       </c>
       <c r="N10" t="n">
-        <v>56.14868940472984</v>
+        <v>62.94839337892879</v>
       </c>
       <c r="O10" t="n">
-        <v>0.35874072116415</v>
+        <v>0</v>
       </c>
       <c r="P10" t="n">
-        <v>29.7937136845741</v>
+        <v>32.52825343106613</v>
       </c>
     </row>
     <row r="11">
@@ -1725,34 +1725,34 @@
         <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>0</v>
+        <v>0.1466975215289837</v>
       </c>
       <c r="H11" t="n">
-        <v>0.1230265384525975</v>
+        <v>0.2854598834573609</v>
       </c>
       <c r="I11" t="n">
-        <v>0.3300017794581777</v>
+        <v>0.5386032995395821</v>
       </c>
       <c r="J11" t="n">
-        <v>0.7549248582574809</v>
+        <v>1.016232161105944</v>
       </c>
       <c r="K11" t="n">
-        <v>1.72699535908807</v>
+        <v>1.917418267115837</v>
       </c>
       <c r="L11" t="n">
-        <v>3.411698473554981</v>
+        <v>4.686555379607684</v>
       </c>
       <c r="M11" t="n">
-        <v>10.17144041519669</v>
+        <v>14.13309671985435</v>
       </c>
       <c r="N11" t="n">
-        <v>29.1560118248337</v>
+        <v>39.77319429602451</v>
       </c>
       <c r="O11" t="n">
-        <v>7.005582466568661</v>
+        <v>8.002909829898504</v>
       </c>
       <c r="P11" t="n">
-        <v>19.51071636679448</v>
+        <v>26.56081179848189</v>
       </c>
     </row>
     <row r="12">
@@ -1768,43 +1768,43 @@
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>0.01828458821538225</v>
+        <v>0.03085356918810132</v>
       </c>
       <c r="E12" t="n">
-        <v>0.05761816527499006</v>
+        <v>0.05821425401711954</v>
       </c>
       <c r="F12" t="n">
-        <v>0.1318095475869716</v>
+        <v>0.1098381632967329</v>
       </c>
       <c r="G12" t="n">
-        <v>0.3015326286799251</v>
+        <v>0.207241719748773</v>
       </c>
       <c r="H12" t="n">
-        <v>0.689797725757558</v>
+        <v>0.3910219282199746</v>
       </c>
       <c r="I12" t="n">
-        <v>1.596292595320244</v>
+        <v>0.76863044410603</v>
       </c>
       <c r="J12" t="n">
-        <v>3.667530430138346</v>
+        <v>1.565386484469686</v>
       </c>
       <c r="K12" t="n">
-        <v>6.375130832689647</v>
+        <v>2.621169805518732</v>
       </c>
       <c r="L12" t="n">
-        <v>13.12649406684302</v>
+        <v>6.413300507033679</v>
       </c>
       <c r="M12" t="n">
-        <v>29.04987987306738</v>
+        <v>21.08673122979906</v>
       </c>
       <c r="N12" t="n">
-        <v>65.51356755541229</v>
+        <v>61.72824991919323</v>
       </c>
       <c r="O12" t="n">
         <v>0</v>
       </c>
       <c r="P12" t="n">
-        <v>45.86852104358033</v>
+        <v>43.14986594131388</v>
       </c>
     </row>
     <row r="13">
@@ -1823,40 +1823,40 @@
         <v>0</v>
       </c>
       <c r="E13" t="n">
-        <v>0</v>
+        <v>0.05544027426958647</v>
       </c>
       <c r="F13" t="n">
-        <v>0</v>
+        <v>0.1692725046414925</v>
       </c>
       <c r="G13" t="n">
-        <v>0.132646074455596</v>
+        <v>0.3193819335208101</v>
       </c>
       <c r="H13" t="n">
-        <v>0.3034462999600065</v>
+        <v>0.6026071373820008</v>
       </c>
       <c r="I13" t="n">
-        <v>0.694175514332634</v>
+        <v>1.136994062314638</v>
       </c>
       <c r="J13" t="n">
-        <v>1.588022805888514</v>
+        <v>2.200711077657445</v>
       </c>
       <c r="K13" t="n">
-        <v>3.632822506634292</v>
+        <v>4.216951355751301</v>
       </c>
       <c r="L13" t="n">
-        <v>8.44269170415267</v>
+        <v>9.887368424173694</v>
       </c>
       <c r="M13" t="n">
-        <v>20.66638945495711</v>
+        <v>25.5728119760333</v>
       </c>
       <c r="N13" t="n">
-        <v>45.84317884244919</v>
+        <v>55.25167681654703</v>
       </c>
       <c r="O13" t="n">
-        <v>24.92486358610756</v>
+        <v>25.86144329191133</v>
       </c>
       <c r="P13" t="n">
-        <v>43.31612060939361</v>
+        <v>48.41436723171896</v>
       </c>
     </row>
     <row r="14">
@@ -1872,43 +1872,43 @@
         <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>0.03045395284433601</v>
+        <v>0.2476523783741173</v>
       </c>
       <c r="E14" t="n">
-        <v>0.1122162521916266</v>
+        <v>0.8358133976888693</v>
       </c>
       <c r="F14" t="n">
-        <v>0.5625361058663063</v>
+        <v>1.662727007499476</v>
       </c>
       <c r="G14" t="n">
-        <v>1.66796902470636</v>
+        <v>3.283916810019871</v>
       </c>
       <c r="H14" t="n">
-        <v>3.954007587990877</v>
+        <v>6.204738766694224</v>
       </c>
       <c r="I14" t="n">
-        <v>9.124356431741948</v>
+        <v>11.95470113088944</v>
       </c>
       <c r="J14" t="n">
-        <v>20.91577995163885</v>
+        <v>23.03971525356074</v>
       </c>
       <c r="K14" t="n">
-        <v>46.13872066671613</v>
+        <v>43.26240753556995</v>
       </c>
       <c r="L14" t="n">
-        <v>114.9646724826193</v>
+        <v>101.764177760879</v>
       </c>
       <c r="M14" t="n">
-        <v>323.0805639838757</v>
+        <v>305.4937022474451</v>
       </c>
       <c r="N14" t="n">
-        <v>891.1181566434537</v>
+        <v>864.9089284591688</v>
       </c>
       <c r="O14" t="n">
-        <v>352.2342047131249</v>
+        <v>365.4904187851951</v>
       </c>
       <c r="P14" t="n">
-        <v>681.6585435176556</v>
+        <v>670.7447831527196</v>
       </c>
     </row>
   </sheetData>
@@ -1995,43 +1995,43 @@
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>36.334802134545</v>
+        <v>32.90048312109479</v>
       </c>
       <c r="E2" t="n">
-        <v>70.65276613608263</v>
+        <v>52.76490086179703</v>
       </c>
       <c r="F2" t="n">
-        <v>142.6129461243445</v>
+        <v>87.84385565487148</v>
       </c>
       <c r="G2" t="n">
-        <v>282.7473148982843</v>
+        <v>143.6439729114689</v>
       </c>
       <c r="H2" t="n">
-        <v>587.1169096487118</v>
+        <v>246.0084296847223</v>
       </c>
       <c r="I2" t="n">
-        <v>1202.653291198394</v>
+        <v>677.0039933181038</v>
       </c>
       <c r="J2" t="n">
-        <v>4023.975235739762</v>
+        <v>1414.766269697059</v>
       </c>
       <c r="K2" t="n">
-        <v>7434.672826436908</v>
+        <v>2546.619742453563</v>
       </c>
       <c r="L2" t="n">
-        <v>16377.78453455448</v>
+        <v>5191.600299173556</v>
       </c>
       <c r="M2" t="n">
-        <v>53238.07895691019</v>
+        <v>14693.58382533309</v>
       </c>
       <c r="N2" t="n">
-        <v>154748.6060318575</v>
+        <v>32779.51982619567</v>
       </c>
       <c r="O2" t="n">
-        <v>69243.56397605714</v>
+        <v>86604.86070963995</v>
       </c>
       <c r="P2" t="n">
-        <v>221899.9985072915</v>
+        <v>162420.2364525321</v>
       </c>
     </row>
     <row r="3">
@@ -2047,43 +2047,43 @@
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>2.23585771271615</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>361.3572843030948</v>
       </c>
       <c r="F3" t="n">
-        <v>140.1480452961073</v>
+        <v>601.5934191802884</v>
       </c>
       <c r="G3" t="n">
-        <v>460.1523815601393</v>
+        <v>983.7372023829084</v>
       </c>
       <c r="H3" t="n">
-        <v>955.4935802883662</v>
+        <v>1684.774094418956</v>
       </c>
       <c r="I3" t="n">
-        <v>1926.489072228524</v>
+        <v>2802.832347630103</v>
       </c>
       <c r="J3" t="n">
-        <v>4152.854646172969</v>
+        <v>5189.507441292425</v>
       </c>
       <c r="K3" t="n">
-        <v>8808.790960374134</v>
+        <v>8992.211192229963</v>
       </c>
       <c r="L3" t="n">
-        <v>15240.85964599142</v>
+        <v>19206.55597392482</v>
       </c>
       <c r="M3" t="n">
-        <v>43057.30921328883</v>
+        <v>54438.80976035608</v>
       </c>
       <c r="N3" t="n">
-        <v>126701.4151275895</v>
+        <v>159871.8660529156</v>
       </c>
       <c r="O3" t="n">
-        <v>24937.59144317116</v>
+        <v>27985.74903001313</v>
       </c>
       <c r="P3" t="n">
-        <v>80265.32362654642</v>
+        <v>100715.097471533</v>
       </c>
     </row>
     <row r="4">
@@ -2099,43 +2099,43 @@
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>5.761789645054906</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>49.23935199435816</v>
       </c>
       <c r="F4" t="n">
-        <v>9.428217981414186</v>
+        <v>81.97446519346113</v>
       </c>
       <c r="G4" t="n">
-        <v>48.43769079508581</v>
+        <v>134.0462320318094</v>
       </c>
       <c r="H4" t="n">
-        <v>100.5795133381236</v>
+        <v>229.5710873133782</v>
       </c>
       <c r="I4" t="n">
-        <v>202.7908269959074</v>
+        <v>384.7579121055185</v>
       </c>
       <c r="J4" t="n">
-        <v>437.1479912507461</v>
+        <v>707.133894012802</v>
       </c>
       <c r="K4" t="n">
-        <v>924.057967363217</v>
+        <v>1225.29881459491</v>
       </c>
       <c r="L4" t="n">
-        <v>2765.875344055415</v>
+        <v>2617.024983207448</v>
       </c>
       <c r="M4" t="n">
-        <v>7399.815580108991</v>
+        <v>8300.916844970328</v>
       </c>
       <c r="N4" t="n">
-        <v>15089.98456618284</v>
+        <v>16646.32666810305</v>
       </c>
       <c r="O4" t="n">
-        <v>4048.569647271489</v>
+        <v>5165.469518745473</v>
       </c>
       <c r="P4" t="n">
-        <v>9917.173567292499</v>
+        <v>10124.95435155647</v>
       </c>
     </row>
     <row r="5">
@@ -2151,43 +2151,43 @@
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>91.55318113585399</v>
       </c>
       <c r="E5" t="n">
-        <v>14.88679775723331</v>
+        <v>146.830504234089</v>
       </c>
       <c r="F5" t="n">
-        <v>92.74613694587546</v>
+        <v>244.4457851527939</v>
       </c>
       <c r="G5" t="n">
-        <v>183.8803692181658</v>
+        <v>399.7224789263154</v>
       </c>
       <c r="H5" t="n">
-        <v>381.8224557119877</v>
+        <v>684.5751851416247</v>
       </c>
       <c r="I5" t="n">
-        <v>769.8395924738792</v>
+        <v>1186.011646182998</v>
       </c>
       <c r="J5" t="n">
-        <v>1668.093902374384</v>
+        <v>2108.655415099923</v>
       </c>
       <c r="K5" t="n">
-        <v>3542.104590488475</v>
+        <v>3653.810123354515</v>
       </c>
       <c r="L5" t="n">
-        <v>10495.99418858519</v>
+        <v>7802.494562686706</v>
       </c>
       <c r="M5" t="n">
-        <v>31124.73638781154</v>
+        <v>24763.57241288684</v>
       </c>
       <c r="N5" t="n">
-        <v>90704.75890581335</v>
+        <v>77779.27968348903</v>
       </c>
       <c r="O5" t="n">
-        <v>34986.52854553245</v>
+        <v>31350.23560638283</v>
       </c>
       <c r="P5" t="n">
-        <v>61788.89985150804</v>
+        <v>48971.52581038671</v>
       </c>
     </row>
     <row r="6">
@@ -2203,43 +2203,43 @@
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>148.0521740449266</v>
       </c>
       <c r="E6" t="n">
-        <v>54.00225795809853</v>
+        <v>237.4420538780867</v>
       </c>
       <c r="F6" t="n">
-        <v>183.9847218520395</v>
+        <v>395.2973504469215</v>
       </c>
       <c r="G6" t="n">
-        <v>364.7718352344709</v>
+        <v>646.3978781016099</v>
       </c>
       <c r="H6" t="n">
-        <v>757.4385373272069</v>
+        <v>1107.03793358125</v>
       </c>
       <c r="I6" t="n">
-        <v>1807.196151770621</v>
+        <v>2186.948131479051</v>
       </c>
       <c r="J6" t="n">
-        <v>4097.201150952627</v>
+        <v>4176.461203786987</v>
       </c>
       <c r="K6" t="n">
-        <v>7180.252736198318</v>
+        <v>6219.588598750239</v>
       </c>
       <c r="L6" t="n">
-        <v>13269.42048334036</v>
+        <v>12617.54390888223</v>
       </c>
       <c r="M6" t="n">
-        <v>36801.72767432078</v>
+        <v>34934.55213132688</v>
       </c>
       <c r="N6" t="n">
-        <v>92822.14230213036</v>
+        <v>95833.45597825578</v>
       </c>
       <c r="O6" t="n">
-        <v>106663.6513383801</v>
+        <v>105893.7729167154</v>
       </c>
       <c r="P6" t="n">
-        <v>85711.58335285266</v>
+        <v>85557.66680171025</v>
       </c>
     </row>
     <row r="7">
@@ -2255,40 +2255,40 @@
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>99.45016813041953</v>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>181.7395097026266</v>
       </c>
       <c r="F7" t="n">
-        <v>68.00203503447565</v>
+        <v>302.5628589527674</v>
       </c>
       <c r="G7" t="n">
-        <v>166.0631939530453</v>
+        <v>494.7566428115647</v>
       </c>
       <c r="H7" t="n">
-        <v>344.8255884416824</v>
+        <v>847.3331829186695</v>
       </c>
       <c r="I7" t="n">
-        <v>695.2456213857411</v>
+        <v>1460.774040108754</v>
       </c>
       <c r="J7" t="n">
-        <v>1498.712892081589</v>
+        <v>2609.98900242881</v>
       </c>
       <c r="K7" t="n">
-        <v>3189.43623974045</v>
+        <v>4522.504801224916</v>
       </c>
       <c r="L7" t="n">
-        <v>9480.513080704442</v>
+        <v>9657.803020693467</v>
       </c>
       <c r="M7" t="n">
-        <v>26149.77011308997</v>
+        <v>27643.97631100707</v>
       </c>
       <c r="N7" t="n">
-        <v>76212.78803496259</v>
+        <v>80473.11707004509</v>
       </c>
       <c r="O7" t="n">
-        <v>112390.06358121</v>
+        <v>112448.0399357743</v>
       </c>
       <c r="P7" t="n">
         <v>0</v>
@@ -2307,43 +2307,43 @@
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>264.8498854381823</v>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>682.3536130188461</v>
       </c>
       <c r="F8" t="n">
-        <v>256.7207884820584</v>
+        <v>1135.993270310602</v>
       </c>
       <c r="G8" t="n">
-        <v>694.1573243801578</v>
+        <v>1857.598181814983</v>
       </c>
       <c r="H8" t="n">
-        <v>1441.39831441621</v>
+        <v>3181.371292028729</v>
       </c>
       <c r="I8" t="n">
-        <v>2906.181850655029</v>
+        <v>5428.135407731846</v>
       </c>
       <c r="J8" t="n">
-        <v>6264.738780560626</v>
+        <v>9799.385002528225</v>
       </c>
       <c r="K8" t="n">
-        <v>13315.57662996108</v>
+        <v>16980.05841470751</v>
       </c>
       <c r="L8" t="n">
-        <v>35851.17682575743</v>
+        <v>36262.94698960765</v>
       </c>
       <c r="M8" t="n">
-        <v>98903.70928240292</v>
+        <v>111431.5533832266</v>
       </c>
       <c r="N8" t="n">
-        <v>285865.770778105</v>
+        <v>321670.3430098767</v>
       </c>
       <c r="O8" t="n">
-        <v>26350.11007664648</v>
+        <v>19187.39790917316</v>
       </c>
       <c r="P8" t="n">
-        <v>168962.0266462875</v>
+        <v>193762.1547203013</v>
       </c>
     </row>
     <row r="9">
@@ -2362,40 +2362,40 @@
         <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>0</v>
+        <v>66.76360867424565</v>
       </c>
       <c r="F9" t="n">
-        <v>0</v>
+        <v>170.7187561653825</v>
       </c>
       <c r="G9" t="n">
-        <v>75.95322124027602</v>
+        <v>279.1626142008936</v>
       </c>
       <c r="H9" t="n">
-        <v>191.7048543490229</v>
+        <v>478.1012036514097</v>
       </c>
       <c r="I9" t="n">
-        <v>386.5199250057692</v>
+        <v>795.051194706269</v>
       </c>
       <c r="J9" t="n">
-        <v>1006.51794399316</v>
+        <v>1452.039149273602</v>
       </c>
       <c r="K9" t="n">
-        <v>1750.475132630677</v>
+        <v>2551.788402216336</v>
       </c>
       <c r="L9" t="n">
-        <v>5268.650122728573</v>
+        <v>5451.199864243907</v>
       </c>
       <c r="M9" t="n">
-        <v>14575.56900008318</v>
+        <v>17250.43409206005</v>
       </c>
       <c r="N9" t="n">
-        <v>44257.68788587421</v>
+        <v>48060.15918884776</v>
       </c>
       <c r="O9" t="n">
-        <v>13231.66404415296</v>
+        <v>15813.77897907715</v>
       </c>
       <c r="P9" t="n">
-        <v>34183.67359734662</v>
+        <v>38066.57353476624</v>
       </c>
     </row>
     <row r="10">
@@ -2411,43 +2411,43 @@
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>0</v>
+        <v>57.22125594118082</v>
       </c>
       <c r="E10" t="n">
-        <v>0</v>
+        <v>162.342920278014</v>
       </c>
       <c r="F10" t="n">
-        <v>105.2726949765467</v>
+        <v>270.2711048930888</v>
       </c>
       <c r="G10" t="n">
-        <v>218.1567557247811</v>
+        <v>441.9525415931881</v>
       </c>
       <c r="H10" t="n">
-        <v>452.9964158499586</v>
+        <v>756.8994963646771</v>
       </c>
       <c r="I10" t="n">
-        <v>913.3422378727612</v>
+        <v>1288.42966896859</v>
       </c>
       <c r="J10" t="n">
-        <v>1968.854955251977</v>
+        <v>2331.431603623775</v>
       </c>
       <c r="K10" t="n">
-        <v>4199.516678095668</v>
+        <v>4039.829520853947</v>
       </c>
       <c r="L10" t="n">
-        <v>8254.889380415776</v>
+        <v>8627.649065089841</v>
       </c>
       <c r="M10" t="n">
-        <v>21494.62551740417</v>
+        <v>24019.11904705509</v>
       </c>
       <c r="N10" t="n">
-        <v>63523.94531549441</v>
+        <v>71216.80561193044</v>
       </c>
       <c r="O10" t="n">
-        <v>395.7155641634444</v>
+        <v>0</v>
       </c>
       <c r="P10" t="n">
-        <v>32864.50498553986</v>
+        <v>35880.88945117546</v>
       </c>
     </row>
     <row r="11">
@@ -2472,34 +2472,34 @@
         <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>0</v>
+        <v>259.6912346168967</v>
       </c>
       <c r="H11" t="n">
-        <v>197.6842067086128</v>
+        <v>458.6889245050525</v>
       </c>
       <c r="I11" t="n">
-        <v>467.3484249225582</v>
+        <v>762.7698375178528</v>
       </c>
       <c r="J11" t="n">
-        <v>1007.44411468483</v>
+        <v>1356.15763431444</v>
       </c>
       <c r="K11" t="n">
-        <v>2116.532016011443</v>
+        <v>2349.906228224493</v>
       </c>
       <c r="L11" t="n">
-        <v>3809.567349578732</v>
+        <v>5233.096797543903</v>
       </c>
       <c r="M11" t="n">
-        <v>11080.60844874758</v>
+        <v>15396.37499984868</v>
       </c>
       <c r="N11" t="n">
-        <v>31762.10426159089</v>
+        <v>43328.29714970964</v>
       </c>
       <c r="O11" t="n">
-        <v>7440.977901978752</v>
+        <v>8500.288945277476</v>
       </c>
       <c r="P11" t="n">
-        <v>20723.30316999345</v>
+        <v>28211.56050824761</v>
       </c>
     </row>
     <row r="12">
@@ -2515,43 +2515,43 @@
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>51.71577441184373</v>
+        <v>87.26563623618927</v>
       </c>
       <c r="E12" t="n">
-        <v>138.521185270505</v>
+        <v>139.9542562246407</v>
       </c>
       <c r="F12" t="n">
-        <v>279.6056745182967</v>
+        <v>232.9980968652488</v>
       </c>
       <c r="G12" t="n">
-        <v>554.351872314884</v>
+        <v>381.0029974780548</v>
       </c>
       <c r="H12" t="n">
-        <v>1151.096194312496</v>
+        <v>652.5157109969133</v>
       </c>
       <c r="I12" t="n">
-        <v>2347.759956465571</v>
+        <v>2110.614994572949</v>
       </c>
       <c r="J12" t="n">
-        <v>5638.211169407834</v>
+        <v>4050.473109375884</v>
       </c>
       <c r="K12" t="n">
-        <v>8114.083338797996</v>
+        <v>6096.845355843755</v>
       </c>
       <c r="L12" t="n">
-        <v>15221.95562585042</v>
+        <v>7437.09441654358</v>
       </c>
       <c r="M12" t="n">
-        <v>32888.02787910107</v>
+        <v>23856.52053013808</v>
       </c>
       <c r="N12" t="n">
-        <v>74177.80009229733</v>
+        <v>70686.61735953824</v>
       </c>
       <c r="O12" t="n">
         <v>0</v>
       </c>
       <c r="P12" t="n">
-        <v>50600.80130804253</v>
+        <v>47646.2613771669</v>
       </c>
     </row>
     <row r="13">
@@ -2570,40 +2570,40 @@
         <v>0</v>
       </c>
       <c r="E13" t="n">
-        <v>0</v>
+        <v>172.8395956577657</v>
       </c>
       <c r="F13" t="n">
-        <v>0</v>
+        <v>465.636085440869</v>
       </c>
       <c r="G13" t="n">
-        <v>316.2326478094794</v>
+        <v>761.4171389113128</v>
       </c>
       <c r="H13" t="n">
-        <v>656.6482690692304</v>
+        <v>1304.02293171084</v>
       </c>
       <c r="I13" t="n">
-        <v>1323.949988526208</v>
+        <v>2168.505291061753</v>
       </c>
       <c r="J13" t="n">
-        <v>2853.985491229149</v>
+        <v>3955.105344036573</v>
       </c>
       <c r="K13" t="n">
-        <v>5995.917368883907</v>
+        <v>6960.013001326932</v>
       </c>
       <c r="L13" t="n">
-        <v>12695.90702363262</v>
+        <v>14868.37546845003</v>
       </c>
       <c r="M13" t="n">
-        <v>30319.60551855663</v>
+        <v>37517.80507202096</v>
       </c>
       <c r="N13" t="n">
-        <v>67256.40689435008</v>
+        <v>81059.58948309015</v>
       </c>
       <c r="O13" t="n">
-        <v>35653.02165393562</v>
+        <v>36992.72393219684</v>
       </c>
       <c r="P13" t="n">
-        <v>61960.24225833581</v>
+        <v>69252.8758406589</v>
       </c>
     </row>
     <row r="14">
@@ -2619,43 +2619,43 @@
         <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>88.05057654638873</v>
+        <v>789.2904314056183</v>
       </c>
       <c r="E14" t="n">
-        <v>278.0630071219195</v>
+        <v>2253.627598827564</v>
       </c>
       <c r="F14" t="n">
-        <v>1278.521261211158</v>
+        <v>3989.335048256295</v>
       </c>
       <c r="G14" t="n">
-        <v>3364.90460712877</v>
+        <v>6783.129115781006</v>
       </c>
       <c r="H14" t="n">
-        <v>7218.804839461611</v>
+        <v>11630.89947231622</v>
       </c>
       <c r="I14" t="n">
-        <v>14949.31693950096</v>
+        <v>21251.83446538378</v>
       </c>
       <c r="J14" t="n">
-        <v>34617.73827369965</v>
+        <v>39151.1050694705</v>
       </c>
       <c r="K14" t="n">
-        <v>66571.41648498227</v>
+        <v>66138.47419578109</v>
       </c>
       <c r="L14" t="n">
-        <v>148732.5936051948</v>
+        <v>134973.3853500471</v>
       </c>
       <c r="M14" t="n">
-        <v>407033.5835718259</v>
+        <v>394247.2184102298</v>
       </c>
       <c r="N14" t="n">
-        <v>1123123.410196248</v>
+        <v>1099405.377081997</v>
       </c>
       <c r="O14" t="n">
-        <v>435341.4577724996</v>
+        <v>449942.3174829958</v>
       </c>
       <c r="P14" t="n">
-        <v>828877.5308710368</v>
+        <v>820609.796320035</v>
       </c>
     </row>
   </sheetData>
@@ -2730,43 +2730,43 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.05556787446237497</v>
+        <v>0.05031567005800005</v>
       </c>
       <c r="C2" t="n">
-        <v>0.1826870973376393</v>
+        <v>0.1452508517849684</v>
       </c>
       <c r="D2" t="n">
-        <v>0.4734899574569805</v>
+        <v>0.3243737516518167</v>
       </c>
       <c r="E2" t="n">
-        <v>1.138741848876815</v>
+        <v>0.6623413277711184</v>
       </c>
       <c r="F2" t="n">
-        <v>2.66059785419962</v>
+        <v>1.300015698791594</v>
       </c>
       <c r="G2" t="n">
-        <v>6.142054623896273</v>
+        <v>2.503174321655522</v>
       </c>
       <c r="H2" t="n">
-        <v>14.10637003670417</v>
+        <v>4.773283859624302</v>
       </c>
       <c r="I2" t="n">
-        <v>32.32584659226574</v>
+        <v>9.056507381814567</v>
       </c>
       <c r="J2" t="n">
-        <v>151.2729646907119</v>
+        <v>29.31718612605808</v>
       </c>
       <c r="K2" t="n">
-        <v>546.5674472957708</v>
+        <v>94.6100008525667</v>
       </c>
       <c r="L2" t="n">
-        <v>1646.81924608404</v>
+        <v>305.0250470968311</v>
       </c>
       <c r="M2" t="n">
-        <v>1926.143686842733</v>
+        <v>939.7365411296132</v>
       </c>
       <c r="N2" t="n">
-        <v>2872.753559213782</v>
+        <v>2050.63040030939</v>
       </c>
     </row>
     <row r="3">
@@ -2776,43 +2776,43 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>0.003748684452011819</v>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>0.7165239340123314</v>
       </c>
       <c r="D3" t="n">
-        <v>0.3133000789172986</v>
+        <v>2.061382260841575</v>
       </c>
       <c r="E3" t="n">
-        <v>1.500224430828757</v>
+        <v>4.59884960466086</v>
       </c>
       <c r="F3" t="n">
-        <v>4.215478571580045</v>
+        <v>9.386521579098375</v>
       </c>
       <c r="G3" t="n">
-        <v>10.42699916006064</v>
+        <v>18.4198606644848</v>
       </c>
       <c r="H3" t="n">
-        <v>24.63671435469166</v>
+        <v>35.46388863199337</v>
       </c>
       <c r="I3" t="n">
-        <v>57.14340946039334</v>
+        <v>67.62241679210258</v>
       </c>
       <c r="J3" t="n">
-        <v>179.2482962255729</v>
+        <v>219.7745370523016</v>
       </c>
       <c r="K3" t="n">
-        <v>525.5280866320961</v>
+        <v>655.8312822421666</v>
       </c>
       <c r="L3" t="n">
-        <v>1485.429344470224</v>
+        <v>1875.12987067581</v>
       </c>
       <c r="M3" t="n">
-        <v>1457.042457303169</v>
+        <v>1809.028073457925</v>
       </c>
       <c r="N3" t="n">
-        <v>1435.615641038481</v>
+        <v>1776.687727205056</v>
       </c>
     </row>
     <row r="4">
@@ -2822,43 +2822,43 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
+        <v>0.008233046499655602</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>0.09100754775622043</v>
       </c>
       <c r="D4" t="n">
-        <v>0.01796269604450473</v>
+        <v>0.2471857783172527</v>
       </c>
       <c r="E4" t="n">
-        <v>0.1244439712194432</v>
+        <v>0.5418615459859881</v>
       </c>
       <c r="F4" t="n">
-        <v>0.3680346624590454</v>
+        <v>1.097853298096569</v>
       </c>
       <c r="G4" t="n">
-        <v>0.9252821668780447</v>
+        <v>2.146893844798404</v>
       </c>
       <c r="H4" t="n">
-        <v>2.200063151327743</v>
+        <v>4.126214697035813</v>
       </c>
       <c r="I4" t="n">
-        <v>5.11630152911802</v>
+        <v>7.86078058051767</v>
       </c>
       <c r="J4" t="n">
-        <v>24.16690984720768</v>
+        <v>25.5294673703469</v>
       </c>
       <c r="K4" t="n">
-        <v>75.71862122470215</v>
+        <v>82.46923269567216</v>
       </c>
       <c r="L4" t="n">
-        <v>170.3183129062486</v>
+        <v>187.3568076891547</v>
       </c>
       <c r="M4" t="n">
-        <v>163.9115618167432</v>
+        <v>186.4341746994472</v>
       </c>
       <c r="N4" t="n">
-        <v>156.2423461624012</v>
+        <v>171.508888356182</v>
       </c>
     </row>
     <row r="5">
@@ -2868,43 +2868,43 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
+        <v>0.1308207421508001</v>
       </c>
       <c r="C5" t="n">
-        <v>0.02502565955383665</v>
+        <v>0.377652214640918</v>
       </c>
       <c r="D5" t="n">
-        <v>0.2017261421418393</v>
+        <v>0.8433717542947233</v>
       </c>
       <c r="E5" t="n">
-        <v>0.6059530132538544</v>
+        <v>1.722087452204908</v>
       </c>
       <c r="F5" t="n">
-        <v>1.530678067400955</v>
+        <v>3.380040816858143</v>
       </c>
       <c r="G5" t="n">
-        <v>3.646114934363711</v>
+        <v>6.508253236304355</v>
       </c>
       <c r="H5" t="n">
-        <v>8.485470284406304</v>
+        <v>12.41053803502318</v>
       </c>
       <c r="I5" t="n">
-        <v>19.55616710818355</v>
+        <v>23.54691919271787</v>
       </c>
       <c r="J5" t="n">
-        <v>91.84944180721345</v>
+        <v>76.22468392775099</v>
       </c>
       <c r="K5" t="n">
-        <v>309.210813721548</v>
+        <v>245.9860022166734</v>
       </c>
       <c r="L5" t="n">
-        <v>906.9934333839457</v>
+        <v>759.812384536697</v>
       </c>
       <c r="M5" t="n">
-        <v>1015.599123596564</v>
+        <v>873.8832984103292</v>
       </c>
       <c r="N5" t="n">
-        <v>1033.163809100982</v>
+        <v>866.4228450818368</v>
       </c>
     </row>
     <row r="6">
@@ -2914,43 +2914,43 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0</v>
+        <v>0.2264205152610002</v>
       </c>
       <c r="C6" t="n">
-        <v>0.09716144803051388</v>
+        <v>0.6536288330323581</v>
       </c>
       <c r="D6" t="n">
-        <v>0.472325728601402</v>
+        <v>1.459681882433175</v>
       </c>
       <c r="E6" t="n">
-        <v>1.330566074451237</v>
+        <v>2.980535974970033</v>
       </c>
       <c r="F6" t="n">
-        <v>3.293909946430722</v>
+        <v>5.850070644562171</v>
       </c>
       <c r="G6" t="n">
-        <v>7.785331467546031</v>
+        <v>11.26428444744985</v>
       </c>
       <c r="H6" t="n">
-        <v>18.06008138183335</v>
+        <v>21.47977736830935</v>
       </c>
       <c r="I6" t="n">
-        <v>41.56499743231618</v>
+        <v>40.75428321816555</v>
       </c>
       <c r="J6" t="n">
-        <v>138.7168530759426</v>
+        <v>131.9273375672613</v>
       </c>
       <c r="K6" t="n">
-        <v>408.9454490920587</v>
+        <v>386.37683754813</v>
       </c>
       <c r="L6" t="n">
-        <v>1039.335320925734</v>
+        <v>1045.480905649687</v>
       </c>
       <c r="M6" t="n">
-        <v>1685.605174588491</v>
+        <v>1694.949372873396</v>
       </c>
       <c r="N6" t="n">
-        <v>1863.129196814246</v>
+        <v>1867.007285528228</v>
       </c>
     </row>
     <row r="7">
@@ -2960,43 +2960,43 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0</v>
+        <v>0.1354347876867726</v>
       </c>
       <c r="C7" t="n">
-        <v>0</v>
+        <v>0.4266104928735815</v>
       </c>
       <c r="D7" t="n">
-        <v>0.1234767971444062</v>
+        <v>0.9759983566250405</v>
       </c>
       <c r="E7" t="n">
-        <v>0.4714010790455078</v>
+        <v>2.012578742491193</v>
       </c>
       <c r="F7" t="n">
-        <v>1.267326148388391</v>
+        <v>3.968389868396446</v>
       </c>
       <c r="G7" t="n">
-        <v>3.088115179113607</v>
+        <v>7.658597798598102</v>
       </c>
       <c r="H7" t="n">
-        <v>7.253422721375551</v>
+        <v>14.62125098517318</v>
       </c>
       <c r="I7" t="n">
-        <v>16.78214166072123</v>
+        <v>27.75832627021676</v>
       </c>
       <c r="J7" t="n">
-        <v>79.01625977525381</v>
+        <v>89.90160021151155</v>
       </c>
       <c r="K7" t="n">
-        <v>252.7733047110168</v>
+        <v>269.7039043509836</v>
       </c>
       <c r="L7" t="n">
-        <v>728.4949241503405</v>
+        <v>768.2674587401721</v>
       </c>
       <c r="M7" t="n">
-        <v>1392.88235835371</v>
+        <v>1427.383750851408</v>
       </c>
       <c r="N7" t="n">
-        <v>1044.379897511316</v>
+        <v>1059.28946145385</v>
       </c>
     </row>
     <row r="8">
@@ -3006,43 +3006,43 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0</v>
+        <v>0.342595984570463</v>
       </c>
       <c r="C8" t="n">
-        <v>0</v>
+        <v>1.381015995880731</v>
       </c>
       <c r="D8" t="n">
-        <v>0.4427741455338221</v>
+        <v>3.340298111552099</v>
       </c>
       <c r="E8" t="n">
-        <v>1.824198259971985</v>
+        <v>7.037055075957986</v>
       </c>
       <c r="F8" t="n">
-        <v>4.984397594345159</v>
+        <v>14.01206492501213</v>
       </c>
       <c r="G8" t="n">
-        <v>12.21379204938144</v>
+        <v>27.1724546565619</v>
       </c>
       <c r="H8" t="n">
-        <v>28.75203494375755</v>
+        <v>52.00336696126166</v>
       </c>
       <c r="I8" t="n">
-        <v>66.5855602458445</v>
+        <v>98.85412278694659</v>
       </c>
       <c r="J8" t="n">
-        <v>289.8445761246546</v>
+        <v>320.48866585766</v>
       </c>
       <c r="K8" t="n">
-        <v>912.4493344637521</v>
+        <v>1011.273708355151</v>
       </c>
       <c r="L8" t="n">
-        <v>2601.698827002968</v>
+        <v>2915.599411843873</v>
       </c>
       <c r="M8" t="n">
-        <v>2343.542391826816</v>
+        <v>2568.116018450805</v>
       </c>
       <c r="N8" t="n">
-        <v>2220.070967252413</v>
+        <v>2452.857462222711</v>
       </c>
     </row>
     <row r="9">
@@ -3055,40 +3055,40 @@
         <v>0</v>
       </c>
       <c r="C9" t="n">
-        <v>0</v>
+        <v>0.0950667709775731</v>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>0.370570727575005</v>
       </c>
       <c r="E9" t="n">
-        <v>0.1414297281278096</v>
+        <v>0.890389268318406</v>
       </c>
       <c r="F9" t="n">
-        <v>0.534698049424167</v>
+        <v>1.871178505024118</v>
       </c>
       <c r="G9" t="n">
-        <v>1.434353900369164</v>
+        <v>3.721723361431271</v>
       </c>
       <c r="H9" t="n">
-        <v>3.492441486655162</v>
+        <v>7.213315782528062</v>
       </c>
       <c r="I9" t="n">
-        <v>8.200602399936979</v>
+        <v>13.80122290234244</v>
       </c>
       <c r="J9" t="n">
-        <v>38.96919719118263</v>
+        <v>44.9754610967549</v>
       </c>
       <c r="K9" t="n">
-        <v>125.0086627297128</v>
+        <v>145.2357592692406</v>
       </c>
       <c r="L9" t="n">
-        <v>371.4414764750706</v>
+        <v>411.3327793681321</v>
       </c>
       <c r="M9" t="n">
-        <v>393.9330804843264</v>
+        <v>441.1974771445059</v>
       </c>
       <c r="N9" t="n">
-        <v>427.9928642042339</v>
+        <v>479.8039875631497</v>
       </c>
     </row>
     <row r="10">
@@ -3098,43 +3098,43 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0</v>
+        <v>0.09237945981457447</v>
       </c>
       <c r="C10" t="n">
-        <v>0</v>
+        <v>0.4007213005874471</v>
       </c>
       <c r="D10" t="n">
-        <v>0.2266065767624175</v>
+        <v>0.9824980841234222</v>
       </c>
       <c r="E10" t="n">
-        <v>0.7684494210872431</v>
+        <v>2.080189610557489</v>
       </c>
       <c r="F10" t="n">
-        <v>2.007990108174931</v>
+        <v>4.151304720861033</v>
       </c>
       <c r="G10" t="n">
-        <v>4.84361141615835</v>
+        <v>8.059067235948017</v>
       </c>
       <c r="H10" t="n">
-        <v>11.3304886006269</v>
+        <v>15.43220057766792</v>
       </c>
       <c r="I10" t="n">
-        <v>26.17012021430805</v>
+        <v>29.34376635601248</v>
       </c>
       <c r="J10" t="n">
-        <v>90.01779799442055</v>
+        <v>95.15538274684637</v>
       </c>
       <c r="K10" t="n">
-        <v>256.8263350352461</v>
+        <v>280.1643476752449</v>
       </c>
       <c r="L10" t="n">
-        <v>718.7854268621205</v>
+        <v>802.729001447505</v>
       </c>
       <c r="M10" t="n">
-        <v>602.8032686726104</v>
+        <v>671.813867686446</v>
       </c>
       <c r="N10" t="n">
-        <v>531.7515847108235</v>
+        <v>584.4972555297353</v>
       </c>
     </row>
     <row r="11">
@@ -3153,34 +3153,34 @@
         <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>0</v>
+        <v>0.6698516897808605</v>
       </c>
       <c r="F11" t="n">
-        <v>0.5617650101476354</v>
+        <v>1.973321464222696</v>
       </c>
       <c r="G11" t="n">
-        <v>2.06862243552736</v>
+        <v>4.432697236613331</v>
       </c>
       <c r="H11" t="n">
-        <v>5.515767872551252</v>
+        <v>9.073026692976903</v>
       </c>
       <c r="I11" t="n">
-        <v>13.40159135117279</v>
+        <v>17.82836115846391</v>
       </c>
       <c r="J11" t="n">
-        <v>44.27777221996195</v>
+        <v>59.30636666129892</v>
       </c>
       <c r="K11" t="n">
-        <v>133.656325447547</v>
+        <v>182.9444664198378</v>
       </c>
       <c r="L11" t="n">
-        <v>374.7333430728298</v>
+        <v>513.6946862391508</v>
       </c>
       <c r="M11" t="n">
-        <v>376.6877998769639</v>
+        <v>500.846136414828</v>
       </c>
       <c r="N11" t="n">
-        <v>375.290450546456</v>
+        <v>497.2631801999037</v>
       </c>
     </row>
     <row r="12">
@@ -3190,43 +3190,43 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.08349126955496056</v>
+        <v>0.1408838761624001</v>
       </c>
       <c r="C12" t="n">
-        <v>0.3465879120152729</v>
+        <v>0.4067023849979116</v>
       </c>
       <c r="D12" t="n">
-        <v>0.9484579863023784</v>
+        <v>0.9082465046250864</v>
       </c>
       <c r="E12" t="n">
-        <v>2.325319290706939</v>
+        <v>1.854555717759131</v>
       </c>
       <c r="F12" t="n">
-        <v>5.475080564038358</v>
+        <v>3.640043956616461</v>
       </c>
       <c r="G12" t="n">
-        <v>12.68059650616065</v>
+        <v>7.008888100635455</v>
       </c>
       <c r="H12" t="n">
-        <v>29.16421398910235</v>
+        <v>13.36519480694804</v>
       </c>
       <c r="I12" t="n">
-        <v>57.67253007435104</v>
+        <v>25.35822066908078</v>
       </c>
       <c r="J12" t="n">
-        <v>174.5974450791992</v>
+        <v>82.08812115296256</v>
       </c>
       <c r="K12" t="n">
-        <v>422.6559041185533</v>
+        <v>264.9080023871866</v>
       </c>
       <c r="L12" t="n">
-        <v>923.5314470377555</v>
+        <v>785.5856670529024</v>
       </c>
       <c r="M12" t="n">
-        <v>730.7458799024362</v>
+        <v>656.8384684189492</v>
       </c>
       <c r="N12" t="n">
-        <v>717.9917062243093</v>
+        <v>674.3387114248378</v>
       </c>
     </row>
     <row r="13">
@@ -3239,40 +3239,40 @@
         <v>0</v>
       </c>
       <c r="C13" t="n">
-        <v>0</v>
+        <v>0.2531519347725284</v>
       </c>
       <c r="D13" t="n">
-        <v>0</v>
+        <v>1.026085738191558</v>
       </c>
       <c r="E13" t="n">
-        <v>0.6056898316398871</v>
+        <v>2.484450716853616</v>
       </c>
       <c r="F13" t="n">
-        <v>1.991289360980268</v>
+        <v>5.236081453638681</v>
       </c>
       <c r="G13" t="n">
-        <v>5.161040536281085</v>
+        <v>10.4278351109204</v>
       </c>
       <c r="H13" t="n">
-        <v>12.41228615275728</v>
+        <v>20.22359210605807</v>
       </c>
       <c r="I13" t="n">
-        <v>29.00051661077584</v>
+        <v>38.70614375278419</v>
       </c>
       <c r="J13" t="n">
-        <v>104.8042335873037</v>
+        <v>126.1675645500219</v>
       </c>
       <c r="K13" t="n">
-        <v>286.050208225334</v>
+        <v>348.1172006055585</v>
       </c>
       <c r="L13" t="n">
-        <v>645.9444149970182</v>
+        <v>783.2709785112825</v>
       </c>
       <c r="M13" t="n">
-        <v>740.65056022852</v>
+        <v>857.5299101139701</v>
       </c>
       <c r="N13" t="n">
-        <v>832.5349105488585</v>
+        <v>930.6086567386969</v>
       </c>
     </row>
     <row r="14">
@@ -3282,43 +3282,43 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.1390591440173355</v>
+        <v>1.130832766655678</v>
       </c>
       <c r="C14" t="n">
-        <v>0.6514621169372627</v>
+        <v>4.94733226131657</v>
       </c>
       <c r="D14" t="n">
-        <v>3.22012010890505</v>
+        <v>12.53969295023076</v>
       </c>
       <c r="E14" t="n">
-        <v>10.83641694920948</v>
+        <v>27.53474672731159</v>
       </c>
       <c r="F14" t="n">
-        <v>28.89124593756929</v>
+        <v>55.86688693117842</v>
       </c>
       <c r="G14" t="n">
-        <v>70.41591437573638</v>
+        <v>109.3237300154014</v>
       </c>
       <c r="H14" t="n">
-        <v>165.4093549757893</v>
+        <v>210.1856505045998</v>
       </c>
       <c r="I14" t="n">
-        <v>373.5197846793872</v>
+        <v>400.4910710611654</v>
       </c>
       <c r="J14" t="n">
-        <v>1406.781747618625</v>
+        <v>1300.856374320775</v>
       </c>
       <c r="K14" t="n">
-        <v>4255.390492697338</v>
+        <v>3967.620744618412</v>
       </c>
       <c r="L14" t="n">
-        <v>11613.5255173683</v>
+        <v>11153.2849988512</v>
       </c>
       <c r="M14" t="n">
-        <v>12829.54734349308</v>
+        <v>12627.75708965162</v>
       </c>
       <c r="N14" t="n">
-        <v>13510.9169333283</v>
+        <v>13410.91586161358</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Run assumptions check for SSPs
</commit_message>
<xml_diff>
--- a/tutorial/dac_scenarios/SSPs/get_report_output.xlsx
+++ b/tutorial/dac_scenarios/SSPs/get_report_output.xlsx
@@ -513,19 +513,19 @@
         <v>0.7252637611620123</v>
       </c>
       <c r="H2" t="n">
-        <v>1.423517204411967</v>
+        <v>1.423517204411968</v>
       </c>
       <c r="I2" t="n">
         <v>2.740975909622556</v>
       </c>
       <c r="J2" t="n">
-        <v>5.226745878556069</v>
+        <v>5.226745878556068</v>
       </c>
       <c r="K2" t="n">
         <v>9.916875682255711</v>
       </c>
       <c r="L2" t="n">
-        <v>32.10231912905679</v>
+        <v>32.10231912905678</v>
       </c>
       <c r="M2" t="n">
         <v>103.5979519695401</v>
@@ -534,10 +534,10 @@
         <v>334.0024299110544</v>
       </c>
       <c r="O2" t="n">
-        <v>1029.011522827042</v>
+        <v>1076.512445508014</v>
       </c>
       <c r="P2" t="n">
-        <v>2245.440310793185</v>
+        <v>2689.637897038697</v>
       </c>
     </row>
     <row r="3">
@@ -553,43 +553,43 @@
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>0.004104809516001037</v>
+        <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>0.78459371558944</v>
+        <v>0.4490310465577787</v>
       </c>
       <c r="F3" t="n">
-        <v>2.257213598193661</v>
+        <v>1.624076785574742</v>
       </c>
       <c r="G3" t="n">
-        <v>5.035740367461045</v>
+        <v>3.841143171503525</v>
       </c>
       <c r="H3" t="n">
-        <v>10.27824123189513</v>
+        <v>8.024285321976325</v>
       </c>
       <c r="I3" t="n">
-        <v>20.16974762930833</v>
+        <v>15.91700263622652</v>
       </c>
       <c r="J3" t="n">
-        <v>38.83295844036233</v>
+        <v>30.80891506995142</v>
       </c>
       <c r="K3" t="n">
-        <v>74.0465471278178</v>
+        <v>58.90684979939245</v>
       </c>
       <c r="L3" t="n">
-        <v>240.6531204788015</v>
+        <v>191.8633703841186</v>
       </c>
       <c r="M3" t="n">
-        <v>718.1352612365251</v>
+        <v>614.8433783229875</v>
       </c>
       <c r="N3" t="n">
-        <v>2053.267228922684</v>
+        <v>1809.312429258334</v>
       </c>
       <c r="O3" t="n">
-        <v>1980.885760245286</v>
+        <v>1798.609849551534</v>
       </c>
       <c r="P3" t="n">
-        <v>1945.473080744267</v>
+        <v>1678.268352400397</v>
       </c>
     </row>
     <row r="4">
@@ -605,43 +605,43 @@
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>0.009015186007274745</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>0.09965326578959403</v>
+        <v>0.06411708104522686</v>
       </c>
       <c r="F4" t="n">
-        <v>0.270668429964076</v>
+        <v>0.2036190564249627</v>
       </c>
       <c r="G4" t="n">
-        <v>0.593338398788041</v>
+        <v>0.4668302065235313</v>
       </c>
       <c r="H4" t="n">
-        <v>1.202149373437236</v>
+        <v>0.9634547836854316</v>
       </c>
       <c r="I4" t="n">
-        <v>2.35084878356274</v>
+        <v>1.900481845604636</v>
       </c>
       <c r="J4" t="n">
-        <v>4.518205138436267</v>
+        <v>3.668456599867956</v>
       </c>
       <c r="K4" t="n">
-        <v>8.607554821742397</v>
+        <v>7.004256448925</v>
       </c>
       <c r="L4" t="n">
-        <v>27.95476705007753</v>
+        <v>22.78791825250593</v>
       </c>
       <c r="M4" t="n">
-        <v>90.30381070479915</v>
+        <v>73.65293214745677</v>
       </c>
       <c r="N4" t="n">
-        <v>205.1557064711814</v>
+        <v>193.1532793462594</v>
       </c>
       <c r="O4" t="n">
-        <v>204.145423337349</v>
+        <v>192.3426258223748</v>
       </c>
       <c r="P4" t="n">
-        <v>187.8022346280416</v>
+        <v>176.8034122364053</v>
       </c>
     </row>
     <row r="5">
@@ -657,43 +657,43 @@
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>0.1432487140876133</v>
+        <v>0.1113706490214261</v>
       </c>
       <c r="E5" t="n">
-        <v>0.413529179167097</v>
+        <v>0.353381914971389</v>
       </c>
       <c r="F5" t="n">
-        <v>0.9234920801876429</v>
+        <v>0.8100067295957228</v>
       </c>
       <c r="G5" t="n">
-        <v>1.885685779021232</v>
+        <v>1.671562577057043</v>
       </c>
       <c r="H5" t="n">
-        <v>3.701144731471113</v>
+        <v>3.297138880669598</v>
       </c>
       <c r="I5" t="n">
-        <v>7.126537365018643</v>
+        <v>6.364262534525709</v>
       </c>
       <c r="J5" t="n">
-        <v>13.58953928424577</v>
+        <v>12.15128556576559</v>
       </c>
       <c r="K5" t="n">
-        <v>25.78387677386484</v>
+        <v>23.07019179310217</v>
       </c>
       <c r="L5" t="n">
-        <v>83.46602973554762</v>
+        <v>74.72080787443954</v>
       </c>
       <c r="M5" t="n">
-        <v>269.3546751208041</v>
+        <v>241.1719988182259</v>
       </c>
       <c r="N5" t="n">
-        <v>831.994569387629</v>
+        <v>744.9949372904075</v>
       </c>
       <c r="O5" t="n">
-        <v>956.9022213283326</v>
+        <v>862.3636606708116</v>
       </c>
       <c r="P5" t="n">
-        <v>948.7330248519417</v>
+        <v>912.5130953676722</v>
       </c>
     </row>
     <row r="6">
@@ -709,43 +709,43 @@
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>0.2479304666900999</v>
+        <v>0.2149352065978835</v>
       </c>
       <c r="E6" t="n">
-        <v>0.7157235793276679</v>
+        <v>0.6534684009831808</v>
       </c>
       <c r="F6" t="n">
-        <v>1.598351677247844</v>
+        <v>1.480889132025533</v>
       </c>
       <c r="G6" t="n">
-        <v>3.263686925229055</v>
+        <v>3.042059585993825</v>
       </c>
       <c r="H6" t="n">
-        <v>6.405827419853852</v>
+        <v>5.987662826165495</v>
       </c>
       <c r="I6" t="n">
-        <v>12.3343915933015</v>
+        <v>11.54540216619406</v>
       </c>
       <c r="J6" t="n">
-        <v>23.52035645350231</v>
+        <v>22.03169785953429</v>
       </c>
       <c r="K6" t="n">
-        <v>44.62594057015069</v>
+        <v>41.81715209560873</v>
       </c>
       <c r="L6" t="n">
-        <v>144.4604360807555</v>
+        <v>135.4087301735026</v>
       </c>
       <c r="M6" t="n">
-        <v>423.0826413460287</v>
+        <v>413.5563609619434</v>
       </c>
       <c r="N6" t="n">
-        <v>1144.801603134423</v>
+        <v>1139.426504425004</v>
       </c>
       <c r="O6" t="n">
-        <v>1855.969581856064</v>
+        <v>1786.424826561195</v>
       </c>
       <c r="P6" t="n">
-        <v>2044.372998097139</v>
+        <v>2042.839007233536</v>
       </c>
     </row>
     <row r="7">
@@ -761,43 +761,43 @@
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>0.1483010940000269</v>
+        <v>0.09076758564109094</v>
       </c>
       <c r="E7" t="n">
-        <v>0.4671384943679568</v>
+        <v>0.3585847562352932</v>
       </c>
       <c r="F7" t="n">
-        <v>1.068718211191602</v>
+        <v>0.8638999340050573</v>
       </c>
       <c r="G7" t="n">
-        <v>2.203773745065594</v>
+        <v>1.817324347824236</v>
       </c>
       <c r="H7" t="n">
-        <v>4.345386949347978</v>
+        <v>3.616237487299772</v>
       </c>
       <c r="I7" t="n">
-        <v>8.386164673326569</v>
+        <v>7.010411620532601</v>
       </c>
       <c r="J7" t="n">
-        <v>16.01026998886734</v>
+        <v>13.41451073677205</v>
       </c>
       <c r="K7" t="n">
-        <v>30.39536756984104</v>
+        <v>25.49771091470636</v>
       </c>
       <c r="L7" t="n">
-        <v>98.44225321602769</v>
+        <v>82.65888324039852</v>
       </c>
       <c r="M7" t="n">
-        <v>295.3257782175849</v>
+        <v>266.8685971065668</v>
       </c>
       <c r="N7" t="n">
-        <v>841.252875733017</v>
+        <v>775.659730958687</v>
       </c>
       <c r="O7" t="n">
-        <v>1562.985222812144</v>
+        <v>1479.514496631615</v>
       </c>
       <c r="P7" t="n">
-        <v>1159.921971891186</v>
+        <v>1086.100236099329</v>
       </c>
     </row>
     <row r="8">
@@ -813,43 +813,43 @@
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>0.3751426068560831</v>
+        <v>0.01000162769697045</v>
       </c>
       <c r="E8" t="n">
-        <v>1.512212530611525</v>
+        <v>0.8232676120111231</v>
       </c>
       <c r="F8" t="n">
-        <v>3.657626468725813</v>
+        <v>2.357731009283324</v>
       </c>
       <c r="G8" t="n">
-        <v>7.705575385229749</v>
+        <v>5.252943600221599</v>
       </c>
       <c r="H8" t="n">
-        <v>15.3432112463204</v>
+        <v>10.7156062884477</v>
       </c>
       <c r="I8" t="n">
-        <v>29.75383814647366</v>
+        <v>21.02251215737629</v>
       </c>
       <c r="J8" t="n">
-        <v>56.9436873920184</v>
+        <v>40.46949518635249</v>
       </c>
       <c r="K8" t="n">
-        <v>108.2452655341592</v>
+        <v>77.16189868150549</v>
       </c>
       <c r="L8" t="n">
-        <v>350.9350926234887</v>
+        <v>250.7646818191099</v>
       </c>
       <c r="M8" t="n">
-        <v>1107.344721722338</v>
+        <v>810.2234491434962</v>
       </c>
       <c r="N8" t="n">
-        <v>3192.581387894855</v>
+        <v>2403.452475869918</v>
       </c>
       <c r="O8" t="n">
-        <v>2812.087068324503</v>
+        <v>2232.721781867871</v>
       </c>
       <c r="P8" t="n">
-        <v>2685.878947992658</v>
+        <v>2122.267785739251</v>
       </c>
     </row>
     <row r="9">
@@ -868,40 +868,40 @@
         <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>0.1040981152614237</v>
+        <v>0.01003999271368437</v>
       </c>
       <c r="F9" t="n">
-        <v>0.40577495075238</v>
+        <v>0.2283068787447144</v>
       </c>
       <c r="G9" t="n">
-        <v>0.9749762585584173</v>
+        <v>0.6401309976812113</v>
       </c>
       <c r="H9" t="n">
-        <v>2.048940483490814</v>
+        <v>1.41715727052459</v>
       </c>
       <c r="I9" t="n">
-        <v>4.075287121520113</v>
+        <v>2.883243885966301</v>
       </c>
       <c r="J9" t="n">
-        <v>7.898580860854038</v>
+        <v>5.649443741875904</v>
       </c>
       <c r="K9" t="n">
-        <v>15.11233922918836</v>
+        <v>10.86868629019486</v>
       </c>
       <c r="L9" t="n">
-        <v>49.24813039342792</v>
+        <v>35.572377048391</v>
       </c>
       <c r="M9" t="n">
-        <v>159.0331579901501</v>
+        <v>115.1834070685054</v>
       </c>
       <c r="N9" t="n">
-        <v>450.4093979121987</v>
+        <v>361.0064383641163</v>
       </c>
       <c r="O9" t="n">
-        <v>483.1112423043464</v>
+        <v>361.3402700804563</v>
       </c>
       <c r="P9" t="n">
-        <v>525.3853716355027</v>
+        <v>348.8626731340805</v>
       </c>
     </row>
     <row r="10">
@@ -917,43 +917,43 @@
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>0.1011555095085142</v>
+        <v>0.01844540961689184</v>
       </c>
       <c r="E10" t="n">
-        <v>0.4387898285311529</v>
+        <v>0.2827331099221077</v>
       </c>
       <c r="F10" t="n">
-        <v>1.075835412873501</v>
+        <v>0.7813889129305183</v>
       </c>
       <c r="G10" t="n">
-        <v>2.277807646338527</v>
+        <v>1.722248474638449</v>
       </c>
       <c r="H10" t="n">
-        <v>4.545678714799618</v>
+        <v>3.497454357166423</v>
       </c>
       <c r="I10" t="n">
-        <v>8.824678711609867</v>
+        <v>6.846897838020571</v>
       </c>
       <c r="J10" t="n">
-        <v>16.89825980152898</v>
+        <v>13.16659953676681</v>
       </c>
       <c r="K10" t="n">
-        <v>32.13142448114791</v>
+        <v>25.09055937947814</v>
       </c>
       <c r="L10" t="n">
-        <v>104.1951451497482</v>
+        <v>81.50499214940612</v>
       </c>
       <c r="M10" t="n">
-        <v>306.7799637721929</v>
+        <v>263.3082354289302</v>
       </c>
       <c r="N10" t="n">
-        <v>878.9882653749007</v>
+        <v>849.194109736127</v>
       </c>
       <c r="O10" t="n">
-        <v>735.6361924730203</v>
+        <v>672.4045526568398</v>
       </c>
       <c r="P10" t="n">
-        <v>640.0245012053052</v>
+        <v>578.9248991203031</v>
       </c>
     </row>
     <row r="11">
@@ -978,34 +978,34 @@
         <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>0.7334876076449184</v>
+        <v>0.5061045565799114</v>
       </c>
       <c r="H11" t="n">
-        <v>2.160787024931722</v>
+        <v>1.731762602726761</v>
       </c>
       <c r="I11" t="n">
-        <v>4.853803522629633</v>
+        <v>4.044323862706872</v>
       </c>
       <c r="J11" t="n">
-        <v>9.934964328159353</v>
+        <v>8.407644935801718</v>
       </c>
       <c r="K11" t="n">
-        <v>19.52205566373853</v>
+        <v>16.64032232099552</v>
       </c>
       <c r="L11" t="n">
-        <v>64.94047214352705</v>
+        <v>55.65369139871215</v>
       </c>
       <c r="M11" t="n">
-        <v>200.3241927329644</v>
+        <v>180.3845236731346</v>
       </c>
       <c r="N11" t="n">
-        <v>562.4956870568271</v>
+        <v>509.3115116425636</v>
       </c>
       <c r="O11" t="n">
-        <v>548.4265248585019</v>
+        <v>515.4011497452815</v>
       </c>
       <c r="P11" t="n">
-        <v>544.5031877639265</v>
+        <v>498.6908336565305</v>
       </c>
     </row>
     <row r="12">
@@ -1033,31 +1033,31 @@
         <v>2.030738531253633</v>
       </c>
       <c r="H12" t="n">
-        <v>3.985848172353506</v>
+        <v>3.985848172353507</v>
       </c>
       <c r="I12" t="n">
         <v>7.674732546943149</v>
       </c>
       <c r="J12" t="n">
-        <v>14.66140288272231</v>
+        <v>14.63488845995698</v>
       </c>
       <c r="K12" t="n">
-        <v>27.76725191031598</v>
+        <v>27.76725191031597</v>
       </c>
       <c r="L12" t="n">
-        <v>89.88649356135896</v>
+        <v>89.88649356135898</v>
       </c>
       <c r="M12" t="n">
-        <v>290.0742655147121</v>
+        <v>290.074265514712</v>
       </c>
       <c r="N12" t="n">
-        <v>860.2163140250913</v>
+        <v>935.2068037509518</v>
       </c>
       <c r="O12" t="n">
-        <v>719.2381301111308</v>
+        <v>718.4354212212122</v>
       </c>
       <c r="P12" t="n">
-        <v>738.4008963942065</v>
+        <v>802.5898699042621</v>
       </c>
     </row>
     <row r="13">
@@ -1076,40 +1076,40 @@
         <v>0</v>
       </c>
       <c r="E13" t="n">
-        <v>0.2772013713479323</v>
+        <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>1.123563894555395</v>
+        <v>0.5278279031582536</v>
       </c>
       <c r="G13" t="n">
-        <v>2.720473562159445</v>
+        <v>1.596443920113747</v>
       </c>
       <c r="H13" t="n">
-        <v>5.733509249069449</v>
+        <v>3.612699604457729</v>
       </c>
       <c r="I13" t="n">
-        <v>11.41847956064264</v>
+        <v>7.41695381752062</v>
       </c>
       <c r="J13" t="n">
-        <v>22.14483357758193</v>
+        <v>14.59478856833276</v>
       </c>
       <c r="K13" t="n">
-        <v>42.38322783313097</v>
+        <v>28.13786661318441</v>
       </c>
       <c r="L13" t="n">
-        <v>138.1534845638089</v>
+        <v>92.24585518044336</v>
       </c>
       <c r="M13" t="n">
-        <v>381.1883384749701</v>
+        <v>298.8426367024072</v>
       </c>
       <c r="N13" t="n">
-        <v>857.6817300466716</v>
+        <v>778.7726452463081</v>
       </c>
       <c r="O13" t="n">
-        <v>938.9952609647501</v>
+        <v>811.3654051449073</v>
       </c>
       <c r="P13" t="n">
-        <v>1019.016489319038</v>
+        <v>763.9925736767213</v>
       </c>
     </row>
     <row r="14">
@@ -1125,43 +1125,43 @@
         <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>1.238261891870587</v>
+        <v>0.6548839837792361</v>
       </c>
       <c r="E14" t="n">
-        <v>5.417328880314932</v>
+        <v>3.599012714760926</v>
       </c>
       <c r="F14" t="n">
-        <v>13.73096391781231</v>
+        <v>10.22746553586323</v>
       </c>
       <c r="G14" t="n">
-        <v>30.15054796791167</v>
+        <v>23.31279373055272</v>
       </c>
       <c r="H14" t="n">
-        <v>61.17424180138279</v>
+        <v>48.27282479988531</v>
       </c>
       <c r="I14" t="n">
-        <v>119.7094855639594</v>
+        <v>95.36720082123988</v>
       </c>
       <c r="J14" t="n">
-        <v>230.1798040268351</v>
+        <v>184.224472139534</v>
       </c>
       <c r="K14" t="n">
-        <v>438.5377271973533</v>
+        <v>351.8796219296648</v>
       </c>
       <c r="L14" t="n">
-        <v>1424.437744125627</v>
+        <v>1145.170120211444</v>
       </c>
       <c r="M14" t="n">
-        <v>4344.544758802609</v>
+        <v>3671.707736857906</v>
       </c>
       <c r="N14" t="n">
-        <v>12212.84719587053</v>
+        <v>10833.49329579973</v>
       </c>
       <c r="O14" t="n">
-        <v>13827.39415144247</v>
+        <v>12507.43648546211</v>
       </c>
       <c r="P14" t="n">
-        <v>14684.9530153164</v>
+        <v>13701.49063560719</v>
       </c>
     </row>
   </sheetData>
@@ -1260,31 +1260,31 @@
         <v>0.07401489991027609</v>
       </c>
       <c r="H2" t="n">
-        <v>0.139650688649991</v>
+        <v>0.1506698205028844</v>
       </c>
       <c r="I2" t="n">
-        <v>0.274510872895011</v>
+        <v>0.2842825460482318</v>
       </c>
       <c r="J2" t="n">
-        <v>0.5179447987928169</v>
+        <v>0.5363819092498215</v>
       </c>
       <c r="K2" t="n">
-        <v>1.015187933466584</v>
+        <v>1.012040860650204</v>
       </c>
       <c r="L2" t="n">
-        <v>2.271497438165975</v>
+        <v>2.364949891443608</v>
       </c>
       <c r="M2" t="n">
-        <v>7.451217592356535</v>
+        <v>7.741835090347848</v>
       </c>
       <c r="N2" t="n">
-        <v>24.81327667966593</v>
+        <v>25.6584079007576</v>
       </c>
       <c r="O2" t="n">
-        <v>74.36226680686001</v>
+        <v>81.99283665004386</v>
       </c>
       <c r="P2" t="n">
-        <v>137.7751259326255</v>
+        <v>186.9709530538258</v>
       </c>
     </row>
     <row r="3">
@@ -1300,43 +1300,43 @@
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>0.0008209619032002075</v>
+        <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>0.1560977812146878</v>
+        <v>0.08980620931155575</v>
       </c>
       <c r="F3" t="n">
-        <v>0.2945239765208442</v>
+        <v>0.2350091478033926</v>
       </c>
       <c r="G3" t="n">
-        <v>0.5557053538534771</v>
+        <v>0.4434132771857567</v>
       </c>
       <c r="H3" t="n">
-        <v>1.048500172886818</v>
+        <v>0.83662843009456</v>
       </c>
       <c r="I3" t="n">
-        <v>1.97912224138584</v>
+        <v>1.668349672161594</v>
       </c>
       <c r="J3" t="n">
-        <v>3.888739943425488</v>
+        <v>3.213391634548375</v>
       </c>
       <c r="K3" t="n">
-        <v>7.33724171401194</v>
+        <v>6.063000223073961</v>
       </c>
       <c r="L3" t="n">
-        <v>17.20063505524681</v>
+        <v>14.13105369156029</v>
       </c>
       <c r="M3" t="n">
-        <v>49.97208522554337</v>
+        <v>45.83753408496997</v>
       </c>
       <c r="N3" t="n">
-        <v>146.7543201391017</v>
+        <v>135.0937088408634</v>
       </c>
       <c r="O3" t="n">
-        <v>26.34821327265524</v>
+        <v>44.76727611428996</v>
       </c>
       <c r="P3" t="n">
-        <v>94.82193473222063</v>
+        <v>123.0595591257497</v>
       </c>
     </row>
     <row r="4">
@@ -1352,43 +1352,43 @@
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>0.001803037201454949</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>0.01812761595646386</v>
+        <v>0.01282341620904537</v>
       </c>
       <c r="F4" t="n">
-        <v>0.0342030328348964</v>
+        <v>0.02790039507594718</v>
       </c>
       <c r="G4" t="n">
-        <v>0.06453399376479298</v>
+        <v>0.05264223001971372</v>
       </c>
       <c r="H4" t="n">
-        <v>0.1217621949298391</v>
+        <v>0.09932491543238006</v>
       </c>
       <c r="I4" t="n">
-        <v>0.2315429192265556</v>
+        <v>0.2002288285928862</v>
       </c>
       <c r="J4" t="n">
-        <v>0.4515988869311694</v>
+        <v>0.3814953459286113</v>
       </c>
       <c r="K4" t="n">
-        <v>0.8520729694961222</v>
+        <v>0.7198021998311225</v>
       </c>
       <c r="L4" t="n">
-        <v>1.99742876844837</v>
+        <v>1.678085845222505</v>
       </c>
       <c r="M4" t="n">
-        <v>6.494016095550691</v>
+        <v>5.507256819565391</v>
       </c>
       <c r="N4" t="n">
-        <v>13.02284016734327</v>
+        <v>13.80807111506055</v>
       </c>
       <c r="O4" t="n">
-        <v>4.144694118616285</v>
+        <v>5.426191467176933</v>
       </c>
       <c r="P4" t="n">
-        <v>8.124109260516244</v>
+        <v>12.2541497564636</v>
       </c>
     </row>
     <row r="5">
@@ -1404,43 +1404,43 @@
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>0.02864974281752266</v>
+        <v>0.02227412980428522</v>
       </c>
       <c r="E5" t="n">
-        <v>0.05405609301589675</v>
+        <v>0.04840225318999258</v>
       </c>
       <c r="F5" t="n">
-        <v>0.1019925802041092</v>
+        <v>0.09132496292486678</v>
       </c>
       <c r="G5" t="n">
-        <v>0.1924387397667178</v>
+        <v>0.172311169492264</v>
       </c>
       <c r="H5" t="n">
-        <v>0.3630917904899764</v>
+        <v>0.3473893905267964</v>
       </c>
       <c r="I5" t="n">
-        <v>0.7137282695270286</v>
+        <v>0.6618269839612148</v>
       </c>
       <c r="J5" t="n">
-        <v>1.346656476861323</v>
+        <v>1.248729569172843</v>
       </c>
       <c r="K5" t="n">
-        <v>2.540860078127922</v>
+        <v>2.356092414959581</v>
       </c>
       <c r="L5" t="n">
-        <v>5.955207613674132</v>
+        <v>5.504213049387438</v>
       </c>
       <c r="M5" t="n">
-        <v>19.37316574012699</v>
+        <v>18.02396372869525</v>
       </c>
       <c r="N5" t="n">
-        <v>60.84868739179885</v>
+        <v>56.4755300003455</v>
       </c>
       <c r="O5" t="n">
-        <v>25.15495187097093</v>
+        <v>29.76083606673566</v>
       </c>
       <c r="P5" t="n">
-        <v>39.29400691832382</v>
+        <v>61.49047347003157</v>
       </c>
     </row>
     <row r="6">
@@ -1456,43 +1456,43 @@
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>0.04958609333801998</v>
+        <v>0.0429870413195767</v>
       </c>
       <c r="E6" t="n">
-        <v>0.09355862252751362</v>
+        <v>0.08770663887705948</v>
       </c>
       <c r="F6" t="n">
-        <v>0.1765256195840351</v>
+        <v>0.1654841462084704</v>
       </c>
       <c r="G6" t="n">
-        <v>0.3330670495962424</v>
+        <v>0.3122340907936585</v>
       </c>
       <c r="H6" t="n">
-        <v>0.6284280989249593</v>
+        <v>0.6321076893539106</v>
       </c>
       <c r="I6" t="n">
-        <v>1.235298928027549</v>
+        <v>1.199254506882773</v>
       </c>
       <c r="J6" t="n">
-        <v>2.330751594567675</v>
+        <v>2.262743284876516</v>
       </c>
       <c r="K6" t="n">
-        <v>4.397642442913712</v>
+        <v>4.269324938008547</v>
       </c>
       <c r="L6" t="n">
-        <v>10.30709010058985</v>
+        <v>9.975025279187044</v>
       </c>
       <c r="M6" t="n">
-        <v>29.21966491391426</v>
+        <v>30.31327958250516</v>
       </c>
       <c r="N6" t="n">
-        <v>80.10695034923313</v>
+        <v>83.62937085999521</v>
       </c>
       <c r="O6" t="n">
-        <v>90.93915608027595</v>
+        <v>95.01311179612425</v>
       </c>
       <c r="P6" t="n">
-        <v>73.46513192919078</v>
+        <v>109.2707889272293</v>
       </c>
     </row>
     <row r="7">
@@ -1508,43 +1508,43 @@
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>0.02966021880000538</v>
+        <v>0.01815351712821819</v>
       </c>
       <c r="E7" t="n">
-        <v>0.06376748007358599</v>
+        <v>0.05356343411884045</v>
       </c>
       <c r="F7" t="n">
-        <v>0.120315943364729</v>
+        <v>0.1010630355539528</v>
       </c>
       <c r="G7" t="n">
-        <v>0.2270111067747985</v>
+        <v>0.1906848827638358</v>
       </c>
       <c r="H7" t="n">
-        <v>0.4283226408564767</v>
+        <v>0.3779361450233254</v>
       </c>
       <c r="I7" t="n">
-        <v>0.8378157635957237</v>
+        <v>0.7323982607654062</v>
       </c>
       <c r="J7" t="n">
-        <v>1.588588543181739</v>
+        <v>1.381882858801843</v>
       </c>
       <c r="K7" t="n">
-        <v>2.997335459559469</v>
+        <v>2.607324918350697</v>
       </c>
       <c r="L7" t="n">
-        <v>7.025274778220184</v>
+        <v>6.088184870272232</v>
       </c>
       <c r="M7" t="n">
-        <v>20.61148817796314</v>
+        <v>19.94684361079677</v>
       </c>
       <c r="N7" t="n">
-        <v>60.00116200622848</v>
+        <v>57.61912948507193</v>
       </c>
       <c r="O7" t="n">
-        <v>85.99161618600436</v>
+        <v>90.33232017808962</v>
       </c>
       <c r="P7" t="n">
-        <v>0</v>
+        <v>18.27770343184332</v>
       </c>
     </row>
     <row r="8">
@@ -1560,43 +1560,43 @@
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>0.07502852137121663</v>
+        <v>0.00200032553939409</v>
       </c>
       <c r="E8" t="n">
-        <v>0.2274139847510885</v>
+        <v>0.1626531968628305</v>
       </c>
       <c r="F8" t="n">
-        <v>0.4290827876228576</v>
+        <v>0.3068926794544402</v>
       </c>
       <c r="G8" t="n">
-        <v>0.8095897833007872</v>
+        <v>0.5790425181876552</v>
       </c>
       <c r="H8" t="n">
-        <v>1.527527172218131</v>
+        <v>1.094532863184615</v>
       </c>
       <c r="I8" t="n">
-        <v>2.957153901401869</v>
+        <v>2.224034370648548</v>
       </c>
       <c r="J8" t="n">
-        <v>5.665383833860036</v>
+        <v>4.19628928524968</v>
       </c>
       <c r="K8" t="n">
-        <v>10.68939841605102</v>
+        <v>7.917523217218257</v>
       </c>
       <c r="L8" t="n">
-        <v>25.05565939363787</v>
+        <v>18.46355333801489</v>
       </c>
       <c r="M8" t="n">
-        <v>78.91776761210542</v>
+        <v>60.57941077203017</v>
       </c>
       <c r="N8" t="n">
-        <v>227.8125414805612</v>
+        <v>179.7658368149616</v>
       </c>
       <c r="O8" t="n">
-        <v>13.93728154583635</v>
+        <v>43.50634137182551</v>
       </c>
       <c r="P8" t="n">
-        <v>140.7443425131489</v>
+        <v>168.7204372020996</v>
       </c>
     </row>
     <row r="9">
@@ -1615,40 +1615,40 @@
         <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>0.02081962305228474</v>
+        <v>0.002007998542736875</v>
       </c>
       <c r="F9" t="n">
-        <v>0.06033536709819126</v>
+        <v>0.04365337720620601</v>
       </c>
       <c r="G9" t="n">
-        <v>0.1138402615612075</v>
+        <v>0.08236482378729937</v>
       </c>
       <c r="H9" t="n">
-        <v>0.2147928449864793</v>
+        <v>0.1554052545686758</v>
       </c>
       <c r="I9" t="n">
-        <v>0.4052693276058599</v>
+        <v>0.295225321631079</v>
       </c>
       <c r="J9" t="n">
-        <v>0.7854783709190696</v>
+        <v>0.5968933483881268</v>
       </c>
       <c r="K9" t="n">
-        <v>1.503087040765057</v>
+        <v>1.12621333345109</v>
       </c>
       <c r="L9" t="n">
-        <v>3.52419745845118</v>
+        <v>2.621878033511722</v>
       </c>
       <c r="M9" t="n">
-        <v>11.43120522745154</v>
+        <v>8.61490933997605</v>
       </c>
       <c r="N9" t="n">
-        <v>31.84763583454274</v>
+        <v>27.48573449643558</v>
       </c>
       <c r="O9" t="n">
-        <v>10.74788578216613</v>
+        <v>8.648292511610057</v>
       </c>
       <c r="P9" t="n">
-        <v>25.86683346411277</v>
+        <v>26.23797480179799</v>
       </c>
     </row>
     <row r="10">
@@ -1664,43 +1664,43 @@
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>0.02023110190170283</v>
+        <v>0.003689081923378368</v>
       </c>
       <c r="E10" t="n">
-        <v>0.06752686380452776</v>
+        <v>0.05285754006104318</v>
       </c>
       <c r="F10" t="n">
-        <v>0.1274091168684697</v>
+        <v>0.09973116060168212</v>
       </c>
       <c r="G10" t="n">
-        <v>0.2403944466930051</v>
+        <v>0.1881719123415862</v>
       </c>
       <c r="H10" t="n">
-        <v>0.4535742136922183</v>
+        <v>0.3587302584289732</v>
       </c>
       <c r="I10" t="n">
-        <v>0.8760311012637527</v>
+        <v>0.7227462362318726</v>
       </c>
       <c r="J10" t="n">
-        <v>1.682243081788349</v>
+        <v>1.36367150035093</v>
       </c>
       <c r="K10" t="n">
-        <v>3.174042052792257</v>
+        <v>2.572963880883852</v>
       </c>
       <c r="L10" t="n">
-        <v>7.439962843629591</v>
+        <v>6.001494965265253</v>
       </c>
       <c r="M10" t="n">
-        <v>21.23045173674648</v>
+        <v>19.68608760740681</v>
       </c>
       <c r="N10" t="n">
-        <v>62.94839337892879</v>
+        <v>65.23332336620589</v>
       </c>
       <c r="O10" t="n">
-        <v>0</v>
+        <v>2.007131899478092</v>
       </c>
       <c r="P10" t="n">
-        <v>32.52825343106613</v>
+        <v>55.88535801255222</v>
       </c>
     </row>
     <row r="11">
@@ -1725,34 +1725,34 @@
         <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>0.1466975215289837</v>
+        <v>0.1012209113159823</v>
       </c>
       <c r="H11" t="n">
-        <v>0.2854598834573609</v>
+        <v>0.2451316092293698</v>
       </c>
       <c r="I11" t="n">
-        <v>0.5386032995395821</v>
+        <v>0.4625122519960223</v>
       </c>
       <c r="J11" t="n">
-        <v>1.016232161105944</v>
+        <v>0.8726642146189694</v>
       </c>
       <c r="K11" t="n">
-        <v>1.917418267115837</v>
+        <v>1.747756388354743</v>
       </c>
       <c r="L11" t="n">
-        <v>4.686555379607684</v>
+        <v>4.139530775385353</v>
       </c>
       <c r="M11" t="n">
-        <v>14.13309671985435</v>
+        <v>13.46198249483943</v>
       </c>
       <c r="N11" t="n">
-        <v>39.77319429602451</v>
+        <v>37.46916866941694</v>
       </c>
       <c r="O11" t="n">
-        <v>8.002909829898504</v>
+        <v>14.07094630511121</v>
       </c>
       <c r="P11" t="n">
-        <v>26.56081179848189</v>
+        <v>35.79813706054184</v>
       </c>
     </row>
     <row r="12">
@@ -1780,31 +1780,31 @@
         <v>0.207241719748773</v>
       </c>
       <c r="H12" t="n">
-        <v>0.3910219282199746</v>
+        <v>0.4218754974080759</v>
       </c>
       <c r="I12" t="n">
-        <v>0.76863044410603</v>
+        <v>0.7959911289350483</v>
       </c>
       <c r="J12" t="n">
-        <v>1.565386484469686</v>
+        <v>1.5018693458995</v>
       </c>
       <c r="K12" t="n">
-        <v>2.621169805518732</v>
+        <v>2.833714409820571</v>
       </c>
       <c r="L12" t="n">
-        <v>6.413300507033679</v>
+        <v>6.6218596960421</v>
       </c>
       <c r="M12" t="n">
-        <v>21.08673122979906</v>
+        <v>21.67713825297396</v>
       </c>
       <c r="N12" t="n">
-        <v>61.72824991919323</v>
+        <v>71.84354212212122</v>
       </c>
       <c r="O12" t="n">
         <v>0</v>
       </c>
       <c r="P12" t="n">
-        <v>43.14986594131388</v>
+        <v>80.25898699042621</v>
       </c>
     </row>
     <row r="13">
@@ -1823,40 +1823,40 @@
         <v>0</v>
       </c>
       <c r="E13" t="n">
-        <v>0.05544027426958647</v>
+        <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>0.1692725046414925</v>
+        <v>0.1055655806316507</v>
       </c>
       <c r="G13" t="n">
-        <v>0.3193819335208101</v>
+        <v>0.2137232033910986</v>
       </c>
       <c r="H13" t="n">
-        <v>0.6026071373820008</v>
+        <v>0.4032511368687965</v>
       </c>
       <c r="I13" t="n">
-        <v>1.136994062314638</v>
+        <v>0.7608508426125781</v>
       </c>
       <c r="J13" t="n">
-        <v>2.200711077657445</v>
+        <v>1.541132530794079</v>
       </c>
       <c r="K13" t="n">
-        <v>4.216951355751301</v>
+        <v>2.922338812361429</v>
       </c>
       <c r="L13" t="n">
-        <v>9.887368424173694</v>
+        <v>6.802637135813439</v>
       </c>
       <c r="M13" t="n">
-        <v>25.5728119760333</v>
+        <v>22.35104183133693</v>
       </c>
       <c r="N13" t="n">
-        <v>55.25167681654703</v>
+        <v>55.5262226932939</v>
       </c>
       <c r="O13" t="n">
-        <v>25.86144329191133</v>
+        <v>25.61031782119684</v>
       </c>
       <c r="P13" t="n">
-        <v>48.41436723171896</v>
+        <v>50.7889395464753</v>
       </c>
     </row>
     <row r="14">
@@ -1872,43 +1872,43 @@
         <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>0.2476523783741173</v>
+        <v>0.1309767967558472</v>
       </c>
       <c r="E14" t="n">
-        <v>0.8358133976888693</v>
+        <v>0.5888257461963379</v>
       </c>
       <c r="F14" t="n">
-        <v>1.662727007499476</v>
+        <v>1.325690564220461</v>
       </c>
       <c r="G14" t="n">
-        <v>3.283916810019871</v>
+        <v>2.6170656389379</v>
       </c>
       <c r="H14" t="n">
-        <v>6.204738766694224</v>
+        <v>5.122983010622363</v>
       </c>
       <c r="I14" t="n">
-        <v>11.95470113088944</v>
+        <v>10.00770095046725</v>
       </c>
       <c r="J14" t="n">
-        <v>23.03971525356074</v>
+        <v>19.09714482787929</v>
       </c>
       <c r="K14" t="n">
-        <v>43.26240753556995</v>
+        <v>36.14809559696405</v>
       </c>
       <c r="L14" t="n">
-        <v>101.764177760879</v>
+        <v>84.39246657110587</v>
       </c>
       <c r="M14" t="n">
-        <v>305.4937022474451</v>
+        <v>273.7412832154437</v>
       </c>
       <c r="N14" t="n">
-        <v>864.9089284591688</v>
+        <v>809.6080463645295</v>
       </c>
       <c r="O14" t="n">
-        <v>365.4904187851951</v>
+        <v>441.135602181682</v>
       </c>
       <c r="P14" t="n">
-        <v>670.7447831527196</v>
+        <v>929.0134613790367</v>
       </c>
     </row>
   </sheetData>
@@ -1995,43 +1995,43 @@
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>32.90048312109479</v>
+        <v>45.65589958004852</v>
       </c>
       <c r="E2" t="n">
-        <v>52.76490086179703</v>
+        <v>73.22169119008542</v>
       </c>
       <c r="F2" t="n">
-        <v>87.84385565487148</v>
+        <v>121.9006492318534</v>
       </c>
       <c r="G2" t="n">
-        <v>143.6439729114689</v>
+        <v>199.3343009094087</v>
       </c>
       <c r="H2" t="n">
-        <v>246.0084296847223</v>
+        <v>368.3221245566874</v>
       </c>
       <c r="I2" t="n">
-        <v>677.0039933181038</v>
+        <v>612.4957287893706</v>
       </c>
       <c r="J2" t="n">
-        <v>1414.766269697059</v>
+        <v>1088.979555465511</v>
       </c>
       <c r="K2" t="n">
-        <v>2546.619742453563</v>
+        <v>1886.948666621015</v>
       </c>
       <c r="L2" t="n">
-        <v>5191.600299173556</v>
+        <v>4017.494811823167</v>
       </c>
       <c r="M2" t="n">
-        <v>14693.58382533309</v>
+        <v>12830.79103395638</v>
       </c>
       <c r="N2" t="n">
-        <v>32779.51982619567</v>
+        <v>42524.50048297839</v>
       </c>
       <c r="O2" t="n">
-        <v>86604.86070963995</v>
+        <v>132492.1181521182</v>
       </c>
       <c r="P2" t="n">
-        <v>162420.2364525321</v>
+        <v>302126.1199774382</v>
       </c>
     </row>
     <row r="3">
@@ -2047,43 +2047,43 @@
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>2.23585771271615</v>
+        <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>361.3572843030948</v>
+        <v>288.4968516401092</v>
       </c>
       <c r="F3" t="n">
-        <v>601.5934191802884</v>
+        <v>666.1343329707612</v>
       </c>
       <c r="G3" t="n">
-        <v>983.7372023829084</v>
+        <v>1089.275753748692</v>
       </c>
       <c r="H3" t="n">
-        <v>1684.774094418956</v>
+        <v>1865.522181278812</v>
       </c>
       <c r="I3" t="n">
-        <v>2802.832347630103</v>
+        <v>3278.734201545154</v>
       </c>
       <c r="J3" t="n">
-        <v>5189.507441292425</v>
+        <v>5950.802349043279</v>
       </c>
       <c r="K3" t="n">
-        <v>8992.211192229963</v>
+        <v>10311.35846535923</v>
       </c>
       <c r="L3" t="n">
-        <v>19206.55597392482</v>
+        <v>21896.47422280704</v>
       </c>
       <c r="M3" t="n">
-        <v>54438.80976035608</v>
+        <v>69294.22218238768</v>
       </c>
       <c r="N3" t="n">
-        <v>159871.8660529156</v>
+        <v>204225.9397835081</v>
       </c>
       <c r="O3" t="n">
-        <v>27985.74903001313</v>
+        <v>65984.36845485878</v>
       </c>
       <c r="P3" t="n">
-        <v>100715.097471533</v>
+        <v>181382.6525990934</v>
       </c>
     </row>
     <row r="4">
@@ -2099,43 +2099,43 @@
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>5.761789645054906</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>49.23935199435816</v>
+        <v>48.33592169498279</v>
       </c>
       <c r="F4" t="n">
-        <v>81.97446519346113</v>
+        <v>92.7937993184777</v>
       </c>
       <c r="G4" t="n">
-        <v>134.0462320318094</v>
+        <v>151.7382165922325</v>
       </c>
       <c r="H4" t="n">
-        <v>229.5710873133782</v>
+        <v>259.8708433804044</v>
       </c>
       <c r="I4" t="n">
-        <v>384.7579121055185</v>
+        <v>461.7185153388618</v>
       </c>
       <c r="J4" t="n">
-        <v>707.133894012802</v>
+        <v>828.9582620646664</v>
       </c>
       <c r="K4" t="n">
-        <v>1225.29881459491</v>
+        <v>1436.392152117805</v>
       </c>
       <c r="L4" t="n">
-        <v>2617.024983207448</v>
+        <v>3051.022223980327</v>
       </c>
       <c r="M4" t="n">
-        <v>8300.916844970328</v>
+        <v>9768.832452615385</v>
       </c>
       <c r="N4" t="n">
-        <v>16646.32666810305</v>
+        <v>24492.90774630507</v>
       </c>
       <c r="O4" t="n">
-        <v>5165.469518745473</v>
+        <v>9384.411896787971</v>
       </c>
       <c r="P4" t="n">
-        <v>10124.95435155647</v>
+        <v>21193.13139891986</v>
       </c>
     </row>
     <row r="5">
@@ -2151,43 +2151,43 @@
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>91.55318113585399</v>
+        <v>98.77523838766632</v>
       </c>
       <c r="E5" t="n">
-        <v>146.830504234089</v>
+        <v>182.4449492953313</v>
       </c>
       <c r="F5" t="n">
-        <v>244.4457851527939</v>
+        <v>303.7372861333868</v>
       </c>
       <c r="G5" t="n">
-        <v>399.7224789263154</v>
+        <v>496.6770888673728</v>
       </c>
       <c r="H5" t="n">
-        <v>684.5751851416247</v>
+        <v>908.8995797742508</v>
       </c>
       <c r="I5" t="n">
-        <v>1186.011646182998</v>
+        <v>1526.14273675387</v>
       </c>
       <c r="J5" t="n">
-        <v>2108.655415099923</v>
+        <v>2713.387475096445</v>
       </c>
       <c r="K5" t="n">
-        <v>3653.810123354515</v>
+        <v>4701.670341249631</v>
       </c>
       <c r="L5" t="n">
-        <v>7802.494562686706</v>
+        <v>10007.51921423715</v>
       </c>
       <c r="M5" t="n">
-        <v>24763.57241288684</v>
+        <v>31971.10422962547</v>
       </c>
       <c r="N5" t="n">
-        <v>77779.27968348903</v>
+        <v>100176.9135381572</v>
       </c>
       <c r="O5" t="n">
-        <v>31350.23560638283</v>
+        <v>51470.3444823953</v>
       </c>
       <c r="P5" t="n">
-        <v>48971.52581038671</v>
+        <v>106345.6633002872</v>
       </c>
     </row>
     <row r="6">
@@ -2203,43 +2203,43 @@
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>148.0521740449266</v>
+        <v>178.1094979106417</v>
       </c>
       <c r="E6" t="n">
-        <v>237.4420538780867</v>
+        <v>308.8879158497139</v>
       </c>
       <c r="F6" t="n">
-        <v>395.2973504469215</v>
+        <v>514.2415706324564</v>
       </c>
       <c r="G6" t="n">
-        <v>646.3978781016099</v>
+        <v>840.8977690152578</v>
       </c>
       <c r="H6" t="n">
-        <v>1107.03793358125</v>
+        <v>1545.228143993136</v>
       </c>
       <c r="I6" t="n">
-        <v>2186.948131479051</v>
+        <v>2583.831731521353</v>
       </c>
       <c r="J6" t="n">
-        <v>4176.461203786987</v>
+        <v>4593.893145918432</v>
       </c>
       <c r="K6" t="n">
-        <v>6219.588598750239</v>
+        <v>7960.149942929527</v>
       </c>
       <c r="L6" t="n">
-        <v>12617.54390888223</v>
+        <v>16945.22681090576</v>
       </c>
       <c r="M6" t="n">
-        <v>34934.55213132688</v>
+        <v>50239.16827703245</v>
       </c>
       <c r="N6" t="n">
-        <v>95833.45597825578</v>
+        <v>138601.6324661376</v>
       </c>
       <c r="O6" t="n">
-        <v>105893.7729167154</v>
+        <v>153531.5638343118</v>
       </c>
       <c r="P6" t="n">
-        <v>85557.66680171025</v>
+        <v>176570.5257754842</v>
       </c>
     </row>
     <row r="7">
@@ -2255,43 +2255,43 @@
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>99.45016813041953</v>
+        <v>84.46690466986298</v>
       </c>
       <c r="E7" t="n">
-        <v>181.7395097026266</v>
+        <v>211.8425225160794</v>
       </c>
       <c r="F7" t="n">
-        <v>302.5628589527674</v>
+        <v>352.678838878284</v>
       </c>
       <c r="G7" t="n">
-        <v>494.7566428115647</v>
+        <v>576.7072631387975</v>
       </c>
       <c r="H7" t="n">
-        <v>847.3331829186695</v>
+        <v>1037.519435128178</v>
       </c>
       <c r="I7" t="n">
-        <v>1460.774040108754</v>
+        <v>1772.051944009644</v>
       </c>
       <c r="J7" t="n">
-        <v>2609.98900242881</v>
+        <v>3150.598849176669</v>
       </c>
       <c r="K7" t="n">
-        <v>4522.504801224916</v>
+        <v>5459.256115208037</v>
       </c>
       <c r="L7" t="n">
-        <v>9657.803020693467</v>
+        <v>11614.41897133392</v>
       </c>
       <c r="M7" t="n">
-        <v>27643.97631100707</v>
+        <v>37124.44538075489</v>
       </c>
       <c r="N7" t="n">
-        <v>80473.11707004509</v>
+        <v>107238.9329957629</v>
       </c>
       <c r="O7" t="n">
-        <v>112448.0399357743</v>
+        <v>163920.6141183324</v>
       </c>
       <c r="P7" t="n">
-        <v>0</v>
+        <v>33167.44621762988</v>
       </c>
     </row>
     <row r="8">
@@ -2307,43 +2307,43 @@
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>264.8498854381823</v>
+        <v>9.798705624281491</v>
       </c>
       <c r="E8" t="n">
-        <v>682.3536130188461</v>
+        <v>677.2508519195619</v>
       </c>
       <c r="F8" t="n">
-        <v>1135.993270310602</v>
+        <v>1127.498111556853</v>
       </c>
       <c r="G8" t="n">
-        <v>1857.598181814983</v>
+        <v>1843.706733804135</v>
       </c>
       <c r="H8" t="n">
-        <v>3181.371292028729</v>
+        <v>3163.361670701379</v>
       </c>
       <c r="I8" t="n">
-        <v>5428.135407731846</v>
+        <v>5665.168987190257</v>
       </c>
       <c r="J8" t="n">
-        <v>9799.385002528225</v>
+        <v>10072.32036948453</v>
       </c>
       <c r="K8" t="n">
-        <v>16980.05841470751</v>
+        <v>17452.99201953701</v>
       </c>
       <c r="L8" t="n">
-        <v>36262.94698960765</v>
+        <v>37082.34352535135</v>
       </c>
       <c r="M8" t="n">
-        <v>111431.5533832266</v>
+        <v>118700.6417420148</v>
       </c>
       <c r="N8" t="n">
-        <v>321670.3430098767</v>
+        <v>352237.1697130845</v>
       </c>
       <c r="O8" t="n">
-        <v>19187.39790917316</v>
+        <v>83116.1084351538</v>
       </c>
       <c r="P8" t="n">
-        <v>193762.1547203013</v>
+        <v>322329.7043956388</v>
       </c>
     </row>
     <row r="9">
@@ -2362,40 +2362,40 @@
         <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>66.76360867424565</v>
+        <v>8.935625586803306</v>
       </c>
       <c r="F9" t="n">
-        <v>170.7187561653825</v>
+        <v>171.4043168793209</v>
       </c>
       <c r="G9" t="n">
-        <v>279.1626142008936</v>
+        <v>280.283656348782</v>
       </c>
       <c r="H9" t="n">
-        <v>478.1012036514097</v>
+        <v>480.0211297911746</v>
       </c>
       <c r="I9" t="n">
-        <v>795.051194706269</v>
+        <v>803.7104073184553</v>
       </c>
       <c r="J9" t="n">
-        <v>1452.039149273602</v>
+        <v>1531.21249128949</v>
       </c>
       <c r="K9" t="n">
-        <v>2551.788402216336</v>
+        <v>2653.235640881278</v>
       </c>
       <c r="L9" t="n">
-        <v>5451.199864243907</v>
+        <v>5627.804284110681</v>
       </c>
       <c r="M9" t="n">
-        <v>17250.43409206005</v>
+        <v>18040.69842808191</v>
       </c>
       <c r="N9" t="n">
-        <v>48060.15918884776</v>
+        <v>57558.56823977912</v>
       </c>
       <c r="O9" t="n">
-        <v>15813.77897907715</v>
+        <v>17657.84179363448</v>
       </c>
       <c r="P9" t="n">
-        <v>38066.57353476624</v>
+        <v>53571.96318389365</v>
       </c>
     </row>
     <row r="10">
@@ -2411,43 +2411,43 @@
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>57.22125594118082</v>
+        <v>14.47940703819858</v>
       </c>
       <c r="E10" t="n">
-        <v>162.342920278014</v>
+        <v>176.3430510506853</v>
       </c>
       <c r="F10" t="n">
-        <v>270.2711048930888</v>
+        <v>293.5787477893591</v>
       </c>
       <c r="G10" t="n">
-        <v>441.9525415931881</v>
+        <v>480.0656503571744</v>
       </c>
       <c r="H10" t="n">
-        <v>756.8994963646771</v>
+        <v>830.7158546734534</v>
       </c>
       <c r="I10" t="n">
-        <v>1288.42966896859</v>
+        <v>1475.10066777665</v>
       </c>
       <c r="J10" t="n">
-        <v>2331.431603623775</v>
+        <v>2622.637830695306</v>
       </c>
       <c r="K10" t="n">
-        <v>4039.829520853947</v>
+        <v>4544.422283065603</v>
       </c>
       <c r="L10" t="n">
-        <v>8627.649065089841</v>
+        <v>9657.746019280681</v>
       </c>
       <c r="M10" t="n">
-        <v>24019.11904705509</v>
+        <v>30906.64630144563</v>
       </c>
       <c r="N10" t="n">
-        <v>71216.80561193044</v>
+        <v>102414.6235938008</v>
       </c>
       <c r="O10" t="n">
-        <v>0</v>
+        <v>3072.366333588993</v>
       </c>
       <c r="P10" t="n">
-        <v>35880.88945117546</v>
+        <v>85545.09673379212</v>
       </c>
     </row>
     <row r="11">
@@ -2472,34 +2472,34 @@
         <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>259.6912346168967</v>
+        <v>248.6562539773849</v>
       </c>
       <c r="H11" t="n">
-        <v>458.6889245050525</v>
+        <v>546.5968378558126</v>
       </c>
       <c r="I11" t="n">
-        <v>762.7698375178528</v>
+        <v>908.9549778184318</v>
       </c>
       <c r="J11" t="n">
-        <v>1356.15763431444</v>
+        <v>1616.065779984028</v>
       </c>
       <c r="K11" t="n">
-        <v>2349.906228224493</v>
+        <v>2972.413321355654</v>
       </c>
       <c r="L11" t="n">
-        <v>5233.096797543903</v>
+        <v>6414.322024116064</v>
       </c>
       <c r="M11" t="n">
-        <v>15396.37499984868</v>
+        <v>20350.95527354496</v>
       </c>
       <c r="N11" t="n">
-        <v>43328.29714970964</v>
+        <v>56643.46807912795</v>
       </c>
       <c r="O11" t="n">
-        <v>8500.288945277476</v>
+        <v>20739.75872766183</v>
       </c>
       <c r="P11" t="n">
-        <v>28211.56050824761</v>
+        <v>52764.37770682964</v>
       </c>
     </row>
     <row r="12">
@@ -2515,43 +2515,43 @@
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>87.26563623618927</v>
+        <v>121.0982559169156</v>
       </c>
       <c r="E12" t="n">
-        <v>139.9542562246407</v>
+        <v>194.2140923728768</v>
       </c>
       <c r="F12" t="n">
-        <v>232.9980968652488</v>
+        <v>323.3307448303586</v>
       </c>
       <c r="G12" t="n">
-        <v>381.0029974780548</v>
+        <v>528.7166917437264</v>
       </c>
       <c r="H12" t="n">
-        <v>652.5157109969133</v>
+        <v>976.9420230396514</v>
       </c>
       <c r="I12" t="n">
-        <v>2110.614994572949</v>
+        <v>1624.59102098967</v>
       </c>
       <c r="J12" t="n">
-        <v>4050.473109375884</v>
+        <v>2888.422440671385</v>
       </c>
       <c r="K12" t="n">
-        <v>6096.845355843755</v>
+        <v>5004.965286729578</v>
       </c>
       <c r="L12" t="n">
-        <v>7437.09441654358</v>
+        <v>10656.05144881751</v>
       </c>
       <c r="M12" t="n">
-        <v>23856.52053013808</v>
+        <v>34032.54410795829</v>
       </c>
       <c r="N12" t="n">
-        <v>70686.61735953824</v>
+        <v>112792.4953750576</v>
       </c>
       <c r="O12" t="n">
         <v>0</v>
       </c>
       <c r="P12" t="n">
-        <v>47646.2613771669</v>
+        <v>122854.4121397608</v>
       </c>
     </row>
     <row r="13">
@@ -2570,40 +2570,40 @@
         <v>0</v>
       </c>
       <c r="E13" t="n">
-        <v>172.8395956577657</v>
+        <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>465.636085440869</v>
+        <v>402.9741417083473</v>
       </c>
       <c r="G13" t="n">
-        <v>761.4171389113128</v>
+        <v>707.063805675211</v>
       </c>
       <c r="H13" t="n">
-        <v>1304.02293171084</v>
+        <v>1210.935989832778</v>
       </c>
       <c r="I13" t="n">
-        <v>2168.505291061753</v>
+        <v>2013.707763286301</v>
       </c>
       <c r="J13" t="n">
-        <v>3955.105344036573</v>
+        <v>3843.524401525563</v>
       </c>
       <c r="K13" t="n">
-        <v>6960.013001326932</v>
+        <v>6693.243958756352</v>
       </c>
       <c r="L13" t="n">
-        <v>14868.37546845003</v>
+        <v>14195.63215396112</v>
       </c>
       <c r="M13" t="n">
-        <v>37517.80507202096</v>
+        <v>45504.18470049401</v>
       </c>
       <c r="N13" t="n">
-        <v>81059.58948309015</v>
+        <v>113045.0881092228</v>
       </c>
       <c r="O13" t="n">
-        <v>36992.72393219684</v>
+        <v>50836.20822415945</v>
       </c>
       <c r="P13" t="n">
-        <v>69252.8758406589</v>
+        <v>100815.5042938161</v>
       </c>
     </row>
     <row r="14">
@@ -2619,43 +2619,43 @@
         <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>789.2904314056183</v>
+        <v>552.3839091276152</v>
       </c>
       <c r="E14" t="n">
-        <v>2253.627598827564</v>
+        <v>2169.973473116229</v>
       </c>
       <c r="F14" t="n">
-        <v>3989.335048256295</v>
+        <v>4370.272539929459</v>
       </c>
       <c r="G14" t="n">
-        <v>6783.129115781006</v>
+        <v>7443.123184178175</v>
       </c>
       <c r="H14" t="n">
-        <v>11630.89947231622</v>
+        <v>13193.93581400572</v>
       </c>
       <c r="I14" t="n">
-        <v>21251.83446538378</v>
+        <v>22726.20868233802</v>
       </c>
       <c r="J14" t="n">
-        <v>39151.1050694705</v>
+        <v>40900.8029504153</v>
       </c>
       <c r="K14" t="n">
-        <v>66138.47419578109</v>
+        <v>71077.04819381073</v>
       </c>
       <c r="L14" t="n">
-        <v>134973.3853500471</v>
+        <v>151166.0557107247</v>
       </c>
       <c r="M14" t="n">
-        <v>394247.2184102298</v>
+        <v>478764.2341099118</v>
       </c>
       <c r="N14" t="n">
-        <v>1099405.377081997</v>
+        <v>1411952.240122922</v>
       </c>
       <c r="O14" t="n">
-        <v>449942.3174829958</v>
+        <v>752205.704453003</v>
       </c>
       <c r="P14" t="n">
-        <v>820609.796320035</v>
+        <v>1558666.597722584</v>
       </c>
     </row>
   </sheetData>
@@ -2748,25 +2748,25 @@
         <v>2.503174321655522</v>
       </c>
       <c r="H2" t="n">
-        <v>4.773283859624302</v>
+        <v>4.773283859624301</v>
       </c>
       <c r="I2" t="n">
-        <v>9.056507381814567</v>
+        <v>9.056507381814569</v>
       </c>
       <c r="J2" t="n">
         <v>29.31718612605808</v>
       </c>
       <c r="K2" t="n">
-        <v>94.6100008525667</v>
+        <v>94.61000085256671</v>
       </c>
       <c r="L2" t="n">
         <v>305.0250470968311</v>
       </c>
       <c r="M2" t="n">
-        <v>939.7365411296132</v>
+        <v>983.1163787606301</v>
       </c>
       <c r="N2" t="n">
-        <v>2050.63040030939</v>
+        <v>2456.290292367414</v>
       </c>
     </row>
     <row r="3">
@@ -2776,43 +2776,43 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.003748684452011819</v>
+        <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>0.7165239340123314</v>
+        <v>0.4100740110205189</v>
       </c>
       <c r="D3" t="n">
-        <v>2.061382260841575</v>
+        <v>1.483175131811848</v>
       </c>
       <c r="E3" t="n">
-        <v>4.59884960466086</v>
+        <v>3.507893272230222</v>
       </c>
       <c r="F3" t="n">
-        <v>9.386521579098375</v>
+        <v>7.328114376012302</v>
       </c>
       <c r="G3" t="n">
-        <v>18.4198606644848</v>
+        <v>14.53607532151277</v>
       </c>
       <c r="H3" t="n">
-        <v>35.46388863199337</v>
+        <v>28.13599521631258</v>
       </c>
       <c r="I3" t="n">
-        <v>67.62241679210258</v>
+        <v>53.79620932449675</v>
       </c>
       <c r="J3" t="n">
-        <v>219.7745370523016</v>
+        <v>175.2176880963332</v>
       </c>
       <c r="K3" t="n">
-        <v>655.8312822421666</v>
+        <v>561.5007965064417</v>
       </c>
       <c r="L3" t="n">
-        <v>1875.12987067581</v>
+        <v>1652.340101520739</v>
       </c>
       <c r="M3" t="n">
-        <v>1809.028073457925</v>
+        <v>1642.566056224142</v>
       </c>
       <c r="N3" t="n">
-        <v>1776.687727205056</v>
+        <v>1532.665146682843</v>
       </c>
     </row>
     <row r="4">
@@ -2822,43 +2822,43 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.008233046499655602</v>
+        <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>0.09100754775622043</v>
+        <v>0.05855441132790506</v>
       </c>
       <c r="D4" t="n">
-        <v>0.2471857783172527</v>
+        <v>0.1859534743276458</v>
       </c>
       <c r="E4" t="n">
-        <v>0.5418615459859881</v>
+        <v>0.4263289514659627</v>
       </c>
       <c r="F4" t="n">
-        <v>1.097853298096569</v>
+        <v>0.8798673735624508</v>
       </c>
       <c r="G4" t="n">
-        <v>2.146893844798404</v>
+        <v>1.735599841643668</v>
       </c>
       <c r="H4" t="n">
-        <v>4.126214697035813</v>
+        <v>3.350188642176612</v>
       </c>
       <c r="I4" t="n">
-        <v>7.86078058051767</v>
+        <v>6.396581167929164</v>
       </c>
       <c r="J4" t="n">
-        <v>25.5294673703469</v>
+        <v>20.81088404075502</v>
       </c>
       <c r="K4" t="n">
-        <v>82.46923269567216</v>
+        <v>67.2629510602077</v>
       </c>
       <c r="L4" t="n">
-        <v>187.3568076891547</v>
+        <v>176.3956871367366</v>
       </c>
       <c r="M4" t="n">
-        <v>186.4341746994472</v>
+        <v>175.6553642912772</v>
       </c>
       <c r="N4" t="n">
-        <v>171.508888356182</v>
+        <v>161.4643017975993</v>
       </c>
     </row>
     <row r="5">
@@ -2868,43 +2868,43 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.1308207421508001</v>
+        <v>0.1017083542536252</v>
       </c>
       <c r="C5" t="n">
-        <v>0.377652214640918</v>
+        <v>0.3227232067923012</v>
       </c>
       <c r="D5" t="n">
-        <v>0.8433717542947233</v>
+        <v>0.739732165749457</v>
       </c>
       <c r="E5" t="n">
-        <v>1.722087452204908</v>
+        <v>1.526541150996727</v>
       </c>
       <c r="F5" t="n">
-        <v>3.380040816858143</v>
+        <v>3.011085705660465</v>
       </c>
       <c r="G5" t="n">
-        <v>6.508253236304355</v>
+        <v>5.812111845555327</v>
       </c>
       <c r="H5" t="n">
-        <v>12.41053803502318</v>
+        <v>11.0970643326509</v>
       </c>
       <c r="I5" t="n">
-        <v>23.54691919271787</v>
+        <v>21.06866809351621</v>
       </c>
       <c r="J5" t="n">
-        <v>76.22468392775099</v>
+        <v>68.23818002486891</v>
       </c>
       <c r="K5" t="n">
-        <v>245.9860022166734</v>
+        <v>220.2483985447542</v>
       </c>
       <c r="L5" t="n">
-        <v>759.812384536697</v>
+        <v>680.3606665209663</v>
       </c>
       <c r="M5" t="n">
-        <v>873.8832984103292</v>
+        <v>787.5467141983332</v>
       </c>
       <c r="N5" t="n">
-        <v>866.4228450818368</v>
+        <v>833.3452842397636</v>
       </c>
     </row>
     <row r="6">
@@ -2914,43 +2914,43 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.2264205152610002</v>
+        <v>0.1962878579438643</v>
       </c>
       <c r="C6" t="n">
-        <v>0.6536288330323581</v>
+        <v>0.5967747894506821</v>
       </c>
       <c r="D6" t="n">
-        <v>1.459681882433175</v>
+        <v>1.352410152709262</v>
       </c>
       <c r="E6" t="n">
-        <v>2.980535974970033</v>
+        <v>2.778136580432172</v>
       </c>
       <c r="F6" t="n">
-        <v>5.850070644562171</v>
+        <v>5.468185174693028</v>
       </c>
       <c r="G6" t="n">
-        <v>11.26428444744985</v>
+        <v>10.5437461650594</v>
       </c>
       <c r="H6" t="n">
-        <v>21.47977736830935</v>
+        <v>20.12027181663681</v>
       </c>
       <c r="I6" t="n">
-        <v>40.75428321816555</v>
+        <v>38.1891796140979</v>
       </c>
       <c r="J6" t="n">
-        <v>131.9273375672613</v>
+        <v>123.6609395611099</v>
       </c>
       <c r="K6" t="n">
-        <v>386.37683754813</v>
+        <v>377.6770381976071</v>
       </c>
       <c r="L6" t="n">
-        <v>1045.480905649687</v>
+        <v>1040.572139754099</v>
       </c>
       <c r="M6" t="n">
-        <v>1694.949372873396</v>
+        <v>1631.438181458398</v>
       </c>
       <c r="N6" t="n">
-        <v>1867.007285528228</v>
+        <v>1865.606380643969</v>
       </c>
     </row>
     <row r="7">
@@ -2960,43 +2960,43 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.1354347876867726</v>
+        <v>0.08289277144604118</v>
       </c>
       <c r="C7" t="n">
-        <v>0.4266104928735815</v>
+        <v>0.3274746599538316</v>
       </c>
       <c r="D7" t="n">
-        <v>0.9759983566250405</v>
+        <v>0.7889497035306465</v>
       </c>
       <c r="E7" t="n">
-        <v>2.012578742491193</v>
+        <v>1.659656922055701</v>
       </c>
       <c r="F7" t="n">
-        <v>3.968389868396446</v>
+        <v>3.302499955376618</v>
       </c>
       <c r="G7" t="n">
-        <v>7.658597798598102</v>
+        <v>6.402202329158432</v>
       </c>
       <c r="H7" t="n">
-        <v>14.62125098517318</v>
+        <v>12.25069461427118</v>
       </c>
       <c r="I7" t="n">
-        <v>27.75832627021676</v>
+        <v>23.28558051116826</v>
       </c>
       <c r="J7" t="n">
-        <v>89.90160021151155</v>
+        <v>75.48756384822804</v>
       </c>
       <c r="K7" t="n">
-        <v>269.7039043509836</v>
+        <v>243.7156113587952</v>
       </c>
       <c r="L7" t="n">
-        <v>768.2674587401721</v>
+        <v>708.3650440201732</v>
       </c>
       <c r="M7" t="n">
-        <v>1427.383750851408</v>
+        <v>1351.15477793285</v>
       </c>
       <c r="N7" t="n">
-        <v>1059.28946145385</v>
+        <v>991.8723518158238</v>
       </c>
     </row>
     <row r="8">
@@ -3006,43 +3006,43 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.342595984570463</v>
+        <v>0.009133906481236687</v>
       </c>
       <c r="C8" t="n">
-        <v>1.381015995880731</v>
+        <v>0.751842560528262</v>
       </c>
       <c r="D8" t="n">
-        <v>3.340298111552099</v>
+        <v>2.153178982379921</v>
       </c>
       <c r="E8" t="n">
-        <v>7.037055075957986</v>
+        <v>4.797208719353574</v>
       </c>
       <c r="F8" t="n">
-        <v>14.01206492501213</v>
+        <v>9.785941718074557</v>
       </c>
       <c r="G8" t="n">
-        <v>27.1724546565619</v>
+        <v>19.19864104762664</v>
       </c>
       <c r="H8" t="n">
-        <v>52.00336696126166</v>
+        <v>36.95844272297492</v>
       </c>
       <c r="I8" t="n">
-        <v>98.85412278694659</v>
+        <v>70.46748667569543</v>
       </c>
       <c r="J8" t="n">
-        <v>320.48866585766</v>
+        <v>229.0088395538476</v>
       </c>
       <c r="K8" t="n">
-        <v>1011.273708355151</v>
+        <v>739.9300831427047</v>
       </c>
       <c r="L8" t="n">
-        <v>2915.599411843873</v>
+        <v>2194.933745968395</v>
       </c>
       <c r="M8" t="n">
-        <v>2568.116018450805</v>
+        <v>2039.015305516578</v>
       </c>
       <c r="N8" t="n">
-        <v>2452.857462222711</v>
+        <v>1938.144077184085</v>
       </c>
     </row>
     <row r="9">
@@ -3055,40 +3055,40 @@
         <v>0</v>
       </c>
       <c r="C9" t="n">
-        <v>0.0950667709775731</v>
+        <v>0.009168943025830545</v>
       </c>
       <c r="D9" t="n">
-        <v>0.370570727575005</v>
+        <v>0.2084994305585804</v>
       </c>
       <c r="E9" t="n">
-        <v>0.890389268318406</v>
+        <v>0.5845945125843847</v>
       </c>
       <c r="F9" t="n">
-        <v>1.871178505024118</v>
+        <v>1.294207540048418</v>
       </c>
       <c r="G9" t="n">
-        <v>3.721723361431271</v>
+        <v>2.633099412907636</v>
       </c>
       <c r="H9" t="n">
-        <v>7.213315782528062</v>
+        <v>5.159309301718235</v>
       </c>
       <c r="I9" t="n">
-        <v>13.80122290234244</v>
+        <v>9.925740805030133</v>
       </c>
       <c r="J9" t="n">
-        <v>44.9754610967549</v>
+        <v>32.48618876042669</v>
       </c>
       <c r="K9" t="n">
-        <v>145.2357592692406</v>
+        <v>105.190325038056</v>
       </c>
       <c r="L9" t="n">
-        <v>411.3327793681321</v>
+        <v>329.6862417845222</v>
       </c>
       <c r="M9" t="n">
-        <v>441.1974771445059</v>
+        <v>329.9911109288161</v>
       </c>
       <c r="N9" t="n">
-        <v>479.8039875631497</v>
+        <v>318.596045338314</v>
       </c>
     </row>
     <row r="10">
@@ -3098,43 +3098,43 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.09237945981457447</v>
+        <v>0.01684512276934954</v>
       </c>
       <c r="C10" t="n">
-        <v>0.4007213005874471</v>
+        <v>0.2582037507714855</v>
       </c>
       <c r="D10" t="n">
-        <v>0.9824980841234222</v>
+        <v>0.7135971736224923</v>
       </c>
       <c r="E10" t="n">
-        <v>2.080189610557489</v>
+        <v>1.572829641475767</v>
       </c>
       <c r="F10" t="n">
-        <v>4.151304720861033</v>
+        <v>3.194022212047379</v>
       </c>
       <c r="G10" t="n">
-        <v>8.059067235948017</v>
+        <v>6.252874675389581</v>
       </c>
       <c r="H10" t="n">
-        <v>15.43220057766792</v>
+        <v>12.02429169415599</v>
       </c>
       <c r="I10" t="n">
-        <v>29.34376635601248</v>
+        <v>22.91375262883337</v>
       </c>
       <c r="J10" t="n">
-        <v>95.15538274684637</v>
+        <v>74.43378204050794</v>
       </c>
       <c r="K10" t="n">
-        <v>280.1643476752449</v>
+        <v>240.4641395395871</v>
       </c>
       <c r="L10" t="n">
-        <v>802.729001447505</v>
+        <v>775.51972716364</v>
       </c>
       <c r="M10" t="n">
-        <v>671.813867686446</v>
+        <v>614.0680784774377</v>
       </c>
       <c r="N10" t="n">
-        <v>584.4972555297353</v>
+        <v>528.6985327224238</v>
       </c>
     </row>
     <row r="11">
@@ -3153,34 +3153,34 @@
         <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>0.6698516897808605</v>
+        <v>0.4621959374601514</v>
       </c>
       <c r="F11" t="n">
-        <v>1.973321464222696</v>
+        <v>1.581518342839392</v>
       </c>
       <c r="G11" t="n">
-        <v>4.432697236613331</v>
+        <v>3.693446413026149</v>
       </c>
       <c r="H11" t="n">
-        <v>9.073026692976903</v>
+        <v>7.678214476461433</v>
       </c>
       <c r="I11" t="n">
-        <v>17.82836115846391</v>
+        <v>15.19664123707059</v>
       </c>
       <c r="J11" t="n">
-        <v>59.30636666129892</v>
+        <v>50.82528844034267</v>
       </c>
       <c r="K11" t="n">
-        <v>182.9444664198378</v>
+        <v>164.7347231683008</v>
       </c>
       <c r="L11" t="n">
-        <v>513.6946862391508</v>
+        <v>465.1246635154781</v>
       </c>
       <c r="M11" t="n">
-        <v>500.846136414828</v>
+        <v>470.6859767956803</v>
       </c>
       <c r="N11" t="n">
-        <v>497.2631801999037</v>
+        <v>455.4254143101572</v>
       </c>
     </row>
     <row r="12">
@@ -3208,25 +3208,25 @@
         <v>7.008888100635455</v>
       </c>
       <c r="H12" t="n">
-        <v>13.36519480694804</v>
+        <v>13.36519480694803</v>
       </c>
       <c r="I12" t="n">
         <v>25.35822066908078</v>
       </c>
       <c r="J12" t="n">
-        <v>82.08812115296256</v>
+        <v>82.08812115296257</v>
       </c>
       <c r="K12" t="n">
         <v>264.9080023871866</v>
       </c>
       <c r="L12" t="n">
-        <v>785.5856670529024</v>
+        <v>854.0701318711267</v>
       </c>
       <c r="M12" t="n">
-        <v>656.8384684189492</v>
+        <v>656.1054009469023</v>
       </c>
       <c r="N12" t="n">
-        <v>674.3387114248378</v>
+        <v>732.958777971108</v>
       </c>
     </row>
     <row r="13">
@@ -3239,40 +3239,40 @@
         <v>0</v>
       </c>
       <c r="C13" t="n">
-        <v>0.2531519347725284</v>
+        <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>1.026085738191558</v>
+        <v>0.4820346099360497</v>
       </c>
       <c r="E13" t="n">
-        <v>2.484450716853616</v>
+        <v>1.457939638492518</v>
       </c>
       <c r="F13" t="n">
-        <v>5.236081453638681</v>
+        <v>3.299269012174185</v>
       </c>
       <c r="G13" t="n">
-        <v>10.4278351109204</v>
+        <v>6.773473738220165</v>
       </c>
       <c r="H13" t="n">
-        <v>20.22359210605807</v>
+        <v>13.32857390172135</v>
       </c>
       <c r="I13" t="n">
-        <v>38.70614375278419</v>
+        <v>25.69668158155775</v>
       </c>
       <c r="J13" t="n">
-        <v>126.1675645500219</v>
+        <v>84.24278927669846</v>
       </c>
       <c r="K13" t="n">
-        <v>348.1172006055585</v>
+        <v>272.9156472273797</v>
       </c>
       <c r="L13" t="n">
-        <v>783.2709785112825</v>
+        <v>711.2078880900289</v>
       </c>
       <c r="M13" t="n">
-        <v>857.5299101139701</v>
+        <v>740.9729653253454</v>
       </c>
       <c r="N13" t="n">
-        <v>930.6086567386969</v>
+        <v>697.7101059696763</v>
       </c>
     </row>
     <row r="14">
@@ -3282,43 +3282,43 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>1.130832766655678</v>
+        <v>0.598067559114517</v>
       </c>
       <c r="C14" t="n">
-        <v>4.94733226131657</v>
+        <v>3.286769569653697</v>
       </c>
       <c r="D14" t="n">
-        <v>12.53969295023076</v>
+        <v>9.340151080902807</v>
       </c>
       <c r="E14" t="n">
-        <v>27.53474672731159</v>
+        <v>21.29022237207743</v>
       </c>
       <c r="F14" t="n">
-        <v>55.86688693117842</v>
+        <v>44.08477106589685</v>
       </c>
       <c r="G14" t="n">
-        <v>109.3237300154014</v>
+        <v>87.09333321239075</v>
       </c>
       <c r="H14" t="n">
-        <v>210.1856505045998</v>
+        <v>168.2415253856523</v>
       </c>
       <c r="I14" t="n">
-        <v>400.4910710611654</v>
+        <v>321.3512496902909</v>
       </c>
       <c r="J14" t="n">
-        <v>1300.856374320775</v>
+        <v>1045.817450922139</v>
       </c>
       <c r="K14" t="n">
-        <v>3967.620744618412</v>
+        <v>3353.157717023588</v>
       </c>
       <c r="L14" t="n">
-        <v>11153.2849988512</v>
+        <v>9893.601084442736</v>
       </c>
       <c r="M14" t="n">
-        <v>12627.75708965162</v>
+        <v>11422.31631085639</v>
       </c>
       <c r="N14" t="n">
-        <v>13410.91586161358</v>
+        <v>12512.77671104317</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add co2 storage share to test
</commit_message>
<xml_diff>
--- a/tutorial/dac_scenarios/SSPs/get_report_output.xlsx
+++ b/tutorial/dac_scenarios/SSPs/get_report_output.xlsx
@@ -537,7 +537,7 @@
         <v>1076.512445508014</v>
       </c>
       <c r="P2" t="n">
-        <v>2689.637897038697</v>
+        <v>2549.929988284399</v>
       </c>
     </row>
     <row r="3">
@@ -556,40 +556,40 @@
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>0.4490310465577787</v>
+        <v>0.5677495884918854</v>
       </c>
       <c r="F3" t="n">
-        <v>1.624076785574742</v>
+        <v>1.848073928808317</v>
       </c>
       <c r="G3" t="n">
-        <v>3.841143171503525</v>
+        <v>4.263779091380739</v>
       </c>
       <c r="H3" t="n">
-        <v>8.024285321976325</v>
+        <v>8.821711209610077</v>
       </c>
       <c r="I3" t="n">
-        <v>15.91700263622652</v>
+        <v>17.42157907273295</v>
       </c>
       <c r="J3" t="n">
-        <v>30.80891506995142</v>
+        <v>33.64773719548809</v>
       </c>
       <c r="K3" t="n">
-        <v>58.90684979939245</v>
+        <v>64.26311543329334</v>
       </c>
       <c r="L3" t="n">
-        <v>191.8633703841186</v>
+        <v>209.1246706630947</v>
       </c>
       <c r="M3" t="n">
-        <v>614.8433783229875</v>
+        <v>659.3736072645478</v>
       </c>
       <c r="N3" t="n">
-        <v>1809.312429258334</v>
+        <v>1929.578841213178</v>
       </c>
       <c r="O3" t="n">
-        <v>1798.609849551534</v>
+        <v>1897.653199332078</v>
       </c>
       <c r="P3" t="n">
-        <v>1678.268352400397</v>
+        <v>1857.304118185554</v>
       </c>
     </row>
     <row r="4">
@@ -608,40 +608,40 @@
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>0.06411708104522686</v>
+        <v>0.06290082651422882</v>
       </c>
       <c r="F4" t="n">
-        <v>0.2036190564249627</v>
+        <v>0.2013242376380232</v>
       </c>
       <c r="G4" t="n">
-        <v>0.4668302065235313</v>
+        <v>0.4625003617988673</v>
       </c>
       <c r="H4" t="n">
-        <v>0.9634547836854316</v>
+        <v>0.9552852691920004</v>
       </c>
       <c r="I4" t="n">
-        <v>1.900481845604636</v>
+        <v>1.885067674588708</v>
       </c>
       <c r="J4" t="n">
-        <v>3.668456599867956</v>
+        <v>3.639373272052172</v>
       </c>
       <c r="K4" t="n">
-        <v>7.004256448925</v>
+        <v>6.949382271392757</v>
       </c>
       <c r="L4" t="n">
-        <v>22.78791825250593</v>
+        <v>22.61107869287862</v>
       </c>
       <c r="M4" t="n">
-        <v>73.65293214745677</v>
+        <v>73.08304242417474</v>
       </c>
       <c r="N4" t="n">
-        <v>193.1532793462594</v>
+        <v>192.8151147551188</v>
       </c>
       <c r="O4" t="n">
-        <v>192.3426258223748</v>
+        <v>192.2495735159291</v>
       </c>
       <c r="P4" t="n">
-        <v>176.8034122364053</v>
+        <v>176.8703036643627</v>
       </c>
     </row>
     <row r="5">
@@ -657,43 +657,43 @@
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>0.1113706490214261</v>
+        <v>0.1059984610390926</v>
       </c>
       <c r="E5" t="n">
-        <v>0.353381914971389</v>
+        <v>0.3432457160141582</v>
       </c>
       <c r="F5" t="n">
-        <v>0.8100067295957228</v>
+        <v>0.7908818349273985</v>
       </c>
       <c r="G5" t="n">
-        <v>1.671562577057043</v>
+        <v>1.635477887163147</v>
       </c>
       <c r="H5" t="n">
-        <v>3.297138880669598</v>
+        <v>3.229054592242367</v>
       </c>
       <c r="I5" t="n">
-        <v>6.364262534525709</v>
+        <v>6.235801673582392</v>
       </c>
       <c r="J5" t="n">
-        <v>12.15128556576559</v>
+        <v>11.90890669722625</v>
       </c>
       <c r="K5" t="n">
-        <v>23.07019179310217</v>
+        <v>22.61287338901386</v>
       </c>
       <c r="L5" t="n">
-        <v>74.72080787443954</v>
+        <v>73.24703662491294</v>
       </c>
       <c r="M5" t="n">
-        <v>241.1719988182259</v>
+        <v>236.4225689319277</v>
       </c>
       <c r="N5" t="n">
-        <v>744.9949372904075</v>
+        <v>737.6657013446001</v>
       </c>
       <c r="O5" t="n">
-        <v>862.3636606708116</v>
+        <v>851.6441665932373</v>
       </c>
       <c r="P5" t="n">
-        <v>912.5130953676722</v>
+        <v>892.6089386627436</v>
       </c>
     </row>
     <row r="6">
@@ -709,43 +709,43 @@
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>0.2149352065978835</v>
+        <v>0.2176664078599483</v>
       </c>
       <c r="E6" t="n">
-        <v>0.6534684009831808</v>
+        <v>0.6586216084799341</v>
       </c>
       <c r="F6" t="n">
-        <v>1.480889132025533</v>
+        <v>1.490612160450218</v>
       </c>
       <c r="G6" t="n">
-        <v>3.042059585993825</v>
+        <v>3.060404913987469</v>
       </c>
       <c r="H6" t="n">
-        <v>5.987662826165495</v>
+        <v>6.022276636235198</v>
       </c>
       <c r="I6" t="n">
-        <v>11.54540216619406</v>
+        <v>11.61071121097956</v>
       </c>
       <c r="J6" t="n">
-        <v>22.03169785953429</v>
+        <v>22.15492241419049</v>
       </c>
       <c r="K6" t="n">
-        <v>41.81715209560873</v>
+        <v>42.04965114562687</v>
       </c>
       <c r="L6" t="n">
-        <v>135.4087301735026</v>
+        <v>136.1579902347549</v>
       </c>
       <c r="M6" t="n">
-        <v>413.5563609619434</v>
+        <v>413.7126980136905</v>
       </c>
       <c r="N6" t="n">
-        <v>1139.426504425004</v>
+        <v>1139.315674625472</v>
       </c>
       <c r="O6" t="n">
-        <v>1786.424826561195</v>
+        <v>1737.620694376152</v>
       </c>
       <c r="P6" t="n">
-        <v>2042.839007233536</v>
+        <v>2042.797556084721</v>
       </c>
     </row>
     <row r="7">
@@ -761,43 +761,43 @@
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>0.09076758564109094</v>
+        <v>0.09328771196663604</v>
       </c>
       <c r="E7" t="n">
-        <v>0.3585847562352932</v>
+        <v>0.3633397093227658</v>
       </c>
       <c r="F7" t="n">
-        <v>0.8638999340050573</v>
+        <v>0.8728715393705838</v>
       </c>
       <c r="G7" t="n">
-        <v>1.817324347824236</v>
+        <v>1.834251897129991</v>
       </c>
       <c r="H7" t="n">
-        <v>3.616237487299772</v>
+        <v>3.648176244503674</v>
       </c>
       <c r="I7" t="n">
-        <v>7.010411620532601</v>
+        <v>7.070673398141659</v>
       </c>
       <c r="J7" t="n">
-        <v>13.41451073677205</v>
+        <v>13.52821215030608</v>
       </c>
       <c r="K7" t="n">
-        <v>25.49771091470636</v>
+        <v>25.71224178240668</v>
       </c>
       <c r="L7" t="n">
-        <v>82.65888324039852</v>
+        <v>83.35023837092959</v>
       </c>
       <c r="M7" t="n">
-        <v>266.8685971065668</v>
+        <v>269.0965837904191</v>
       </c>
       <c r="N7" t="n">
-        <v>775.659730958687</v>
+        <v>782.2115354499407</v>
       </c>
       <c r="O7" t="n">
-        <v>1479.514496631615</v>
+        <v>1477.887186176543</v>
       </c>
       <c r="P7" t="n">
-        <v>1086.100236099329</v>
+        <v>1086.098499154616</v>
       </c>
     </row>
     <row r="8">
@@ -813,43 +813,43 @@
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>0.01000162769697045</v>
+        <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>0.8232676120111231</v>
+        <v>0.804396625261213</v>
       </c>
       <c r="F8" t="n">
-        <v>2.357731009283324</v>
+        <v>2.322125390707545</v>
       </c>
       <c r="G8" t="n">
-        <v>5.252943600221599</v>
+        <v>5.185763219515227</v>
       </c>
       <c r="H8" t="n">
-        <v>10.7156062884477</v>
+        <v>10.58885091296538</v>
       </c>
       <c r="I8" t="n">
-        <v>21.02251215737629</v>
+        <v>20.78335118441472</v>
       </c>
       <c r="J8" t="n">
-        <v>40.46949518635249</v>
+        <v>40.0182482804893</v>
       </c>
       <c r="K8" t="n">
-        <v>77.16189868150549</v>
+        <v>76.31048982691858</v>
       </c>
       <c r="L8" t="n">
-        <v>250.7646818191099</v>
+        <v>248.0209000682224</v>
       </c>
       <c r="M8" t="n">
-        <v>810.2234491434962</v>
+        <v>801.3812363147882</v>
       </c>
       <c r="N8" t="n">
-        <v>2403.452475869918</v>
+        <v>2377.601168957217</v>
       </c>
       <c r="O8" t="n">
-        <v>2232.721781867871</v>
+        <v>2234.56535062146</v>
       </c>
       <c r="P8" t="n">
-        <v>2122.267785739251</v>
+        <v>2120.473730945449</v>
       </c>
     </row>
     <row r="9">
@@ -868,40 +868,40 @@
         <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>0.01003999271368437</v>
+        <v>0.0123417173298066</v>
       </c>
       <c r="F9" t="n">
-        <v>0.2283068787447144</v>
+        <v>0.2326497533296124</v>
       </c>
       <c r="G9" t="n">
-        <v>0.6401309976812113</v>
+        <v>0.6483250968049924</v>
       </c>
       <c r="H9" t="n">
-        <v>1.41715727052459</v>
+        <v>1.432617827613629</v>
       </c>
       <c r="I9" t="n">
-        <v>2.883243885966301</v>
+        <v>2.912414734633449</v>
       </c>
       <c r="J9" t="n">
-        <v>5.649443741875904</v>
+        <v>5.704483053012044</v>
       </c>
       <c r="K9" t="n">
-        <v>10.86868629019486</v>
+        <v>10.97253399805234</v>
       </c>
       <c r="L9" t="n">
-        <v>35.572377048391</v>
+        <v>35.90704052311973</v>
       </c>
       <c r="M9" t="n">
-        <v>115.1834070685054</v>
+        <v>116.2619059937895</v>
       </c>
       <c r="N9" t="n">
-        <v>361.0064383641163</v>
+        <v>359.6553935835182</v>
       </c>
       <c r="O9" t="n">
-        <v>361.3402700804563</v>
+        <v>343.1258449179838</v>
       </c>
       <c r="P9" t="n">
-        <v>348.8626731340805</v>
+        <v>319.7742841148242</v>
       </c>
     </row>
     <row r="10">
@@ -917,43 +917,43 @@
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>0.01844540961689184</v>
+        <v>0.01267356759353133</v>
       </c>
       <c r="E10" t="n">
-        <v>0.2827331099221077</v>
+        <v>0.2718428470923482</v>
       </c>
       <c r="F10" t="n">
-        <v>0.7813889129305183</v>
+        <v>0.7608412569099205</v>
       </c>
       <c r="G10" t="n">
-        <v>1.722248474638449</v>
+        <v>1.683479330629633</v>
       </c>
       <c r="H10" t="n">
-        <v>3.497454357166423</v>
+        <v>3.424305063365242</v>
       </c>
       <c r="I10" t="n">
-        <v>6.846897838020571</v>
+        <v>6.708880367673668</v>
       </c>
       <c r="J10" t="n">
-        <v>13.16659953676681</v>
+        <v>12.90618933823868</v>
       </c>
       <c r="K10" t="n">
-        <v>25.09055937947814</v>
+        <v>24.59921961410631</v>
       </c>
       <c r="L10" t="n">
-        <v>81.50499214940612</v>
+        <v>79.92158239926121</v>
       </c>
       <c r="M10" t="n">
-        <v>263.3082354289302</v>
+        <v>258.2054804443899</v>
       </c>
       <c r="N10" t="n">
-        <v>849.194109736127</v>
+        <v>832.7497822776986</v>
       </c>
       <c r="O10" t="n">
-        <v>672.4045526568398</v>
+        <v>684.1166709308459</v>
       </c>
       <c r="P10" t="n">
-        <v>578.9248991203031</v>
+        <v>579.5186851346975</v>
       </c>
     </row>
     <row r="11">
@@ -978,34 +978,34 @@
         <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>0.5061045565799114</v>
+        <v>0.459680735841237</v>
       </c>
       <c r="H11" t="n">
-        <v>1.731762602726761</v>
+        <v>1.644170529458017</v>
       </c>
       <c r="I11" t="n">
-        <v>4.044323862706872</v>
+        <v>3.879055877921525</v>
       </c>
       <c r="J11" t="n">
-        <v>8.407644935801718</v>
+        <v>8.095818696557348</v>
       </c>
       <c r="K11" t="n">
-        <v>16.64032232099552</v>
+        <v>16.05197120382314</v>
       </c>
       <c r="L11" t="n">
-        <v>55.65369139871215</v>
+        <v>53.75764926840662</v>
       </c>
       <c r="M11" t="n">
-        <v>180.3845236731346</v>
+        <v>175.2693657851947</v>
       </c>
       <c r="N11" t="n">
-        <v>509.3115116425636</v>
+        <v>495.024948693582</v>
       </c>
       <c r="O11" t="n">
-        <v>515.4011497452815</v>
+        <v>491.1724913513273</v>
       </c>
       <c r="P11" t="n">
-        <v>498.6908336565305</v>
+        <v>486.5767336032999</v>
       </c>
     </row>
     <row r="12">
@@ -1057,7 +1057,7 @@
         <v>718.4354212212122</v>
       </c>
       <c r="P12" t="n">
-        <v>802.5898699042621</v>
+        <v>792.3323765467517</v>
       </c>
     </row>
     <row r="13">
@@ -1079,37 +1079,37 @@
         <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>0.5278279031582536</v>
+        <v>0.5253006187890602</v>
       </c>
       <c r="G13" t="n">
-        <v>1.596443920113747</v>
+        <v>1.591675461289914</v>
       </c>
       <c r="H13" t="n">
-        <v>3.612699604457729</v>
+        <v>3.603702516582793</v>
       </c>
       <c r="I13" t="n">
-        <v>7.41695381752062</v>
+        <v>7.39997818803112</v>
       </c>
       <c r="J13" t="n">
-        <v>14.59478856833276</v>
+        <v>14.56275909384385</v>
       </c>
       <c r="K13" t="n">
-        <v>28.13786661318441</v>
+        <v>28.07743367096741</v>
       </c>
       <c r="L13" t="n">
-        <v>92.24585518044336</v>
+        <v>92.05110173958575</v>
       </c>
       <c r="M13" t="n">
-        <v>298.8426367024072</v>
+        <v>298.2150170411024</v>
       </c>
       <c r="N13" t="n">
-        <v>778.7726452463081</v>
+        <v>683.1478321236802</v>
       </c>
       <c r="O13" t="n">
-        <v>811.3654051449073</v>
+        <v>797.3896347198831</v>
       </c>
       <c r="P13" t="n">
-        <v>763.9925736767213</v>
+        <v>751.0526546848929</v>
       </c>
     </row>
     <row r="14">
@@ -1125,43 +1125,43 @@
         <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>0.6548839837792361</v>
+        <v>0.6389896536641816</v>
       </c>
       <c r="E14" t="n">
-        <v>3.599012714760926</v>
+        <v>3.688827438827482</v>
       </c>
       <c r="F14" t="n">
-        <v>10.22746553586323</v>
+        <v>10.39439991505108</v>
       </c>
       <c r="G14" t="n">
-        <v>23.31279373055272</v>
+        <v>23.58134028795686</v>
       </c>
       <c r="H14" t="n">
-        <v>48.27282479988531</v>
+        <v>48.77951617853385</v>
       </c>
       <c r="I14" t="n">
-        <v>95.36720082123988</v>
+        <v>96.32322183926544</v>
       </c>
       <c r="J14" t="n">
-        <v>184.224472139534</v>
+        <v>186.0282845299174</v>
       </c>
       <c r="K14" t="n">
-        <v>351.8796219296648</v>
+        <v>355.2830399281729</v>
       </c>
       <c r="L14" t="n">
-        <v>1145.170120211444</v>
+        <v>1156.138101275582</v>
       </c>
       <c r="M14" t="n">
-        <v>3671.707736857906</v>
+        <v>3694.693723488276</v>
       </c>
       <c r="N14" t="n">
-        <v>10833.49329579973</v>
+        <v>10798.97522668601</v>
       </c>
       <c r="O14" t="n">
-        <v>12507.43648546211</v>
+        <v>12502.37267926467</v>
       </c>
       <c r="P14" t="n">
-        <v>13701.49063560719</v>
+        <v>13655.33786906631</v>
       </c>
     </row>
   </sheetData>
@@ -1284,7 +1284,7 @@
         <v>81.99283665004386</v>
       </c>
       <c r="P2" t="n">
-        <v>186.9709530538258</v>
+        <v>173.0001621783961</v>
       </c>
     </row>
     <row r="3">
@@ -1303,40 +1303,40 @@
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>0.08980620931155575</v>
+        <v>0.1135499176983771</v>
       </c>
       <c r="F3" t="n">
-        <v>0.2350091478033926</v>
+        <v>0.2560648680632862</v>
       </c>
       <c r="G3" t="n">
-        <v>0.4434132771857567</v>
+        <v>0.4831410325144844</v>
       </c>
       <c r="H3" t="n">
-        <v>0.83662843009456</v>
+        <v>0.9115864236458679</v>
       </c>
       <c r="I3" t="n">
-        <v>1.668349672161594</v>
+        <v>1.833523490322952</v>
       </c>
       <c r="J3" t="n">
-        <v>3.213391634548375</v>
+        <v>3.501296492614314</v>
       </c>
       <c r="K3" t="n">
-        <v>6.063000223073961</v>
+        <v>6.606216680075535</v>
       </c>
       <c r="L3" t="n">
-        <v>14.13105369156029</v>
+        <v>15.40032960738381</v>
       </c>
       <c r="M3" t="n">
-        <v>45.83753408496997</v>
+        <v>48.88547694905209</v>
       </c>
       <c r="N3" t="n">
-        <v>135.0937088408634</v>
+        <v>144.0724071722657</v>
       </c>
       <c r="O3" t="n">
-        <v>44.76727611428996</v>
+        <v>45.69291276094204</v>
       </c>
       <c r="P3" t="n">
-        <v>123.0595591257497</v>
+        <v>140.0374990576134</v>
       </c>
     </row>
     <row r="4">
@@ -1355,40 +1355,40 @@
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>0.01282341620904537</v>
+        <v>0.01258016530284576</v>
       </c>
       <c r="F4" t="n">
-        <v>0.02790039507594718</v>
+        <v>0.02768468222475888</v>
       </c>
       <c r="G4" t="n">
-        <v>0.05264223001971372</v>
+        <v>0.05223522483216882</v>
       </c>
       <c r="H4" t="n">
-        <v>0.09932491543238006</v>
+        <v>0.09855698147862663</v>
       </c>
       <c r="I4" t="n">
-        <v>0.2002288285928862</v>
+        <v>0.1985366463821873</v>
       </c>
       <c r="J4" t="n">
-        <v>0.3814953459286113</v>
+        <v>0.3785458017174517</v>
       </c>
       <c r="K4" t="n">
-        <v>0.7198021998311225</v>
+        <v>0.7142370247002858</v>
       </c>
       <c r="L4" t="n">
-        <v>1.678085845222505</v>
+        <v>1.665082294483447</v>
       </c>
       <c r="M4" t="n">
-        <v>5.507256819565391</v>
+        <v>5.464662691758956</v>
       </c>
       <c r="N4" t="n">
-        <v>13.80807111506055</v>
+        <v>13.81684878375293</v>
       </c>
       <c r="O4" t="n">
-        <v>5.426191467176933</v>
+        <v>5.408108567839985</v>
       </c>
       <c r="P4" t="n">
-        <v>12.2541497564636</v>
+        <v>12.27892179859629</v>
       </c>
     </row>
     <row r="5">
@@ -1404,43 +1404,43 @@
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>0.02227412980428522</v>
+        <v>0.02119969220781852</v>
       </c>
       <c r="E5" t="n">
-        <v>0.04840225318999258</v>
+        <v>0.04744945099501312</v>
       </c>
       <c r="F5" t="n">
-        <v>0.09132496292486678</v>
+        <v>0.08952722378264805</v>
       </c>
       <c r="G5" t="n">
-        <v>0.172311169492264</v>
+        <v>0.1689192104471497</v>
       </c>
       <c r="H5" t="n">
-        <v>0.3473893905267964</v>
+        <v>0.3399150332236625</v>
       </c>
       <c r="I5" t="n">
-        <v>0.6618269839612148</v>
+        <v>0.6487988672630183</v>
       </c>
       <c r="J5" t="n">
-        <v>1.248729569172843</v>
+        <v>1.22414822851142</v>
       </c>
       <c r="K5" t="n">
-        <v>2.356092414959581</v>
+        <v>2.30971254880467</v>
       </c>
       <c r="L5" t="n">
-        <v>5.504213049387438</v>
+        <v>5.395573557017493</v>
       </c>
       <c r="M5" t="n">
-        <v>18.02396372869525</v>
+        <v>17.66925519897411</v>
       </c>
       <c r="N5" t="n">
-        <v>56.4755300003455</v>
+        <v>56.0973149354859</v>
       </c>
       <c r="O5" t="n">
-        <v>29.76083606673566</v>
+        <v>29.06710172383784</v>
       </c>
       <c r="P5" t="n">
-        <v>61.49047347003157</v>
+        <v>60.19379214243652</v>
       </c>
     </row>
     <row r="6">
@@ -1456,43 +1456,43 @@
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0429870413195767</v>
+        <v>0.04353328157198966</v>
       </c>
       <c r="E6" t="n">
-        <v>0.08770663887705948</v>
+        <v>0.08819104012399716</v>
       </c>
       <c r="F6" t="n">
-        <v>0.1654841462084704</v>
+        <v>0.1663981103940569</v>
       </c>
       <c r="G6" t="n">
-        <v>0.3122340907936585</v>
+        <v>0.3139585507074502</v>
       </c>
       <c r="H6" t="n">
-        <v>0.6321076893539106</v>
+        <v>0.6359076260215353</v>
       </c>
       <c r="I6" t="n">
-        <v>1.199254506882773</v>
+        <v>1.205877955072869</v>
       </c>
       <c r="J6" t="n">
-        <v>2.262743284876516</v>
+        <v>2.275240351036245</v>
       </c>
       <c r="K6" t="n">
-        <v>4.269324938008547</v>
+        <v>4.292904296994726</v>
       </c>
       <c r="L6" t="n">
-        <v>9.975025279187044</v>
+        <v>10.03025721069179</v>
       </c>
       <c r="M6" t="n">
-        <v>30.31327958250516</v>
+        <v>30.26778651642858</v>
       </c>
       <c r="N6" t="n">
-        <v>83.62937085999521</v>
+        <v>83.66378094611866</v>
       </c>
       <c r="O6" t="n">
-        <v>95.01311179612425</v>
+        <v>90.09828849149655</v>
       </c>
       <c r="P6" t="n">
-        <v>109.2707889272293</v>
+        <v>114.1814671169756</v>
       </c>
     </row>
     <row r="7">
@@ -1508,43 +1508,43 @@
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>0.01815351712821819</v>
+        <v>0.01865754239332721</v>
       </c>
       <c r="E7" t="n">
-        <v>0.05356343411884045</v>
+        <v>0.05401039947122595</v>
       </c>
       <c r="F7" t="n">
-        <v>0.1010630355539528</v>
+        <v>0.1019063660095636</v>
       </c>
       <c r="G7" t="n">
-        <v>0.1906848827638358</v>
+        <v>0.1922760715518815</v>
       </c>
       <c r="H7" t="n">
-        <v>0.3779361450233254</v>
+        <v>0.3814424118680638</v>
       </c>
       <c r="I7" t="n">
-        <v>0.7323982607654062</v>
+        <v>0.738509830198823</v>
       </c>
       <c r="J7" t="n">
-        <v>1.381882858801843</v>
+        <v>1.393414116442447</v>
       </c>
       <c r="K7" t="n">
-        <v>2.607324918350697</v>
+        <v>2.629081997972003</v>
       </c>
       <c r="L7" t="n">
-        <v>6.088184870272232</v>
+        <v>6.139148322336029</v>
       </c>
       <c r="M7" t="n">
-        <v>19.94684361079677</v>
+        <v>20.11323955721289</v>
       </c>
       <c r="N7" t="n">
-        <v>57.61912948507193</v>
+        <v>58.10791398778119</v>
       </c>
       <c r="O7" t="n">
-        <v>90.33232017808962</v>
+        <v>89.68080462987311</v>
       </c>
       <c r="P7" t="n">
-        <v>18.27770343184332</v>
+        <v>18.92904528558854</v>
       </c>
     </row>
     <row r="8">
@@ -1560,43 +1560,43 @@
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>0.00200032553939409</v>
+        <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>0.1626531968628305</v>
+        <v>0.1608793250522426</v>
       </c>
       <c r="F8" t="n">
-        <v>0.3068926794544402</v>
+        <v>0.3035457530892663</v>
       </c>
       <c r="G8" t="n">
-        <v>0.5790425181876552</v>
+        <v>0.5727275657615364</v>
       </c>
       <c r="H8" t="n">
-        <v>1.094532863184615</v>
+        <v>1.080617538690031</v>
       </c>
       <c r="I8" t="n">
-        <v>2.224034370648548</v>
+        <v>2.199779379342111</v>
       </c>
       <c r="J8" t="n">
-        <v>4.19628928524968</v>
+        <v>4.150525172304183</v>
       </c>
       <c r="K8" t="n">
-        <v>7.917523217218257</v>
+        <v>7.831175875047393</v>
       </c>
       <c r="L8" t="n">
-        <v>18.46355333801489</v>
+        <v>18.26129463831092</v>
       </c>
       <c r="M8" t="n">
-        <v>60.57941077203017</v>
+        <v>59.91903502440606</v>
       </c>
       <c r="N8" t="n">
-        <v>179.7658368149616</v>
+        <v>177.8410818713157</v>
       </c>
       <c r="O8" t="n">
-        <v>43.50634137182551</v>
+        <v>45.61545319083035</v>
       </c>
       <c r="P8" t="n">
-        <v>168.7204372020996</v>
+        <v>166.4319199037145</v>
       </c>
     </row>
     <row r="9">
@@ -1615,40 +1615,40 @@
         <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>0.002007998542736875</v>
+        <v>0.002468343465961319</v>
       </c>
       <c r="F9" t="n">
-        <v>0.04365337720620601</v>
+        <v>0.04406160719996115</v>
       </c>
       <c r="G9" t="n">
-        <v>0.08236482378729937</v>
+        <v>0.08313506869507602</v>
       </c>
       <c r="H9" t="n">
-        <v>0.1554052545686758</v>
+        <v>0.1568585461617273</v>
       </c>
       <c r="I9" t="n">
-        <v>0.295225321631079</v>
+        <v>0.2984277248699254</v>
       </c>
       <c r="J9" t="n">
-        <v>0.5968933483881268</v>
+        <v>0.6024752708756802</v>
       </c>
       <c r="K9" t="n">
-        <v>1.12621333345109</v>
+        <v>1.136745257703135</v>
       </c>
       <c r="L9" t="n">
-        <v>2.621878033511722</v>
+        <v>2.646486856805085</v>
       </c>
       <c r="M9" t="n">
-        <v>8.61490933997605</v>
+        <v>8.695517428148086</v>
       </c>
       <c r="N9" t="n">
-        <v>27.48573449643558</v>
+        <v>27.27002193020374</v>
       </c>
       <c r="O9" t="n">
-        <v>8.648292511610057</v>
+        <v>7.04256256159465</v>
       </c>
       <c r="P9" t="n">
-        <v>26.23797480179799</v>
+        <v>24.93486584988777</v>
       </c>
     </row>
     <row r="10">
@@ -1664,43 +1664,43 @@
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>0.003689081923378368</v>
+        <v>0.002534713518706266</v>
       </c>
       <c r="E10" t="n">
-        <v>0.05285754006104318</v>
+        <v>0.05183385589976339</v>
       </c>
       <c r="F10" t="n">
-        <v>0.09973116060168212</v>
+        <v>0.09779968196351449</v>
       </c>
       <c r="G10" t="n">
-        <v>0.1881719123415862</v>
+        <v>0.1845276147439426</v>
       </c>
       <c r="H10" t="n">
-        <v>0.3587302584289732</v>
+        <v>0.350699860065828</v>
       </c>
       <c r="I10" t="n">
-        <v>0.7227462362318726</v>
+        <v>0.7087489167614486</v>
       </c>
       <c r="J10" t="n">
-        <v>1.36367150035093</v>
+        <v>1.337261476076517</v>
       </c>
       <c r="K10" t="n">
-        <v>2.572963880883852</v>
+        <v>2.523133669917469</v>
       </c>
       <c r="L10" t="n">
-        <v>6.001494965265253</v>
+        <v>5.884773437738766</v>
       </c>
       <c r="M10" t="n">
-        <v>19.68608760740681</v>
+        <v>19.30499118922086</v>
       </c>
       <c r="N10" t="n">
-        <v>65.23332336620589</v>
+        <v>63.96998703854901</v>
       </c>
       <c r="O10" t="n">
-        <v>2.007131899478092</v>
+        <v>4.44168005453558</v>
       </c>
       <c r="P10" t="n">
-        <v>55.88535801255222</v>
+        <v>53.51018845893417</v>
       </c>
     </row>
     <row r="11">
@@ -1725,34 +1725,34 @@
         <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>0.1012209113159823</v>
+        <v>0.09193614716824741</v>
       </c>
       <c r="H11" t="n">
-        <v>0.2451316092293698</v>
+        <v>0.2368979587233561</v>
       </c>
       <c r="I11" t="n">
-        <v>0.4625122519960223</v>
+        <v>0.4469770696927016</v>
       </c>
       <c r="J11" t="n">
-        <v>0.8726642146189694</v>
+        <v>0.8433525637271645</v>
       </c>
       <c r="K11" t="n">
-        <v>1.747756388354743</v>
+        <v>1.683166648621405</v>
       </c>
       <c r="L11" t="n">
-        <v>4.139530775385353</v>
+        <v>4.000761053243203</v>
       </c>
       <c r="M11" t="n">
-        <v>13.46198249483943</v>
+        <v>13.10538386312092</v>
       </c>
       <c r="N11" t="n">
-        <v>37.46916866941694</v>
+        <v>36.39711100623728</v>
       </c>
       <c r="O11" t="n">
-        <v>14.07094630511121</v>
+        <v>12.72013812889545</v>
       </c>
       <c r="P11" t="n">
-        <v>35.79813706054184</v>
+        <v>35.93753523143455</v>
       </c>
     </row>
     <row r="12">
@@ -1804,7 +1804,7 @@
         <v>0</v>
       </c>
       <c r="P12" t="n">
-        <v>80.25898699042621</v>
+        <v>79.23323765467518</v>
       </c>
     </row>
     <row r="13">
@@ -1826,37 +1826,37 @@
         <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>0.1055655806316507</v>
+        <v>0.105060123757812</v>
       </c>
       <c r="G13" t="n">
-        <v>0.2137232033910986</v>
+        <v>0.2132749685001708</v>
       </c>
       <c r="H13" t="n">
-        <v>0.4032511368687965</v>
+        <v>0.4024054110585758</v>
       </c>
       <c r="I13" t="n">
-        <v>0.7608508426125781</v>
+        <v>0.7592551342896655</v>
       </c>
       <c r="J13" t="n">
-        <v>1.541132530794079</v>
+        <v>1.537616304920357</v>
       </c>
       <c r="K13" t="n">
-        <v>2.922338812361429</v>
+        <v>2.916209883924884</v>
       </c>
       <c r="L13" t="n">
-        <v>6.802637135813439</v>
+        <v>6.788383295963538</v>
       </c>
       <c r="M13" t="n">
-        <v>22.35104183133693</v>
+        <v>22.30406593716549</v>
       </c>
       <c r="N13" t="n">
-        <v>55.5262226932939</v>
+        <v>46.01071727520255</v>
       </c>
       <c r="O13" t="n">
-        <v>25.61031782119684</v>
+        <v>33.72824619678578</v>
       </c>
       <c r="P13" t="n">
-        <v>50.7889395464753</v>
+        <v>41.37701927170352</v>
       </c>
     </row>
     <row r="14">
@@ -1872,43 +1872,43 @@
         <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>0.1309767967558472</v>
+        <v>0.1277979307328363</v>
       </c>
       <c r="E14" t="n">
-        <v>0.5888257461963379</v>
+        <v>0.60996755703266</v>
       </c>
       <c r="F14" t="n">
-        <v>1.325690564220461</v>
+        <v>1.34111449524472</v>
       </c>
       <c r="G14" t="n">
-        <v>2.6170656389379</v>
+        <v>2.637388074581157</v>
       </c>
       <c r="H14" t="n">
-        <v>5.122983010622363</v>
+        <v>5.167433108848234</v>
       </c>
       <c r="I14" t="n">
-        <v>10.00770095046725</v>
+        <v>10.11870868917898</v>
       </c>
       <c r="J14" t="n">
-        <v>19.09714482787929</v>
+        <v>19.2821270333751</v>
       </c>
       <c r="K14" t="n">
-        <v>36.14809559696405</v>
+        <v>36.48833915423229</v>
       </c>
       <c r="L14" t="n">
-        <v>84.39246657110587</v>
+        <v>85.19889986145978</v>
       </c>
       <c r="M14" t="n">
-        <v>273.7412832154437</v>
+        <v>275.1483876988099</v>
       </c>
       <c r="N14" t="n">
-        <v>809.6080463645295</v>
+        <v>804.7491349697914</v>
       </c>
       <c r="O14" t="n">
-        <v>441.135602181682</v>
+        <v>445.4881329566752</v>
       </c>
       <c r="P14" t="n">
-        <v>929.0134613790367</v>
+        <v>920.0456539499561</v>
       </c>
     </row>
   </sheetData>
@@ -2031,7 +2031,7 @@
         <v>132492.1181521182</v>
       </c>
       <c r="P2" t="n">
-        <v>302126.1199774382</v>
+        <v>279550.7371638594</v>
       </c>
     </row>
     <row r="3">
@@ -2050,40 +2050,40 @@
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>288.4968516401092</v>
+        <v>364.7720353759557</v>
       </c>
       <c r="F3" t="n">
-        <v>666.1343329707612</v>
+        <v>725.8168529987781</v>
       </c>
       <c r="G3" t="n">
-        <v>1089.275753748692</v>
+        <v>1186.869765603945</v>
       </c>
       <c r="H3" t="n">
-        <v>1865.522181278812</v>
+        <v>2032.664241725304</v>
       </c>
       <c r="I3" t="n">
-        <v>3278.734201545154</v>
+        <v>3603.343038554588</v>
       </c>
       <c r="J3" t="n">
-        <v>5950.802349043279</v>
+        <v>6483.96640139837</v>
       </c>
       <c r="K3" t="n">
-        <v>10311.35846535923</v>
+        <v>11235.20794685995</v>
       </c>
       <c r="L3" t="n">
-        <v>21896.47422280704</v>
+        <v>23863.25376940648</v>
       </c>
       <c r="M3" t="n">
-        <v>69294.22218238768</v>
+        <v>73901.90525782132</v>
       </c>
       <c r="N3" t="n">
-        <v>204225.9397835081</v>
+        <v>217799.355751555</v>
       </c>
       <c r="O3" t="n">
-        <v>65984.36845485878</v>
+        <v>67348.70318436256</v>
       </c>
       <c r="P3" t="n">
-        <v>181382.6525990934</v>
+        <v>206407.151324647</v>
       </c>
     </row>
     <row r="4">
@@ -2102,40 +2102,40 @@
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>48.33592169498279</v>
+        <v>47.4190243126765</v>
       </c>
       <c r="F4" t="n">
-        <v>92.7937993184777</v>
+        <v>92.07636091055923</v>
       </c>
       <c r="G4" t="n">
-        <v>151.7382165922325</v>
+        <v>150.5650474221817</v>
       </c>
       <c r="H4" t="n">
-        <v>259.8708433804044</v>
+        <v>257.8616431374078</v>
       </c>
       <c r="I4" t="n">
-        <v>461.7185153388618</v>
+        <v>457.8164206030667</v>
       </c>
       <c r="J4" t="n">
-        <v>828.9582620646664</v>
+        <v>822.5491431350129</v>
       </c>
       <c r="K4" t="n">
-        <v>1436.392152117805</v>
+        <v>1425.286637457013</v>
       </c>
       <c r="L4" t="n">
-        <v>3051.022223980327</v>
+        <v>3027.379737269369</v>
       </c>
       <c r="M4" t="n">
-        <v>9768.832452615385</v>
+        <v>9693.278522294193</v>
       </c>
       <c r="N4" t="n">
-        <v>24492.90774630507</v>
+        <v>24508.47767114965</v>
       </c>
       <c r="O4" t="n">
-        <v>9384.411896787971</v>
+        <v>9353.138143052489</v>
       </c>
       <c r="P4" t="n">
-        <v>21193.13139891986</v>
+        <v>21235.973795526</v>
       </c>
     </row>
     <row r="5">
@@ -2151,43 +2151,43 @@
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>98.77523838766632</v>
+        <v>94.01061545262118</v>
       </c>
       <c r="E5" t="n">
-        <v>182.4449492953313</v>
+        <v>178.8535059906331</v>
       </c>
       <c r="F5" t="n">
-        <v>303.7372861333868</v>
+        <v>297.758193552944</v>
       </c>
       <c r="G5" t="n">
-        <v>496.6770888673728</v>
+        <v>486.8999609594786</v>
       </c>
       <c r="H5" t="n">
-        <v>908.8995797742508</v>
+        <v>889.3438869489773</v>
       </c>
       <c r="I5" t="n">
-        <v>1526.14273675387</v>
+        <v>1496.100495874644</v>
       </c>
       <c r="J5" t="n">
-        <v>2713.387475096445</v>
+        <v>2659.974227329785</v>
       </c>
       <c r="K5" t="n">
-        <v>4701.670341249631</v>
+        <v>4609.11758748364</v>
       </c>
       <c r="L5" t="n">
-        <v>10007.51921423715</v>
+        <v>9809.995645007175</v>
       </c>
       <c r="M5" t="n">
-        <v>31971.10422962547</v>
+        <v>31341.91835544413</v>
       </c>
       <c r="N5" t="n">
-        <v>100176.9135381572</v>
+        <v>99506.03151454385</v>
       </c>
       <c r="O5" t="n">
-        <v>51470.3444823953</v>
+        <v>50270.55474772016</v>
       </c>
       <c r="P5" t="n">
-        <v>106345.6633002872</v>
+        <v>104103.0974508081</v>
       </c>
     </row>
     <row r="6">
@@ -2203,43 +2203,43 @@
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>178.1094979106417</v>
+        <v>180.3727515356719</v>
       </c>
       <c r="E6" t="n">
-        <v>308.8879158497139</v>
+        <v>310.593894935417</v>
       </c>
       <c r="F6" t="n">
-        <v>514.2415706324564</v>
+        <v>517.0817120542558</v>
       </c>
       <c r="G6" t="n">
-        <v>840.8977690152578</v>
+        <v>845.5420232367547</v>
       </c>
       <c r="H6" t="n">
-        <v>1545.228143993136</v>
+        <v>1554.517335033046</v>
       </c>
       <c r="I6" t="n">
-        <v>2583.831731521353</v>
+        <v>2598.102159947877</v>
       </c>
       <c r="J6" t="n">
-        <v>4593.893145918432</v>
+        <v>4619.265085792911</v>
       </c>
       <c r="K6" t="n">
-        <v>7960.149942929527</v>
+        <v>8004.11362239022</v>
       </c>
       <c r="L6" t="n">
-        <v>16945.22681090576</v>
+        <v>17039.052899598</v>
       </c>
       <c r="M6" t="n">
-        <v>50239.16827703245</v>
+        <v>50163.77116284562</v>
       </c>
       <c r="N6" t="n">
-        <v>138601.6324661376</v>
+        <v>138658.6614029928</v>
       </c>
       <c r="O6" t="n">
-        <v>153531.5638343118</v>
+        <v>145589.7072456342</v>
       </c>
       <c r="P6" t="n">
-        <v>176570.5257754842</v>
+        <v>184505.6842784135</v>
       </c>
     </row>
     <row r="7">
@@ -2255,43 +2255,43 @@
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>84.46690466986298</v>
+        <v>86.81209506566726</v>
       </c>
       <c r="E7" t="n">
-        <v>211.8425225160794</v>
+        <v>213.6102633132164</v>
       </c>
       <c r="F7" t="n">
-        <v>352.678838878284</v>
+        <v>355.6218021906884</v>
       </c>
       <c r="G7" t="n">
-        <v>576.7072631387975</v>
+        <v>581.5196537058439</v>
       </c>
       <c r="H7" t="n">
-        <v>1037.519435128178</v>
+        <v>1047.144923571304</v>
       </c>
       <c r="I7" t="n">
-        <v>1772.051944009644</v>
+        <v>1786.839006016206</v>
       </c>
       <c r="J7" t="n">
-        <v>3150.598849176669</v>
+        <v>3176.889331630113</v>
       </c>
       <c r="K7" t="n">
-        <v>5459.256115208037</v>
+        <v>5504.811415637111</v>
       </c>
       <c r="L7" t="n">
-        <v>11614.41897133392</v>
+        <v>11711.64185419752</v>
       </c>
       <c r="M7" t="n">
-        <v>37124.44538075489</v>
+        <v>37434.13634464054</v>
       </c>
       <c r="N7" t="n">
-        <v>107238.9329957629</v>
+        <v>108148.6435207889</v>
       </c>
       <c r="O7" t="n">
-        <v>163920.6141183324</v>
+        <v>162738.3481413184</v>
       </c>
       <c r="P7" t="n">
-        <v>33167.44621762988</v>
+        <v>34349.39700176114</v>
       </c>
     </row>
     <row r="8">
@@ -2307,43 +2307,43 @@
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>9.798705624281491</v>
+        <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>677.2508519195619</v>
+        <v>669.8648538691831</v>
       </c>
       <c r="F8" t="n">
-        <v>1127.498111556853</v>
+        <v>1115.201783202062</v>
       </c>
       <c r="G8" t="n">
-        <v>1843.706733804135</v>
+        <v>1823.599539693193</v>
       </c>
       <c r="H8" t="n">
-        <v>3163.361670701379</v>
+        <v>3123.144327191508</v>
       </c>
       <c r="I8" t="n">
-        <v>5665.168987190257</v>
+        <v>5603.38548854148</v>
       </c>
       <c r="J8" t="n">
-        <v>10072.32036948453</v>
+        <v>9962.473126914147</v>
       </c>
       <c r="K8" t="n">
-        <v>17452.99201953701</v>
+        <v>17262.65225892362</v>
       </c>
       <c r="L8" t="n">
-        <v>37082.34352535135</v>
+        <v>36676.12558636065</v>
       </c>
       <c r="M8" t="n">
-        <v>118700.6417420148</v>
+        <v>117406.6868481841</v>
       </c>
       <c r="N8" t="n">
-        <v>352237.1697130845</v>
+        <v>348465.762165615</v>
       </c>
       <c r="O8" t="n">
-        <v>83116.1084351538</v>
+        <v>87145.43292263633</v>
       </c>
       <c r="P8" t="n">
-        <v>322329.7043956388</v>
+        <v>317957.6371077312</v>
       </c>
     </row>
     <row r="9">
@@ -2362,40 +2362,40 @@
         <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>8.935625586803306</v>
+        <v>10.98416784775174</v>
       </c>
       <c r="F9" t="n">
-        <v>171.4043168793209</v>
+        <v>173.0072256961742</v>
       </c>
       <c r="G9" t="n">
-        <v>280.283656348782</v>
+        <v>282.9047638690649</v>
       </c>
       <c r="H9" t="n">
-        <v>480.0211297911746</v>
+        <v>484.5101071706643</v>
       </c>
       <c r="I9" t="n">
-        <v>803.7104073184553</v>
+        <v>812.4285104854574</v>
       </c>
       <c r="J9" t="n">
-        <v>1531.21249128949</v>
+        <v>1545.531815606694</v>
       </c>
       <c r="K9" t="n">
-        <v>2653.235640881278</v>
+        <v>2678.047704424301</v>
       </c>
       <c r="L9" t="n">
-        <v>5627.804284110681</v>
+        <v>5680.626589110052</v>
       </c>
       <c r="M9" t="n">
-        <v>18040.69842808191</v>
+        <v>18209.50185388557</v>
       </c>
       <c r="N9" t="n">
-        <v>57558.56823977912</v>
+        <v>57106.83912680076</v>
       </c>
       <c r="O9" t="n">
-        <v>17657.84179363448</v>
+        <v>14379.30728724392</v>
       </c>
       <c r="P9" t="n">
-        <v>53571.96318389365</v>
+        <v>50911.31176839062</v>
       </c>
     </row>
     <row r="10">
@@ -2411,43 +2411,43 @@
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>14.47940703819858</v>
+        <v>9.948585996421192</v>
       </c>
       <c r="E10" t="n">
-        <v>176.3430510506853</v>
+        <v>172.9278412602966</v>
       </c>
       <c r="F10" t="n">
-        <v>293.5787477893591</v>
+        <v>287.893051598177</v>
       </c>
       <c r="G10" t="n">
-        <v>480.0656503571744</v>
+        <v>470.7682899034418</v>
       </c>
       <c r="H10" t="n">
-        <v>830.7158546734534</v>
+        <v>812.1197672711154</v>
       </c>
       <c r="I10" t="n">
-        <v>1475.10066777665</v>
+        <v>1446.532611295922</v>
       </c>
       <c r="J10" t="n">
-        <v>2622.637830695306</v>
+        <v>2571.845591689188</v>
       </c>
       <c r="K10" t="n">
-        <v>4544.422283065603</v>
+        <v>4456.411128782433</v>
       </c>
       <c r="L10" t="n">
-        <v>9657.746019280681</v>
+        <v>9469.915008114705</v>
       </c>
       <c r="M10" t="n">
-        <v>30906.64630144563</v>
+        <v>30308.33482186096</v>
       </c>
       <c r="N10" t="n">
-        <v>102414.6235938008</v>
+        <v>100431.2183678702</v>
       </c>
       <c r="O10" t="n">
-        <v>3072.366333588993</v>
+        <v>6798.989278022677</v>
       </c>
       <c r="P10" t="n">
-        <v>85545.09673379212</v>
+        <v>81909.36608001735</v>
       </c>
     </row>
     <row r="11">
@@ -2472,34 +2472,34 @@
         <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>248.6562539773849</v>
+        <v>225.8475809272861</v>
       </c>
       <c r="H11" t="n">
-        <v>546.5968378558126</v>
+        <v>528.2373641643316</v>
       </c>
       <c r="I11" t="n">
-        <v>908.9549778184318</v>
+        <v>878.4243676022043</v>
       </c>
       <c r="J11" t="n">
-        <v>1616.065779984028</v>
+        <v>1561.784241715879</v>
       </c>
       <c r="K11" t="n">
-        <v>2972.413321355654</v>
+        <v>2862.56540199717</v>
       </c>
       <c r="L11" t="n">
-        <v>6414.322024116064</v>
+        <v>6199.294347474622</v>
       </c>
       <c r="M11" t="n">
-        <v>20350.95527354496</v>
+        <v>19811.87250416143</v>
       </c>
       <c r="N11" t="n">
-        <v>56643.46807912795</v>
+        <v>55022.80057622532</v>
       </c>
       <c r="O11" t="n">
-        <v>20739.75872766183</v>
+        <v>18748.7458238679</v>
       </c>
       <c r="P11" t="n">
-        <v>52764.37770682964</v>
+        <v>52969.84252552077</v>
       </c>
     </row>
     <row r="12">
@@ -2551,7 +2551,7 @@
         <v>0</v>
       </c>
       <c r="P12" t="n">
-        <v>122854.4121397608</v>
+        <v>121284.2723165224</v>
       </c>
     </row>
     <row r="13">
@@ -2573,37 +2573,37 @@
         <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>402.9741417083473</v>
+        <v>401.0446676441024</v>
       </c>
       <c r="G13" t="n">
-        <v>707.063805675211</v>
+        <v>705.580903197674</v>
       </c>
       <c r="H13" t="n">
-        <v>1210.935989832778</v>
+        <v>1208.396332216239</v>
       </c>
       <c r="I13" t="n">
-        <v>2013.707763286301</v>
+        <v>2009.484477909162</v>
       </c>
       <c r="J13" t="n">
-        <v>3843.524401525563</v>
+        <v>3834.755071388874</v>
       </c>
       <c r="K13" t="n">
-        <v>6693.243958756352</v>
+        <v>6679.20643064427</v>
       </c>
       <c r="L13" t="n">
-        <v>14195.63215396112</v>
+        <v>14165.88747358924</v>
       </c>
       <c r="M13" t="n">
-        <v>45504.18470049401</v>
+        <v>45408.54711093651</v>
       </c>
       <c r="N13" t="n">
-        <v>113045.0881092228</v>
+        <v>93672.59892814554</v>
       </c>
       <c r="O13" t="n">
-        <v>50836.20822415945</v>
+        <v>66950.20962513721</v>
       </c>
       <c r="P13" t="n">
-        <v>100815.5042938161</v>
+        <v>82132.9427489736</v>
       </c>
     </row>
     <row r="14">
@@ -2619,43 +2619,43 @@
         <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>552.3839091276152</v>
+        <v>537.8982035473457</v>
       </c>
       <c r="E14" t="n">
-        <v>2169.973473116229</v>
+        <v>2236.461370468092</v>
       </c>
       <c r="F14" t="n">
-        <v>4370.272539929459</v>
+        <v>4410.733043909953</v>
       </c>
       <c r="G14" t="n">
-        <v>7443.123184178175</v>
+        <v>7488.148521171997</v>
       </c>
       <c r="H14" t="n">
-        <v>13193.93581400572</v>
+        <v>13283.20407602624</v>
       </c>
       <c r="I14" t="n">
-        <v>22726.20868233802</v>
+        <v>22929.54332660965</v>
       </c>
       <c r="J14" t="n">
-        <v>40900.8029504153</v>
+        <v>41216.43603273787</v>
       </c>
       <c r="K14" t="n">
-        <v>71077.04819381073</v>
+        <v>71609.33408795032</v>
       </c>
       <c r="L14" t="n">
-        <v>151166.0557107247</v>
+        <v>152316.7191707685</v>
       </c>
       <c r="M14" t="n">
-        <v>478764.2341099118</v>
+        <v>480543.2879239891</v>
       </c>
       <c r="N14" t="n">
-        <v>1411952.240122922</v>
+        <v>1398637.384883723</v>
       </c>
       <c r="O14" t="n">
-        <v>752205.704453003</v>
+        <v>761815.254551114</v>
       </c>
       <c r="P14" t="n">
-        <v>1558666.597722584</v>
+        <v>1537317.413562171</v>
       </c>
     </row>
   </sheetData>
@@ -2766,7 +2766,7 @@
         <v>983.1163787606301</v>
       </c>
       <c r="N2" t="n">
-        <v>2456.290292367414</v>
+        <v>2328.703162360821</v>
       </c>
     </row>
     <row r="3">
@@ -2779,40 +2779,40 @@
         <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>0.4100740110205189</v>
+        <v>0.5184927696935063</v>
       </c>
       <c r="D3" t="n">
-        <v>1.483175131811848</v>
+        <v>1.687738730892764</v>
       </c>
       <c r="E3" t="n">
-        <v>3.507893272230222</v>
+        <v>3.893862144970728</v>
       </c>
       <c r="F3" t="n">
-        <v>7.328114376012302</v>
+        <v>8.056357188486725</v>
       </c>
       <c r="G3" t="n">
-        <v>14.53607532151277</v>
+        <v>15.91011771554078</v>
       </c>
       <c r="H3" t="n">
-        <v>28.13599521631258</v>
+        <v>30.72852681188193</v>
       </c>
       <c r="I3" t="n">
-        <v>53.79620932449675</v>
+        <v>58.68777606453168</v>
       </c>
       <c r="J3" t="n">
-        <v>175.2176880963332</v>
+        <v>190.9814324857059</v>
       </c>
       <c r="K3" t="n">
-        <v>561.5007965064417</v>
+        <v>602.1676718454901</v>
       </c>
       <c r="L3" t="n">
-        <v>1652.340101520739</v>
+        <v>1762.172440107205</v>
       </c>
       <c r="M3" t="n">
-        <v>1642.566056224142</v>
+        <v>1733.016603064425</v>
       </c>
       <c r="N3" t="n">
-        <v>1532.665146682843</v>
+        <v>1696.168127500012</v>
       </c>
     </row>
     <row r="4">
@@ -2825,40 +2825,40 @@
         <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>0.05855441132790506</v>
+        <v>0.05744367660750735</v>
       </c>
       <c r="D4" t="n">
-        <v>0.1859534743276458</v>
+        <v>0.1838577494290236</v>
       </c>
       <c r="E4" t="n">
-        <v>0.4263289514659627</v>
+        <v>0.4223747554099211</v>
       </c>
       <c r="F4" t="n">
-        <v>0.8798673735624508</v>
+        <v>0.8724066298074407</v>
       </c>
       <c r="G4" t="n">
-        <v>1.735599841643668</v>
+        <v>1.721522973276741</v>
       </c>
       <c r="H4" t="n">
-        <v>3.350188642176612</v>
+        <v>3.323628525715469</v>
       </c>
       <c r="I4" t="n">
-        <v>6.396581167929164</v>
+        <v>6.346467764291264</v>
       </c>
       <c r="J4" t="n">
-        <v>20.81088404075502</v>
+        <v>20.64938672764186</v>
       </c>
       <c r="K4" t="n">
-        <v>67.2629510602077</v>
+        <v>66.74250382953818</v>
       </c>
       <c r="L4" t="n">
-        <v>176.3956871367366</v>
+        <v>176.0868610291942</v>
       </c>
       <c r="M4" t="n">
-        <v>175.6553642912772</v>
+        <v>175.5703850168341</v>
       </c>
       <c r="N4" t="n">
-        <v>161.4643017975993</v>
+        <v>161.5253898590499</v>
       </c>
     </row>
     <row r="5">
@@ -2868,43 +2868,43 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.1017083542536252</v>
+        <v>0.09680224655626299</v>
       </c>
       <c r="C5" t="n">
-        <v>0.3227232067923012</v>
+        <v>0.3134664041842018</v>
       </c>
       <c r="D5" t="n">
-        <v>0.739732165749457</v>
+        <v>0.7222665086927671</v>
       </c>
       <c r="E5" t="n">
-        <v>1.526541150996727</v>
+        <v>1.493587096628646</v>
       </c>
       <c r="F5" t="n">
-        <v>3.011085705660465</v>
+        <v>2.948908273928603</v>
       </c>
       <c r="G5" t="n">
-        <v>5.812111845555327</v>
+        <v>5.69479599198573</v>
       </c>
       <c r="H5" t="n">
-        <v>11.0970643326509</v>
+        <v>10.8757137699883</v>
       </c>
       <c r="I5" t="n">
-        <v>21.06866809351621</v>
+        <v>20.65102571952979</v>
       </c>
       <c r="J5" t="n">
-        <v>68.23818002486891</v>
+        <v>66.89227022140872</v>
       </c>
       <c r="K5" t="n">
-        <v>220.2483985447542</v>
+        <v>215.9110196965315</v>
       </c>
       <c r="L5" t="n">
-        <v>680.3606665209663</v>
+        <v>673.6673004273453</v>
       </c>
       <c r="M5" t="n">
-        <v>787.5467141983332</v>
+        <v>777.7572219879412</v>
       </c>
       <c r="N5" t="n">
-        <v>833.3452842397636</v>
+        <v>815.1679723622412</v>
       </c>
     </row>
     <row r="6">
@@ -2914,43 +2914,43 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.1962878579438643</v>
+        <v>0.1987821056468349</v>
       </c>
       <c r="C6" t="n">
-        <v>0.5967747894506821</v>
+        <v>0.6014809149714319</v>
       </c>
       <c r="D6" t="n">
-        <v>1.352410152709262</v>
+        <v>1.361289630633878</v>
       </c>
       <c r="E6" t="n">
-        <v>2.778136580432172</v>
+        <v>2.794890304459744</v>
       </c>
       <c r="F6" t="n">
-        <v>5.468185174693028</v>
+        <v>5.499795959828703</v>
       </c>
       <c r="G6" t="n">
-        <v>10.5437461650594</v>
+        <v>10.60338912773739</v>
       </c>
       <c r="H6" t="n">
-        <v>20.12027181663681</v>
+        <v>20.23280565538015</v>
       </c>
       <c r="I6" t="n">
-        <v>38.1891796140979</v>
+        <v>38.40150751153457</v>
       </c>
       <c r="J6" t="n">
-        <v>123.6609395611099</v>
+        <v>124.345195317968</v>
       </c>
       <c r="K6" t="n">
-        <v>377.6770381976071</v>
+        <v>377.8198117594187</v>
       </c>
       <c r="L6" t="n">
-        <v>1040.572139754099</v>
+        <v>1040.470925326316</v>
       </c>
       <c r="M6" t="n">
-        <v>1631.438181458398</v>
+        <v>1586.868198173466</v>
       </c>
       <c r="N6" t="n">
-        <v>1865.606380643969</v>
+        <v>1865.568525713923</v>
       </c>
     </row>
     <row r="7">
@@ -2960,43 +2960,43 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.08289277144604118</v>
+        <v>0.08519425665183464</v>
       </c>
       <c r="C7" t="n">
-        <v>0.3274746599538316</v>
+        <v>0.3318170828213413</v>
       </c>
       <c r="D7" t="n">
-        <v>0.7889497035306465</v>
+        <v>0.7971429503578707</v>
       </c>
       <c r="E7" t="n">
-        <v>1.659656922055701</v>
+        <v>1.675115871038788</v>
       </c>
       <c r="F7" t="n">
-        <v>3.302499955376618</v>
+        <v>3.331667769883024</v>
       </c>
       <c r="G7" t="n">
-        <v>6.402202329158432</v>
+        <v>6.457235915465684</v>
       </c>
       <c r="H7" t="n">
-        <v>12.25069461427118</v>
+        <v>12.35453152056982</v>
       </c>
       <c r="I7" t="n">
-        <v>23.28558051116826</v>
+        <v>23.48149910984864</v>
       </c>
       <c r="J7" t="n">
-        <v>75.48756384822804</v>
+        <v>76.11893839034448</v>
       </c>
       <c r="K7" t="n">
-        <v>243.7156113587952</v>
+        <v>245.7503023739299</v>
       </c>
       <c r="L7" t="n">
-        <v>708.3650440201732</v>
+        <v>714.3484270573747</v>
       </c>
       <c r="M7" t="n">
-        <v>1351.15477793285</v>
+        <v>1349.668649678238</v>
       </c>
       <c r="N7" t="n">
-        <v>991.8723518158238</v>
+        <v>991.8707655649602</v>
       </c>
     </row>
     <row r="8">
@@ -3006,43 +3006,43 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.009133906481236687</v>
+        <v>0</v>
       </c>
       <c r="C8" t="n">
-        <v>0.751842560528262</v>
+        <v>0.7346087828468006</v>
       </c>
       <c r="D8" t="n">
-        <v>2.153178982379921</v>
+        <v>2.12066243606054</v>
       </c>
       <c r="E8" t="n">
-        <v>4.797208719353574</v>
+        <v>4.735856774116524</v>
       </c>
       <c r="F8" t="n">
-        <v>9.785941718074557</v>
+        <v>9.67018338545833</v>
       </c>
       <c r="G8" t="n">
-        <v>19.19864104762664</v>
+        <v>18.98022920235727</v>
       </c>
       <c r="H8" t="n">
-        <v>36.95844272297492</v>
+        <v>36.54634509617061</v>
       </c>
       <c r="I8" t="n">
-        <v>70.46748667569543</v>
+        <v>69.68994435051478</v>
       </c>
       <c r="J8" t="n">
-        <v>229.0088395538476</v>
+        <v>226.5031028201035</v>
       </c>
       <c r="K8" t="n">
-        <v>739.9300831427047</v>
+        <v>731.8550030145899</v>
       </c>
       <c r="L8" t="n">
-        <v>2194.933745968395</v>
+        <v>2171.325246740827</v>
       </c>
       <c r="M8" t="n">
-        <v>2039.015305516578</v>
+        <v>2040.698929932244</v>
       </c>
       <c r="N8" t="n">
-        <v>1938.144077184085</v>
+        <v>1936.505670996083</v>
       </c>
     </row>
     <row r="9">
@@ -3055,40 +3055,40 @@
         <v>0</v>
       </c>
       <c r="C9" t="n">
-        <v>0.009168943025830545</v>
+        <v>0.01127097461770724</v>
       </c>
       <c r="D9" t="n">
-        <v>0.2084994305585804</v>
+        <v>0.2124655260302418</v>
       </c>
       <c r="E9" t="n">
-        <v>0.5845945125843847</v>
+        <v>0.5920777080563848</v>
       </c>
       <c r="F9" t="n">
-        <v>1.294207540048418</v>
+        <v>1.308326770125526</v>
       </c>
       <c r="G9" t="n">
-        <v>2.633099412907636</v>
+        <v>2.65973945708612</v>
       </c>
       <c r="H9" t="n">
-        <v>5.159309301718235</v>
+        <v>5.209573512298824</v>
       </c>
       <c r="I9" t="n">
-        <v>9.925740805030133</v>
+        <v>10.02057889344931</v>
       </c>
       <c r="J9" t="n">
-        <v>32.48618876042669</v>
+        <v>32.79181750141491</v>
       </c>
       <c r="K9" t="n">
-        <v>105.190325038056</v>
+        <v>106.1752555535803</v>
       </c>
       <c r="L9" t="n">
-        <v>329.6862417845222</v>
+        <v>328.4524109469994</v>
       </c>
       <c r="M9" t="n">
-        <v>329.9911109288161</v>
+        <v>313.3569328645894</v>
       </c>
       <c r="N9" t="n">
-        <v>318.596045338314</v>
+        <v>292.0313067735902</v>
       </c>
     </row>
     <row r="10">
@@ -3098,43 +3098,43 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.01684512276934954</v>
+        <v>0.01157403421625174</v>
       </c>
       <c r="C10" t="n">
-        <v>0.2582037507714855</v>
+        <v>0.2482583053643103</v>
       </c>
       <c r="D10" t="n">
-        <v>0.7135971736224923</v>
+        <v>0.6948321911429297</v>
       </c>
       <c r="E10" t="n">
-        <v>1.572829641475767</v>
+        <v>1.537424030862867</v>
       </c>
       <c r="F10" t="n">
-        <v>3.194022212047379</v>
+        <v>3.1272192046778</v>
       </c>
       <c r="G10" t="n">
-        <v>6.252874675389581</v>
+        <v>6.126831324735035</v>
       </c>
       <c r="H10" t="n">
-        <v>12.02429169415599</v>
+        <v>11.78647416363177</v>
       </c>
       <c r="I10" t="n">
-        <v>22.91375262883337</v>
+        <v>22.46504051882567</v>
       </c>
       <c r="J10" t="n">
-        <v>74.43378204050794</v>
+        <v>72.9877457534661</v>
       </c>
       <c r="K10" t="n">
-        <v>240.4641395395871</v>
+        <v>235.8040893719955</v>
       </c>
       <c r="L10" t="n">
-        <v>775.51972716364</v>
+        <v>760.5020766668499</v>
       </c>
       <c r="M10" t="n">
-        <v>614.0680784774377</v>
+        <v>624.7640767942275</v>
       </c>
       <c r="N10" t="n">
-        <v>528.6985327224238</v>
+        <v>529.2408030497813</v>
       </c>
     </row>
     <row r="11">
@@ -3153,34 +3153,34 @@
         <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>0.4621959374601514</v>
+        <v>0.419799754561123</v>
       </c>
       <c r="F11" t="n">
-        <v>1.581518342839392</v>
+        <v>1.501525582663298</v>
       </c>
       <c r="G11" t="n">
-        <v>3.693446413026149</v>
+        <v>3.542516748064809</v>
       </c>
       <c r="H11" t="n">
-        <v>7.678214476461433</v>
+        <v>7.393441658081425</v>
       </c>
       <c r="I11" t="n">
-        <v>15.19664123707059</v>
+        <v>14.65933428612185</v>
       </c>
       <c r="J11" t="n">
-        <v>50.82528844034267</v>
+        <v>49.09374313317821</v>
       </c>
       <c r="K11" t="n">
-        <v>164.7347231683008</v>
+        <v>160.0633461484028</v>
       </c>
       <c r="L11" t="n">
-        <v>465.1246635154781</v>
+        <v>452.0775741948242</v>
       </c>
       <c r="M11" t="n">
-        <v>470.6859767956803</v>
+        <v>448.5593483466688</v>
       </c>
       <c r="N11" t="n">
-        <v>455.4254143101572</v>
+        <v>444.3623093493448</v>
       </c>
     </row>
     <row r="12">
@@ -3226,7 +3226,7 @@
         <v>656.1054009469023</v>
       </c>
       <c r="N12" t="n">
-        <v>732.958777971108</v>
+        <v>723.5912042223085</v>
       </c>
     </row>
     <row r="13">
@@ -3242,37 +3242,37 @@
         <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>0.4820346099360497</v>
+        <v>0.4797265877041589</v>
       </c>
       <c r="E13" t="n">
-        <v>1.457939638492518</v>
+        <v>1.453584881619324</v>
       </c>
       <c r="F13" t="n">
-        <v>3.299269012174185</v>
+        <v>3.291052493649103</v>
       </c>
       <c r="G13" t="n">
-        <v>6.773473738220165</v>
+        <v>6.757970880393916</v>
       </c>
       <c r="H13" t="n">
-        <v>13.32857390172135</v>
+        <v>13.29932324038014</v>
       </c>
       <c r="I13" t="n">
-        <v>25.69668158155775</v>
+        <v>25.64149168054162</v>
       </c>
       <c r="J13" t="n">
-        <v>84.24278927669846</v>
+        <v>84.06493225486275</v>
       </c>
       <c r="K13" t="n">
-        <v>272.9156472273797</v>
+        <v>272.3424785926504</v>
       </c>
       <c r="L13" t="n">
-        <v>711.2078880900289</v>
+        <v>623.879292504294</v>
       </c>
       <c r="M13" t="n">
-        <v>740.9729653253454</v>
+        <v>728.2097047908555</v>
       </c>
       <c r="N13" t="n">
-        <v>697.7101059696763</v>
+        <v>685.8928284697409</v>
       </c>
     </row>
     <row r="14">
@@ -3282,43 +3282,43 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.598067559114517</v>
+        <v>0.5835521892915844</v>
       </c>
       <c r="C14" t="n">
-        <v>3.286769569653697</v>
+        <v>3.368792147889686</v>
       </c>
       <c r="D14" t="n">
-        <v>9.340151080902807</v>
+        <v>9.492602567221075</v>
       </c>
       <c r="E14" t="n">
-        <v>21.29022237207743</v>
+        <v>21.53547036725429</v>
       </c>
       <c r="F14" t="n">
-        <v>44.08477106589685</v>
+        <v>44.54750291391661</v>
       </c>
       <c r="G14" t="n">
-        <v>87.09333321239075</v>
+        <v>87.96641175893446</v>
       </c>
       <c r="H14" t="n">
-        <v>168.2415253856523</v>
+        <v>169.8888426206708</v>
       </c>
       <c r="I14" t="n">
-        <v>321.3512496902909</v>
+        <v>324.4593939500845</v>
       </c>
       <c r="J14" t="n">
-        <v>1045.817450922139</v>
+        <v>1055.833871885115</v>
       </c>
       <c r="K14" t="n">
-        <v>3353.157717023588</v>
+        <v>3374.14948542588</v>
       </c>
       <c r="L14" t="n">
-        <v>9893.601084442736</v>
+        <v>9862.077733969189</v>
       </c>
       <c r="M14" t="n">
-        <v>11422.31631085639</v>
+        <v>11417.69183035702</v>
       </c>
       <c r="N14" t="n">
-        <v>12512.77671104317</v>
+        <v>12470.62806622185</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finalized single runner script
</commit_message>
<xml_diff>
--- a/tutorial/dac_scenarios/SSPs/get_report_output.xlsx
+++ b/tutorial/dac_scenarios/SSPs/get_report_output.xlsx
@@ -534,10 +534,10 @@
         <v>334.0024299110544</v>
       </c>
       <c r="O2" t="n">
-        <v>1076.512445508014</v>
+        <v>1001.40060567106</v>
       </c>
       <c r="P2" t="n">
-        <v>2549.929988284399</v>
+        <v>2409.075372001149</v>
       </c>
     </row>
     <row r="3">
@@ -556,40 +556,40 @@
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>0.5677495884918854</v>
+        <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>1.848073928808317</v>
+        <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>4.263779091380739</v>
+        <v>0</v>
       </c>
       <c r="H3" t="n">
-        <v>8.821711209610077</v>
+        <v>0.7490225269059768</v>
       </c>
       <c r="I3" t="n">
-        <v>17.42157907273295</v>
+        <v>2.190098179517606</v>
       </c>
       <c r="J3" t="n">
-        <v>33.64773719548809</v>
+        <v>4.909107561789412</v>
       </c>
       <c r="K3" t="n">
-        <v>64.26311543329334</v>
+        <v>10.03931152261819</v>
       </c>
       <c r="L3" t="n">
-        <v>209.1246706630947</v>
+        <v>34.38102918898286</v>
       </c>
       <c r="M3" t="n">
-        <v>659.3736072645478</v>
+        <v>90.88385009147881</v>
       </c>
       <c r="N3" t="n">
-        <v>1929.578841213178</v>
+        <v>258.7932365018313</v>
       </c>
       <c r="O3" t="n">
-        <v>1897.653199332078</v>
+        <v>760.0098772670457</v>
       </c>
       <c r="P3" t="n">
-        <v>1857.304118185554</v>
+        <v>1211.301409696401</v>
       </c>
     </row>
     <row r="4">
@@ -608,40 +608,40 @@
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>0.06290082651422882</v>
+        <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>0.2013242376380232</v>
+        <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>0.4625003617988673</v>
+        <v>0.04699829397759718</v>
       </c>
       <c r="H4" t="n">
-        <v>0.9552852691920004</v>
+        <v>0.1713194734255249</v>
       </c>
       <c r="I4" t="n">
-        <v>1.885067674588708</v>
+        <v>0.4058876258479235</v>
       </c>
       <c r="J4" t="n">
-        <v>3.639373272052172</v>
+        <v>0.8484688366697193</v>
       </c>
       <c r="K4" t="n">
-        <v>6.949382271392757</v>
+        <v>1.683527330969317</v>
       </c>
       <c r="L4" t="n">
-        <v>22.61107869287862</v>
+        <v>5.641139267753242</v>
       </c>
       <c r="M4" t="n">
-        <v>73.08304242417474</v>
+        <v>17.77809781504941</v>
       </c>
       <c r="N4" t="n">
-        <v>192.8151147551188</v>
+        <v>47.86375910798161</v>
       </c>
       <c r="O4" t="n">
-        <v>192.2495735159291</v>
+        <v>134.4997279765825</v>
       </c>
       <c r="P4" t="n">
-        <v>176.8703036643627</v>
+        <v>199.8912406405004</v>
       </c>
     </row>
     <row r="5">
@@ -657,43 +657,43 @@
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>0.1059984610390926</v>
+        <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>0.3432457160141582</v>
+        <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>0.7908818349273985</v>
+        <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>1.635477887163147</v>
+        <v>0</v>
       </c>
       <c r="H5" t="n">
-        <v>3.229054592242367</v>
+        <v>0.09506722576947955</v>
       </c>
       <c r="I5" t="n">
-        <v>6.235801673582392</v>
+        <v>0.3226207535397499</v>
       </c>
       <c r="J5" t="n">
-        <v>11.90890669722625</v>
+        <v>0.7519668297538058</v>
       </c>
       <c r="K5" t="n">
-        <v>22.61287338901386</v>
+        <v>1.562053383746968</v>
       </c>
       <c r="L5" t="n">
-        <v>73.24703662491294</v>
+        <v>5.40788336675824</v>
       </c>
       <c r="M5" t="n">
-        <v>236.4225689319277</v>
+        <v>17.80159769983561</v>
       </c>
       <c r="N5" t="n">
-        <v>737.6657013446001</v>
+        <v>57.74204115377529</v>
       </c>
       <c r="O5" t="n">
-        <v>851.6441665932373</v>
+        <v>186.4555954947728</v>
       </c>
       <c r="P5" t="n">
-        <v>892.6089386627436</v>
+        <v>573.8304817236946</v>
       </c>
     </row>
     <row r="6">
@@ -709,43 +709,43 @@
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>0.2176664078599483</v>
+        <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>0.6586216084799341</v>
+        <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>1.490612160450218</v>
+        <v>0.08093629557070771</v>
       </c>
       <c r="G6" t="n">
-        <v>3.060404913987469</v>
+        <v>0.4006403862729174</v>
       </c>
       <c r="H6" t="n">
-        <v>6.022276636235198</v>
+        <v>1.003855367106582</v>
       </c>
       <c r="I6" t="n">
-        <v>11.61071121097956</v>
+        <v>2.141996303317139</v>
       </c>
       <c r="J6" t="n">
-        <v>22.15492241419049</v>
+        <v>4.28943101869507</v>
       </c>
       <c r="K6" t="n">
-        <v>42.04965114562687</v>
+        <v>8.34119272068974</v>
       </c>
       <c r="L6" t="n">
-        <v>136.1579902347549</v>
+        <v>24.75916003128892</v>
       </c>
       <c r="M6" t="n">
-        <v>413.7126980136905</v>
+        <v>63.3518280540851</v>
       </c>
       <c r="N6" t="n">
-        <v>1139.315674625472</v>
+        <v>180.5104356837037</v>
       </c>
       <c r="O6" t="n">
-        <v>1737.620694376152</v>
+        <v>527.7867086345261</v>
       </c>
       <c r="P6" t="n">
-        <v>2042.797556084721</v>
+        <v>1288.185549445848</v>
       </c>
     </row>
     <row r="7">
@@ -761,43 +761,43 @@
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>0.09328771196663604</v>
+        <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>0.3633397093227658</v>
+        <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>0.8728715393705838</v>
+        <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>1.834251897129991</v>
+        <v>0.1542448882277084</v>
       </c>
       <c r="H7" t="n">
-        <v>3.648176244503674</v>
+        <v>0.4783531951659825</v>
       </c>
       <c r="I7" t="n">
-        <v>7.070673398141659</v>
+        <v>1.089878014033279</v>
       </c>
       <c r="J7" t="n">
-        <v>13.52821215030608</v>
+        <v>2.243697882531434</v>
       </c>
       <c r="K7" t="n">
-        <v>25.71224178240668</v>
+        <v>4.420715475058614</v>
       </c>
       <c r="L7" t="n">
-        <v>83.35023837092959</v>
+        <v>14.73537605664297</v>
       </c>
       <c r="M7" t="n">
-        <v>269.0965837904191</v>
+        <v>47.97578378540958</v>
       </c>
       <c r="N7" t="n">
-        <v>782.2115354499407</v>
+        <v>155.0975545150604</v>
       </c>
       <c r="O7" t="n">
-        <v>1477.887186176543</v>
+        <v>500.3121456804159</v>
       </c>
       <c r="P7" t="n">
-        <v>1086.098499154616</v>
+        <v>950.593322126976</v>
       </c>
     </row>
     <row r="8">
@@ -816,40 +816,40 @@
         <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>0.804396625261213</v>
+        <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>2.322125390707545</v>
+        <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>5.185763219515227</v>
+        <v>0.1975066009671017</v>
       </c>
       <c r="H8" t="n">
-        <v>10.58885091296538</v>
+        <v>1.177050413503995</v>
       </c>
       <c r="I8" t="n">
-        <v>20.78335118441472</v>
+        <v>3.025245414097688</v>
       </c>
       <c r="J8" t="n">
-        <v>40.0182482804893</v>
+        <v>6.512404147072551</v>
       </c>
       <c r="K8" t="n">
-        <v>76.31048982691858</v>
+        <v>13.09194582154771</v>
       </c>
       <c r="L8" t="n">
-        <v>248.0209000682224</v>
+        <v>44.29047557812049</v>
       </c>
       <c r="M8" t="n">
-        <v>801.3812363147882</v>
+        <v>116.6922575069934</v>
       </c>
       <c r="N8" t="n">
-        <v>2377.601168957217</v>
+        <v>326.8189167537113</v>
       </c>
       <c r="O8" t="n">
-        <v>2234.56535062146</v>
+        <v>930.497705759633</v>
       </c>
       <c r="P8" t="n">
-        <v>2120.473730945449</v>
+        <v>1993.946216746609</v>
       </c>
     </row>
     <row r="9">
@@ -868,40 +868,40 @@
         <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>0.0123417173298066</v>
+        <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>0.2326497533296124</v>
+        <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>0.6483250968049924</v>
+        <v>0</v>
       </c>
       <c r="H9" t="n">
-        <v>1.432617827613629</v>
+        <v>0</v>
       </c>
       <c r="I9" t="n">
-        <v>2.912414734633449</v>
+        <v>0.08451607566513439</v>
       </c>
       <c r="J9" t="n">
-        <v>5.704483053012044</v>
+        <v>0.3688277236655604</v>
       </c>
       <c r="K9" t="n">
-        <v>10.97253399805234</v>
+        <v>0.9052645422332346</v>
       </c>
       <c r="L9" t="n">
-        <v>35.90704052311973</v>
+        <v>3.463884611208588</v>
       </c>
       <c r="M9" t="n">
-        <v>116.2619059937895</v>
+        <v>9.378227969686918</v>
       </c>
       <c r="N9" t="n">
-        <v>359.6553935835182</v>
+        <v>30.76917078827705</v>
       </c>
       <c r="O9" t="n">
-        <v>343.1258449179838</v>
+        <v>99.70441643874031</v>
       </c>
       <c r="P9" t="n">
-        <v>319.7742841148242</v>
+        <v>80.91906142598346</v>
       </c>
     </row>
     <row r="10">
@@ -917,43 +917,43 @@
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>0.01267356759353133</v>
+        <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>0.2718428470923482</v>
+        <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>0.7608412569099205</v>
+        <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>1.683479330629633</v>
+        <v>0.07954195729000565</v>
       </c>
       <c r="H10" t="n">
-        <v>3.424305063365242</v>
+        <v>0.398009560569618</v>
       </c>
       <c r="I10" t="n">
-        <v>6.708880367673668</v>
+        <v>0.9988915473671883</v>
       </c>
       <c r="J10" t="n">
-        <v>12.90618933823868</v>
+        <v>2.13263061011508</v>
       </c>
       <c r="K10" t="n">
-        <v>24.59921961410631</v>
+        <v>4.271759907784462</v>
       </c>
       <c r="L10" t="n">
-        <v>79.92158239926121</v>
+        <v>14.41355686766155</v>
       </c>
       <c r="M10" t="n">
-        <v>258.2054804443899</v>
+        <v>36.76093422324562</v>
       </c>
       <c r="N10" t="n">
-        <v>832.7497822776986</v>
+        <v>111.2390888979279</v>
       </c>
       <c r="O10" t="n">
-        <v>684.1166709308459</v>
+        <v>272.0609652791752</v>
       </c>
       <c r="P10" t="n">
-        <v>579.5186851346975</v>
+        <v>470.2914390475262</v>
       </c>
     </row>
     <row r="11">
@@ -978,34 +978,34 @@
         <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>0.459680735841237</v>
+        <v>0</v>
       </c>
       <c r="H11" t="n">
-        <v>1.644170529458017</v>
+        <v>0</v>
       </c>
       <c r="I11" t="n">
-        <v>3.879055877921525</v>
+        <v>0</v>
       </c>
       <c r="J11" t="n">
-        <v>8.095818696557348</v>
+        <v>0.7768487956289797</v>
       </c>
       <c r="K11" t="n">
-        <v>16.05197120382314</v>
+        <v>2.242600548560026</v>
       </c>
       <c r="L11" t="n">
-        <v>53.75764926840662</v>
+        <v>9.054139623697999</v>
       </c>
       <c r="M11" t="n">
-        <v>175.2693657851947</v>
+        <v>26.21616270336694</v>
       </c>
       <c r="N11" t="n">
-        <v>495.024948693582</v>
+        <v>68.18771317517826</v>
       </c>
       <c r="O11" t="n">
-        <v>491.1724913513273</v>
+        <v>210.905231801663</v>
       </c>
       <c r="P11" t="n">
-        <v>486.5767336032999</v>
+        <v>465.4573882606065</v>
       </c>
     </row>
     <row r="12">
@@ -1021,43 +1021,43 @@
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>0.1542678459405066</v>
+        <v>0.001013373681047842</v>
       </c>
       <c r="E12" t="n">
-        <v>0.4453391160261043</v>
+        <v>0.1561798708515672</v>
       </c>
       <c r="F12" t="n">
-        <v>0.9945299325097688</v>
+        <v>0.4489467084955834</v>
       </c>
       <c r="G12" t="n">
-        <v>2.030738531253633</v>
+        <v>1.001336707542121</v>
       </c>
       <c r="H12" t="n">
-        <v>3.985848172353507</v>
+        <v>2.043581496952511</v>
       </c>
       <c r="I12" t="n">
-        <v>7.674732546943149</v>
+        <v>4.010080171671626</v>
       </c>
       <c r="J12" t="n">
-        <v>14.63488845995698</v>
+        <v>7.720453278799082</v>
       </c>
       <c r="K12" t="n">
-        <v>27.76725191031597</v>
+        <v>14.72115395105408</v>
       </c>
       <c r="L12" t="n">
-        <v>89.88649356135898</v>
+        <v>47.84365443880544</v>
       </c>
       <c r="M12" t="n">
-        <v>290.074265514712</v>
+        <v>132.5277377361002</v>
       </c>
       <c r="N12" t="n">
-        <v>935.2068037509518</v>
+        <v>383.7674989814658</v>
       </c>
       <c r="O12" t="n">
-        <v>718.4354212212122</v>
+        <v>858.1197703795244</v>
       </c>
       <c r="P12" t="n">
-        <v>792.3323765467517</v>
+        <v>875.4100064453289</v>
       </c>
     </row>
     <row r="13">
@@ -1079,37 +1079,37 @@
         <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>0.5253006187890602</v>
+        <v>0</v>
       </c>
       <c r="G13" t="n">
-        <v>1.591675461289914</v>
+        <v>0.05134124663742765</v>
       </c>
       <c r="H13" t="n">
-        <v>3.603702516582793</v>
+        <v>0.6974129169464165</v>
       </c>
       <c r="I13" t="n">
-        <v>7.39997818803112</v>
+        <v>1.916415493255699</v>
       </c>
       <c r="J13" t="n">
-        <v>14.56275909384385</v>
+        <v>4.216419268901817</v>
       </c>
       <c r="K13" t="n">
-        <v>28.07743367096741</v>
+        <v>8.556046986509054</v>
       </c>
       <c r="L13" t="n">
-        <v>92.05110173958575</v>
+        <v>27.71307147664887</v>
       </c>
       <c r="M13" t="n">
-        <v>298.2150170411024</v>
+        <v>69.34565573808554</v>
       </c>
       <c r="N13" t="n">
-        <v>683.1478321236802</v>
+        <v>192.3816830009706</v>
       </c>
       <c r="O13" t="n">
-        <v>797.3896347198831</v>
+        <v>407.424235680982</v>
       </c>
       <c r="P13" t="n">
-        <v>751.0526546848929</v>
+        <v>532.9147395122502</v>
       </c>
     </row>
     <row r="14">
@@ -1125,43 +1125,43 @@
         <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>0.6389896536641816</v>
+        <v>0.05610903294551449</v>
       </c>
       <c r="E14" t="n">
-        <v>3.688827438827482</v>
+        <v>0.3152295551466045</v>
       </c>
       <c r="F14" t="n">
-        <v>10.39439991505108</v>
+        <v>0.885072265676923</v>
       </c>
       <c r="G14" t="n">
-        <v>23.58134028795686</v>
+        <v>2.656873842076891</v>
       </c>
       <c r="H14" t="n">
-        <v>48.77951617853385</v>
+        <v>8.237189380758053</v>
       </c>
       <c r="I14" t="n">
-        <v>96.32322183926544</v>
+        <v>18.92660548793559</v>
       </c>
       <c r="J14" t="n">
-        <v>186.0282845299174</v>
+        <v>39.99700183217858</v>
       </c>
       <c r="K14" t="n">
-        <v>355.2830399281729</v>
+        <v>79.75244787302712</v>
       </c>
       <c r="L14" t="n">
-        <v>1156.138101275582</v>
+        <v>263.805689636626</v>
       </c>
       <c r="M14" t="n">
-        <v>3694.693723488276</v>
+        <v>732.3100852928773</v>
       </c>
       <c r="N14" t="n">
-        <v>10798.97522668601</v>
+        <v>2147.173528470938</v>
       </c>
       <c r="O14" t="n">
-        <v>12502.37267926467</v>
+        <v>5889.176986064121</v>
       </c>
       <c r="P14" t="n">
-        <v>13655.33786906631</v>
+        <v>11051.81622707287</v>
       </c>
     </row>
   </sheetData>
@@ -1281,10 +1281,10 @@
         <v>25.6584079007576</v>
       </c>
       <c r="O2" t="n">
-        <v>81.99283665004386</v>
+        <v>74.48165266634837</v>
       </c>
       <c r="P2" t="n">
-        <v>173.0001621783961</v>
+        <v>166.4258845337665</v>
       </c>
     </row>
     <row r="3">
@@ -1303,40 +1303,40 @@
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>0.1135499176983771</v>
+        <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>0.2560648680632862</v>
+        <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>0.4831410325144844</v>
+        <v>0</v>
       </c>
       <c r="H3" t="n">
-        <v>0.9115864236458679</v>
+        <v>0.1498045053811954</v>
       </c>
       <c r="I3" t="n">
-        <v>1.833523490322952</v>
+        <v>0.2882151305223259</v>
       </c>
       <c r="J3" t="n">
-        <v>3.501296492614314</v>
+        <v>0.5438018764543611</v>
       </c>
       <c r="K3" t="n">
-        <v>6.606216680075535</v>
+        <v>1.026040792165756</v>
       </c>
       <c r="L3" t="n">
-        <v>15.40032960738381</v>
+        <v>2.581127801957646</v>
       </c>
       <c r="M3" t="n">
-        <v>48.88547694905209</v>
+        <v>6.250747009148796</v>
       </c>
       <c r="N3" t="n">
-        <v>144.0724071722657</v>
+        <v>19.62857664103433</v>
       </c>
       <c r="O3" t="n">
-        <v>45.69291276094204</v>
+        <v>56.37241108567024</v>
       </c>
       <c r="P3" t="n">
-        <v>140.0374990576134</v>
+        <v>64.75772988396982</v>
       </c>
     </row>
     <row r="4">
@@ -1355,40 +1355,40 @@
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>0.01258016530284576</v>
+        <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>0.02768468222475888</v>
+        <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>0.05223522483216882</v>
+        <v>0.009399658795519437</v>
       </c>
       <c r="H4" t="n">
-        <v>0.09855698147862663</v>
+        <v>0.02486423588958555</v>
       </c>
       <c r="I4" t="n">
-        <v>0.1985366463821873</v>
+        <v>0.04691363048447973</v>
       </c>
       <c r="J4" t="n">
-        <v>0.3785458017174517</v>
+        <v>0.08851624216435915</v>
       </c>
       <c r="K4" t="n">
-        <v>0.7142370247002858</v>
+        <v>0.176411357655439</v>
       </c>
       <c r="L4" t="n">
-        <v>1.665082294483447</v>
+        <v>0.4199217192443052</v>
       </c>
       <c r="M4" t="n">
-        <v>5.464662691758956</v>
+        <v>1.313785222846776</v>
       </c>
       <c r="N4" t="n">
-        <v>13.81684878375293</v>
+        <v>3.472590687951385</v>
       </c>
       <c r="O4" t="n">
-        <v>5.408108567839985</v>
+        <v>9.977382109706866</v>
       </c>
       <c r="P4" t="n">
-        <v>12.27892179859629</v>
+        <v>10.01174195434318</v>
       </c>
     </row>
     <row r="5">
@@ -1404,43 +1404,43 @@
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>0.02119969220781852</v>
+        <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>0.04744945099501312</v>
+        <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>0.08952722378264805</v>
+        <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>0.1689192104471497</v>
+        <v>0</v>
       </c>
       <c r="H5" t="n">
-        <v>0.3399150332236625</v>
+        <v>0.01901344515389591</v>
       </c>
       <c r="I5" t="n">
-        <v>0.6487988672630183</v>
+        <v>0.04551070555405407</v>
       </c>
       <c r="J5" t="n">
-        <v>1.22414822851142</v>
+        <v>0.08586921524281117</v>
       </c>
       <c r="K5" t="n">
-        <v>2.30971254880467</v>
+        <v>0.1620173107986325</v>
       </c>
       <c r="L5" t="n">
-        <v>5.395573557017493</v>
+        <v>0.4054673972665887</v>
       </c>
       <c r="M5" t="n">
-        <v>17.66925519897411</v>
+        <v>1.334188045017314</v>
       </c>
       <c r="N5" t="n">
-        <v>56.0973149354859</v>
+        <v>4.440016070360215</v>
       </c>
       <c r="O5" t="n">
-        <v>29.06710172383784</v>
+        <v>14.20554347911706</v>
       </c>
       <c r="P5" t="n">
-        <v>60.19379214243652</v>
+        <v>43.1775046932524</v>
       </c>
     </row>
     <row r="6">
@@ -1456,43 +1456,43 @@
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>0.04353328157198966</v>
+        <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>0.08819104012399716</v>
+        <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>0.1663981103940569</v>
+        <v>0.01618725911414154</v>
       </c>
       <c r="G6" t="n">
-        <v>0.3139585507074502</v>
+        <v>0.06394081814044193</v>
       </c>
       <c r="H6" t="n">
-        <v>0.6359076260215353</v>
+        <v>0.1206429961667329</v>
       </c>
       <c r="I6" t="n">
-        <v>1.205877955072869</v>
+        <v>0.2276281872421115</v>
       </c>
       <c r="J6" t="n">
-        <v>2.275240351036245</v>
+        <v>0.4456742021897278</v>
       </c>
       <c r="K6" t="n">
-        <v>4.292904296994726</v>
+        <v>0.8742931585393763</v>
       </c>
       <c r="L6" t="n">
-        <v>10.03025721069179</v>
+        <v>1.759025275953812</v>
       </c>
       <c r="M6" t="n">
-        <v>30.26778651642858</v>
+        <v>4.357584239819854</v>
       </c>
       <c r="N6" t="n">
-        <v>83.66378094611866</v>
+        <v>13.69345932855052</v>
       </c>
       <c r="O6" t="n">
-        <v>90.09828849149655</v>
+        <v>39.0852115349021</v>
       </c>
       <c r="P6" t="n">
-        <v>114.1814671169756</v>
+        <v>89.7333434096827</v>
       </c>
     </row>
     <row r="7">
@@ -1508,43 +1508,43 @@
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>0.01865754239332721</v>
+        <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>0.05401039947122595</v>
+        <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>0.1019063660095636</v>
+        <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>0.1922760715518815</v>
+        <v>0.03084897764554169</v>
       </c>
       <c r="H7" t="n">
-        <v>0.3814424118680638</v>
+        <v>0.06482166138765481</v>
       </c>
       <c r="I7" t="n">
-        <v>0.738509830198823</v>
+        <v>0.1223049637734592</v>
       </c>
       <c r="J7" t="n">
-        <v>1.393414116442447</v>
+        <v>0.2307639736996311</v>
       </c>
       <c r="K7" t="n">
-        <v>2.629081997972003</v>
+        <v>0.4662524961509776</v>
       </c>
       <c r="L7" t="n">
-        <v>6.139148322336029</v>
+        <v>1.094453129795627</v>
       </c>
       <c r="M7" t="n">
-        <v>20.11323955721289</v>
+        <v>3.586562124707586</v>
       </c>
       <c r="N7" t="n">
-        <v>58.10791398778119</v>
+        <v>11.92319332679846</v>
       </c>
       <c r="O7" t="n">
-        <v>89.68080462987311</v>
+        <v>38.10802124124313</v>
       </c>
       <c r="P7" t="n">
-        <v>18.92904528558854</v>
+        <v>56.95131097145446</v>
       </c>
     </row>
     <row r="8">
@@ -1563,40 +1563,40 @@
         <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>0.1608793250522426</v>
+        <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>0.3035457530892663</v>
+        <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>0.5727275657615364</v>
+        <v>0.03950132019342035</v>
       </c>
       <c r="H8" t="n">
-        <v>1.080617538690031</v>
+        <v>0.1959087625073787</v>
       </c>
       <c r="I8" t="n">
-        <v>2.199779379342111</v>
+        <v>0.3696390001187385</v>
       </c>
       <c r="J8" t="n">
-        <v>4.150525172304183</v>
+        <v>0.6974317465949726</v>
       </c>
       <c r="K8" t="n">
-        <v>7.831175875047393</v>
+        <v>1.355409655088453</v>
       </c>
       <c r="L8" t="n">
-        <v>18.26129463831092</v>
+        <v>3.310217106940652</v>
       </c>
       <c r="M8" t="n">
-        <v>59.91903502440606</v>
+        <v>8.020156229986574</v>
       </c>
       <c r="N8" t="n">
-        <v>177.8410818713157</v>
+        <v>24.66173544538455</v>
       </c>
       <c r="O8" t="n">
-        <v>45.61545319083035</v>
+        <v>68.38803513057876</v>
       </c>
       <c r="P8" t="n">
-        <v>166.4319199037145</v>
+        <v>131.0065865440822</v>
       </c>
     </row>
     <row r="9">
@@ -1615,40 +1615,40 @@
         <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>0.002468343465961319</v>
+        <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>0.04406160719996115</v>
+        <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>0.08313506869507602</v>
+        <v>0</v>
       </c>
       <c r="H9" t="n">
-        <v>0.1568585461617273</v>
+        <v>0</v>
       </c>
       <c r="I9" t="n">
-        <v>0.2984277248699254</v>
+        <v>0.01690321513302688</v>
       </c>
       <c r="J9" t="n">
-        <v>0.6024752708756802</v>
+        <v>0.05686232960008519</v>
       </c>
       <c r="K9" t="n">
-        <v>1.136745257703135</v>
+        <v>0.1072873637135348</v>
       </c>
       <c r="L9" t="n">
-        <v>2.646486856805085</v>
+        <v>0.2600878106807921</v>
       </c>
       <c r="M9" t="n">
-        <v>8.695517428148086</v>
+        <v>0.6509131453595161</v>
       </c>
       <c r="N9" t="n">
-        <v>27.27002193020374</v>
+        <v>2.426003933468189</v>
       </c>
       <c r="O9" t="n">
-        <v>7.04256256159465</v>
+        <v>7.544437710405842</v>
       </c>
       <c r="P9" t="n">
-        <v>24.93486584988777</v>
+        <v>0.5474684321925044</v>
       </c>
     </row>
     <row r="10">
@@ -1664,43 +1664,43 @@
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>0.002534713518706266</v>
+        <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>0.05183385589976339</v>
+        <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>0.09779968196351449</v>
+        <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>0.1845276147439426</v>
+        <v>0.01590839145800113</v>
       </c>
       <c r="H10" t="n">
-        <v>0.350699860065828</v>
+        <v>0.06369352065592247</v>
       </c>
       <c r="I10" t="n">
-        <v>0.7087489167614486</v>
+        <v>0.1201763973595141</v>
       </c>
       <c r="J10" t="n">
-        <v>1.337261476076517</v>
+        <v>0.2267478125495784</v>
       </c>
       <c r="K10" t="n">
-        <v>2.523133669917469</v>
+        <v>0.4437342509918776</v>
       </c>
       <c r="L10" t="n">
-        <v>5.884773437738766</v>
+        <v>1.076070555655549</v>
       </c>
       <c r="M10" t="n">
-        <v>19.30499118922086</v>
+        <v>2.489089303921044</v>
       </c>
       <c r="N10" t="n">
-        <v>63.96998703854901</v>
+        <v>8.634819585871742</v>
       </c>
       <c r="O10" t="n">
-        <v>4.44168005453558</v>
+        <v>18.57127694204577</v>
       </c>
       <c r="P10" t="n">
-        <v>53.51018845893417</v>
+        <v>28.45786696270685</v>
       </c>
     </row>
     <row r="11">
@@ -1725,34 +1725,34 @@
         <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>0.09193614716824741</v>
+        <v>0</v>
       </c>
       <c r="H11" t="n">
-        <v>0.2368979587233561</v>
+        <v>0</v>
       </c>
       <c r="I11" t="n">
-        <v>0.4469770696927016</v>
+        <v>0</v>
       </c>
       <c r="J11" t="n">
-        <v>0.8433525637271645</v>
+        <v>0.155369759125796</v>
       </c>
       <c r="K11" t="n">
-        <v>1.683166648621405</v>
+        <v>0.2931503505862093</v>
       </c>
       <c r="L11" t="n">
-        <v>4.000761053243203</v>
+        <v>0.6811539075137975</v>
       </c>
       <c r="M11" t="n">
-        <v>13.10538386312092</v>
+        <v>1.867174775176345</v>
       </c>
       <c r="N11" t="n">
-        <v>36.39711100623728</v>
+        <v>4.951596542341481</v>
       </c>
       <c r="O11" t="n">
-        <v>12.72013812889545</v>
+        <v>16.13892663782482</v>
       </c>
       <c r="P11" t="n">
-        <v>35.93753523143455</v>
+        <v>30.40681218823584</v>
       </c>
     </row>
     <row r="12">
@@ -1768,43 +1768,43 @@
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>0.03085356918810132</v>
+        <v>0.0002026747362095685</v>
       </c>
       <c r="E12" t="n">
-        <v>0.05821425401711954</v>
+        <v>0.03103329943410387</v>
       </c>
       <c r="F12" t="n">
-        <v>0.1098381632967329</v>
+        <v>0.05855336752880325</v>
       </c>
       <c r="G12" t="n">
-        <v>0.207241719748773</v>
+        <v>0.1104779998093075</v>
       </c>
       <c r="H12" t="n">
-        <v>0.4218754974080759</v>
+        <v>0.2086516326182876</v>
       </c>
       <c r="I12" t="n">
-        <v>0.7959911289350483</v>
+        <v>0.4243330343779269</v>
       </c>
       <c r="J12" t="n">
-        <v>1.5018693458995</v>
+        <v>0.8006279889542948</v>
       </c>
       <c r="K12" t="n">
-        <v>2.833714409820571</v>
+        <v>1.510618134260307</v>
       </c>
       <c r="L12" t="n">
-        <v>6.6218596960421</v>
+        <v>3.522659123678761</v>
       </c>
       <c r="M12" t="n">
-        <v>21.67713825297396</v>
+        <v>9.352460116366181</v>
       </c>
       <c r="N12" t="n">
-        <v>71.84354212212122</v>
+        <v>29.0242897817804</v>
       </c>
       <c r="O12" t="n">
-        <v>0</v>
+        <v>56.78768725617203</v>
       </c>
       <c r="P12" t="n">
-        <v>79.23323765467518</v>
+        <v>30.75331338836086</v>
       </c>
     </row>
     <row r="13">
@@ -1826,37 +1826,37 @@
         <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>0.105060123757812</v>
+        <v>0</v>
       </c>
       <c r="G13" t="n">
-        <v>0.2132749685001708</v>
+        <v>0.01026824932748553</v>
       </c>
       <c r="H13" t="n">
-        <v>0.4024054110585758</v>
+        <v>0.1292143340617978</v>
       </c>
       <c r="I13" t="n">
-        <v>0.7592551342896655</v>
+        <v>0.2438005152618565</v>
       </c>
       <c r="J13" t="n">
-        <v>1.537616304920357</v>
+        <v>0.4600007551292235</v>
       </c>
       <c r="K13" t="n">
-        <v>2.916209883924884</v>
+        <v>0.8781937928489332</v>
       </c>
       <c r="L13" t="n">
-        <v>6.788383295963538</v>
+        <v>2.041259744860345</v>
       </c>
       <c r="M13" t="n">
-        <v>22.30406593716549</v>
+        <v>4.673757380735977</v>
       </c>
       <c r="N13" t="n">
-        <v>46.01071727520255</v>
+        <v>14.56441091936108</v>
       </c>
       <c r="O13" t="n">
-        <v>33.72824619678578</v>
+        <v>26.17801264873712</v>
       </c>
       <c r="P13" t="n">
-        <v>41.37701927170352</v>
+        <v>27.1134613024879</v>
       </c>
     </row>
     <row r="14">
@@ -1872,43 +1872,43 @@
         <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>0.1277979307328363</v>
+        <v>0.0112218065891029</v>
       </c>
       <c r="E14" t="n">
-        <v>0.60996755703266</v>
+        <v>0.051824104440218</v>
       </c>
       <c r="F14" t="n">
-        <v>1.34111449524472</v>
+        <v>0.1139685421060637</v>
       </c>
       <c r="G14" t="n">
-        <v>2.637388074581157</v>
+        <v>0.3543603152799936</v>
       </c>
       <c r="H14" t="n">
-        <v>5.167433108848234</v>
+        <v>1.127284914325335</v>
       </c>
       <c r="I14" t="n">
-        <v>10.11870868917898</v>
+        <v>2.189707325875725</v>
       </c>
       <c r="J14" t="n">
-        <v>19.2821270333751</v>
+        <v>4.328047810954661</v>
       </c>
       <c r="K14" t="n">
-        <v>36.48833915423229</v>
+        <v>8.305449523449701</v>
       </c>
       <c r="L14" t="n">
-        <v>85.19889986145978</v>
+        <v>19.51639346499148</v>
       </c>
       <c r="M14" t="n">
-        <v>275.1483876988099</v>
+        <v>51.63825268343381</v>
       </c>
       <c r="N14" t="n">
-        <v>804.7491349697914</v>
+        <v>163.0791001636599</v>
       </c>
       <c r="O14" t="n">
-        <v>445.4881329566752</v>
+        <v>425.8385984427521</v>
       </c>
       <c r="P14" t="n">
-        <v>920.0456539499561</v>
+        <v>679.3430242645352</v>
       </c>
     </row>
   </sheetData>
@@ -2028,10 +2028,10 @@
         <v>42524.50048297839</v>
       </c>
       <c r="O2" t="n">
-        <v>132492.1181521182</v>
+        <v>120354.8057174039</v>
       </c>
       <c r="P2" t="n">
-        <v>279550.7371638594</v>
+        <v>268927.3704644634</v>
       </c>
     </row>
     <row r="3">
@@ -2050,40 +2050,40 @@
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>364.7720353759557</v>
+        <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>725.8168529987781</v>
+        <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>1186.869765603945</v>
+        <v>0</v>
       </c>
       <c r="H3" t="n">
-        <v>2032.664241725304</v>
+        <v>334.0355378701805</v>
       </c>
       <c r="I3" t="n">
-        <v>3603.343038554588</v>
+        <v>566.4165142442761</v>
       </c>
       <c r="J3" t="n">
-        <v>6483.96640139837</v>
+        <v>1007.053559555795</v>
       </c>
       <c r="K3" t="n">
-        <v>11235.20794685995</v>
+        <v>1744.98994208155</v>
       </c>
       <c r="L3" t="n">
-        <v>23863.25376940648</v>
+        <v>3999.531784037524</v>
       </c>
       <c r="M3" t="n">
-        <v>73901.90525782132</v>
+        <v>9449.475428912257</v>
       </c>
       <c r="N3" t="n">
-        <v>217799.355751555</v>
+        <v>29673.21384188175</v>
       </c>
       <c r="O3" t="n">
-        <v>67348.70318436256</v>
+        <v>83089.6642956189</v>
       </c>
       <c r="P3" t="n">
-        <v>206407.151324647</v>
+        <v>95449.13784915584</v>
       </c>
     </row>
     <row r="4">
@@ -2102,40 +2102,40 @@
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>47.4190243126765</v>
+        <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>92.07636091055923</v>
+        <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>150.5650474221817</v>
+        <v>27.09397876331395</v>
       </c>
       <c r="H4" t="n">
-        <v>257.8616431374078</v>
+        <v>65.05406949009553</v>
       </c>
       <c r="I4" t="n">
-        <v>457.8164206030667</v>
+        <v>108.1806849127195</v>
       </c>
       <c r="J4" t="n">
-        <v>822.5491431350129</v>
+        <v>192.3385725465524</v>
       </c>
       <c r="K4" t="n">
-        <v>1425.286637457013</v>
+        <v>352.0354477107333</v>
       </c>
       <c r="L4" t="n">
-        <v>3027.379737269369</v>
+        <v>763.4832874575162</v>
       </c>
       <c r="M4" t="n">
-        <v>9693.278522294193</v>
+        <v>2330.406614617427</v>
       </c>
       <c r="N4" t="n">
-        <v>24508.47767114965</v>
+        <v>6159.719388170197</v>
       </c>
       <c r="O4" t="n">
-        <v>9353.138143052489</v>
+        <v>17255.5399004094</v>
       </c>
       <c r="P4" t="n">
-        <v>21235.973795526</v>
+        <v>17314.96407235896</v>
       </c>
     </row>
     <row r="5">
@@ -2151,43 +2151,43 @@
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>94.01061545262118</v>
+        <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>178.8535059906331</v>
+        <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>297.758193552944</v>
+        <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>486.8999609594786</v>
+        <v>0</v>
       </c>
       <c r="H5" t="n">
-        <v>889.3438869489773</v>
+        <v>49.74622939471648</v>
       </c>
       <c r="I5" t="n">
-        <v>1496.100495874644</v>
+        <v>104.9456042274849</v>
       </c>
       <c r="J5" t="n">
-        <v>2659.974227329785</v>
+        <v>186.586799006082</v>
       </c>
       <c r="K5" t="n">
-        <v>4609.11758748364</v>
+        <v>323.3115900354112</v>
       </c>
       <c r="L5" t="n">
-        <v>9809.995645007175</v>
+        <v>737.2030719893183</v>
       </c>
       <c r="M5" t="n">
-        <v>31341.91835544413</v>
+        <v>2366.597364000389</v>
       </c>
       <c r="N5" t="n">
-        <v>99506.03151454385</v>
+        <v>7875.749125077405</v>
       </c>
       <c r="O5" t="n">
-        <v>50270.55474772016</v>
+        <v>24567.99986365429</v>
       </c>
       <c r="P5" t="n">
-        <v>104103.0974508081</v>
+        <v>74674.01236539596</v>
       </c>
     </row>
     <row r="6">
@@ -2203,43 +2203,43 @@
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>180.3727515356719</v>
+        <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>310.593894935417</v>
+        <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>517.0817120542558</v>
+        <v>50.30186722904705</v>
       </c>
       <c r="G6" t="n">
-        <v>845.5420232367547</v>
+        <v>172.2031415167942</v>
       </c>
       <c r="H6" t="n">
-        <v>1554.517335033046</v>
+        <v>294.9196097314305</v>
       </c>
       <c r="I6" t="n">
-        <v>2598.102159947877</v>
+        <v>490.432122463846</v>
       </c>
       <c r="J6" t="n">
-        <v>4619.265085792911</v>
+        <v>904.8218931577946</v>
       </c>
       <c r="K6" t="n">
-        <v>8004.11362239022</v>
+        <v>1630.118282656929</v>
       </c>
       <c r="L6" t="n">
-        <v>17039.052899598</v>
+        <v>2988.17110061326</v>
       </c>
       <c r="M6" t="n">
-        <v>50163.77116284562</v>
+        <v>7221.963803349118</v>
       </c>
       <c r="N6" t="n">
-        <v>138658.6614029928</v>
+        <v>22694.60833590529</v>
       </c>
       <c r="O6" t="n">
-        <v>145589.7072456342</v>
+        <v>63157.7425084733</v>
       </c>
       <c r="P6" t="n">
-        <v>184505.6842784135</v>
+        <v>144999.9929623599</v>
       </c>
     </row>
     <row r="7">
@@ -2255,43 +2255,43 @@
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>86.81209506566726</v>
+        <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>213.6102633132164</v>
+        <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>355.6218021906884</v>
+        <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>581.5196537058439</v>
+        <v>93.29963241304415</v>
       </c>
       <c r="H7" t="n">
-        <v>1047.144923571304</v>
+        <v>177.9499907394115</v>
       </c>
       <c r="I7" t="n">
-        <v>1786.839006016206</v>
+        <v>295.9192565398627</v>
       </c>
       <c r="J7" t="n">
-        <v>3176.889331630113</v>
+        <v>526.1261512425694</v>
       </c>
       <c r="K7" t="n">
-        <v>5504.811415637111</v>
+        <v>976.2464865534911</v>
       </c>
       <c r="L7" t="n">
-        <v>11711.64185419752</v>
+        <v>2087.886203325118</v>
       </c>
       <c r="M7" t="n">
-        <v>37434.13634464054</v>
+        <v>6675.197956197962</v>
       </c>
       <c r="N7" t="n">
-        <v>108148.6435207889</v>
+        <v>22191.07684713178</v>
       </c>
       <c r="O7" t="n">
-        <v>162738.3481413184</v>
+        <v>69152.32811892487</v>
       </c>
       <c r="P7" t="n">
-        <v>34349.39700176114</v>
+        <v>103346.1096856592</v>
       </c>
     </row>
     <row r="8">
@@ -2310,40 +2310,40 @@
         <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>669.8648538691831</v>
+        <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>1115.201783202062</v>
+        <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>1823.599539693193</v>
+        <v>125.7746154163416</v>
       </c>
       <c r="H8" t="n">
-        <v>3123.144327191508</v>
+        <v>566.2052653834762</v>
       </c>
       <c r="I8" t="n">
-        <v>5603.38548854148</v>
+        <v>941.5625170028487</v>
       </c>
       <c r="J8" t="n">
-        <v>9962.473126914147</v>
+        <v>1674.039969609898</v>
       </c>
       <c r="K8" t="n">
-        <v>17262.65225892362</v>
+        <v>2987.797224518083</v>
       </c>
       <c r="L8" t="n">
-        <v>36676.12558636065</v>
+        <v>6648.265675401434</v>
       </c>
       <c r="M8" t="n">
-        <v>117406.6868481841</v>
+        <v>15714.87208670848</v>
       </c>
       <c r="N8" t="n">
-        <v>348465.762165615</v>
+        <v>48322.75168299455</v>
       </c>
       <c r="O8" t="n">
-        <v>87145.43292263633</v>
+        <v>130651.0077462252</v>
       </c>
       <c r="P8" t="n">
-        <v>317957.6371077312</v>
+        <v>250279.7824311838</v>
       </c>
     </row>
     <row r="9">
@@ -2362,40 +2362,40 @@
         <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>10.98416784775174</v>
+        <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>173.0072256961742</v>
+        <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>282.9047638690649</v>
+        <v>0</v>
       </c>
       <c r="H9" t="n">
-        <v>484.5101071706643</v>
+        <v>0</v>
       </c>
       <c r="I9" t="n">
-        <v>812.4285104854574</v>
+        <v>46.01668259517735</v>
       </c>
       <c r="J9" t="n">
-        <v>1545.531815606694</v>
+        <v>145.8691231902535</v>
       </c>
       <c r="K9" t="n">
-        <v>2678.047704424301</v>
+        <v>252.7573140593666</v>
       </c>
       <c r="L9" t="n">
-        <v>5680.626589110052</v>
+        <v>558.2728397300124</v>
       </c>
       <c r="M9" t="n">
-        <v>18209.50185388557</v>
+        <v>1363.09359679668</v>
       </c>
       <c r="N9" t="n">
-        <v>57106.83912680076</v>
+        <v>5080.355883253178</v>
       </c>
       <c r="O9" t="n">
-        <v>14379.30728724392</v>
+        <v>15404.02193073774</v>
       </c>
       <c r="P9" t="n">
-        <v>50911.31176839062</v>
+        <v>1117.805734448339</v>
       </c>
     </row>
     <row r="10">
@@ -2411,43 +2411,43 @@
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>9.948585996421192</v>
+        <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>172.9278412602966</v>
+        <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>287.893051598177</v>
+        <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>470.7682899034418</v>
+        <v>40.58561236045868</v>
       </c>
       <c r="H10" t="n">
-        <v>812.1197672711154</v>
+        <v>147.495830657179</v>
       </c>
       <c r="I10" t="n">
-        <v>1446.532611295922</v>
+        <v>245.2759697791612</v>
       </c>
       <c r="J10" t="n">
-        <v>2571.845591689188</v>
+        <v>436.0855169789036</v>
       </c>
       <c r="K10" t="n">
-        <v>4456.411128782433</v>
+        <v>783.7326567033696</v>
       </c>
       <c r="L10" t="n">
-        <v>9469.915008114705</v>
+        <v>1731.637897806385</v>
       </c>
       <c r="M10" t="n">
-        <v>30308.33482186096</v>
+        <v>3907.805566203762</v>
       </c>
       <c r="N10" t="n">
-        <v>100431.2183678702</v>
+        <v>13556.44250597174</v>
       </c>
       <c r="O10" t="n">
-        <v>6798.989278022677</v>
+        <v>28427.5119454459</v>
       </c>
       <c r="P10" t="n">
-        <v>81909.36608001735</v>
+        <v>43561.1592863976</v>
       </c>
     </row>
     <row r="11">
@@ -2472,34 +2472,34 @@
         <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>225.8475809272861</v>
+        <v>0</v>
       </c>
       <c r="H11" t="n">
-        <v>528.2373641643316</v>
+        <v>0</v>
       </c>
       <c r="I11" t="n">
-        <v>878.4243676022043</v>
+        <v>0</v>
       </c>
       <c r="J11" t="n">
-        <v>1561.784241715879</v>
+        <v>287.7255039926122</v>
       </c>
       <c r="K11" t="n">
-        <v>2862.56540199717</v>
+        <v>498.5614774738662</v>
       </c>
       <c r="L11" t="n">
-        <v>6199.294347474622</v>
+        <v>1055.467575397296</v>
       </c>
       <c r="M11" t="n">
-        <v>19811.87250416143</v>
+        <v>2822.67417537289</v>
       </c>
       <c r="N11" t="n">
-        <v>55022.80057622532</v>
+        <v>7485.503699359351</v>
       </c>
       <c r="O11" t="n">
-        <v>18748.7458238679</v>
+        <v>23787.84179357834</v>
       </c>
       <c r="P11" t="n">
-        <v>52969.84252552077</v>
+        <v>44817.87754617929</v>
       </c>
     </row>
     <row r="12">
@@ -2515,43 +2515,43 @@
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>121.0982559169156</v>
+        <v>0.79548518110718</v>
       </c>
       <c r="E12" t="n">
-        <v>194.2140923728768</v>
+        <v>103.533132644073</v>
       </c>
       <c r="F12" t="n">
-        <v>323.3307448303586</v>
+        <v>172.363624510615</v>
       </c>
       <c r="G12" t="n">
-        <v>528.7166917437264</v>
+        <v>281.8523347540737</v>
       </c>
       <c r="H12" t="n">
-        <v>976.9420230396514</v>
+        <v>483.1770257646963</v>
       </c>
       <c r="I12" t="n">
-        <v>1624.59102098967</v>
+        <v>866.0493974122322</v>
       </c>
       <c r="J12" t="n">
-        <v>2888.422440671385</v>
+        <v>1539.782309452593</v>
       </c>
       <c r="K12" t="n">
-        <v>5004.965286729578</v>
+        <v>2668.085145516047</v>
       </c>
       <c r="L12" t="n">
-        <v>10656.05144881751</v>
+        <v>5668.745425247172</v>
       </c>
       <c r="M12" t="n">
-        <v>34032.54410795829</v>
+        <v>14683.11950192437</v>
       </c>
       <c r="N12" t="n">
-        <v>112792.4953750576</v>
+        <v>45567.3812047164</v>
       </c>
       <c r="O12" t="n">
-        <v>0</v>
+        <v>86926.3143760563</v>
       </c>
       <c r="P12" t="n">
-        <v>121284.2723165224</v>
+        <v>47074.85578066907</v>
       </c>
     </row>
     <row r="13">
@@ -2573,37 +2573,37 @@
         <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>401.0446676441024</v>
+        <v>0</v>
       </c>
       <c r="G13" t="n">
-        <v>705.580903197674</v>
+        <v>33.97060932980678</v>
       </c>
       <c r="H13" t="n">
-        <v>1208.396332216239</v>
+        <v>388.0219377251655</v>
       </c>
       <c r="I13" t="n">
-        <v>2009.484477909162</v>
+        <v>645.2552363485871</v>
       </c>
       <c r="J13" t="n">
-        <v>3834.755071388874</v>
+        <v>1147.223935470605</v>
       </c>
       <c r="K13" t="n">
-        <v>6679.20643064427</v>
+        <v>2011.390764732613</v>
       </c>
       <c r="L13" t="n">
-        <v>14165.88747358924</v>
+        <v>4259.667521610501</v>
       </c>
       <c r="M13" t="n">
-        <v>45408.54711093651</v>
+        <v>9515.23963416008</v>
       </c>
       <c r="N13" t="n">
-        <v>93672.59892814554</v>
+        <v>29651.48781562889</v>
       </c>
       <c r="O13" t="n">
-        <v>66950.20962513721</v>
+        <v>51963.07641307078</v>
       </c>
       <c r="P13" t="n">
-        <v>82132.9427489736</v>
+        <v>53819.93203185288</v>
       </c>
     </row>
     <row r="14">
@@ -2619,43 +2619,43 @@
         <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>537.8982035473457</v>
+        <v>46.4513847611557</v>
       </c>
       <c r="E14" t="n">
-        <v>2236.461370468092</v>
+        <v>176.7548238341584</v>
       </c>
       <c r="F14" t="n">
-        <v>4410.733043909953</v>
+        <v>344.5661409715154</v>
       </c>
       <c r="G14" t="n">
-        <v>7488.148521171997</v>
+        <v>974.1142254632417</v>
       </c>
       <c r="H14" t="n">
-        <v>13283.20407602624</v>
+        <v>2874.927621313039</v>
       </c>
       <c r="I14" t="n">
-        <v>22929.54332660965</v>
+        <v>4922.549714315566</v>
       </c>
       <c r="J14" t="n">
-        <v>41216.43603273787</v>
+        <v>9136.632889669168</v>
       </c>
       <c r="K14" t="n">
-        <v>71609.33408795032</v>
+        <v>16115.97499866247</v>
       </c>
       <c r="L14" t="n">
-        <v>152316.7191707685</v>
+        <v>34515.8271944387</v>
       </c>
       <c r="M14" t="n">
-        <v>480543.2879239891</v>
+        <v>88881.23676219981</v>
       </c>
       <c r="N14" t="n">
-        <v>1398637.384883723</v>
+        <v>280782.7908130689</v>
       </c>
       <c r="O14" t="n">
-        <v>761815.254551114</v>
+        <v>714737.8546095989</v>
       </c>
       <c r="P14" t="n">
-        <v>1537317.413562171</v>
+        <v>1145383.000210124</v>
       </c>
     </row>
   </sheetData>
@@ -2763,10 +2763,10 @@
         <v>305.0250470968311</v>
       </c>
       <c r="M2" t="n">
-        <v>983.1163787606301</v>
+        <v>914.5210919242497</v>
       </c>
       <c r="N2" t="n">
-        <v>2328.703162360821</v>
+        <v>2200.068810877073</v>
       </c>
     </row>
     <row r="3">
@@ -2779,40 +2779,40 @@
         <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>0.5184927696935063</v>
+        <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>1.687738730892764</v>
+        <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>3.893862144970728</v>
+        <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>8.056357188486725</v>
+        <v>0.684038830516668</v>
       </c>
       <c r="G3" t="n">
-        <v>15.91011771554078</v>
+        <v>2.000089641659017</v>
       </c>
       <c r="H3" t="n">
-        <v>30.72852681188193</v>
+        <v>4.483203207943685</v>
       </c>
       <c r="I3" t="n">
-        <v>58.68777606453168</v>
+        <v>9.168320933538883</v>
       </c>
       <c r="J3" t="n">
-        <v>190.9814324857059</v>
+        <v>31.39819985860508</v>
       </c>
       <c r="K3" t="n">
-        <v>602.1676718454901</v>
+        <v>82.99894902524228</v>
       </c>
       <c r="L3" t="n">
-        <v>1762.172440107205</v>
+        <v>236.3408528894054</v>
       </c>
       <c r="M3" t="n">
-        <v>1733.016603064425</v>
+        <v>694.0729403351113</v>
       </c>
       <c r="N3" t="n">
-        <v>1696.168127500012</v>
+        <v>1106.21132199396</v>
       </c>
     </row>
     <row r="4">
@@ -2825,40 +2825,40 @@
         <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>0.05744367660750735</v>
+        <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>0.1838577494290236</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>0.4223747554099211</v>
+        <v>0.0429208159886888</v>
       </c>
       <c r="F4" t="n">
-        <v>0.8724066298074407</v>
+        <v>0.1564561385500732</v>
       </c>
       <c r="G4" t="n">
-        <v>1.721522973276741</v>
+        <v>0.3706736272046093</v>
       </c>
       <c r="H4" t="n">
-        <v>3.323628525715469</v>
+        <v>0.7748573773379277</v>
       </c>
       <c r="I4" t="n">
-        <v>6.346467764291264</v>
+        <v>1.537467866789081</v>
       </c>
       <c r="J4" t="n">
-        <v>20.64938672764186</v>
+        <v>5.151725307161506</v>
       </c>
       <c r="K4" t="n">
-        <v>66.74250382953818</v>
+        <v>16.23570560481135</v>
       </c>
       <c r="L4" t="n">
-        <v>176.0868610291942</v>
+        <v>43.71119509529134</v>
       </c>
       <c r="M4" t="n">
-        <v>175.5703850168341</v>
+        <v>122.8308005767901</v>
       </c>
       <c r="N4" t="n">
-        <v>161.5253898590499</v>
+        <v>182.5490763850119</v>
       </c>
     </row>
     <row r="5">
@@ -2868,43 +2868,43 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.09680224655626299</v>
+        <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>0.3134664041842018</v>
+        <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>0.7222665086927671</v>
+        <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>1.493587096628646</v>
+        <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>2.948908273928603</v>
+        <v>0.08681938339617104</v>
       </c>
       <c r="G5" t="n">
-        <v>5.69479599198573</v>
+        <v>0.2946308222041483</v>
       </c>
       <c r="H5" t="n">
-        <v>10.8757137699883</v>
+        <v>0.686727691538025</v>
       </c>
       <c r="I5" t="n">
-        <v>20.65102571952979</v>
+        <v>1.426532756279849</v>
       </c>
       <c r="J5" t="n">
-        <v>66.89227022140872</v>
+        <v>4.938706221625027</v>
       </c>
       <c r="K5" t="n">
-        <v>215.9110196965315</v>
+        <v>16.25716668659327</v>
       </c>
       <c r="L5" t="n">
-        <v>673.6673004273453</v>
+        <v>52.73245714735605</v>
       </c>
       <c r="M5" t="n">
-        <v>777.7572219879412</v>
+        <v>170.2790809408372</v>
       </c>
       <c r="N5" t="n">
-        <v>815.1679723622412</v>
+        <v>524.0460967903102</v>
       </c>
     </row>
     <row r="6">
@@ -2914,43 +2914,43 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.1987821056468349</v>
+        <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>0.6014809149714319</v>
+        <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>1.361289630633878</v>
+        <v>0.07391442443958424</v>
       </c>
       <c r="E6" t="n">
-        <v>2.794890304459744</v>
+        <v>0.3658816276406516</v>
       </c>
       <c r="F6" t="n">
-        <v>5.499795959828703</v>
+        <v>0.9167628831671488</v>
       </c>
       <c r="G6" t="n">
-        <v>10.60338912773739</v>
+        <v>1.95616098803395</v>
       </c>
       <c r="H6" t="n">
-        <v>20.23280565538015</v>
+        <v>3.917288562375123</v>
       </c>
       <c r="I6" t="n">
-        <v>38.40150751153457</v>
+        <v>7.61752752262814</v>
       </c>
       <c r="J6" t="n">
-        <v>124.345195317968</v>
+        <v>22.61110482529435</v>
       </c>
       <c r="K6" t="n">
-        <v>377.8198117594187</v>
+        <v>57.85555015576878</v>
       </c>
       <c r="L6" t="n">
-        <v>1040.470925326316</v>
+        <v>164.8497113046569</v>
       </c>
       <c r="M6" t="n">
-        <v>1586.868198173466</v>
+        <v>481.9969893668119</v>
       </c>
       <c r="N6" t="n">
-        <v>1865.568525713923</v>
+        <v>1176.425147547025</v>
       </c>
     </row>
     <row r="7">
@@ -2960,43 +2960,43 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.08519425665183464</v>
+        <v>0</v>
       </c>
       <c r="C7" t="n">
-        <v>0.3318170828213413</v>
+        <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>0.7971429503578707</v>
+        <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>1.675115871038788</v>
+        <v>0.1408629102148489</v>
       </c>
       <c r="F7" t="n">
-        <v>3.331667769883024</v>
+        <v>0.4368522286597721</v>
       </c>
       <c r="G7" t="n">
-        <v>6.457235915465684</v>
+        <v>0.9953223772917794</v>
       </c>
       <c r="H7" t="n">
-        <v>12.35453152056982</v>
+        <v>2.049039141638772</v>
       </c>
       <c r="I7" t="n">
-        <v>23.48149910984864</v>
+        <v>4.037183041873478</v>
       </c>
       <c r="J7" t="n">
-        <v>76.11893839034448</v>
+        <v>13.45696430072073</v>
       </c>
       <c r="K7" t="n">
-        <v>245.7503023739299</v>
+        <v>43.81350073575501</v>
       </c>
       <c r="L7" t="n">
-        <v>714.3484270573747</v>
+        <v>141.6416008804428</v>
       </c>
       <c r="M7" t="n">
-        <v>1349.668649678238</v>
+        <v>456.9060645454744</v>
       </c>
       <c r="N7" t="n">
-        <v>991.8707655649602</v>
+        <v>868.1217466858836</v>
       </c>
     </row>
     <row r="8">
@@ -3009,40 +3009,40 @@
         <v>0</v>
       </c>
       <c r="C8" t="n">
-        <v>0.7346087828468006</v>
+        <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>2.12066243606054</v>
+        <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>4.735856774116524</v>
+        <v>0.1803713232803979</v>
       </c>
       <c r="F8" t="n">
-        <v>9.67018338545833</v>
+        <v>1.074931873729215</v>
       </c>
       <c r="G8" t="n">
-        <v>18.98022920235727</v>
+        <v>2.7627811724614</v>
       </c>
       <c r="H8" t="n">
-        <v>36.54634509617061</v>
+        <v>5.94740098808083</v>
       </c>
       <c r="I8" t="n">
-        <v>69.68994435051478</v>
+        <v>11.95611478596188</v>
       </c>
       <c r="J8" t="n">
-        <v>226.5031028201035</v>
+        <v>40.44792249791391</v>
       </c>
       <c r="K8" t="n">
-        <v>731.8550030145899</v>
+        <v>106.5682706302017</v>
       </c>
       <c r="L8" t="n">
-        <v>2171.325246740827</v>
+        <v>298.4647611739928</v>
       </c>
       <c r="M8" t="n">
-        <v>2040.698929932244</v>
+        <v>849.7695858033387</v>
       </c>
       <c r="N8" t="n">
-        <v>1936.505670996083</v>
+        <v>1820.955430874107</v>
       </c>
     </row>
     <row r="9">
@@ -3055,40 +3055,40 @@
         <v>0</v>
       </c>
       <c r="C9" t="n">
-        <v>0.01127097461770724</v>
+        <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>0.2124655260302418</v>
+        <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>0.5920777080563848</v>
+        <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>1.308326770125526</v>
+        <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>2.65973945708612</v>
+        <v>0.07718362997257865</v>
       </c>
       <c r="H9" t="n">
-        <v>5.209573512298824</v>
+        <v>0.3368289680157837</v>
       </c>
       <c r="I9" t="n">
-        <v>10.02057889344931</v>
+        <v>0.8267256010781635</v>
       </c>
       <c r="J9" t="n">
-        <v>32.79181750141491</v>
+        <v>3.163364910109354</v>
       </c>
       <c r="K9" t="n">
-        <v>106.1752555535803</v>
+        <v>8.56459166749282</v>
       </c>
       <c r="L9" t="n">
-        <v>328.4524109469994</v>
+        <v>28.09969906902771</v>
       </c>
       <c r="M9" t="n">
-        <v>313.3569328645894</v>
+        <v>91.05426067734807</v>
       </c>
       <c r="N9" t="n">
-        <v>292.0313067735902</v>
+        <v>73.89868549478798</v>
       </c>
     </row>
     <row r="10">
@@ -3098,43 +3098,43 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.01157403421625174</v>
+        <v>0</v>
       </c>
       <c r="C10" t="n">
-        <v>0.2482583053643103</v>
+        <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>0.6948321911429297</v>
+        <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>1.537424030862867</v>
+        <v>0.07264105615943933</v>
       </c>
       <c r="F10" t="n">
-        <v>3.1272192046778</v>
+        <v>0.363479047113719</v>
       </c>
       <c r="G10" t="n">
-        <v>6.126831324735035</v>
+        <v>0.9122297145007057</v>
       </c>
       <c r="H10" t="n">
-        <v>11.78647416363177</v>
+        <v>1.947607843642716</v>
       </c>
       <c r="I10" t="n">
-        <v>22.46504051882567</v>
+        <v>3.901150561704898</v>
       </c>
       <c r="J10" t="n">
-        <v>72.9877457534661</v>
+        <v>13.16306550093697</v>
       </c>
       <c r="K10" t="n">
-        <v>235.8040893719955</v>
+        <v>33.57162909190527</v>
       </c>
       <c r="L10" t="n">
-        <v>760.5020766668499</v>
+        <v>101.5882080233214</v>
       </c>
       <c r="M10" t="n">
-        <v>624.7640767942275</v>
+        <v>248.4575000534845</v>
       </c>
       <c r="N10" t="n">
-        <v>529.2408030497813</v>
+        <v>429.4898943786409</v>
       </c>
     </row>
     <row r="11">
@@ -3153,34 +3153,34 @@
         <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>0.419799754561123</v>
+        <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>1.501525582663298</v>
+        <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>3.542516748064809</v>
+        <v>0</v>
       </c>
       <c r="H11" t="n">
-        <v>7.393441658081425</v>
+        <v>0.7094509478178006</v>
       </c>
       <c r="I11" t="n">
-        <v>14.65933428612185</v>
+        <v>2.048037010168055</v>
       </c>
       <c r="J11" t="n">
-        <v>49.09374313317821</v>
+        <v>8.268620578225208</v>
       </c>
       <c r="K11" t="n">
-        <v>160.0633461484028</v>
+        <v>23.94170085954823</v>
       </c>
       <c r="L11" t="n">
-        <v>452.0775741948242</v>
+        <v>62.27188355552613</v>
       </c>
       <c r="M11" t="n">
-        <v>448.5593483466688</v>
+        <v>192.6075157010143</v>
       </c>
       <c r="N11" t="n">
-        <v>444.3623093493448</v>
+        <v>425.0752361698928</v>
       </c>
     </row>
     <row r="12">
@@ -3190,43 +3190,43 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.1408838761624001</v>
+        <v>0.0009254554072274934</v>
       </c>
       <c r="C12" t="n">
-        <v>0.4067023849979116</v>
+        <v>0.1426300176162269</v>
       </c>
       <c r="D12" t="n">
-        <v>0.9082465046250864</v>
+        <v>0.4099969899599236</v>
       </c>
       <c r="E12" t="n">
-        <v>1.854555717759131</v>
+        <v>0.9144627374691814</v>
       </c>
       <c r="F12" t="n">
-        <v>3.640043956616461</v>
+        <v>1.866284453439905</v>
       </c>
       <c r="G12" t="n">
-        <v>7.008888100635455</v>
+        <v>3.662173636137738</v>
       </c>
       <c r="H12" t="n">
-        <v>13.36519480694803</v>
+        <v>7.050642193237032</v>
       </c>
       <c r="I12" t="n">
-        <v>25.35822066908078</v>
+        <v>13.44397607656853</v>
       </c>
       <c r="J12" t="n">
-        <v>82.08812115296257</v>
+        <v>43.69283466700355</v>
       </c>
       <c r="K12" t="n">
-        <v>264.9080023871866</v>
+        <v>121.0298962655916</v>
       </c>
       <c r="L12" t="n">
-        <v>854.0701318711267</v>
+        <v>350.4725983048318</v>
       </c>
       <c r="M12" t="n">
-        <v>656.1054009469023</v>
+        <v>783.6710153409375</v>
       </c>
       <c r="N12" t="n">
-        <v>723.5912042223085</v>
+        <v>799.461185106145</v>
       </c>
     </row>
     <row r="13">
@@ -3242,37 +3242,37 @@
         <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>0.4797265877041589</v>
+        <v>0</v>
       </c>
       <c r="E13" t="n">
-        <v>1.453584881619324</v>
+        <v>0.0468869827616577</v>
       </c>
       <c r="F13" t="n">
-        <v>3.291052493649103</v>
+        <v>0.6369067670979792</v>
       </c>
       <c r="G13" t="n">
-        <v>6.757970880393916</v>
+        <v>1.750151117891821</v>
       </c>
       <c r="H13" t="n">
-        <v>13.29932324038014</v>
+        <v>3.850611165970432</v>
       </c>
       <c r="I13" t="n">
-        <v>25.64149168054162</v>
+        <v>7.813741462053502</v>
       </c>
       <c r="J13" t="n">
-        <v>84.06493225486275</v>
+        <v>25.30874082147777</v>
       </c>
       <c r="K13" t="n">
-        <v>272.3424785926504</v>
+        <v>63.32936533756072</v>
       </c>
       <c r="L13" t="n">
-        <v>623.879292504294</v>
+        <v>175.6910329471724</v>
       </c>
       <c r="M13" t="n">
-        <v>728.2097047908555</v>
+        <v>372.0769238417713</v>
       </c>
       <c r="N13" t="n">
-        <v>685.8928284697409</v>
+        <v>486.6801225416463</v>
       </c>
     </row>
     <row r="14">
@@ -3282,43 +3282,43 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.5835521892915844</v>
+        <v>0.05124112546522754</v>
       </c>
       <c r="C14" t="n">
-        <v>3.368792147889686</v>
+        <v>0.2878808694011954</v>
       </c>
       <c r="D14" t="n">
-        <v>9.492602567221075</v>
+        <v>0.8082851660513246</v>
       </c>
       <c r="E14" t="n">
-        <v>21.53547036725429</v>
+        <v>2.426368781285984</v>
       </c>
       <c r="F14" t="n">
-        <v>44.54750291391661</v>
+        <v>7.522547304462246</v>
       </c>
       <c r="G14" t="n">
-        <v>87.96641175893446</v>
+        <v>17.28457104901327</v>
       </c>
       <c r="H14" t="n">
-        <v>169.8888426206708</v>
+        <v>36.52694194722243</v>
       </c>
       <c r="I14" t="n">
-        <v>324.4593939500845</v>
+        <v>72.83328500045901</v>
       </c>
       <c r="J14" t="n">
-        <v>1055.833871885115</v>
+        <v>240.9184356151315</v>
       </c>
       <c r="K14" t="n">
-        <v>3374.14948542588</v>
+        <v>668.7763269130378</v>
       </c>
       <c r="L14" t="n">
-        <v>9862.077733969189</v>
+        <v>1960.889047487856</v>
       </c>
       <c r="M14" t="n">
-        <v>11417.69183035702</v>
+        <v>5378.243769107169</v>
       </c>
       <c r="N14" t="n">
-        <v>12470.62806622185</v>
+        <v>10092.98275484448</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implement pipelines cost curve
</commit_message>
<xml_diff>
--- a/tutorial/dac_scenarios/SSPs/get_report_output.xlsx
+++ b/tutorial/dac_scenarios/SSPs/get_report_output.xlsx
@@ -501,43 +501,43 @@
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>0.05529194511868137</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>0.1596163206428224</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>0.3564546721448534</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>0.727847612935295</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>1.428588679990762</v>
       </c>
       <c r="I2" t="n">
-        <v>0</v>
+        <v>2.750741012808266</v>
       </c>
       <c r="J2" t="n">
-        <v>0</v>
+        <v>5.245366878708023</v>
       </c>
       <c r="K2" t="n">
-        <v>0</v>
+        <v>9.952205914081944</v>
       </c>
       <c r="L2" t="n">
-        <v>0</v>
+        <v>32.21668805061326</v>
       </c>
       <c r="M2" t="n">
-        <v>0</v>
+        <v>103.9670339039195</v>
       </c>
       <c r="N2" t="n">
-        <v>0</v>
+        <v>335.1923594470671</v>
       </c>
       <c r="O2" t="n">
-        <v>0</v>
+        <v>779.9949950850662</v>
       </c>
       <c r="P2" t="n">
-        <v>0</v>
+        <v>985.7507147372517</v>
       </c>
     </row>
     <row r="3">
@@ -556,40 +556,40 @@
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>0.3338248112832123</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>1.409474263455727</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>3.439000574022576</v>
       </c>
       <c r="H3" t="n">
-        <v>0</v>
+        <v>7.268293692671865</v>
       </c>
       <c r="I3" t="n">
-        <v>0</v>
+        <v>14.49337163927865</v>
       </c>
       <c r="J3" t="n">
-        <v>0</v>
+        <v>28.12558774734117</v>
       </c>
       <c r="K3" t="n">
-        <v>0</v>
+        <v>53.84673807821013</v>
       </c>
       <c r="L3" t="n">
-        <v>0</v>
+        <v>175.5636916149057</v>
       </c>
       <c r="M3" t="n">
-        <v>0</v>
+        <v>125.5462466553449</v>
       </c>
       <c r="N3" t="n">
-        <v>0</v>
+        <v>89.99052310125347</v>
       </c>
       <c r="O3" t="n">
-        <v>0</v>
+        <v>69.10144002739311</v>
       </c>
       <c r="P3" t="n">
-        <v>0</v>
+        <v>51.45846723032821</v>
       </c>
     </row>
     <row r="4">
@@ -605,43 +605,43 @@
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>0.004725193092549785</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>0.09185337213622827</v>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>0.2562460852118302</v>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>0.5664208691793595</v>
       </c>
       <c r="H4" t="n">
-        <v>0</v>
+        <v>1.151656034469554</v>
       </c>
       <c r="I4" t="n">
-        <v>0</v>
+        <v>2.255872806417387</v>
       </c>
       <c r="J4" t="n">
-        <v>0</v>
+        <v>4.339299694899545</v>
       </c>
       <c r="K4" t="n">
-        <v>0</v>
+        <v>8.270291969173311</v>
       </c>
       <c r="L4" t="n">
-        <v>0</v>
+        <v>26.86865988264025</v>
       </c>
       <c r="M4" t="n">
-        <v>0</v>
+        <v>21.90458427646609</v>
       </c>
       <c r="N4" t="n">
-        <v>0</v>
+        <v>18.93240884187747</v>
       </c>
       <c r="O4" t="n">
-        <v>0</v>
+        <v>21.13646764141426</v>
       </c>
       <c r="P4" t="n">
-        <v>0</v>
+        <v>21.59248346329874</v>
       </c>
     </row>
     <row r="5">
@@ -657,43 +657,43 @@
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>0.1437590573085715</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>0.4150024336713384</v>
       </c>
       <c r="F5" t="n">
-        <v>0</v>
+        <v>0.926782147576619</v>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>1.892403793631766</v>
       </c>
       <c r="H5" t="n">
-        <v>0</v>
+        <v>3.714330567975981</v>
       </c>
       <c r="I5" t="n">
-        <v>0</v>
+        <v>7.151926633301487</v>
       </c>
       <c r="J5" t="n">
-        <v>0</v>
+        <v>13.63795388464085</v>
       </c>
       <c r="K5" t="n">
-        <v>0</v>
+        <v>25.87573537661305</v>
       </c>
       <c r="L5" t="n">
-        <v>0</v>
+        <v>83.76338893159448</v>
       </c>
       <c r="M5" t="n">
-        <v>0</v>
+        <v>97.14926289525408</v>
       </c>
       <c r="N5" t="n">
-        <v>0</v>
+        <v>99.10168003507428</v>
       </c>
       <c r="O5" t="n">
-        <v>0</v>
+        <v>59.33583657758152</v>
       </c>
       <c r="P5" t="n">
-        <v>0</v>
+        <v>51.9567798547119</v>
       </c>
     </row>
     <row r="6">
@@ -709,43 +709,43 @@
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>0.2488137530340661</v>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>0.7182734428927011</v>
       </c>
       <c r="F6" t="n">
-        <v>0</v>
+        <v>1.60404602465184</v>
       </c>
       <c r="G6" t="n">
-        <v>0</v>
+        <v>3.275314258208827</v>
       </c>
       <c r="H6" t="n">
-        <v>0</v>
+        <v>6.428649059958429</v>
       </c>
       <c r="I6" t="n">
-        <v>0</v>
+        <v>12.37833455763719</v>
       </c>
       <c r="J6" t="n">
-        <v>0</v>
+        <v>23.6041509541861</v>
       </c>
       <c r="K6" t="n">
-        <v>0</v>
+        <v>44.78492661336874</v>
       </c>
       <c r="L6" t="n">
-        <v>0</v>
+        <v>144.9750962277597</v>
       </c>
       <c r="M6" t="n">
-        <v>0</v>
+        <v>407.94928033531</v>
       </c>
       <c r="N6" t="n">
-        <v>0</v>
+        <v>396.5232583889402</v>
       </c>
       <c r="O6" t="n">
-        <v>0</v>
+        <v>274.6144210329214</v>
       </c>
       <c r="P6" t="n">
-        <v>0</v>
+        <v>200.7362908976964</v>
       </c>
     </row>
     <row r="7">
@@ -761,43 +761,43 @@
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>0.1879926134035166</v>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>0.5426954901855964</v>
       </c>
       <c r="F7" t="n">
-        <v>0</v>
+        <v>1.211945885292502</v>
       </c>
       <c r="G7" t="n">
-        <v>0</v>
+        <v>2.474681883980002</v>
       </c>
       <c r="H7" t="n">
-        <v>0</v>
+        <v>4.857201511968591</v>
       </c>
       <c r="I7" t="n">
-        <v>0</v>
+        <v>9.352519443548099</v>
       </c>
       <c r="J7" t="n">
-        <v>0</v>
+        <v>17.83424738760727</v>
       </c>
       <c r="K7" t="n">
-        <v>0</v>
+        <v>33.8375001078786</v>
       </c>
       <c r="L7" t="n">
-        <v>0</v>
+        <v>109.5367393720851</v>
       </c>
       <c r="M7" t="n">
-        <v>0</v>
+        <v>261.514947429779</v>
       </c>
       <c r="N7" t="n">
-        <v>0</v>
+        <v>340.9728082641385</v>
       </c>
       <c r="O7" t="n">
-        <v>0</v>
+        <v>402.0012503860937</v>
       </c>
       <c r="P7" t="n">
-        <v>0</v>
+        <v>368.7197571139581</v>
       </c>
     </row>
     <row r="8">
@@ -813,43 +813,43 @@
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>0.6453103761304461</v>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>2.024828571609375</v>
       </c>
       <c r="F8" t="n">
-        <v>0</v>
+        <v>4.627691863154245</v>
       </c>
       <c r="G8" t="n">
-        <v>0</v>
+        <v>9.538752359982086</v>
       </c>
       <c r="H8" t="n">
-        <v>0</v>
+        <v>18.80489986832391</v>
       </c>
       <c r="I8" t="n">
-        <v>0</v>
+        <v>36.2881888039437</v>
       </c>
       <c r="J8" t="n">
-        <v>0</v>
+        <v>69.27551085242069</v>
       </c>
       <c r="K8" t="n">
-        <v>0</v>
+        <v>131.5157117629573</v>
       </c>
       <c r="L8" t="n">
-        <v>0</v>
+        <v>425.9347767989062</v>
       </c>
       <c r="M8" t="n">
-        <v>0</v>
+        <v>571.7077935088872</v>
       </c>
       <c r="N8" t="n">
-        <v>0</v>
+        <v>501.5221502405046</v>
       </c>
       <c r="O8" t="n">
-        <v>0</v>
+        <v>344.1317947426065</v>
       </c>
       <c r="P8" t="n">
-        <v>0</v>
+        <v>351.5928856159968</v>
       </c>
     </row>
     <row r="9">
@@ -865,43 +865,43 @@
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>0.1738088628439262</v>
       </c>
       <c r="E9" t="n">
-        <v>0</v>
+        <v>0.5380504873526288</v>
       </c>
       <c r="F9" t="n">
-        <v>0</v>
+        <v>1.225298511186943</v>
       </c>
       <c r="G9" t="n">
-        <v>0</v>
+        <v>2.521992283902326</v>
       </c>
       <c r="H9" t="n">
-        <v>0</v>
+        <v>4.968583153408003</v>
       </c>
       <c r="I9" t="n">
-        <v>0</v>
+        <v>9.584790162880857</v>
       </c>
       <c r="J9" t="n">
-        <v>0</v>
+        <v>18.29461059910759</v>
       </c>
       <c r="K9" t="n">
-        <v>0</v>
+        <v>34.72822630907028</v>
       </c>
       <c r="L9" t="n">
-        <v>0</v>
+        <v>112.4649627325595</v>
       </c>
       <c r="M9" t="n">
-        <v>0</v>
+        <v>110.4071797103971</v>
       </c>
       <c r="N9" t="n">
-        <v>0</v>
+        <v>91.87717505298582</v>
       </c>
       <c r="O9" t="n">
-        <v>0</v>
+        <v>55.01025857709347</v>
       </c>
       <c r="P9" t="n">
-        <v>0</v>
+        <v>54.56857857275376</v>
       </c>
     </row>
     <row r="10">
@@ -917,43 +917,43 @@
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>0</v>
+        <v>0.2488137530340661</v>
       </c>
       <c r="E10" t="n">
-        <v>0</v>
+        <v>0.7182734428927011</v>
       </c>
       <c r="F10" t="n">
-        <v>0</v>
+        <v>1.60404602465184</v>
       </c>
       <c r="G10" t="n">
-        <v>0</v>
+        <v>3.275314258208827</v>
       </c>
       <c r="H10" t="n">
-        <v>0</v>
+        <v>6.428649059958429</v>
       </c>
       <c r="I10" t="n">
-        <v>0</v>
+        <v>12.37833455763719</v>
       </c>
       <c r="J10" t="n">
-        <v>0</v>
+        <v>23.6041509541861</v>
       </c>
       <c r="K10" t="n">
-        <v>0</v>
+        <v>44.78492661336874</v>
       </c>
       <c r="L10" t="n">
-        <v>0</v>
+        <v>144.9750962277597</v>
       </c>
       <c r="M10" t="n">
-        <v>0</v>
+        <v>158.4608023326292</v>
       </c>
       <c r="N10" t="n">
-        <v>0</v>
+        <v>167.3540844406837</v>
       </c>
       <c r="O10" t="n">
-        <v>0</v>
+        <v>100.2010722870562</v>
       </c>
       <c r="P10" t="n">
-        <v>0</v>
+        <v>77.66671616028765</v>
       </c>
     </row>
     <row r="11">
@@ -978,34 +978,34 @@
         <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>0</v>
+        <v>0.3734343367679739</v>
       </c>
       <c r="H11" t="n">
-        <v>0</v>
+        <v>1.484209181935004</v>
       </c>
       <c r="I11" t="n">
-        <v>0</v>
+        <v>3.580009787633402</v>
       </c>
       <c r="J11" t="n">
-        <v>0</v>
+        <v>7.53434868714753</v>
       </c>
       <c r="K11" t="n">
-        <v>0</v>
+        <v>14.99536195801632</v>
       </c>
       <c r="L11" t="n">
-        <v>0</v>
+        <v>50.3598060537445</v>
       </c>
       <c r="M11" t="n">
-        <v>0</v>
+        <v>41.44034304756279</v>
       </c>
       <c r="N11" t="n">
-        <v>0</v>
+        <v>36.0999310675916</v>
       </c>
       <c r="O11" t="n">
-        <v>0</v>
+        <v>24.81186415728618</v>
       </c>
       <c r="P11" t="n">
-        <v>0</v>
+        <v>14.85577960233197</v>
       </c>
     </row>
     <row r="12">
@@ -1030,34 +1030,34 @@
         <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>0</v>
+        <v>0.1548174463323078</v>
       </c>
       <c r="H12" t="n">
-        <v>0</v>
+        <v>0.4469256977999028</v>
       </c>
       <c r="I12" t="n">
-        <v>0</v>
+        <v>0.9980730820055893</v>
       </c>
       <c r="J12" t="n">
-        <v>0</v>
+        <v>2.037973316218824</v>
       </c>
       <c r="K12" t="n">
-        <v>0</v>
+        <v>4.000048303974133</v>
       </c>
       <c r="L12" t="n">
-        <v>0</v>
+        <v>13.29485650551321</v>
       </c>
       <c r="M12" t="n">
-        <v>0</v>
+        <v>7.96012169172443</v>
       </c>
       <c r="N12" t="n">
-        <v>0</v>
+        <v>4.766018897668112</v>
       </c>
       <c r="O12" t="n">
-        <v>0</v>
+        <v>4.766018897668113</v>
       </c>
       <c r="P12" t="n">
-        <v>0</v>
+        <v>2.853591567142078</v>
       </c>
     </row>
     <row r="13">
@@ -1073,43 +1073,43 @@
         <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>0</v>
+        <v>0.03396171656945288</v>
       </c>
       <c r="E13" t="n">
-        <v>0</v>
+        <v>0.666760882064887</v>
       </c>
       <c r="F13" t="n">
-        <v>0</v>
+        <v>1.860721008278714</v>
       </c>
       <c r="G13" t="n">
-        <v>0</v>
+        <v>4.113474900380398</v>
       </c>
       <c r="H13" t="n">
-        <v>0</v>
+        <v>8.363951936386892</v>
       </c>
       <c r="I13" t="n">
-        <v>0</v>
+        <v>16.38371614452396</v>
       </c>
       <c r="J13" t="n">
-        <v>0</v>
+        <v>31.51533958567646</v>
       </c>
       <c r="K13" t="n">
-        <v>0</v>
+        <v>60.06555902137026</v>
       </c>
       <c r="L13" t="n">
-        <v>0</v>
+        <v>195.1428060608981</v>
       </c>
       <c r="M13" t="n">
-        <v>0</v>
+        <v>167.3620052122577</v>
       </c>
       <c r="N13" t="n">
-        <v>0</v>
+        <v>140.720085441743</v>
       </c>
       <c r="O13" t="n">
-        <v>0</v>
+        <v>161.9048618027862</v>
       </c>
       <c r="P13" t="n">
-        <v>0</v>
+        <v>157.1964238197903</v>
       </c>
     </row>
     <row r="14">
@@ -1125,43 +1125,43 @@
         <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>0</v>
+        <v>1.742477270535277</v>
       </c>
       <c r="E14" t="n">
-        <v>0</v>
+        <v>6.209179254731491</v>
       </c>
       <c r="F14" t="n">
-        <v>0</v>
+        <v>15.08270648560511</v>
       </c>
       <c r="G14" t="n">
-        <v>0</v>
+        <v>32.35345457753175</v>
       </c>
       <c r="H14" t="n">
-        <v>0</v>
+        <v>65.34593844484733</v>
       </c>
       <c r="I14" t="n">
-        <v>0</v>
+        <v>127.5958786316158</v>
       </c>
       <c r="J14" t="n">
-        <v>0</v>
+        <v>245.0485405421402</v>
       </c>
       <c r="K14" t="n">
-        <v>0</v>
+        <v>466.6572320280828</v>
       </c>
       <c r="L14" t="n">
-        <v>0</v>
+        <v>1515.09656845898</v>
       </c>
       <c r="M14" t="n">
-        <v>0</v>
+        <v>2075.369600999532</v>
       </c>
       <c r="N14" t="n">
-        <v>0</v>
+        <v>2223.052483219528</v>
       </c>
       <c r="O14" t="n">
-        <v>0</v>
+        <v>2297.010281214967</v>
       </c>
       <c r="P14" t="n">
-        <v>0</v>
+        <v>2338.948468635547</v>
       </c>
     </row>
   </sheetData>
@@ -1248,43 +1248,43 @@
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>0.01105838902373627</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>0.02086487510482822</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>0.03936767030040619</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>0.07427858815808831</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>0.1512066024348298</v>
       </c>
       <c r="I2" t="n">
-        <v>0</v>
+        <v>0.2852953416683288</v>
       </c>
       <c r="J2" t="n">
-        <v>0</v>
+        <v>0.5382928434803577</v>
       </c>
       <c r="K2" t="n">
-        <v>0</v>
+        <v>1.015646395232873</v>
       </c>
       <c r="L2" t="n">
-        <v>0</v>
+        <v>2.373375350287629</v>
       </c>
       <c r="M2" t="n">
-        <v>0</v>
+        <v>7.515504842487882</v>
       </c>
       <c r="N2" t="n">
-        <v>0</v>
+        <v>23.37644415312299</v>
       </c>
       <c r="O2" t="n">
-        <v>0</v>
+        <v>47.31140263256781</v>
       </c>
       <c r="P2" t="n">
-        <v>0</v>
+        <v>27.88722468803438</v>
       </c>
     </row>
     <row r="3">
@@ -1303,40 +1303,40 @@
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>0.06676496225664245</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>0.215129890434503</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>0.4059052621133699</v>
       </c>
       <c r="H3" t="n">
-        <v>0</v>
+        <v>0.7658586237298577</v>
       </c>
       <c r="I3" t="n">
-        <v>0</v>
+        <v>1.511780551578001</v>
       </c>
       <c r="J3" t="n">
-        <v>0</v>
+        <v>2.941573112047007</v>
       </c>
       <c r="K3" t="n">
-        <v>0</v>
+        <v>5.550135328287162</v>
       </c>
       <c r="L3" t="n">
-        <v>0</v>
+        <v>12.55462466553449</v>
       </c>
       <c r="M3" t="n">
         <v>0</v>
       </c>
       <c r="N3" t="n">
-        <v>0</v>
+        <v>3.793219748759835</v>
       </c>
       <c r="O3" t="n">
-        <v>0</v>
+        <v>3.116924253979477</v>
       </c>
       <c r="P3" t="n">
-        <v>0</v>
+        <v>2.271140782231036</v>
       </c>
     </row>
     <row r="4">
@@ -1352,43 +1352,43 @@
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>0.0009450386185099569</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>0.01742563580873569</v>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>0.0328785426151204</v>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>0.06203495679350585</v>
       </c>
       <c r="H4" t="n">
-        <v>0</v>
+        <v>0.1179920716765489</v>
       </c>
       <c r="I4" t="n">
-        <v>0</v>
+        <v>0.2382689901983022</v>
       </c>
       <c r="J4" t="n">
-        <v>0</v>
+        <v>0.4495639203115522</v>
       </c>
       <c r="K4" t="n">
-        <v>0</v>
+        <v>0.8482334116482591</v>
       </c>
       <c r="L4" t="n">
-        <v>0</v>
+        <v>1.978400074734544</v>
       </c>
       <c r="M4" t="n">
         <v>0</v>
       </c>
       <c r="N4" t="n">
-        <v>0</v>
+        <v>0.4434874267288383</v>
       </c>
       <c r="O4" t="n">
-        <v>0</v>
+        <v>1.670159337412588</v>
       </c>
       <c r="P4" t="n">
-        <v>0</v>
+        <v>0.4890890089172863</v>
       </c>
     </row>
     <row r="5">
@@ -1404,43 +1404,43 @@
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>0.02875181146171431</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>0.05424867527255337</v>
       </c>
       <c r="F5" t="n">
-        <v>0</v>
+        <v>0.1023559427810561</v>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>0.1931243292110295</v>
       </c>
       <c r="H5" t="n">
-        <v>0</v>
+        <v>0.3931371663305572</v>
       </c>
       <c r="I5" t="n">
-        <v>0</v>
+        <v>0.7417678883376548</v>
       </c>
       <c r="J5" t="n">
-        <v>0</v>
+        <v>1.39956139304893</v>
       </c>
       <c r="K5" t="n">
-        <v>0</v>
+        <v>2.640680627605468</v>
       </c>
       <c r="L5" t="n">
-        <v>0</v>
+        <v>6.170775910747835</v>
       </c>
       <c r="M5" t="n">
-        <v>0</v>
+        <v>2.22381006497484</v>
       </c>
       <c r="N5" t="n">
-        <v>0</v>
+        <v>0.8554118708833868</v>
       </c>
       <c r="O5" t="n">
-        <v>0</v>
+        <v>3.384377233047236</v>
       </c>
       <c r="P5" t="n">
-        <v>0</v>
+        <v>0.9558888815405675</v>
       </c>
     </row>
     <row r="6">
@@ -1456,43 +1456,43 @@
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>0.04976275060681323</v>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>0.09389193797172701</v>
       </c>
       <c r="F6" t="n">
-        <v>0</v>
+        <v>0.1771545163518279</v>
       </c>
       <c r="G6" t="n">
-        <v>0</v>
+        <v>0.3342536467113974</v>
       </c>
       <c r="H6" t="n">
-        <v>0</v>
+        <v>0.6804297109567337</v>
       </c>
       <c r="I6" t="n">
-        <v>0</v>
+        <v>1.28382903750748</v>
       </c>
       <c r="J6" t="n">
-        <v>0</v>
+        <v>2.422317795661608</v>
       </c>
       <c r="K6" t="n">
-        <v>0</v>
+        <v>4.570408778547926</v>
       </c>
       <c r="L6" t="n">
-        <v>0</v>
+        <v>10.68018907629433</v>
       </c>
       <c r="M6" t="n">
-        <v>0</v>
+        <v>27.82953456796271</v>
       </c>
       <c r="N6" t="n">
         <v>0</v>
       </c>
       <c r="O6" t="n">
-        <v>0</v>
+        <v>0.549242073853624</v>
       </c>
       <c r="P6" t="n">
-        <v>0</v>
+        <v>19.52438701591602</v>
       </c>
     </row>
     <row r="7">
@@ -1508,43 +1508,43 @@
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>0.03759852268070332</v>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>0.07094057535641596</v>
       </c>
       <c r="F7" t="n">
-        <v>0</v>
+        <v>0.1338500790213811</v>
       </c>
       <c r="G7" t="n">
-        <v>0</v>
+        <v>0.2525471997375001</v>
       </c>
       <c r="H7" t="n">
-        <v>0</v>
+        <v>0.514102448278421</v>
       </c>
       <c r="I7" t="n">
-        <v>0</v>
+        <v>0.9700041616723176</v>
       </c>
       <c r="J7" t="n">
-        <v>0</v>
+        <v>1.830195667833216</v>
       </c>
       <c r="K7" t="n">
-        <v>0</v>
+        <v>3.453197743791765</v>
       </c>
       <c r="L7" t="n">
-        <v>0</v>
+        <v>8.069476190977939</v>
       </c>
       <c r="M7" t="n">
-        <v>0</v>
+        <v>16.35541968010408</v>
       </c>
       <c r="N7" t="n">
-        <v>0</v>
+        <v>8.809085519383878</v>
       </c>
       <c r="O7" t="n">
-        <v>0</v>
+        <v>15.72871704600635</v>
       </c>
       <c r="P7" t="n">
-        <v>0</v>
+        <v>12.33417314600558</v>
       </c>
     </row>
     <row r="8">
@@ -1560,43 +1560,43 @@
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>0.1290620752260892</v>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>0.2759036390957859</v>
       </c>
       <c r="F8" t="n">
-        <v>0</v>
+        <v>0.520572658308974</v>
       </c>
       <c r="G8" t="n">
-        <v>0</v>
+        <v>0.9822120993655681</v>
       </c>
       <c r="H8" t="n">
-        <v>0</v>
+        <v>1.982291576894456</v>
       </c>
       <c r="I8" t="n">
-        <v>0</v>
+        <v>3.772561426219741</v>
       </c>
       <c r="J8" t="n">
-        <v>0</v>
+        <v>7.118037068004374</v>
       </c>
       <c r="K8" t="n">
-        <v>0</v>
+        <v>13.4302522814729</v>
       </c>
       <c r="L8" t="n">
-        <v>0</v>
+        <v>31.37619264859705</v>
       </c>
       <c r="M8" t="n">
-        <v>0</v>
+        <v>15.88477756245091</v>
       </c>
       <c r="N8" t="n">
-        <v>0</v>
+        <v>0.1671685306276941</v>
       </c>
       <c r="O8" t="n">
-        <v>0</v>
+        <v>18.88987264705619</v>
       </c>
       <c r="P8" t="n">
-        <v>0</v>
+        <v>16.26941591454349</v>
       </c>
     </row>
     <row r="9">
@@ -1612,40 +1612,40 @@
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>0.03476177256878523</v>
       </c>
       <c r="E9" t="n">
-        <v>0</v>
+        <v>0.07284832490174055</v>
       </c>
       <c r="F9" t="n">
-        <v>0</v>
+        <v>0.1374496047668628</v>
       </c>
       <c r="G9" t="n">
-        <v>0</v>
+        <v>0.2593387545430766</v>
       </c>
       <c r="H9" t="n">
-        <v>0</v>
+        <v>0.5240799464699207</v>
       </c>
       <c r="I9" t="n">
-        <v>0</v>
+        <v>0.9960897267963115</v>
       </c>
       <c r="J9" t="n">
-        <v>0</v>
+        <v>1.87941369201221</v>
       </c>
       <c r="K9" t="n">
-        <v>0</v>
+        <v>3.546061896535614</v>
       </c>
       <c r="L9" t="n">
-        <v>0</v>
+        <v>8.284736047282966</v>
       </c>
       <c r="M9" t="n">
-        <v>0</v>
+        <v>0.1396730547123374</v>
       </c>
       <c r="N9" t="n">
-        <v>0</v>
+        <v>0.04416800043397055</v>
       </c>
       <c r="O9" t="n">
-        <v>0</v>
+        <v>5.456857857275376</v>
       </c>
       <c r="P9" t="n">
         <v>0</v>
@@ -1664,40 +1664,40 @@
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>0</v>
+        <v>0.04976275060681323</v>
       </c>
       <c r="E10" t="n">
-        <v>0</v>
+        <v>0.09389193797172701</v>
       </c>
       <c r="F10" t="n">
-        <v>0</v>
+        <v>0.1771545163518279</v>
       </c>
       <c r="G10" t="n">
-        <v>0</v>
+        <v>0.3342536467113974</v>
       </c>
       <c r="H10" t="n">
-        <v>0</v>
+        <v>0.6804297109567337</v>
       </c>
       <c r="I10" t="n">
-        <v>0</v>
+        <v>1.28382903750748</v>
       </c>
       <c r="J10" t="n">
-        <v>0</v>
+        <v>2.422317795661608</v>
       </c>
       <c r="K10" t="n">
-        <v>0</v>
+        <v>4.570408778547926</v>
       </c>
       <c r="L10" t="n">
-        <v>0</v>
+        <v>10.68018907629433</v>
       </c>
       <c r="M10" t="n">
-        <v>0</v>
+        <v>2.88068676769462</v>
       </c>
       <c r="N10" t="n">
-        <v>0</v>
+        <v>2.031930405442441</v>
       </c>
       <c r="O10" t="n">
-        <v>0</v>
+        <v>6.024824594092747</v>
       </c>
       <c r="P10" t="n">
         <v>0</v>
@@ -1725,34 +1725,34 @@
         <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>0</v>
+        <v>0.07468686735359478</v>
       </c>
       <c r="H11" t="n">
-        <v>0</v>
+        <v>0.2221549690334061</v>
       </c>
       <c r="I11" t="n">
-        <v>0</v>
+        <v>0.4191601211396795</v>
       </c>
       <c r="J11" t="n">
-        <v>0</v>
+        <v>0.7908677799028258</v>
       </c>
       <c r="K11" t="n">
-        <v>0</v>
+        <v>1.566889521527354</v>
       </c>
       <c r="L11" t="n">
-        <v>0</v>
+        <v>3.752311924374441</v>
       </c>
       <c r="M11" t="n">
         <v>0</v>
       </c>
       <c r="N11" t="n">
-        <v>0</v>
+        <v>0.7968592765780311</v>
       </c>
       <c r="O11" t="n">
-        <v>0</v>
+        <v>1.684327139150587</v>
       </c>
       <c r="P11" t="n">
-        <v>0</v>
+        <v>0.4771090842620391</v>
       </c>
     </row>
     <row r="12">
@@ -1777,34 +1777,34 @@
         <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>0</v>
+        <v>0.03096348926646156</v>
       </c>
       <c r="H12" t="n">
-        <v>0</v>
+        <v>0.05842165029351901</v>
       </c>
       <c r="I12" t="n">
-        <v>0</v>
+        <v>0.1102294768411373</v>
       </c>
       <c r="J12" t="n">
-        <v>0</v>
+        <v>0.2079800468426471</v>
       </c>
       <c r="K12" t="n">
-        <v>0</v>
+        <v>0.423378486817523</v>
       </c>
       <c r="L12" t="n">
-        <v>0</v>
+        <v>0.9862490145109517</v>
       </c>
       <c r="M12" t="n">
         <v>0</v>
       </c>
       <c r="N12" t="n">
-        <v>0</v>
+        <v>0.4766018897668112</v>
       </c>
       <c r="O12" t="n">
         <v>0</v>
       </c>
       <c r="P12" t="n">
-        <v>0</v>
+        <v>0.2853591567142079</v>
       </c>
     </row>
     <row r="13">
@@ -1820,43 +1820,43 @@
         <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>0</v>
+        <v>0.006792343313890577</v>
       </c>
       <c r="E13" t="n">
-        <v>0</v>
+        <v>0.1265598330990868</v>
       </c>
       <c r="F13" t="n">
-        <v>0</v>
+        <v>0.2387920252427653</v>
       </c>
       <c r="G13" t="n">
-        <v>0</v>
+        <v>0.450550778420337</v>
       </c>
       <c r="H13" t="n">
-        <v>0</v>
+        <v>0.8568877505151893</v>
       </c>
       <c r="I13" t="n">
-        <v>0</v>
+        <v>1.7305126747265</v>
       </c>
       <c r="J13" t="n">
-        <v>0</v>
+        <v>3.265116713473267</v>
       </c>
       <c r="K13" t="n">
-        <v>0</v>
+        <v>6.160594665559096</v>
       </c>
       <c r="L13" t="n">
-        <v>0</v>
+        <v>13.93616857921038</v>
       </c>
       <c r="M13" t="n">
         <v>0</v>
       </c>
       <c r="N13" t="n">
-        <v>0</v>
+        <v>2.09541215192254</v>
       </c>
       <c r="O13" t="n">
-        <v>0</v>
+        <v>14.09507402835608</v>
       </c>
       <c r="P13" t="n">
-        <v>0</v>
+        <v>1.624568353622946</v>
       </c>
     </row>
     <row r="14">
@@ -1872,43 +1872,43 @@
         <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>0</v>
+        <v>0.3484954541070553</v>
       </c>
       <c r="E14" t="n">
-        <v>0</v>
+        <v>0.8933403968392429</v>
       </c>
       <c r="F14" t="n">
-        <v>0</v>
+        <v>1.774705446174725</v>
       </c>
       <c r="G14" t="n">
-        <v>0</v>
+        <v>3.454149618385326</v>
       </c>
       <c r="H14" t="n">
-        <v>0</v>
+        <v>6.946992227570171</v>
       </c>
       <c r="I14" t="n">
-        <v>0</v>
+        <v>13.34332843419294</v>
       </c>
       <c r="J14" t="n">
-        <v>0</v>
+        <v>25.26523782827961</v>
       </c>
       <c r="K14" t="n">
-        <v>0</v>
+        <v>47.77588791557386</v>
       </c>
       <c r="L14" t="n">
-        <v>0</v>
+        <v>110.8426885588469</v>
       </c>
       <c r="M14" t="n">
-        <v>0</v>
+        <v>72.8294065403874</v>
       </c>
       <c r="N14" t="n">
-        <v>0</v>
+        <v>42.8897889736504</v>
       </c>
       <c r="O14" t="n">
-        <v>0</v>
+        <v>117.9117788427981</v>
       </c>
       <c r="P14" t="n">
-        <v>0</v>
+        <v>82.11835603178754</v>
       </c>
     </row>
   </sheetData>
@@ -1995,43 +1995,43 @@
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>45.81855499371721</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>75.21155478223648</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>128.8594670147678</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>215.4324918711364</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>400.9592653224341</v>
       </c>
       <c r="I2" t="n">
-        <v>0</v>
+        <v>697.4229213168358</v>
       </c>
       <c r="J2" t="n">
-        <v>0</v>
+        <v>1248.981936819384</v>
       </c>
       <c r="K2" t="n">
-        <v>0</v>
+        <v>2413.175835073306</v>
       </c>
       <c r="L2" t="n">
-        <v>0</v>
+        <v>5325.854286045439</v>
       </c>
       <c r="M2" t="n">
-        <v>0</v>
+        <v>16838.10827752913</v>
       </c>
       <c r="N2" t="n">
-        <v>0</v>
+        <v>52456.74067960798</v>
       </c>
       <c r="O2" t="n">
-        <v>0</v>
+        <v>104069.4220179718</v>
       </c>
       <c r="P2" t="n">
-        <v>0</v>
+        <v>61351.89431367564</v>
       </c>
     </row>
     <row r="3">
@@ -2050,40 +2050,40 @@
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>219.5248289551274</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>642.3084482786393</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>1073.837357612941</v>
       </c>
       <c r="H3" t="n">
-        <v>0</v>
+        <v>1852.440928769274</v>
       </c>
       <c r="I3" t="n">
-        <v>0</v>
+        <v>3579.807755796383</v>
       </c>
       <c r="J3" t="n">
-        <v>0</v>
+        <v>6225.6322205226</v>
       </c>
       <c r="K3" t="n">
-        <v>0</v>
+        <v>11326.95354687768</v>
       </c>
       <c r="L3" t="n">
-        <v>0</v>
+        <v>24941.16109493724</v>
       </c>
       <c r="M3" t="n">
         <v>0</v>
       </c>
       <c r="N3" t="n">
-        <v>0</v>
+        <v>7311.289253729716</v>
       </c>
       <c r="O3" t="n">
-        <v>0</v>
+        <v>6254.825408188236</v>
       </c>
       <c r="P3" t="n">
-        <v>0</v>
+        <v>4291.704852612334</v>
       </c>
     </row>
     <row r="4">
@@ -2099,43 +2099,43 @@
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>4.190799624904464</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>67.22877935900529</v>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>115.1826298676769</v>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>192.5669999071206</v>
       </c>
       <c r="H4" t="n">
-        <v>0</v>
+        <v>334.8730060600016</v>
       </c>
       <c r="I4" t="n">
-        <v>0</v>
+        <v>623.4001122949294</v>
       </c>
       <c r="J4" t="n">
-        <v>0</v>
+        <v>1116.417966586764</v>
       </c>
       <c r="K4" t="n">
-        <v>0</v>
+        <v>2031.217713880052</v>
       </c>
       <c r="L4" t="n">
-        <v>0</v>
+        <v>4677.480121136477</v>
       </c>
       <c r="M4" t="n">
         <v>0</v>
       </c>
       <c r="N4" t="n">
-        <v>0</v>
+        <v>1002.995138656754</v>
       </c>
       <c r="O4" t="n">
-        <v>0</v>
+        <v>3932.587572771619</v>
       </c>
       <c r="P4" t="n">
-        <v>0</v>
+        <v>1115.14582168</v>
       </c>
     </row>
     <row r="5">
@@ -2151,43 +2151,43 @@
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>127.5006950287997</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>209.2934949661058</v>
       </c>
       <c r="F5" t="n">
-        <v>0</v>
+        <v>358.5811819616851</v>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>599.4905873640622</v>
       </c>
       <c r="H5" t="n">
-        <v>0</v>
+        <v>1115.761616966256</v>
       </c>
       <c r="I5" t="n">
-        <v>0</v>
+        <v>1940.740104289751</v>
       </c>
       <c r="J5" t="n">
-        <v>0</v>
+        <v>3475.580254434565</v>
       </c>
       <c r="K5" t="n">
-        <v>0</v>
+        <v>6715.218239439039</v>
       </c>
       <c r="L5" t="n">
-        <v>0</v>
+        <v>14820.4176929198</v>
       </c>
       <c r="M5" t="n">
-        <v>0</v>
+        <v>5266.692102982825</v>
       </c>
       <c r="N5" t="n">
-        <v>0</v>
+        <v>2054.451726871634</v>
       </c>
       <c r="O5" t="n">
-        <v>0</v>
+        <v>7925.328166275271</v>
       </c>
       <c r="P5" t="n">
-        <v>0</v>
+        <v>2250.753357653064</v>
       </c>
     </row>
     <row r="6">
@@ -2203,43 +2203,43 @@
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>206.1834974717275</v>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>338.4519965200643</v>
       </c>
       <c r="F6" t="n">
-        <v>0</v>
+        <v>579.8676015664551</v>
       </c>
       <c r="G6" t="n">
-        <v>0</v>
+        <v>969.4462134201138</v>
       </c>
       <c r="H6" t="n">
-        <v>0</v>
+        <v>1804.316693950953</v>
       </c>
       <c r="I6" t="n">
-        <v>0</v>
+        <v>3138.403145925762</v>
       </c>
       <c r="J6" t="n">
-        <v>0</v>
+        <v>5620.418715687223</v>
       </c>
       <c r="K6" t="n">
-        <v>0</v>
+        <v>10859.29125782987</v>
       </c>
       <c r="L6" t="n">
-        <v>0</v>
+        <v>23966.34428720448</v>
       </c>
       <c r="M6" t="n">
-        <v>0</v>
+        <v>62329.3949199468</v>
       </c>
       <c r="N6" t="n">
         <v>0</v>
       </c>
       <c r="O6" t="n">
-        <v>0</v>
+        <v>1137.845580929968</v>
       </c>
       <c r="P6" t="n">
-        <v>0</v>
+        <v>42953.65143501524</v>
       </c>
     </row>
     <row r="7">
@@ -2255,43 +2255,43 @@
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>174.9430046292282</v>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>287.1704569959591</v>
       </c>
       <c r="F7" t="n">
-        <v>0</v>
+        <v>492.0072738560959</v>
       </c>
       <c r="G7" t="n">
-        <v>0</v>
+        <v>822.5577482281213</v>
       </c>
       <c r="H7" t="n">
-        <v>0</v>
+        <v>1530.930397500598</v>
       </c>
       <c r="I7" t="n">
-        <v>0</v>
+        <v>2662.878857030549</v>
       </c>
       <c r="J7" t="n">
-        <v>0</v>
+        <v>4768.824612316504</v>
       </c>
       <c r="K7" t="n">
-        <v>0</v>
+        <v>9213.914130296338</v>
       </c>
       <c r="L7" t="n">
-        <v>0</v>
+        <v>20335.01386383755</v>
       </c>
       <c r="M7" t="n">
-        <v>0</v>
+        <v>41113.63726361902</v>
       </c>
       <c r="N7" t="n">
-        <v>0</v>
+        <v>22198.82330958246</v>
       </c>
       <c r="O7" t="n">
-        <v>0</v>
+        <v>38799.24996392246</v>
       </c>
       <c r="P7" t="n">
-        <v>0</v>
+        <v>30472.5639578931</v>
       </c>
     </row>
     <row r="8">
@@ -2307,43 +2307,43 @@
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>632.2177353104178</v>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>1175.830475402652</v>
       </c>
       <c r="F8" t="n">
-        <v>0</v>
+        <v>2014.542696249275</v>
       </c>
       <c r="G8" t="n">
-        <v>0</v>
+        <v>3367.994320386574</v>
       </c>
       <c r="H8" t="n">
-        <v>0</v>
+        <v>6214.63376545884</v>
       </c>
       <c r="I8" t="n">
-        <v>0</v>
+        <v>10903.25984488704</v>
       </c>
       <c r="J8" t="n">
-        <v>0</v>
+        <v>20611.9096261735</v>
       </c>
       <c r="K8" t="n">
-        <v>0</v>
+        <v>37726.72560220221</v>
       </c>
       <c r="L8" t="n">
-        <v>0</v>
+        <v>83143.78707891017</v>
       </c>
       <c r="M8" t="n">
-        <v>0</v>
+        <v>42060.90041286699</v>
       </c>
       <c r="N8" t="n">
-        <v>0</v>
+        <v>417.6310037504799</v>
       </c>
       <c r="O8" t="n">
-        <v>0</v>
+        <v>49094.80676579378</v>
       </c>
       <c r="P8" t="n">
-        <v>0</v>
+        <v>42316.8321408072</v>
       </c>
     </row>
     <row r="9">
@@ -2359,40 +2359,40 @@
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>181.9887566398835</v>
       </c>
       <c r="E9" t="n">
-        <v>0</v>
+        <v>331.8038848554468</v>
       </c>
       <c r="F9" t="n">
-        <v>0</v>
+        <v>568.4774351453832</v>
       </c>
       <c r="G9" t="n">
-        <v>0</v>
+        <v>950.4036704718546</v>
       </c>
       <c r="H9" t="n">
-        <v>0</v>
+        <v>1755.982405543538</v>
       </c>
       <c r="I9" t="n">
-        <v>0</v>
+        <v>3076.756428585556</v>
       </c>
       <c r="J9" t="n">
-        <v>0</v>
+        <v>5816.325549135056</v>
       </c>
       <c r="K9" t="n">
-        <v>0</v>
+        <v>10645.98543714349</v>
       </c>
       <c r="L9" t="n">
-        <v>0</v>
+        <v>23462.94511401543</v>
       </c>
       <c r="M9" t="n">
-        <v>0</v>
+        <v>372.9283945913953</v>
       </c>
       <c r="N9" t="n">
-        <v>0</v>
+        <v>117.9289844277871</v>
       </c>
       <c r="O9" t="n">
-        <v>0</v>
+        <v>15158.365123374</v>
       </c>
       <c r="P9" t="n">
         <v>0</v>
@@ -2411,40 +2411,40 @@
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>0</v>
+        <v>195.3155653199927</v>
       </c>
       <c r="E10" t="n">
-        <v>0</v>
+        <v>320.6121917834917</v>
       </c>
       <c r="F10" t="n">
-        <v>0</v>
+        <v>549.3027802878872</v>
       </c>
       <c r="G10" t="n">
-        <v>0</v>
+        <v>918.3467035107396</v>
       </c>
       <c r="H10" t="n">
-        <v>0</v>
+        <v>1709.211161012798</v>
       </c>
       <c r="I10" t="n">
-        <v>0</v>
+        <v>2972.977916104015</v>
       </c>
       <c r="J10" t="n">
-        <v>0</v>
+        <v>5324.166445183349</v>
       </c>
       <c r="K10" t="n">
-        <v>0</v>
+        <v>10286.89801562966</v>
       </c>
       <c r="L10" t="n">
-        <v>0</v>
+        <v>22703.07827982594</v>
       </c>
       <c r="M10" t="n">
-        <v>0</v>
+        <v>6009.778704301783</v>
       </c>
       <c r="N10" t="n">
-        <v>0</v>
+        <v>4283.341699448595</v>
       </c>
       <c r="O10" t="n">
-        <v>0</v>
+        <v>12503.34255563018</v>
       </c>
       <c r="P10" t="n">
         <v>0</v>
@@ -2472,34 +2472,34 @@
         <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>0</v>
+        <v>197.586865146311</v>
       </c>
       <c r="H11" t="n">
-        <v>0</v>
+        <v>537.3432437996693</v>
       </c>
       <c r="I11" t="n">
-        <v>0</v>
+        <v>934.6473002420032</v>
       </c>
       <c r="J11" t="n">
-        <v>0</v>
+        <v>1673.815929501033</v>
       </c>
       <c r="K11" t="n">
-        <v>0</v>
+        <v>3197.775148467776</v>
       </c>
       <c r="L11" t="n">
-        <v>0</v>
+        <v>7568.33471682956</v>
       </c>
       <c r="M11" t="n">
         <v>0</v>
       </c>
       <c r="N11" t="n">
-        <v>0</v>
+        <v>1535.916464498157</v>
       </c>
       <c r="O11" t="n">
-        <v>0</v>
+        <v>3379.989799947658</v>
       </c>
       <c r="P11" t="n">
-        <v>0</v>
+        <v>901.5783557641754</v>
       </c>
     </row>
     <row r="12">
@@ -2524,34 +2524,34 @@
         <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>0</v>
+        <v>85.07077956159679</v>
       </c>
       <c r="H12" t="n">
-        <v>0</v>
+        <v>146.7527580270796</v>
       </c>
       <c r="I12" t="n">
-        <v>0</v>
+        <v>255.259688617606</v>
       </c>
       <c r="J12" t="n">
-        <v>0</v>
+        <v>457.1325813031235</v>
       </c>
       <c r="K12" t="n">
-        <v>0</v>
+        <v>897.3358595317186</v>
       </c>
       <c r="L12" t="n">
-        <v>0</v>
+        <v>1974.191308718582</v>
       </c>
       <c r="M12" t="n">
         <v>0</v>
       </c>
       <c r="N12" t="n">
-        <v>0</v>
+        <v>954.0220518882377</v>
       </c>
       <c r="O12" t="n">
         <v>0</v>
       </c>
       <c r="P12" t="n">
-        <v>0</v>
+        <v>560.0080816798837</v>
       </c>
     </row>
     <row r="13">
@@ -2567,43 +2567,43 @@
         <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>0</v>
+        <v>34.57110042529445</v>
       </c>
       <c r="E13" t="n">
-        <v>0</v>
+        <v>560.4136706559798</v>
       </c>
       <c r="F13" t="n">
-        <v>0</v>
+        <v>960.1530924018989</v>
       </c>
       <c r="G13" t="n">
-        <v>0</v>
+        <v>1605.222946096874</v>
       </c>
       <c r="H13" t="n">
-        <v>0</v>
+        <v>2791.241948273994</v>
       </c>
       <c r="I13" t="n">
-        <v>0</v>
+        <v>5518.531462900791</v>
       </c>
       <c r="J13" t="n">
-        <v>0</v>
+        <v>9306.36992976084</v>
       </c>
       <c r="K13" t="n">
-        <v>0</v>
+        <v>17495.46087661915</v>
       </c>
       <c r="L13" t="n">
-        <v>0</v>
+        <v>37967.71124604904</v>
       </c>
       <c r="M13" t="n">
         <v>0</v>
       </c>
       <c r="N13" t="n">
-        <v>0</v>
+        <v>5439.177217685669</v>
       </c>
       <c r="O13" t="n">
-        <v>0</v>
+        <v>38092.02777010609</v>
       </c>
       <c r="P13" t="n">
-        <v>0</v>
+        <v>4192.620769632502</v>
       </c>
     </row>
     <row r="14">
@@ -2619,43 +2619,43 @@
         <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>0</v>
+        <v>1602.729709443965</v>
       </c>
       <c r="E14" t="n">
-        <v>0</v>
+        <v>3585.541334276068</v>
       </c>
       <c r="F14" t="n">
-        <v>0</v>
+        <v>6409.282606629764</v>
       </c>
       <c r="G14" t="n">
-        <v>0</v>
+        <v>10997.95668357744</v>
       </c>
       <c r="H14" t="n">
-        <v>0</v>
+        <v>20194.44719068543</v>
       </c>
       <c r="I14" t="n">
-        <v>0</v>
+        <v>36304.08553799122</v>
       </c>
       <c r="J14" t="n">
-        <v>0</v>
+        <v>65645.57576742394</v>
       </c>
       <c r="K14" t="n">
-        <v>0</v>
+        <v>122809.9516629903</v>
       </c>
       <c r="L14" t="n">
-        <v>0</v>
+        <v>270886.3190904297</v>
       </c>
       <c r="M14" t="n">
-        <v>0</v>
+        <v>173991.4400758379</v>
       </c>
       <c r="N14" t="n">
-        <v>0</v>
+        <v>97772.31753014745</v>
       </c>
       <c r="O14" t="n">
-        <v>0</v>
+        <v>280347.7907249111</v>
       </c>
       <c r="P14" t="n">
-        <v>0</v>
+        <v>190406.7530864131</v>
       </c>
     </row>
   </sheetData>
@@ -2730,43 +2730,43 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>0.05031567005800005</v>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>0.1452508517849684</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>0.3243737516518166</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>0.6623413277711184</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>1.300015698791594</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>2.503174321655522</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>4.773283859624301</v>
       </c>
       <c r="I2" t="n">
-        <v>0</v>
+        <v>9.056507381814569</v>
       </c>
       <c r="J2" t="n">
-        <v>0</v>
+        <v>29.31718612605808</v>
       </c>
       <c r="K2" t="n">
-        <v>0</v>
+        <v>94.61000085256671</v>
       </c>
       <c r="L2" t="n">
-        <v>0</v>
+        <v>305.0250470968311</v>
       </c>
       <c r="M2" t="n">
-        <v>0</v>
+        <v>709.7954455274104</v>
       </c>
       <c r="N2" t="n">
-        <v>0</v>
+        <v>897.033150410899</v>
       </c>
     </row>
     <row r="3">
@@ -2779,40 +2779,40 @@
         <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>0.3037805782677232</v>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>1.282621579744712</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>3.129490522360545</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>6.614147260331396</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>13.18896819174358</v>
       </c>
       <c r="H3" t="n">
-        <v>0</v>
+        <v>25.59428485008047</v>
       </c>
       <c r="I3" t="n">
-        <v>0</v>
+        <v>49.00053165117122</v>
       </c>
       <c r="J3" t="n">
-        <v>0</v>
+        <v>159.7629593695642</v>
       </c>
       <c r="K3" t="n">
-        <v>0</v>
+        <v>114.2470844563639</v>
       </c>
       <c r="L3" t="n">
-        <v>0</v>
+        <v>81.89137602214066</v>
       </c>
       <c r="M3" t="n">
-        <v>0</v>
+        <v>62.88231042492774</v>
       </c>
       <c r="N3" t="n">
-        <v>0</v>
+        <v>46.82720517959868</v>
       </c>
     </row>
     <row r="4">
@@ -2822,43 +2822,43 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
+        <v>0.004299925714220305</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>0.08358656864396773</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>0.2331839375427655</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>0.5154429909532171</v>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>1.048006991367294</v>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>2.052844253839822</v>
       </c>
       <c r="H4" t="n">
-        <v>0</v>
+        <v>3.948762722358587</v>
       </c>
       <c r="I4" t="n">
-        <v>0</v>
+        <v>7.525965691947714</v>
       </c>
       <c r="J4" t="n">
-        <v>0</v>
+        <v>24.45048049320263</v>
       </c>
       <c r="K4" t="n">
-        <v>0</v>
+        <v>19.93317169158414</v>
       </c>
       <c r="L4" t="n">
-        <v>0</v>
+        <v>17.2284920461085</v>
       </c>
       <c r="M4" t="n">
-        <v>0</v>
+        <v>19.23418555368698</v>
       </c>
       <c r="N4" t="n">
-        <v>0</v>
+        <v>19.64915995160185</v>
       </c>
     </row>
     <row r="5">
@@ -2868,43 +2868,43 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
+        <v>0.1308207421508001</v>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>0.377652214640918</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>0.8433717542947233</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>1.722087452204907</v>
       </c>
       <c r="F5" t="n">
-        <v>0</v>
+        <v>3.380040816858143</v>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>6.508253236304355</v>
       </c>
       <c r="H5" t="n">
-        <v>0</v>
+        <v>12.41053803502318</v>
       </c>
       <c r="I5" t="n">
-        <v>0</v>
+        <v>23.54691919271787</v>
       </c>
       <c r="J5" t="n">
-        <v>0</v>
+        <v>76.22468392775099</v>
       </c>
       <c r="K5" t="n">
-        <v>0</v>
+        <v>88.40582923468122</v>
       </c>
       <c r="L5" t="n">
-        <v>0</v>
+        <v>90.18252883191759</v>
       </c>
       <c r="M5" t="n">
-        <v>0</v>
+        <v>53.9956112855992</v>
       </c>
       <c r="N5" t="n">
-        <v>0</v>
+        <v>47.28066966778783</v>
       </c>
     </row>
     <row r="6">
@@ -2914,43 +2914,43 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0</v>
+        <v>0.2264205152610002</v>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>0.6536288330323581</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>1.459681882433175</v>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>2.980535974970033</v>
       </c>
       <c r="F6" t="n">
-        <v>0</v>
+        <v>5.850070644562171</v>
       </c>
       <c r="G6" t="n">
-        <v>0</v>
+        <v>11.26428444744985</v>
       </c>
       <c r="H6" t="n">
-        <v>0</v>
+        <v>21.47977736830935</v>
       </c>
       <c r="I6" t="n">
-        <v>0</v>
+        <v>40.75428321816555</v>
       </c>
       <c r="J6" t="n">
-        <v>0</v>
+        <v>131.9273375672613</v>
       </c>
       <c r="K6" t="n">
-        <v>0</v>
+        <v>371.2338451051322</v>
       </c>
       <c r="L6" t="n">
-        <v>0</v>
+        <v>360.8361651339357</v>
       </c>
       <c r="M6" t="n">
-        <v>0</v>
+        <v>249.8991231399586</v>
       </c>
       <c r="N6" t="n">
-        <v>0</v>
+        <v>182.6700247169037</v>
       </c>
     </row>
     <row r="7">
@@ -2960,43 +2960,43 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0</v>
+        <v>0.1710732781972001</v>
       </c>
       <c r="C7" t="n">
-        <v>0</v>
+        <v>0.4938528960688927</v>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>1.102870755616177</v>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>2.251960514421802</v>
       </c>
       <c r="F7" t="n">
-        <v>0</v>
+        <v>4.420053375891418</v>
       </c>
       <c r="G7" t="n">
-        <v>0</v>
+        <v>8.510792693628771</v>
       </c>
       <c r="H7" t="n">
-        <v>0</v>
+        <v>16.22916512272262</v>
       </c>
       <c r="I7" t="n">
-        <v>0</v>
+        <v>30.79212509816952</v>
       </c>
       <c r="J7" t="n">
-        <v>0</v>
+        <v>99.67843282859744</v>
       </c>
       <c r="K7" t="n">
-        <v>0</v>
+        <v>237.978602161099</v>
       </c>
       <c r="L7" t="n">
-        <v>0</v>
+        <v>310.285255520366</v>
       </c>
       <c r="M7" t="n">
-        <v>0</v>
+        <v>365.8211378513453</v>
       </c>
       <c r="N7" t="n">
-        <v>0</v>
+        <v>335.5349789737019</v>
       </c>
     </row>
     <row r="8">
@@ -3006,43 +3006,43 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0</v>
+        <v>0.587232442278706</v>
       </c>
       <c r="C8" t="n">
-        <v>0</v>
+        <v>1.842594000164532</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>4.211199595470363</v>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>8.680264647583698</v>
       </c>
       <c r="F8" t="n">
-        <v>0</v>
+        <v>17.11245888017476</v>
       </c>
       <c r="G8" t="n">
-        <v>0</v>
+        <v>33.02225181158876</v>
       </c>
       <c r="H8" t="n">
-        <v>0</v>
+        <v>63.04071487570283</v>
       </c>
       <c r="I8" t="n">
-        <v>0</v>
+        <v>119.6792977042912</v>
       </c>
       <c r="J8" t="n">
-        <v>0</v>
+        <v>387.6006468870046</v>
       </c>
       <c r="K8" t="n">
-        <v>0</v>
+        <v>520.2540920930874</v>
       </c>
       <c r="L8" t="n">
-        <v>0</v>
+        <v>456.3851567188592</v>
       </c>
       <c r="M8" t="n">
-        <v>0</v>
+        <v>313.159933215772</v>
       </c>
       <c r="N8" t="n">
-        <v>0</v>
+        <v>319.9495259105572</v>
       </c>
     </row>
     <row r="9">
@@ -3052,43 +3052,43 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0</v>
+        <v>0.1581660651879728</v>
       </c>
       <c r="C9" t="n">
-        <v>0</v>
+        <v>0.4896259434908923</v>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>1.115021645180118</v>
       </c>
       <c r="E9" t="n">
-        <v>0</v>
+        <v>2.295012978351116</v>
       </c>
       <c r="F9" t="n">
-        <v>0</v>
+        <v>4.521410669601283</v>
       </c>
       <c r="G9" t="n">
-        <v>0</v>
+        <v>8.722159048221581</v>
       </c>
       <c r="H9" t="n">
-        <v>0</v>
+        <v>16.64809564518791</v>
       </c>
       <c r="I9" t="n">
-        <v>0</v>
+        <v>31.60268594125396</v>
       </c>
       <c r="J9" t="n">
-        <v>0</v>
+        <v>102.3431160866292</v>
       </c>
       <c r="K9" t="n">
-        <v>0</v>
+        <v>100.4705335364614</v>
       </c>
       <c r="L9" t="n">
-        <v>0</v>
+        <v>83.60822929821711</v>
       </c>
       <c r="M9" t="n">
-        <v>0</v>
+        <v>50.05933530515507</v>
       </c>
       <c r="N9" t="n">
-        <v>0</v>
+        <v>49.65740650120593</v>
       </c>
     </row>
     <row r="10">
@@ -3098,43 +3098,43 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0</v>
+        <v>0.2264205152610002</v>
       </c>
       <c r="C10" t="n">
-        <v>0</v>
+        <v>0.6536288330323581</v>
       </c>
       <c r="D10" t="n">
-        <v>0</v>
+        <v>1.459681882433175</v>
       </c>
       <c r="E10" t="n">
-        <v>0</v>
+        <v>2.980535974970033</v>
       </c>
       <c r="F10" t="n">
-        <v>0</v>
+        <v>5.850070644562171</v>
       </c>
       <c r="G10" t="n">
-        <v>0</v>
+        <v>11.26428444744985</v>
       </c>
       <c r="H10" t="n">
-        <v>0</v>
+        <v>21.47977736830935</v>
       </c>
       <c r="I10" t="n">
-        <v>0</v>
+        <v>40.75428321816555</v>
       </c>
       <c r="J10" t="n">
-        <v>0</v>
+        <v>131.9273375672613</v>
       </c>
       <c r="K10" t="n">
-        <v>0</v>
+        <v>144.1993301226925</v>
       </c>
       <c r="L10" t="n">
-        <v>0</v>
+        <v>152.2922168410222</v>
       </c>
       <c r="M10" t="n">
-        <v>0</v>
+        <v>91.18297578122113</v>
       </c>
       <c r="N10" t="n">
-        <v>0</v>
+        <v>70.67671170586178</v>
       </c>
     </row>
     <row r="11">
@@ -3153,34 +3153,34 @@
         <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>0</v>
+        <v>0.3398252464588563</v>
       </c>
       <c r="F11" t="n">
-        <v>0</v>
+        <v>1.350630355560854</v>
       </c>
       <c r="G11" t="n">
-        <v>0</v>
+        <v>3.257808906746395</v>
       </c>
       <c r="H11" t="n">
-        <v>0</v>
+        <v>6.856257305304252</v>
       </c>
       <c r="I11" t="n">
-        <v>0</v>
+        <v>13.64577938179486</v>
       </c>
       <c r="J11" t="n">
-        <v>0</v>
+        <v>45.8274235089075</v>
       </c>
       <c r="K11" t="n">
-        <v>0</v>
+        <v>37.71071217328214</v>
       </c>
       <c r="L11" t="n">
-        <v>0</v>
+        <v>32.85093727150836</v>
       </c>
       <c r="M11" t="n">
-        <v>0</v>
+        <v>22.57879638313042</v>
       </c>
       <c r="N11" t="n">
-        <v>0</v>
+        <v>13.51875943812209</v>
       </c>
     </row>
     <row r="12">
@@ -3199,34 +3199,34 @@
         <v>0</v>
       </c>
       <c r="E12" t="n">
-        <v>0</v>
+        <v>0.1408838761624001</v>
       </c>
       <c r="F12" t="n">
-        <v>0</v>
+        <v>0.4067023849979116</v>
       </c>
       <c r="G12" t="n">
-        <v>0</v>
+        <v>0.9082465046250864</v>
       </c>
       <c r="H12" t="n">
-        <v>0</v>
+        <v>1.854555717759131</v>
       </c>
       <c r="I12" t="n">
-        <v>0</v>
+        <v>3.640043956616461</v>
       </c>
       <c r="J12" t="n">
-        <v>0</v>
+        <v>12.09831942001702</v>
       </c>
       <c r="K12" t="n">
-        <v>0</v>
+        <v>7.243710739469232</v>
       </c>
       <c r="L12" t="n">
-        <v>0</v>
+        <v>4.337077196877982</v>
       </c>
       <c r="M12" t="n">
-        <v>0</v>
+        <v>4.337077196877983</v>
       </c>
       <c r="N12" t="n">
-        <v>0</v>
+        <v>2.596768326099292</v>
       </c>
     </row>
     <row r="13">
@@ -3236,43 +3236,43 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0</v>
+        <v>0.03090516207820213</v>
       </c>
       <c r="C13" t="n">
-        <v>0</v>
+        <v>0.6067524026790473</v>
       </c>
       <c r="D13" t="n">
-        <v>0</v>
+        <v>1.69325611753363</v>
       </c>
       <c r="E13" t="n">
-        <v>0</v>
+        <v>3.743262159346163</v>
       </c>
       <c r="F13" t="n">
-        <v>0</v>
+        <v>7.611196262112072</v>
       </c>
       <c r="G13" t="n">
-        <v>0</v>
+        <v>14.9091816915168</v>
       </c>
       <c r="H13" t="n">
-        <v>0</v>
+        <v>28.67895902296559</v>
       </c>
       <c r="I13" t="n">
-        <v>0</v>
+        <v>54.65965870944694</v>
       </c>
       <c r="J13" t="n">
-        <v>0</v>
+        <v>177.5799535154173</v>
       </c>
       <c r="K13" t="n">
-        <v>0</v>
+        <v>152.2994247431545</v>
       </c>
       <c r="L13" t="n">
-        <v>0</v>
+        <v>128.0552777519862</v>
       </c>
       <c r="M13" t="n">
-        <v>0</v>
+        <v>147.3334242405355</v>
       </c>
       <c r="N13" t="n">
-        <v>0</v>
+        <v>143.0487456760092</v>
       </c>
     </row>
     <row r="14">
@@ -3282,43 +3282,43 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0</v>
+        <v>1.585654316187102</v>
       </c>
       <c r="C14" t="n">
-        <v>0</v>
+        <v>5.650353121805658</v>
       </c>
       <c r="D14" t="n">
-        <v>0</v>
+        <v>13.72526290190065</v>
       </c>
       <c r="E14" t="n">
-        <v>0</v>
+        <v>29.44164366555389</v>
       </c>
       <c r="F14" t="n">
-        <v>0</v>
+        <v>59.46480398481108</v>
       </c>
       <c r="G14" t="n">
-        <v>0</v>
+        <v>116.1122495547704</v>
       </c>
       <c r="H14" t="n">
-        <v>0</v>
+        <v>222.9941718933476</v>
       </c>
       <c r="I14" t="n">
-        <v>0</v>
+        <v>424.6580811455555</v>
       </c>
       <c r="J14" t="n">
-        <v>0</v>
+        <v>1378.737877297672</v>
       </c>
       <c r="K14" t="n">
-        <v>0</v>
+        <v>1888.586336909574</v>
       </c>
       <c r="L14" t="n">
-        <v>0</v>
+        <v>2022.977759729771</v>
       </c>
       <c r="M14" t="n">
-        <v>0</v>
+        <v>2090.27935590562</v>
       </c>
       <c r="N14" t="n">
-        <v>0</v>
+        <v>2128.443106458348</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
introduce CCS sustaining constraint
</commit_message>
<xml_diff>
--- a/tutorial/dac_scenarios/SSPs/get_report_output.xlsx
+++ b/tutorial/dac_scenarios/SSPs/get_report_output.xlsx
@@ -504,40 +504,40 @@
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>0.05529194511868137</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>0.1596163206428224</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>0.3564546721448534</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>0.727847612935295</v>
       </c>
       <c r="I2" t="n">
-        <v>0</v>
+        <v>1.428588679990762</v>
       </c>
       <c r="J2" t="n">
-        <v>0</v>
+        <v>2.750741012808265</v>
       </c>
       <c r="K2" t="n">
-        <v>0</v>
+        <v>5.245366878708023</v>
       </c>
       <c r="L2" t="n">
-        <v>0</v>
+        <v>17.04825401325482</v>
       </c>
       <c r="M2" t="n">
-        <v>0</v>
+        <v>55.08467582527395</v>
       </c>
       <c r="N2" t="n">
-        <v>0</v>
+        <v>177.6622594088009</v>
       </c>
       <c r="O2" t="n">
-        <v>0</v>
+        <v>572.6853262848947</v>
       </c>
       <c r="P2" t="n">
-        <v>0</v>
+        <v>436.1299058509211</v>
       </c>
     </row>
     <row r="3">
@@ -556,40 +556,40 @@
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>0.7796164261734072</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>2.250590121063797</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>5.026010877242434</v>
       </c>
       <c r="H3" t="n">
-        <v>0</v>
+        <v>10.26265134238766</v>
       </c>
       <c r="I3" t="n">
-        <v>0</v>
+        <v>20.14310038786974</v>
       </c>
       <c r="J3" t="n">
-        <v>0</v>
+        <v>38.78544828059653</v>
       </c>
       <c r="K3" t="n">
-        <v>0</v>
+        <v>73.95967298978309</v>
       </c>
       <c r="L3" t="n">
-        <v>0</v>
+        <v>240.3803815868928</v>
       </c>
       <c r="M3" t="n">
-        <v>0</v>
+        <v>160.3671228142077</v>
       </c>
       <c r="N3" t="n">
-        <v>0</v>
+        <v>96.01772026824392</v>
       </c>
       <c r="O3" t="n">
-        <v>0</v>
+        <v>57.48935594605522</v>
       </c>
       <c r="P3" t="n">
-        <v>0</v>
+        <v>34.4210010179268</v>
       </c>
     </row>
     <row r="4">
@@ -608,40 +608,40 @@
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>0.08293791767802204</v>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>0.2394244809642337</v>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>0.5346820082172803</v>
       </c>
       <c r="H4" t="n">
-        <v>0</v>
+        <v>1.091771419402942</v>
       </c>
       <c r="I4" t="n">
-        <v>0</v>
+        <v>2.142883019986143</v>
       </c>
       <c r="J4" t="n">
-        <v>0</v>
+        <v>4.126111519212397</v>
       </c>
       <c r="K4" t="n">
-        <v>0</v>
+        <v>7.868050318062035</v>
       </c>
       <c r="L4" t="n">
-        <v>0</v>
+        <v>25.57238101988223</v>
       </c>
       <c r="M4" t="n">
-        <v>0</v>
+        <v>23.41783506084621</v>
       </c>
       <c r="N4" t="n">
-        <v>0</v>
+        <v>14.02112288792025</v>
       </c>
       <c r="O4" t="n">
-        <v>0</v>
+        <v>8.394964202598553</v>
       </c>
       <c r="P4" t="n">
-        <v>0</v>
+        <v>5.026375171679616</v>
       </c>
     </row>
     <row r="5">
@@ -660,40 +660,40 @@
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>0.1437590573085715</v>
       </c>
       <c r="F5" t="n">
-        <v>0</v>
+        <v>0.4150024336713384</v>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>0.926782147576619</v>
       </c>
       <c r="H5" t="n">
-        <v>0</v>
+        <v>1.892403793631766</v>
       </c>
       <c r="I5" t="n">
-        <v>0</v>
+        <v>3.714330567975981</v>
       </c>
       <c r="J5" t="n">
-        <v>0</v>
+        <v>7.151926633301487</v>
       </c>
       <c r="K5" t="n">
-        <v>0</v>
+        <v>13.63795388464085</v>
       </c>
       <c r="L5" t="n">
-        <v>0</v>
+        <v>44.32546043446252</v>
       </c>
       <c r="M5" t="n">
-        <v>0</v>
+        <v>143.2201571457123</v>
       </c>
       <c r="N5" t="n">
-        <v>0</v>
+        <v>107.0852825513867</v>
       </c>
       <c r="O5" t="n">
-        <v>0</v>
+        <v>86.79464128246732</v>
       </c>
       <c r="P5" t="n">
-        <v>0</v>
+        <v>280.0829143957978</v>
       </c>
     </row>
     <row r="6">
@@ -712,40 +712,40 @@
         <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>0.2488137530340661</v>
       </c>
       <c r="F6" t="n">
-        <v>0</v>
+        <v>0.7182734428927011</v>
       </c>
       <c r="G6" t="n">
-        <v>0</v>
+        <v>1.60404602465184</v>
       </c>
       <c r="H6" t="n">
-        <v>0</v>
+        <v>3.275314258208827</v>
       </c>
       <c r="I6" t="n">
-        <v>0</v>
+        <v>6.428649059958429</v>
       </c>
       <c r="J6" t="n">
-        <v>0</v>
+        <v>12.37833455763719</v>
       </c>
       <c r="K6" t="n">
-        <v>0</v>
+        <v>23.6041509541861</v>
       </c>
       <c r="L6" t="n">
-        <v>0</v>
+        <v>76.71714305964667</v>
       </c>
       <c r="M6" t="n">
-        <v>0</v>
+        <v>247.8810412137328</v>
       </c>
       <c r="N6" t="n">
-        <v>0</v>
+        <v>799.4801673396042</v>
       </c>
       <c r="O6" t="n">
-        <v>0</v>
+        <v>818.7566782189353</v>
       </c>
       <c r="P6" t="n">
-        <v>0</v>
+        <v>574.5418787636854</v>
       </c>
     </row>
     <row r="7">
@@ -764,40 +764,40 @@
         <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>0.1879926134035166</v>
       </c>
       <c r="F7" t="n">
-        <v>0</v>
+        <v>0.5426954901855964</v>
       </c>
       <c r="G7" t="n">
-        <v>0</v>
+        <v>1.211945885292502</v>
       </c>
       <c r="H7" t="n">
-        <v>0</v>
+        <v>2.474681883980002</v>
       </c>
       <c r="I7" t="n">
-        <v>0</v>
+        <v>4.857201511968591</v>
       </c>
       <c r="J7" t="n">
-        <v>0</v>
+        <v>9.352519443548099</v>
       </c>
       <c r="K7" t="n">
-        <v>0</v>
+        <v>17.83424738760727</v>
       </c>
       <c r="L7" t="n">
-        <v>0</v>
+        <v>57.96406364506636</v>
       </c>
       <c r="M7" t="n">
-        <v>0</v>
+        <v>138.6080276043995</v>
       </c>
       <c r="N7" t="n">
-        <v>0</v>
+        <v>99.42589278615498</v>
       </c>
       <c r="O7" t="n">
-        <v>0</v>
+        <v>136.7914459476741</v>
       </c>
       <c r="P7" t="n">
-        <v>0</v>
+        <v>188.5429306461905</v>
       </c>
     </row>
     <row r="8">
@@ -816,40 +816,40 @@
         <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>0.8072623987327479</v>
       </c>
       <c r="F8" t="n">
-        <v>0</v>
+        <v>2.330398281385208</v>
       </c>
       <c r="G8" t="n">
-        <v>0</v>
+        <v>5.204238213314861</v>
       </c>
       <c r="H8" t="n">
-        <v>0</v>
+        <v>10.62657514885531</v>
       </c>
       <c r="I8" t="n">
-        <v>0</v>
+        <v>20.85739472786513</v>
       </c>
       <c r="J8" t="n">
-        <v>0</v>
+        <v>40.16081878700067</v>
       </c>
       <c r="K8" t="n">
-        <v>0</v>
+        <v>76.58235642913712</v>
       </c>
       <c r="L8" t="n">
-        <v>0</v>
+        <v>248.9045085935203</v>
       </c>
       <c r="M8" t="n">
-        <v>0</v>
+        <v>804.2362670489998</v>
       </c>
       <c r="N8" t="n">
-        <v>0</v>
+        <v>636.7408725602046</v>
       </c>
       <c r="O8" t="n">
-        <v>0</v>
+        <v>381.2402811246716</v>
       </c>
       <c r="P8" t="n">
-        <v>0</v>
+        <v>568.520472817485</v>
       </c>
     </row>
     <row r="9">
@@ -868,40 +868,40 @@
         <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>0</v>
+        <v>0.2101093914509891</v>
       </c>
       <c r="F9" t="n">
-        <v>0</v>
+        <v>0.6065420184427253</v>
       </c>
       <c r="G9" t="n">
-        <v>0</v>
+        <v>1.354527754150443</v>
       </c>
       <c r="H9" t="n">
-        <v>0</v>
+        <v>2.76582092915412</v>
       </c>
       <c r="I9" t="n">
-        <v>0</v>
+        <v>5.428636983964894</v>
       </c>
       <c r="J9" t="n">
-        <v>0</v>
+        <v>10.4528158486714</v>
       </c>
       <c r="K9" t="n">
-        <v>0</v>
+        <v>19.93239413909048</v>
       </c>
       <c r="L9" t="n">
-        <v>0</v>
+        <v>64.78336525036829</v>
       </c>
       <c r="M9" t="n">
-        <v>0</v>
+        <v>108.4559953762829</v>
       </c>
       <c r="N9" t="n">
-        <v>0</v>
+        <v>64.9366107136474</v>
       </c>
       <c r="O9" t="n">
-        <v>0</v>
+        <v>44.51124042849872</v>
       </c>
       <c r="P9" t="n">
-        <v>0</v>
+        <v>41.19434702135365</v>
       </c>
     </row>
     <row r="10">
@@ -920,40 +920,40 @@
         <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>0</v>
+        <v>0.2488137530340661</v>
       </c>
       <c r="F10" t="n">
-        <v>0</v>
+        <v>0.7182734428927011</v>
       </c>
       <c r="G10" t="n">
-        <v>0</v>
+        <v>1.60404602465184</v>
       </c>
       <c r="H10" t="n">
-        <v>0</v>
+        <v>3.275314258208827</v>
       </c>
       <c r="I10" t="n">
-        <v>0</v>
+        <v>6.428649059958429</v>
       </c>
       <c r="J10" t="n">
-        <v>0</v>
+        <v>12.37833455763719</v>
       </c>
       <c r="K10" t="n">
-        <v>0</v>
+        <v>23.6041509541861</v>
       </c>
       <c r="L10" t="n">
-        <v>0</v>
+        <v>76.71714305964667</v>
       </c>
       <c r="M10" t="n">
-        <v>0</v>
+        <v>189.3501290822783</v>
       </c>
       <c r="N10" t="n">
-        <v>0</v>
+        <v>126.4498632552685</v>
       </c>
       <c r="O10" t="n">
-        <v>0</v>
+        <v>75.71020409257103</v>
       </c>
       <c r="P10" t="n">
-        <v>0</v>
+        <v>75.71020409257103</v>
       </c>
     </row>
     <row r="11">
@@ -975,37 +975,37 @@
         <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>0</v>
+        <v>0.4479023184233376</v>
       </c>
       <c r="G11" t="n">
-        <v>0</v>
+        <v>1.624714741398749</v>
       </c>
       <c r="H11" t="n">
-        <v>0</v>
+        <v>3.845114491713937</v>
       </c>
       <c r="I11" t="n">
-        <v>0</v>
+        <v>8.034546005985742</v>
       </c>
       <c r="J11" t="n">
-        <v>0</v>
+        <v>15.93913003878539</v>
       </c>
       <c r="K11" t="n">
-        <v>0</v>
+        <v>30.85343249694398</v>
       </c>
       <c r="L11" t="n">
-        <v>0</v>
+        <v>101.4646122988113</v>
       </c>
       <c r="M11" t="n">
-        <v>0</v>
+        <v>60.75061140879908</v>
       </c>
       <c r="N11" t="n">
-        <v>0</v>
+        <v>36.37363513176451</v>
       </c>
       <c r="O11" t="n">
-        <v>0</v>
+        <v>21.77823896776625</v>
       </c>
       <c r="P11" t="n">
-        <v>0</v>
+        <v>13.03943614156235</v>
       </c>
     </row>
     <row r="12">
@@ -1024,40 +1024,40 @@
         <v>0</v>
       </c>
       <c r="E12" t="n">
-        <v>0</v>
+        <v>0.1548174463323078</v>
       </c>
       <c r="F12" t="n">
-        <v>0</v>
+        <v>0.4469256977999028</v>
       </c>
       <c r="G12" t="n">
-        <v>0</v>
+        <v>0.9980730820055893</v>
       </c>
       <c r="H12" t="n">
-        <v>0</v>
+        <v>2.037973316218825</v>
       </c>
       <c r="I12" t="n">
-        <v>0</v>
+        <v>4.000048303974133</v>
       </c>
       <c r="J12" t="n">
-        <v>0</v>
+        <v>7.702074835863138</v>
       </c>
       <c r="K12" t="n">
-        <v>0</v>
+        <v>14.68702726038245</v>
       </c>
       <c r="L12" t="n">
-        <v>0</v>
+        <v>47.73511123711346</v>
       </c>
       <c r="M12" t="n">
-        <v>0</v>
+        <v>28.58077439631286</v>
       </c>
       <c r="N12" t="n">
-        <v>0</v>
+        <v>17.11236538311099</v>
       </c>
       <c r="O12" t="n">
-        <v>0</v>
+        <v>10.24580527261266</v>
       </c>
       <c r="P12" t="n">
-        <v>0</v>
+        <v>6.134542088956549</v>
       </c>
     </row>
     <row r="13">
@@ -1076,40 +1076,40 @@
         <v>0</v>
       </c>
       <c r="E13" t="n">
-        <v>0</v>
+        <v>0.6026822017936269</v>
       </c>
       <c r="F13" t="n">
-        <v>0</v>
+        <v>1.739817895006764</v>
       </c>
       <c r="G13" t="n">
-        <v>0</v>
+        <v>3.885355926378902</v>
       </c>
       <c r="H13" t="n">
-        <v>0</v>
+        <v>7.933538980994713</v>
       </c>
       <c r="I13" t="n">
-        <v>0</v>
+        <v>15.5716166118993</v>
       </c>
       <c r="J13" t="n">
-        <v>0</v>
+        <v>29.98307703961008</v>
       </c>
       <c r="K13" t="n">
-        <v>0</v>
+        <v>57.17449897791743</v>
       </c>
       <c r="L13" t="n">
-        <v>0</v>
+        <v>185.8259687444774</v>
       </c>
       <c r="M13" t="n">
-        <v>0</v>
+        <v>163.9152677096943</v>
       </c>
       <c r="N13" t="n">
-        <v>0</v>
+        <v>98.14212568294181</v>
       </c>
       <c r="O13" t="n">
-        <v>0</v>
+        <v>85.71537069561224</v>
       </c>
       <c r="P13" t="n">
-        <v>0</v>
+        <v>51.32095869597391</v>
       </c>
     </row>
     <row r="14">
@@ -1128,40 +1128,40 @@
         <v>0</v>
       </c>
       <c r="E14" t="n">
-        <v>0</v>
+        <v>3.522096904060003</v>
       </c>
       <c r="F14" t="n">
-        <v>0</v>
+        <v>10.61546194337113</v>
       </c>
       <c r="G14" t="n">
-        <v>0</v>
+        <v>24.33087735702592</v>
       </c>
       <c r="H14" t="n">
-        <v>0</v>
+        <v>50.20900743569222</v>
       </c>
       <c r="I14" t="n">
-        <v>0</v>
+        <v>99.03564492139729</v>
       </c>
       <c r="J14" t="n">
-        <v>0</v>
+        <v>191.1613325546718</v>
       </c>
       <c r="K14" t="n">
-        <v>0</v>
+        <v>364.9833026706449</v>
       </c>
       <c r="L14" t="n">
-        <v>0</v>
+        <v>1187.438392943143</v>
       </c>
       <c r="M14" t="n">
-        <v>0</v>
+        <v>2123.86790468654</v>
       </c>
       <c r="N14" t="n">
-        <v>0</v>
+        <v>2273.447917969049</v>
       </c>
       <c r="O14" t="n">
-        <v>0</v>
+        <v>2300.113552464358</v>
       </c>
       <c r="P14" t="n">
-        <v>0</v>
+        <v>2274.664966704104</v>
       </c>
     </row>
   </sheetData>
@@ -1251,37 +1251,37 @@
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>0.01105838902373627</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>0.02086487510482822</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>0.03936767030040619</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>0.08533697718182459</v>
       </c>
       <c r="I2" t="n">
-        <v>0</v>
+        <v>0.1610130885159217</v>
       </c>
       <c r="J2" t="n">
-        <v>0</v>
+        <v>0.2644304665635006</v>
       </c>
       <c r="K2" t="n">
-        <v>0</v>
+        <v>0.5382928434803577</v>
       </c>
       <c r="L2" t="n">
-        <v>0</v>
+        <v>1.263210474174572</v>
       </c>
       <c r="M2" t="n">
-        <v>0</v>
+        <v>4.110683897482734</v>
       </c>
       <c r="N2" t="n">
-        <v>0</v>
+        <v>13.65554204339736</v>
       </c>
       <c r="O2" t="n">
-        <v>0</v>
+        <v>43.61299058509212</v>
       </c>
       <c r="P2" t="n">
         <v>0</v>
@@ -1303,40 +1303,40 @@
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>0.1559232852346815</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>0.2941947389780779</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>0.5550841512357274</v>
       </c>
       <c r="H3" t="n">
-        <v>0</v>
+        <v>1.203251378263726</v>
       </c>
       <c r="I3" t="n">
-        <v>0</v>
+        <v>1.976089809096417</v>
       </c>
       <c r="J3" t="n">
-        <v>0</v>
+        <v>4.022664317523437</v>
       </c>
       <c r="K3" t="n">
-        <v>0</v>
+        <v>7.589929093073041</v>
       </c>
       <c r="L3" t="n">
-        <v>0</v>
+        <v>17.73771900111694</v>
       </c>
       <c r="M3" t="n">
         <v>0</v>
       </c>
       <c r="N3" t="n">
-        <v>0</v>
+        <v>9.601772026824392</v>
       </c>
       <c r="O3" t="n">
         <v>0</v>
       </c>
       <c r="P3" t="n">
-        <v>0</v>
+        <v>3.44210010179268</v>
       </c>
     </row>
     <row r="4">
@@ -1355,40 +1355,40 @@
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>0.01658758353560441</v>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>0.03129731265724234</v>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>0.0590515054506093</v>
       </c>
       <c r="H4" t="n">
-        <v>0</v>
+        <v>0.1114178822371324</v>
       </c>
       <c r="I4" t="n">
-        <v>0</v>
+        <v>0.2268099036522445</v>
       </c>
       <c r="J4" t="n">
-        <v>0</v>
+        <v>0.4279430125024933</v>
       </c>
       <c r="K4" t="n">
-        <v>0</v>
+        <v>0.8074392652205367</v>
       </c>
       <c r="L4" t="n">
-        <v>0</v>
+        <v>1.882844487213647</v>
       </c>
       <c r="M4" t="n">
-        <v>0</v>
+        <v>0.2570792025658402</v>
       </c>
       <c r="N4" t="n">
-        <v>0</v>
+        <v>1.145033086226185</v>
       </c>
       <c r="O4" t="n">
         <v>0</v>
       </c>
       <c r="P4" t="n">
-        <v>0</v>
+        <v>0.5026375171679617</v>
       </c>
     </row>
     <row r="5">
@@ -1407,40 +1407,40 @@
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>0.02875181146171431</v>
       </c>
       <c r="F5" t="n">
-        <v>0</v>
+        <v>0.05424867527255337</v>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>0.1023559427810561</v>
       </c>
       <c r="H5" t="n">
-        <v>0</v>
+        <v>0.1931243292110295</v>
       </c>
       <c r="I5" t="n">
-        <v>0</v>
+        <v>0.3931371663305572</v>
       </c>
       <c r="J5" t="n">
-        <v>0</v>
+        <v>0.7417678883376548</v>
       </c>
       <c r="K5" t="n">
-        <v>0</v>
+        <v>1.39956139304893</v>
       </c>
       <c r="L5" t="n">
-        <v>0</v>
+        <v>3.263597111170321</v>
       </c>
       <c r="M5" t="n">
-        <v>0</v>
+        <v>10.70852825513867</v>
       </c>
       <c r="N5" t="n">
         <v>0</v>
       </c>
       <c r="O5" t="n">
-        <v>0</v>
+        <v>8.679464128246734</v>
       </c>
       <c r="P5" t="n">
-        <v>0</v>
+        <v>19.32882731133305</v>
       </c>
     </row>
     <row r="6">
@@ -1459,40 +1459,40 @@
         <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>0.04976275060681323</v>
       </c>
       <c r="F6" t="n">
-        <v>0</v>
+        <v>0.09389193797172701</v>
       </c>
       <c r="G6" t="n">
-        <v>0</v>
+        <v>0.1771545163518279</v>
       </c>
       <c r="H6" t="n">
-        <v>0</v>
+        <v>0.3342536467113974</v>
       </c>
       <c r="I6" t="n">
-        <v>0</v>
+        <v>0.6804297109567337</v>
       </c>
       <c r="J6" t="n">
-        <v>0</v>
+        <v>1.28382903750748</v>
       </c>
       <c r="K6" t="n">
-        <v>0</v>
+        <v>2.422317795661608</v>
       </c>
       <c r="L6" t="n">
-        <v>0</v>
+        <v>5.648533461640941</v>
       </c>
       <c r="M6" t="n">
-        <v>0</v>
+        <v>18.53399121081694</v>
       </c>
       <c r="N6" t="n">
-        <v>0</v>
+        <v>61.41402552314349</v>
       </c>
       <c r="O6" t="n">
-        <v>0</v>
+        <v>20.46164229875005</v>
       </c>
       <c r="P6" t="n">
-        <v>0</v>
+        <v>36.99254557761849</v>
       </c>
     </row>
     <row r="7">
@@ -1511,40 +1511,40 @@
         <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>0.03759852268070332</v>
       </c>
       <c r="F7" t="n">
-        <v>0</v>
+        <v>0.07094057535641596</v>
       </c>
       <c r="G7" t="n">
-        <v>0</v>
+        <v>0.1338500790213811</v>
       </c>
       <c r="H7" t="n">
-        <v>0</v>
+        <v>0.2525471997375001</v>
       </c>
       <c r="I7" t="n">
-        <v>0</v>
+        <v>0.514102448278421</v>
       </c>
       <c r="J7" t="n">
-        <v>0</v>
+        <v>0.9700041616723176</v>
       </c>
       <c r="K7" t="n">
-        <v>0</v>
+        <v>1.830195667833216</v>
       </c>
       <c r="L7" t="n">
-        <v>0</v>
+        <v>4.267780837684264</v>
       </c>
       <c r="M7" t="n">
-        <v>0</v>
+        <v>9.135473005797378</v>
       </c>
       <c r="N7" t="n">
-        <v>0</v>
+        <v>0.8071162728181194</v>
       </c>
       <c r="O7" t="n">
-        <v>0</v>
+        <v>12.87202832194929</v>
       </c>
       <c r="P7" t="n">
-        <v>0</v>
+        <v>5.982264742669759</v>
       </c>
     </row>
     <row r="8">
@@ -1563,40 +1563,40 @@
         <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>0.1614524797465496</v>
       </c>
       <c r="F8" t="n">
-        <v>0</v>
+        <v>0.3046271765304921</v>
       </c>
       <c r="G8" t="n">
-        <v>0</v>
+        <v>0.5747679863859306</v>
       </c>
       <c r="H8" t="n">
-        <v>0</v>
+        <v>1.084467387108089</v>
       </c>
       <c r="I8" t="n">
-        <v>0</v>
+        <v>2.207616395548514</v>
       </c>
       <c r="J8" t="n">
-        <v>0</v>
+        <v>4.1653119883576</v>
       </c>
       <c r="K8" t="n">
-        <v>0</v>
+        <v>7.859075514813219</v>
       </c>
       <c r="L8" t="n">
-        <v>0</v>
+        <v>18.32635300887949</v>
       </c>
       <c r="M8" t="n">
-        <v>0</v>
+        <v>60.13250481731718</v>
       </c>
       <c r="N8" t="n">
         <v>0</v>
       </c>
       <c r="O8" t="n">
-        <v>0</v>
+        <v>38.12402811246717</v>
       </c>
       <c r="P8" t="n">
-        <v>0</v>
+        <v>18.72801916928135</v>
       </c>
     </row>
     <row r="9">
@@ -1615,40 +1615,40 @@
         <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>0</v>
+        <v>0.04202187829019783</v>
       </c>
       <c r="F9" t="n">
-        <v>0</v>
+        <v>0.07928652539834721</v>
       </c>
       <c r="G9" t="n">
-        <v>0</v>
+        <v>0.1495971471415436</v>
       </c>
       <c r="H9" t="n">
-        <v>0</v>
+        <v>0.2822586350007354</v>
       </c>
       <c r="I9" t="n">
-        <v>0</v>
+        <v>0.5745850892523529</v>
       </c>
       <c r="J9" t="n">
-        <v>0</v>
+        <v>1.084122298339649</v>
       </c>
       <c r="K9" t="n">
-        <v>0</v>
+        <v>2.045512805225358</v>
       </c>
       <c r="L9" t="n">
-        <v>0</v>
+        <v>4.769872700941238</v>
       </c>
       <c r="M9" t="n">
-        <v>0</v>
+        <v>5.564348635380715</v>
       </c>
       <c r="N9" t="n">
-        <v>0</v>
+        <v>0.9293124359840251</v>
       </c>
       <c r="O9" t="n">
-        <v>0</v>
+        <v>3.521811606865847</v>
       </c>
       <c r="P9" t="n">
-        <v>0</v>
+        <v>0.5976230952695178</v>
       </c>
     </row>
     <row r="10">
@@ -1667,37 +1667,37 @@
         <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>0</v>
+        <v>0.04976275060681323</v>
       </c>
       <c r="F10" t="n">
-        <v>0</v>
+        <v>0.09389193797172701</v>
       </c>
       <c r="G10" t="n">
-        <v>0</v>
+        <v>0.1771545163518279</v>
       </c>
       <c r="H10" t="n">
-        <v>0</v>
+        <v>0.3840163973182106</v>
       </c>
       <c r="I10" t="n">
-        <v>0</v>
+        <v>0.7245588983216473</v>
       </c>
       <c r="J10" t="n">
-        <v>0</v>
+        <v>1.189937099535753</v>
       </c>
       <c r="K10" t="n">
-        <v>0</v>
+        <v>2.422317795661609</v>
       </c>
       <c r="L10" t="n">
-        <v>0</v>
+        <v>5.684447133785575</v>
       </c>
       <c r="M10" t="n">
-        <v>0</v>
+        <v>12.64498632552685</v>
       </c>
       <c r="N10" t="n">
         <v>0</v>
       </c>
       <c r="O10" t="n">
-        <v>0</v>
+        <v>7.571020409257104</v>
       </c>
       <c r="P10" t="n">
         <v>0</v>
@@ -1722,37 +1722,37 @@
         <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>0</v>
+        <v>0.08958046368466752</v>
       </c>
       <c r="G11" t="n">
-        <v>0</v>
+        <v>0.2353624845950824</v>
       </c>
       <c r="H11" t="n">
-        <v>0</v>
+        <v>0.4440799500630376</v>
       </c>
       <c r="I11" t="n">
-        <v>0</v>
+        <v>0.8378863028543612</v>
       </c>
       <c r="J11" t="n">
-        <v>0</v>
+        <v>1.670497270244597</v>
       </c>
       <c r="K11" t="n">
-        <v>0</v>
+        <v>3.218222976226802</v>
       </c>
       <c r="L11" t="n">
-        <v>0</v>
+        <v>7.492629530931845</v>
       </c>
       <c r="M11" t="n">
         <v>0</v>
       </c>
       <c r="N11" t="n">
-        <v>0</v>
+        <v>3.637363513176451</v>
       </c>
       <c r="O11" t="n">
         <v>0</v>
       </c>
       <c r="P11" t="n">
-        <v>0</v>
+        <v>1.303943614156235</v>
       </c>
     </row>
     <row r="12">
@@ -1771,40 +1771,40 @@
         <v>0</v>
       </c>
       <c r="E12" t="n">
-        <v>0</v>
+        <v>0.03096348926646156</v>
       </c>
       <c r="F12" t="n">
-        <v>0</v>
+        <v>0.05842165029351901</v>
       </c>
       <c r="G12" t="n">
-        <v>0</v>
+        <v>0.1102294768411373</v>
       </c>
       <c r="H12" t="n">
-        <v>0</v>
+        <v>0.2389435361091087</v>
       </c>
       <c r="I12" t="n">
-        <v>0</v>
+        <v>0.3924149975510616</v>
       </c>
       <c r="J12" t="n">
-        <v>0</v>
+        <v>0.7988269566713202</v>
       </c>
       <c r="K12" t="n">
-        <v>0</v>
+        <v>1.507219961745001</v>
       </c>
       <c r="L12" t="n">
-        <v>0</v>
+        <v>3.522383915115421</v>
       </c>
       <c r="M12" t="n">
         <v>0</v>
       </c>
       <c r="N12" t="n">
-        <v>0</v>
+        <v>1.711236538311099</v>
       </c>
       <c r="O12" t="n">
         <v>0</v>
       </c>
       <c r="P12" t="n">
-        <v>0</v>
+        <v>0.6134542088956549</v>
       </c>
     </row>
     <row r="13">
@@ -1823,40 +1823,40 @@
         <v>0</v>
       </c>
       <c r="E13" t="n">
-        <v>0</v>
+        <v>0.1205364403587254</v>
       </c>
       <c r="F13" t="n">
-        <v>0</v>
+        <v>0.2274271386426275</v>
       </c>
       <c r="G13" t="n">
-        <v>0</v>
+        <v>0.4291076062744276</v>
       </c>
       <c r="H13" t="n">
-        <v>0</v>
+        <v>0.8096366109231623</v>
       </c>
       <c r="I13" t="n">
-        <v>0</v>
+        <v>1.648151966539643</v>
       </c>
       <c r="J13" t="n">
-        <v>0</v>
+        <v>3.109719224184783</v>
       </c>
       <c r="K13" t="n">
-        <v>0</v>
+        <v>5.867391993935898</v>
       </c>
       <c r="L13" t="n">
-        <v>0</v>
+        <v>13.68200327375249</v>
       </c>
       <c r="M13" t="n">
-        <v>0</v>
+        <v>1.242675498732958</v>
       </c>
       <c r="N13" t="n">
-        <v>0</v>
+        <v>8.571537069561224</v>
       </c>
       <c r="O13" t="n">
         <v>0</v>
       </c>
       <c r="P13" t="n">
-        <v>0</v>
+        <v>5.132095869597391</v>
       </c>
     </row>
     <row r="14">
@@ -1875,40 +1875,40 @@
         <v>0</v>
       </c>
       <c r="E14" t="n">
-        <v>0</v>
+        <v>0.7044193808120005</v>
       </c>
       <c r="F14" t="n">
-        <v>0</v>
+        <v>1.418673007862225</v>
       </c>
       <c r="G14" t="n">
-        <v>0</v>
+        <v>2.743083082730958</v>
       </c>
       <c r="H14" t="n">
-        <v>0</v>
+        <v>5.423333929864955</v>
       </c>
       <c r="I14" t="n">
-        <v>0</v>
+        <v>10.33679577689787</v>
       </c>
       <c r="J14" t="n">
-        <v>0</v>
+        <v>19.72905372144059</v>
       </c>
       <c r="K14" t="n">
-        <v>0</v>
+        <v>37.50747710592558</v>
       </c>
       <c r="L14" t="n">
-        <v>0</v>
+        <v>87.54137493640675</v>
       </c>
       <c r="M14" t="n">
-        <v>0</v>
+        <v>122.3302708487593</v>
       </c>
       <c r="N14" t="n">
-        <v>0</v>
+        <v>101.4729385094423</v>
       </c>
       <c r="O14" t="n">
-        <v>0</v>
+        <v>134.8429854626283</v>
       </c>
       <c r="P14" t="n">
-        <v>0</v>
+        <v>92.62351120778209</v>
       </c>
     </row>
   </sheetData>
@@ -1998,37 +1998,37 @@
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>30.80839637777545</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>49.62233614368245</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>77.57666140787791</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>144.9674956433754</v>
       </c>
       <c r="I2" t="n">
-        <v>0</v>
+        <v>235.2301649503415</v>
       </c>
       <c r="J2" t="n">
-        <v>0</v>
+        <v>350.3801346714903</v>
       </c>
       <c r="K2" t="n">
-        <v>0</v>
+        <v>640.1032426199339</v>
       </c>
       <c r="L2" t="n">
-        <v>0</v>
+        <v>1373.374796879558</v>
       </c>
       <c r="M2" t="n">
-        <v>0</v>
+        <v>4329.514041873704</v>
       </c>
       <c r="N2" t="n">
-        <v>0</v>
+        <v>14382.48780512901</v>
       </c>
       <c r="O2" t="n">
-        <v>0</v>
+        <v>44452.94102110871</v>
       </c>
       <c r="P2" t="n">
         <v>0</v>
@@ -2050,40 +2050,40 @@
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>396.236490459429</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>638.2084961797854</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>997.7378790150614</v>
       </c>
       <c r="H3" t="n">
-        <v>0</v>
+        <v>1864.472626230578</v>
       </c>
       <c r="I3" t="n">
-        <v>0</v>
+        <v>2633.32688698929</v>
       </c>
       <c r="J3" t="n">
-        <v>0</v>
+        <v>4861.922586766911</v>
       </c>
       <c r="K3" t="n">
-        <v>0</v>
+        <v>8232.569435856392</v>
       </c>
       <c r="L3" t="n">
-        <v>0</v>
+        <v>17590.46776187989</v>
       </c>
       <c r="M3" t="n">
         <v>0</v>
       </c>
       <c r="N3" t="n">
-        <v>0</v>
+        <v>9224.497629543552</v>
       </c>
       <c r="O3" t="n">
         <v>0</v>
       </c>
       <c r="P3" t="n">
-        <v>0</v>
+        <v>3200.179878853869</v>
       </c>
     </row>
     <row r="4">
@@ -2102,40 +2102,40 @@
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>49.46046192540282</v>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>79.66476532529492</v>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>124.5432401224275</v>
       </c>
       <c r="H4" t="n">
-        <v>0</v>
+        <v>202.5751160598343</v>
       </c>
       <c r="I4" t="n">
-        <v>0</v>
+        <v>354.6432206811614</v>
       </c>
       <c r="J4" t="n">
-        <v>0</v>
+        <v>606.8924563414562</v>
       </c>
       <c r="K4" t="n">
-        <v>0</v>
+        <v>1027.635507921759</v>
       </c>
       <c r="L4" t="n">
-        <v>0</v>
+        <v>2190.915470940419</v>
       </c>
       <c r="M4" t="n">
-        <v>0</v>
+        <v>289.7942943756021</v>
       </c>
       <c r="N4" t="n">
-        <v>0</v>
+        <v>1290.746400128001</v>
       </c>
       <c r="O4" t="n">
         <v>0</v>
       </c>
       <c r="P4" t="n">
-        <v>0</v>
+        <v>548.3241181677697</v>
       </c>
     </row>
     <row r="5">
@@ -2154,40 +2154,40 @@
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>85.73146733736489</v>
       </c>
       <c r="F5" t="n">
-        <v>0</v>
+        <v>138.0855932305112</v>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>215.874949545541</v>
       </c>
       <c r="H5" t="n">
-        <v>0</v>
+        <v>351.1302011703793</v>
       </c>
       <c r="I5" t="n">
-        <v>0</v>
+        <v>614.7149158473464</v>
       </c>
       <c r="J5" t="n">
-        <v>0</v>
+        <v>1051.94692432519</v>
       </c>
       <c r="K5" t="n">
-        <v>0</v>
+        <v>1781.234880397714</v>
       </c>
       <c r="L5" t="n">
-        <v>0</v>
+        <v>3797.586816296726</v>
       </c>
       <c r="M5" t="n">
-        <v>0</v>
+        <v>12071.26192444266</v>
       </c>
       <c r="N5" t="n">
         <v>0</v>
       </c>
       <c r="O5" t="n">
-        <v>0</v>
+        <v>9468.373035710656</v>
       </c>
       <c r="P5" t="n">
-        <v>0</v>
+        <v>21085.69660780456</v>
       </c>
     </row>
     <row r="6">
@@ -2206,40 +2206,40 @@
         <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>138.6377836999895</v>
       </c>
       <c r="F6" t="n">
-        <v>0</v>
+        <v>223.3005126465711</v>
       </c>
       <c r="G6" t="n">
-        <v>0</v>
+        <v>349.0949763354506</v>
       </c>
       <c r="H6" t="n">
-        <v>0</v>
+        <v>567.818496431781</v>
       </c>
       <c r="I6" t="n">
-        <v>0</v>
+        <v>994.0657285736027</v>
       </c>
       <c r="J6" t="n">
-        <v>0</v>
+        <v>1701.120891639082</v>
       </c>
       <c r="K6" t="n">
-        <v>0</v>
+        <v>2880.464591789701</v>
       </c>
       <c r="L6" t="n">
-        <v>0</v>
+        <v>6141.140889935687</v>
       </c>
       <c r="M6" t="n">
-        <v>0</v>
+        <v>19520.63870645329</v>
       </c>
       <c r="N6" t="n">
-        <v>0</v>
+        <v>64683.3696050589</v>
       </c>
       <c r="O6" t="n">
-        <v>0</v>
+        <v>20855.71675087729</v>
       </c>
       <c r="P6" t="n">
-        <v>0</v>
+        <v>37704.99167155605</v>
       </c>
     </row>
     <row r="7">
@@ -2258,40 +2258,40 @@
         <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>117.6316763126931</v>
       </c>
       <c r="F7" t="n">
-        <v>0</v>
+        <v>189.4664854203224</v>
       </c>
       <c r="G7" t="n">
-        <v>0</v>
+        <v>296.2008347417205</v>
       </c>
       <c r="H7" t="n">
-        <v>0</v>
+        <v>481.7838239621854</v>
       </c>
       <c r="I7" t="n">
-        <v>0</v>
+        <v>843.4469658729859</v>
       </c>
       <c r="J7" t="n">
-        <v>0</v>
+        <v>1443.370607590457</v>
       </c>
       <c r="K7" t="n">
-        <v>0</v>
+        <v>2444.022613812208</v>
       </c>
       <c r="L7" t="n">
-        <v>0</v>
+        <v>5210.6480504536</v>
       </c>
       <c r="M7" t="n">
-        <v>0</v>
+        <v>10805.18943099316</v>
       </c>
       <c r="N7" t="n">
-        <v>0</v>
+        <v>954.6352132070839</v>
       </c>
       <c r="O7" t="n">
-        <v>0</v>
+        <v>14733.56671595064</v>
       </c>
       <c r="P7" t="n">
-        <v>0</v>
+        <v>6847.413204359432</v>
       </c>
     </row>
     <row r="8">
@@ -2310,40 +2310,40 @@
         <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>531.7903536820032</v>
       </c>
       <c r="F8" t="n">
-        <v>0</v>
+        <v>856.5418129783739</v>
       </c>
       <c r="G8" t="n">
-        <v>0</v>
+        <v>1339.067431543584</v>
       </c>
       <c r="H8" t="n">
-        <v>0</v>
+        <v>2178.052699530156</v>
       </c>
       <c r="I8" t="n">
-        <v>0</v>
+        <v>3813.062725564579</v>
       </c>
       <c r="J8" t="n">
-        <v>0</v>
+        <v>6525.202989238642</v>
       </c>
       <c r="K8" t="n">
-        <v>0</v>
+        <v>11048.95969305984</v>
       </c>
       <c r="L8" t="n">
-        <v>0</v>
+        <v>23838.34886364366</v>
       </c>
       <c r="M8" t="n">
-        <v>0</v>
+        <v>74877.76481098049</v>
       </c>
       <c r="N8" t="n">
         <v>0</v>
       </c>
       <c r="O8" t="n">
-        <v>0</v>
+        <v>46099.44915424455</v>
       </c>
       <c r="P8" t="n">
-        <v>0</v>
+        <v>23966.14237770314</v>
       </c>
     </row>
     <row r="9">
@@ -2362,40 +2362,40 @@
         <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>0</v>
+        <v>147.9264412677375</v>
       </c>
       <c r="F9" t="n">
-        <v>0</v>
+        <v>238.2615279002845</v>
       </c>
       <c r="G9" t="n">
-        <v>0</v>
+        <v>372.4841535659385</v>
       </c>
       <c r="H9" t="n">
-        <v>0</v>
+        <v>605.8620328561786</v>
       </c>
       <c r="I9" t="n">
-        <v>0</v>
+        <v>1060.667602219646</v>
       </c>
       <c r="J9" t="n">
-        <v>0</v>
+        <v>1815.095084114424</v>
       </c>
       <c r="K9" t="n">
-        <v>0</v>
+        <v>3073.45418319183</v>
       </c>
       <c r="L9" t="n">
-        <v>0</v>
+        <v>6552.594054286235</v>
       </c>
       <c r="M9" t="n">
-        <v>0</v>
+        <v>7405.127205270293</v>
       </c>
       <c r="N9" t="n">
-        <v>0</v>
+        <v>1236.744361800842</v>
       </c>
       <c r="O9" t="n">
-        <v>0</v>
+        <v>4580.622715568938</v>
       </c>
       <c r="P9" t="n">
-        <v>0</v>
+        <v>817.3503927133665</v>
       </c>
     </row>
     <row r="10">
@@ -2414,37 +2414,37 @@
         <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>0</v>
+        <v>131.3301861211631</v>
       </c>
       <c r="F10" t="n">
-        <v>0</v>
+        <v>211.5303426249703</v>
       </c>
       <c r="G10" t="n">
-        <v>0</v>
+        <v>330.694180132809</v>
       </c>
       <c r="H10" t="n">
-        <v>0</v>
+        <v>617.9681652660587</v>
       </c>
       <c r="I10" t="n">
-        <v>0</v>
+        <v>1002.740323301141</v>
       </c>
       <c r="J10" t="n">
-        <v>0</v>
+        <v>1493.602189978303</v>
       </c>
       <c r="K10" t="n">
-        <v>0</v>
+        <v>2728.635303156466</v>
       </c>
       <c r="L10" t="n">
-        <v>0</v>
+        <v>5854.428951012163</v>
       </c>
       <c r="M10" t="n">
-        <v>0</v>
+        <v>12616.13674171719</v>
       </c>
       <c r="N10" t="n">
         <v>0</v>
       </c>
       <c r="O10" t="n">
-        <v>0</v>
+        <v>7310.077836530908</v>
       </c>
       <c r="P10" t="n">
         <v>0</v>
@@ -2469,37 +2469,37 @@
         <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>0</v>
+        <v>194.3305077917782</v>
       </c>
       <c r="G11" t="n">
-        <v>0</v>
+        <v>423.0530914219659</v>
       </c>
       <c r="H11" t="n">
-        <v>0</v>
+        <v>688.1146580900917</v>
       </c>
       <c r="I11" t="n">
-        <v>0</v>
+        <v>1116.562880588584</v>
       </c>
       <c r="J11" t="n">
-        <v>0</v>
+        <v>2019.017190660069</v>
       </c>
       <c r="K11" t="n">
-        <v>0</v>
+        <v>3490.710359341245</v>
       </c>
       <c r="L11" t="n">
-        <v>0</v>
+        <v>7430.428805827089</v>
       </c>
       <c r="M11" t="n">
         <v>0</v>
       </c>
       <c r="N11" t="n">
-        <v>0</v>
+        <v>3494.443630961874</v>
       </c>
       <c r="O11" t="n">
         <v>0</v>
       </c>
       <c r="P11" t="n">
-        <v>0</v>
+        <v>1212.298885500022</v>
       </c>
     </row>
     <row r="12">
@@ -2518,40 +2518,40 @@
         <v>0</v>
       </c>
       <c r="E12" t="n">
-        <v>0</v>
+        <v>81.71656025316811</v>
       </c>
       <c r="F12" t="n">
-        <v>0</v>
+        <v>131.618879855537</v>
       </c>
       <c r="G12" t="n">
-        <v>0</v>
+        <v>205.7652676381922</v>
       </c>
       <c r="H12" t="n">
-        <v>0</v>
+        <v>384.5135250544363</v>
       </c>
       <c r="I12" t="n">
-        <v>0</v>
+        <v>543.075714650721</v>
       </c>
       <c r="J12" t="n">
-        <v>0</v>
+        <v>1002.682992540933</v>
       </c>
       <c r="K12" t="n">
-        <v>0</v>
+        <v>1697.817521964023</v>
       </c>
       <c r="L12" t="n">
-        <v>0</v>
+        <v>3627.713634043125</v>
       </c>
       <c r="M12" t="n">
         <v>0</v>
       </c>
       <c r="N12" t="n">
-        <v>0</v>
+        <v>1707.332345719724</v>
       </c>
       <c r="O12" t="n">
         <v>0</v>
       </c>
       <c r="P12" t="n">
-        <v>0</v>
+        <v>592.3109136902663</v>
       </c>
     </row>
     <row r="13">
@@ -2570,40 +2570,40 @@
         <v>0</v>
       </c>
       <c r="E13" t="n">
-        <v>0</v>
+        <v>412.5149015422532</v>
       </c>
       <c r="F13" t="n">
-        <v>0</v>
+        <v>664.4277377375722</v>
       </c>
       <c r="G13" t="n">
-        <v>0</v>
+        <v>1038.727509547778</v>
       </c>
       <c r="H13" t="n">
-        <v>0</v>
+        <v>1689.536466164988</v>
       </c>
       <c r="I13" t="n">
-        <v>0</v>
+        <v>2957.829497883836</v>
       </c>
       <c r="J13" t="n">
-        <v>0</v>
+        <v>5061.662833881689</v>
       </c>
       <c r="K13" t="n">
-        <v>0</v>
+        <v>8570.784498758294</v>
       </c>
       <c r="L13" t="n">
-        <v>0</v>
+        <v>18272.88392788347</v>
       </c>
       <c r="M13" t="n">
-        <v>0</v>
+        <v>1607.78086895255</v>
       </c>
       <c r="N13" t="n">
-        <v>0</v>
+        <v>11089.90507337556</v>
       </c>
       <c r="O13" t="n">
         <v>0</v>
       </c>
       <c r="P13" t="n">
-        <v>0</v>
+        <v>6425.744342010054</v>
       </c>
     </row>
     <row r="14">
@@ -2622,40 +2622,40 @@
         <v>0</v>
       </c>
       <c r="E14" t="n">
-        <v>0</v>
+        <v>2123.78471897898</v>
       </c>
       <c r="F14" t="n">
-        <v>0</v>
+        <v>3615.058997834683</v>
       </c>
       <c r="G14" t="n">
-        <v>0</v>
+        <v>5770.820175018346</v>
       </c>
       <c r="H14" t="n">
-        <v>0</v>
+        <v>9776.795306460042</v>
       </c>
       <c r="I14" t="n">
-        <v>0</v>
+        <v>16169.36662712324</v>
       </c>
       <c r="J14" t="n">
-        <v>0</v>
+        <v>27932.89688174864</v>
       </c>
       <c r="K14" t="n">
-        <v>0</v>
+        <v>47616.39183186941</v>
       </c>
       <c r="L14" t="n">
-        <v>0</v>
+        <v>101880.5320230816</v>
       </c>
       <c r="M14" t="n">
-        <v>0</v>
+        <v>143523.2080250589</v>
       </c>
       <c r="N14" t="n">
-        <v>0</v>
+        <v>108064.1620649245</v>
       </c>
       <c r="O14" t="n">
-        <v>0</v>
+        <v>147500.7472299917</v>
       </c>
       <c r="P14" t="n">
-        <v>0</v>
+        <v>102400.4523923585</v>
       </c>
     </row>
   </sheetData>
@@ -2669,7 +2669,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N14"/>
+  <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2684,42 +2684,39 @@
         </is>
       </c>
       <c r="B1" s="1" t="n">
-        <v>2025</v>
+        <v>2030</v>
       </c>
       <c r="C1" s="1" t="n">
-        <v>2030</v>
+        <v>2035</v>
       </c>
       <c r="D1" s="1" t="n">
-        <v>2035</v>
+        <v>2040</v>
       </c>
       <c r="E1" s="1" t="n">
-        <v>2040</v>
+        <v>2045</v>
       </c>
       <c r="F1" s="1" t="n">
-        <v>2045</v>
+        <v>2050</v>
       </c>
       <c r="G1" s="1" t="n">
-        <v>2050</v>
+        <v>2055</v>
       </c>
       <c r="H1" s="1" t="n">
-        <v>2055</v>
+        <v>2060</v>
       </c>
       <c r="I1" s="1" t="n">
-        <v>2060</v>
+        <v>2070</v>
       </c>
       <c r="J1" s="1" t="n">
-        <v>2070</v>
+        <v>2080</v>
       </c>
       <c r="K1" s="1" t="n">
-        <v>2080</v>
+        <v>2090</v>
       </c>
       <c r="L1" s="1" t="n">
-        <v>2090</v>
+        <v>2100</v>
       </c>
       <c r="M1" s="1" t="n">
-        <v>2100</v>
-      </c>
-      <c r="N1" s="1" t="n">
         <v>2110</v>
       </c>
     </row>
@@ -2730,43 +2727,40 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>0.05031567005800005</v>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>0.1452508517849684</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>0.3243737516518166</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>0.6623413277711185</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>1.300015698791594</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>2.503174321655522</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>4.773283859624302</v>
       </c>
       <c r="I2" t="n">
-        <v>0</v>
+        <v>15.51391115206189</v>
       </c>
       <c r="J2" t="n">
-        <v>0</v>
+        <v>50.1270550009993</v>
       </c>
       <c r="K2" t="n">
-        <v>0</v>
+        <v>161.6726560620089</v>
       </c>
       <c r="L2" t="n">
-        <v>0</v>
+        <v>521.1436469192543</v>
       </c>
       <c r="M2" t="n">
-        <v>0</v>
-      </c>
-      <c r="N2" t="n">
-        <v>0</v>
+        <v>396.8782143243383</v>
       </c>
     </row>
     <row r="3">
@@ -2776,43 +2770,40 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>0.7094509478178006</v>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>2.048037010168055</v>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>4.573669898290615</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>9.33901272157277</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>18.33022135296147</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>35.29475793534285</v>
       </c>
       <c r="H3" t="n">
-        <v>0</v>
+        <v>67.30330242070262</v>
       </c>
       <c r="I3" t="n">
-        <v>0</v>
+        <v>218.7461472440725</v>
       </c>
       <c r="J3" t="n">
-        <v>0</v>
+        <v>145.934081760929</v>
       </c>
       <c r="K3" t="n">
-        <v>0</v>
+        <v>87.37612544410197</v>
       </c>
       <c r="L3" t="n">
-        <v>0</v>
+        <v>52.31531391091026</v>
       </c>
       <c r="M3" t="n">
-        <v>0</v>
-      </c>
-      <c r="N3" t="n">
-        <v>0</v>
+        <v>31.32311092631339</v>
       </c>
     </row>
     <row r="4">
@@ -2822,43 +2813,40 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
+        <v>0.07547350508700007</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>0.2178762776774527</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>0.486560627477725</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>0.9935119916566777</v>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>1.95002354818739</v>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>3.754761482483282</v>
       </c>
       <c r="H4" t="n">
-        <v>0</v>
+        <v>7.159925789436452</v>
       </c>
       <c r="I4" t="n">
-        <v>0</v>
+        <v>23.27086672809283</v>
       </c>
       <c r="J4" t="n">
-        <v>0</v>
+        <v>21.31022990537005</v>
       </c>
       <c r="K4" t="n">
-        <v>0</v>
+        <v>12.75922182800743</v>
       </c>
       <c r="L4" t="n">
-        <v>0</v>
+        <v>7.639417424364685</v>
       </c>
       <c r="M4" t="n">
-        <v>0</v>
-      </c>
-      <c r="N4" t="n">
-        <v>0</v>
+        <v>4.574001406228451</v>
       </c>
     </row>
     <row r="5">
@@ -2868,43 +2856,40 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
+        <v>0.1308207421508001</v>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>0.377652214640918</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>0.8433717542947233</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>1.722087452204907</v>
       </c>
       <c r="F5" t="n">
-        <v>0</v>
+        <v>3.380040816858143</v>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>6.508253236304355</v>
       </c>
       <c r="H5" t="n">
-        <v>0</v>
+        <v>12.41053803502318</v>
       </c>
       <c r="I5" t="n">
-        <v>0</v>
+        <v>40.3361689953609</v>
       </c>
       <c r="J5" t="n">
-        <v>0</v>
+        <v>130.3303430025982</v>
       </c>
       <c r="K5" t="n">
-        <v>0</v>
+        <v>97.44760712176192</v>
       </c>
       <c r="L5" t="n">
-        <v>0</v>
+        <v>78.98312356704527</v>
       </c>
       <c r="M5" t="n">
-        <v>0</v>
-      </c>
-      <c r="N5" t="n">
-        <v>0</v>
+        <v>254.875452100176</v>
       </c>
     </row>
     <row r="6">
@@ -2914,43 +2899,40 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0</v>
+        <v>0.2264205152610002</v>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>0.6536288330323581</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>1.459681882433175</v>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>2.980535974970033</v>
       </c>
       <c r="F6" t="n">
-        <v>0</v>
+        <v>5.850070644562171</v>
       </c>
       <c r="G6" t="n">
-        <v>0</v>
+        <v>11.26428444744985</v>
       </c>
       <c r="H6" t="n">
-        <v>0</v>
+        <v>21.47977736830935</v>
       </c>
       <c r="I6" t="n">
-        <v>0</v>
+        <v>69.81260018427848</v>
       </c>
       <c r="J6" t="n">
-        <v>0</v>
+        <v>225.5717475044969</v>
       </c>
       <c r="K6" t="n">
-        <v>0</v>
+        <v>727.52695227904</v>
       </c>
       <c r="L6" t="n">
-        <v>0</v>
+        <v>745.0685771792312</v>
       </c>
       <c r="M6" t="n">
-        <v>0</v>
-      </c>
-      <c r="N6" t="n">
-        <v>0</v>
+        <v>522.8331096749538</v>
       </c>
     </row>
     <row r="7">
@@ -2960,43 +2942,40 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0</v>
+        <v>0.1710732781972001</v>
       </c>
       <c r="C7" t="n">
-        <v>0</v>
+        <v>0.4938528960688927</v>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>1.102870755616177</v>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>2.251960514421802</v>
       </c>
       <c r="F7" t="n">
-        <v>0</v>
+        <v>4.420053375891418</v>
       </c>
       <c r="G7" t="n">
-        <v>0</v>
+        <v>8.510792693628771</v>
       </c>
       <c r="H7" t="n">
-        <v>0</v>
+        <v>16.22916512272262</v>
       </c>
       <c r="I7" t="n">
-        <v>0</v>
+        <v>52.74729791701039</v>
       </c>
       <c r="J7" t="n">
-        <v>0</v>
+        <v>126.1333051200035</v>
       </c>
       <c r="K7" t="n">
-        <v>0</v>
+        <v>90.47756243540104</v>
       </c>
       <c r="L7" t="n">
-        <v>0</v>
+        <v>124.4802158123834</v>
       </c>
       <c r="M7" t="n">
-        <v>0</v>
-      </c>
-      <c r="N7" t="n">
-        <v>0</v>
+        <v>171.5740668880334</v>
       </c>
     </row>
     <row r="8">
@@ -3006,43 +2985,40 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0</v>
+        <v>0.7346087828468006</v>
       </c>
       <c r="C8" t="n">
-        <v>0</v>
+        <v>2.12066243606054</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>4.735856774116524</v>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>9.67018338545833</v>
       </c>
       <c r="F8" t="n">
-        <v>0</v>
+        <v>18.98022920235727</v>
       </c>
       <c r="G8" t="n">
-        <v>0</v>
+        <v>36.54634509617061</v>
       </c>
       <c r="H8" t="n">
-        <v>0</v>
+        <v>69.68994435051478</v>
       </c>
       <c r="I8" t="n">
-        <v>0</v>
+        <v>226.5031028201035</v>
       </c>
       <c r="J8" t="n">
-        <v>0</v>
+        <v>731.8550030145899</v>
       </c>
       <c r="K8" t="n">
-        <v>0</v>
+        <v>579.4341940297862</v>
       </c>
       <c r="L8" t="n">
-        <v>0</v>
+        <v>346.9286558234512</v>
       </c>
       <c r="M8" t="n">
-        <v>0</v>
-      </c>
-      <c r="N8" t="n">
-        <v>0</v>
+        <v>517.3536302639114</v>
       </c>
     </row>
     <row r="9">
@@ -3052,43 +3028,40 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0</v>
+        <v>0.1911995462204001</v>
       </c>
       <c r="C9" t="n">
-        <v>0</v>
+        <v>0.55195323678288</v>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>1.232620256276903</v>
       </c>
       <c r="E9" t="n">
-        <v>0</v>
+        <v>2.51689704553025</v>
       </c>
       <c r="F9" t="n">
-        <v>0</v>
+        <v>4.940059655408055</v>
       </c>
       <c r="G9" t="n">
-        <v>0</v>
+        <v>9.512062422290978</v>
       </c>
       <c r="H9" t="n">
-        <v>0</v>
+        <v>18.13847866657234</v>
       </c>
       <c r="I9" t="n">
-        <v>0</v>
+        <v>58.95286237783515</v>
       </c>
       <c r="J9" t="n">
-        <v>0</v>
+        <v>98.69495579241746</v>
       </c>
       <c r="K9" t="n">
-        <v>0</v>
+        <v>59.09231574941914</v>
       </c>
       <c r="L9" t="n">
-        <v>0</v>
+        <v>40.50522878993385</v>
       </c>
       <c r="M9" t="n">
-        <v>0</v>
-      </c>
-      <c r="N9" t="n">
-        <v>0</v>
+        <v>37.48685578943183</v>
       </c>
     </row>
     <row r="10">
@@ -3098,43 +3071,40 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0</v>
+        <v>0.2264205152610002</v>
       </c>
       <c r="C10" t="n">
-        <v>0</v>
+        <v>0.6536288330323581</v>
       </c>
       <c r="D10" t="n">
-        <v>0</v>
+        <v>1.459681882433175</v>
       </c>
       <c r="E10" t="n">
-        <v>0</v>
+        <v>2.980535974970033</v>
       </c>
       <c r="F10" t="n">
-        <v>0</v>
+        <v>5.850070644562171</v>
       </c>
       <c r="G10" t="n">
-        <v>0</v>
+        <v>11.26428444744985</v>
       </c>
       <c r="H10" t="n">
-        <v>0</v>
+        <v>21.47977736830935</v>
       </c>
       <c r="I10" t="n">
-        <v>0</v>
+        <v>69.81260018427848</v>
       </c>
       <c r="J10" t="n">
-        <v>0</v>
+        <v>172.3086174648732</v>
       </c>
       <c r="K10" t="n">
-        <v>0</v>
+        <v>115.0693755622944</v>
       </c>
       <c r="L10" t="n">
-        <v>0</v>
+        <v>68.89628572423965</v>
       </c>
       <c r="M10" t="n">
-        <v>0</v>
-      </c>
-      <c r="N10" t="n">
-        <v>0</v>
+        <v>68.89628572423965</v>
       </c>
     </row>
     <row r="11">
@@ -3147,40 +3117,37 @@
         <v>0</v>
       </c>
       <c r="C11" t="n">
-        <v>0</v>
+        <v>0.4075911097652372</v>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
+        <v>1.478490414672862</v>
       </c>
       <c r="E11" t="n">
-        <v>0</v>
+        <v>3.499054187459683</v>
       </c>
       <c r="F11" t="n">
-        <v>0</v>
+        <v>7.311436865447026</v>
       </c>
       <c r="G11" t="n">
-        <v>0</v>
+        <v>14.5046083352947</v>
       </c>
       <c r="H11" t="n">
-        <v>0</v>
+        <v>28.07662357221903</v>
       </c>
       <c r="I11" t="n">
-        <v>0</v>
+        <v>92.33279719191833</v>
       </c>
       <c r="J11" t="n">
-        <v>0</v>
+        <v>55.28305638200717</v>
       </c>
       <c r="K11" t="n">
-        <v>0</v>
+        <v>33.1000079699057</v>
       </c>
       <c r="L11" t="n">
-        <v>0</v>
+        <v>19.81819746066729</v>
       </c>
       <c r="M11" t="n">
-        <v>0</v>
-      </c>
-      <c r="N11" t="n">
-        <v>0</v>
+        <v>11.86588688882174</v>
       </c>
     </row>
     <row r="12">
@@ -3190,43 +3157,40 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0</v>
+        <v>0.1408838761624001</v>
       </c>
       <c r="C12" t="n">
-        <v>0</v>
+        <v>0.4067023849979116</v>
       </c>
       <c r="D12" t="n">
-        <v>0</v>
+        <v>0.9082465046250864</v>
       </c>
       <c r="E12" t="n">
-        <v>0</v>
+        <v>1.854555717759131</v>
       </c>
       <c r="F12" t="n">
-        <v>0</v>
+        <v>3.640043956616461</v>
       </c>
       <c r="G12" t="n">
-        <v>0</v>
+        <v>7.008888100635456</v>
       </c>
       <c r="H12" t="n">
-        <v>0</v>
+        <v>13.36519480694803</v>
       </c>
       <c r="I12" t="n">
-        <v>0</v>
+        <v>43.43895122577325</v>
       </c>
       <c r="J12" t="n">
-        <v>0</v>
+        <v>26.00850470064471</v>
       </c>
       <c r="K12" t="n">
-        <v>0</v>
+        <v>15.572252498631</v>
       </c>
       <c r="L12" t="n">
-        <v>0</v>
+        <v>9.323682798077524</v>
       </c>
       <c r="M12" t="n">
-        <v>0</v>
-      </c>
-      <c r="N12" t="n">
-        <v>0</v>
+        <v>5.582433300950461</v>
       </c>
     </row>
     <row r="13">
@@ -3236,43 +3200,40 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0</v>
+        <v>0.5484408036322005</v>
       </c>
       <c r="C13" t="n">
-        <v>0</v>
+        <v>1.583234284456156</v>
       </c>
       <c r="D13" t="n">
-        <v>0</v>
+        <v>3.535673893004802</v>
       </c>
       <c r="E13" t="n">
-        <v>0</v>
+        <v>7.21952047270519</v>
       </c>
       <c r="F13" t="n">
-        <v>0</v>
+        <v>14.17017111682837</v>
       </c>
       <c r="G13" t="n">
-        <v>0</v>
+        <v>27.28460010604518</v>
       </c>
       <c r="H13" t="n">
-        <v>0</v>
+        <v>52.02879406990486</v>
       </c>
       <c r="I13" t="n">
-        <v>0</v>
+        <v>169.1016315574745</v>
       </c>
       <c r="J13" t="n">
-        <v>0</v>
+        <v>149.1628936158218</v>
       </c>
       <c r="K13" t="n">
-        <v>0</v>
+        <v>89.30933437147706</v>
       </c>
       <c r="L13" t="n">
-        <v>0</v>
+        <v>78.00098733300715</v>
       </c>
       <c r="M13" t="n">
-        <v>0</v>
-      </c>
-      <c r="N13" t="n">
-        <v>0</v>
+        <v>46.70207241333626</v>
       </c>
     </row>
     <row r="14">
@@ -3282,43 +3243,40 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0</v>
+        <v>3.205108182694603</v>
       </c>
       <c r="C14" t="n">
-        <v>0</v>
+        <v>9.660070368467727</v>
       </c>
       <c r="D14" t="n">
-        <v>0</v>
+        <v>22.14109839489358</v>
       </c>
       <c r="E14" t="n">
-        <v>0</v>
+        <v>45.69019676647993</v>
       </c>
       <c r="F14" t="n">
-        <v>0</v>
+        <v>90.12243687847155</v>
       </c>
       <c r="G14" t="n">
-        <v>0</v>
+        <v>173.9568126247514</v>
       </c>
       <c r="H14" t="n">
-        <v>0</v>
+        <v>332.1348054302869</v>
       </c>
       <c r="I14" t="n">
-        <v>0</v>
+        <v>1080.56893757826</v>
       </c>
       <c r="J14" t="n">
-        <v>0</v>
+        <v>1932.719793264751</v>
       </c>
       <c r="K14" t="n">
-        <v>0</v>
+        <v>2068.837605351835</v>
       </c>
       <c r="L14" t="n">
-        <v>0</v>
+        <v>2093.103332742566</v>
       </c>
       <c r="M14" t="n">
-        <v>0</v>
-      </c>
-      <c r="N14" t="n">
-        <v>0</v>
+        <v>2069.945119700734</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
check if SSP2 600f is infeasible
</commit_message>
<xml_diff>
--- a/tutorial/dac_scenarios/SSPs/get_report_output.xlsx
+++ b/tutorial/dac_scenarios/SSPs/get_report_output.xlsx
@@ -504,40 +504,40 @@
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>0.05529194511868137</v>
       </c>
       <c r="F2" t="n">
-        <v>0.06106359831030216</v>
+        <v>0.1596163206428224</v>
       </c>
       <c r="G2" t="n">
-        <v>0.2007550520193839</v>
+        <v>0.3564546721448534</v>
       </c>
       <c r="H2" t="n">
-        <v>0.5203186345681103</v>
+        <v>0.727847612935295</v>
       </c>
       <c r="I2" t="n">
-        <v>1.251364669095401</v>
+        <v>1.428588679990762</v>
       </c>
       <c r="J2" t="n">
-        <v>2.923733905713868</v>
+        <v>2.750741012808266</v>
       </c>
       <c r="K2" t="n">
-        <v>6.749510575710191</v>
+        <v>5.245366878708023</v>
       </c>
       <c r="L2" t="n">
-        <v>31.7341499619147</v>
+        <v>17.04825401325482</v>
       </c>
       <c r="M2" t="n">
-        <v>148.5236565666028</v>
+        <v>15.71994196771707</v>
       </c>
       <c r="N2" t="n">
-        <v>190.9782510179102</v>
+        <v>13.57890037051744</v>
       </c>
       <c r="O2" t="n">
-        <v>365.88714785842</v>
+        <v>8.1301892460665</v>
       </c>
       <c r="P2" t="n">
-        <v>248.2556703917938</v>
+        <v>4.867844624618641</v>
       </c>
     </row>
     <row r="3">
@@ -559,37 +559,37 @@
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>0.8609967361752603</v>
+        <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>2.830646233473312</v>
+        <v>0</v>
       </c>
       <c r="H3" t="n">
-        <v>7.336492747410355</v>
+        <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>17.64424183424514</v>
+        <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>41.22464807056552</v>
+        <v>0</v>
       </c>
       <c r="K3" t="n">
-        <v>112.9324179839768</v>
+        <v>0</v>
       </c>
       <c r="L3" t="n">
-        <v>447.4515144629968</v>
+        <v>0</v>
       </c>
       <c r="M3" t="n">
-        <v>376.999479244196</v>
+        <v>0</v>
       </c>
       <c r="N3" t="n">
-        <v>376.9472250815614</v>
+        <v>0</v>
       </c>
       <c r="O3" t="n">
-        <v>236.2274905388118</v>
+        <v>0</v>
       </c>
       <c r="P3" t="n">
-        <v>141.4381246491713</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -611,37 +611,37 @@
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>0.09159539746545324</v>
+        <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>0.3011325780290759</v>
+        <v>0</v>
       </c>
       <c r="H4" t="n">
-        <v>0.7804779518521656</v>
+        <v>0</v>
       </c>
       <c r="I4" t="n">
-        <v>1.877047003643101</v>
+        <v>0</v>
       </c>
       <c r="J4" t="n">
-        <v>4.385600858570802</v>
+        <v>0</v>
       </c>
       <c r="K4" t="n">
-        <v>10.12426586356529</v>
+        <v>0</v>
       </c>
       <c r="L4" t="n">
-        <v>47.60122494287204</v>
+        <v>0</v>
       </c>
       <c r="M4" t="n">
-        <v>222.7854848499042</v>
+        <v>0</v>
       </c>
       <c r="N4" t="n">
-        <v>203.8361451956195</v>
+        <v>0</v>
       </c>
       <c r="O4" t="n">
-        <v>177.4820682082679</v>
+        <v>0</v>
       </c>
       <c r="P4" t="n">
-        <v>286.0082471725104</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -660,40 +660,40 @@
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>0.1437590573085715</v>
       </c>
       <c r="F5" t="n">
-        <v>0.1587653556067856</v>
+        <v>0.4150024336713384</v>
       </c>
       <c r="G5" t="n">
-        <v>0.5219631352503981</v>
+        <v>0.926782147576619</v>
       </c>
       <c r="H5" t="n">
-        <v>1.352828449877087</v>
+        <v>1.892403793631766</v>
       </c>
       <c r="I5" t="n">
-        <v>3.253548139648038</v>
+        <v>3.714330567975981</v>
       </c>
       <c r="J5" t="n">
-        <v>7.601708154856066</v>
+        <v>7.151926633301487</v>
       </c>
       <c r="K5" t="n">
-        <v>17.54872749684649</v>
+        <v>13.63795388464085</v>
       </c>
       <c r="L5" t="n">
-        <v>82.50878990097821</v>
+        <v>44.32546043446251</v>
       </c>
       <c r="M5" t="n">
-        <v>386.1615070731672</v>
+        <v>41.389714838094</v>
       </c>
       <c r="N5" t="n">
-        <v>522.0699265511394</v>
+        <v>35.42955872964427</v>
       </c>
       <c r="O5" t="n">
-        <v>1041.637273995853</v>
+        <v>21.21298555235359</v>
       </c>
       <c r="P5" t="n">
-        <v>1444.532626403087</v>
+        <v>20.58286074629813</v>
       </c>
     </row>
     <row r="6">
@@ -712,40 +712,40 @@
         <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>0.2488137530340661</v>
       </c>
       <c r="F6" t="n">
-        <v>0.2747861923963597</v>
+        <v>0.7182734428927011</v>
       </c>
       <c r="G6" t="n">
-        <v>0.9033977340872273</v>
+        <v>1.60404602465184</v>
       </c>
       <c r="H6" t="n">
-        <v>2.341433855556496</v>
+        <v>3.275314258208827</v>
       </c>
       <c r="I6" t="n">
-        <v>5.631141010929301</v>
+        <v>6.428649059958429</v>
       </c>
       <c r="J6" t="n">
-        <v>13.1568025757124</v>
+        <v>12.37833455763719</v>
       </c>
       <c r="K6" t="n">
-        <v>30.37279759069585</v>
+        <v>23.6041509541861</v>
       </c>
       <c r="L6" t="n">
-        <v>142.8036748286161</v>
+        <v>76.71714305964667</v>
       </c>
       <c r="M6" t="n">
-        <v>668.3564545497123</v>
+        <v>158.1062696695804</v>
       </c>
       <c r="N6" t="n">
-        <v>1055.53791075729</v>
+        <v>203.2149114614893</v>
       </c>
       <c r="O6" t="n">
-        <v>2581.322934920887</v>
+        <v>149.5705981339387</v>
       </c>
       <c r="P6" t="n">
-        <v>5681.368161750633</v>
+        <v>117.3975917819989</v>
       </c>
     </row>
     <row r="7">
@@ -767,37 +767,37 @@
         <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>0.2076162342550273</v>
+        <v>0.1879926134035166</v>
       </c>
       <c r="G7" t="n">
-        <v>0.6825671768659051</v>
+        <v>0.5426954901855964</v>
       </c>
       <c r="H7" t="n">
-        <v>1.769083357531575</v>
+        <v>1.211945885292502</v>
       </c>
       <c r="I7" t="n">
-        <v>4.254639874924362</v>
+        <v>2.474681883980002</v>
       </c>
       <c r="J7" t="n">
-        <v>9.94069527942715</v>
+        <v>4.857201511968591</v>
       </c>
       <c r="K7" t="n">
-        <v>22.94833595741465</v>
+        <v>9.352519443548099</v>
       </c>
       <c r="L7" t="n">
-        <v>107.8961098705099</v>
+        <v>30.63053261173651</v>
       </c>
       <c r="M7" t="n">
-        <v>190.0407599824657</v>
+        <v>18.33963134319247</v>
       </c>
       <c r="N7" t="n">
-        <v>142.8064549565083</v>
+        <v>10.9806147371833</v>
       </c>
       <c r="O7" t="n">
-        <v>200.4860723172174</v>
+        <v>6.574499658696964</v>
       </c>
       <c r="P7" t="n">
-        <v>912.5965719548772</v>
+        <v>3.936395802671987</v>
       </c>
     </row>
     <row r="8">
@@ -816,40 +816,40 @@
         <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>0.8072623987327479</v>
       </c>
       <c r="F8" t="n">
-        <v>0.8915285353304114</v>
+        <v>2.330398281385208</v>
       </c>
       <c r="G8" t="n">
-        <v>2.931023759483005</v>
+        <v>5.204238213314861</v>
       </c>
       <c r="H8" t="n">
-        <v>7.59665206469441</v>
+        <v>10.62657514885531</v>
       </c>
       <c r="I8" t="n">
-        <v>18.26992416879285</v>
+        <v>20.85739472786513</v>
       </c>
       <c r="J8" t="n">
-        <v>42.68651502342247</v>
+        <v>40.16081878700066</v>
       </c>
       <c r="K8" t="n">
-        <v>122.0292511790938</v>
+        <v>76.58235642913714</v>
       </c>
       <c r="L8" t="n">
-        <v>463.3185894439543</v>
+        <v>248.9045085935203</v>
       </c>
       <c r="M8" t="n">
-        <v>1716.782584667756</v>
+        <v>240.8263962367501</v>
       </c>
       <c r="N8" t="n">
-        <v>1593.175830653631</v>
+        <v>226.5323386248103</v>
       </c>
       <c r="O8" t="n">
-        <v>1425.630442832816</v>
+        <v>137.6293227581042</v>
       </c>
       <c r="P8" t="n">
-        <v>866.8990547283489</v>
+        <v>133.1592310797446</v>
       </c>
     </row>
     <row r="9">
@@ -868,40 +868,40 @@
         <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>0</v>
+        <v>0.1941074700677905</v>
       </c>
       <c r="F9" t="n">
-        <v>0.2320416735791481</v>
+        <v>0.5763497281931176</v>
       </c>
       <c r="G9" t="n">
-        <v>0.7628691976736586</v>
+        <v>1.297561195654932</v>
       </c>
       <c r="H9" t="n">
-        <v>1.977210811358819</v>
+        <v>2.658336907240128</v>
       </c>
       <c r="I9" t="n">
-        <v>4.755185742562521</v>
+        <v>5.22583703831401</v>
       </c>
       <c r="J9" t="n">
-        <v>11.1101888417127</v>
+        <v>10.07017462234186</v>
       </c>
       <c r="K9" t="n">
-        <v>25.64814018769872</v>
+        <v>19.21042990178723</v>
       </c>
       <c r="L9" t="n">
-        <v>120.5897698552757</v>
+        <v>62.45673652383566</v>
       </c>
       <c r="M9" t="n">
-        <v>483.2101525812814</v>
+        <v>60.61942377799791</v>
       </c>
       <c r="N9" t="n">
-        <v>463.4473620126933</v>
+        <v>53.57984118059964</v>
       </c>
       <c r="O9" t="n">
-        <v>482.9065430645629</v>
+        <v>33.90046200218654</v>
       </c>
       <c r="P9" t="n">
-        <v>690.903337325185</v>
+        <v>33.73680997185478</v>
       </c>
     </row>
     <row r="10">
@@ -923,37 +923,37 @@
         <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>0.2747861923963597</v>
+        <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>0.9033977340872272</v>
+        <v>0</v>
       </c>
       <c r="H10" t="n">
-        <v>2.341433855556496</v>
+        <v>0.2488137530340661</v>
       </c>
       <c r="I10" t="n">
-        <v>5.631141010929301</v>
+        <v>0.7182734428927011</v>
       </c>
       <c r="J10" t="n">
-        <v>13.1568025757124</v>
+        <v>1.60404602465184</v>
       </c>
       <c r="K10" t="n">
-        <v>30.37279759069585</v>
+        <v>3.275314258208827</v>
       </c>
       <c r="L10" t="n">
-        <v>142.8036748286161</v>
+        <v>8.162511276248772</v>
       </c>
       <c r="M10" t="n">
-        <v>359.2281226747392</v>
+        <v>4.887197018039945</v>
       </c>
       <c r="N10" t="n">
-        <v>215.0831466586222</v>
+        <v>2.926145384036168</v>
       </c>
       <c r="O10" t="n">
-        <v>217.141683929645</v>
+        <v>1.751991331004326</v>
       </c>
       <c r="P10" t="n">
-        <v>139.1021613015882</v>
+        <v>1.048981927097704</v>
       </c>
     </row>
     <row r="11">
@@ -975,37 +975,37 @@
         <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>0.8609967361752603</v>
+        <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>2.830646233473312</v>
+        <v>0</v>
       </c>
       <c r="H11" t="n">
-        <v>7.336492747410355</v>
+        <v>0</v>
       </c>
       <c r="I11" t="n">
-        <v>17.64424183424515</v>
+        <v>0.7796164261734072</v>
       </c>
       <c r="J11" t="n">
-        <v>41.22464807056552</v>
+        <v>2.250590121063797</v>
       </c>
       <c r="K11" t="n">
-        <v>112.9324179839768</v>
+        <v>2.250590121063797</v>
       </c>
       <c r="L11" t="n">
-        <v>447.4515144629969</v>
+        <v>1.34751144056587</v>
       </c>
       <c r="M11" t="n">
-        <v>1286.056207628592</v>
+        <v>0.8068048755131079</v>
       </c>
       <c r="N11" t="n">
-        <v>1244.475811783189</v>
+        <v>0.4830638817273195</v>
       </c>
       <c r="O11" t="n">
-        <v>1019.181029302101</v>
+        <v>0.2892281900020255</v>
       </c>
       <c r="P11" t="n">
-        <v>610.2213300141605</v>
+        <v>0.1731716012232691</v>
       </c>
     </row>
     <row r="12">
@@ -1027,37 +1027,37 @@
         <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>0.170978075268846</v>
+        <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>0.5621141456542748</v>
+        <v>0</v>
       </c>
       <c r="H12" t="n">
-        <v>1.456892176790709</v>
+        <v>0</v>
       </c>
       <c r="I12" t="n">
-        <v>3.503821073467122</v>
+        <v>0</v>
       </c>
       <c r="J12" t="n">
-        <v>8.186454935998828</v>
+        <v>0</v>
       </c>
       <c r="K12" t="n">
-        <v>18.89862961198854</v>
+        <v>0</v>
       </c>
       <c r="L12" t="n">
-        <v>88.85561989336111</v>
+        <v>0</v>
       </c>
       <c r="M12" t="n">
-        <v>83.19083828569634</v>
+        <v>0</v>
       </c>
       <c r="N12" t="n">
-        <v>49.80942788785277</v>
+        <v>0</v>
       </c>
       <c r="O12" t="n">
-        <v>29.82274439878771</v>
+        <v>0</v>
       </c>
       <c r="P12" t="n">
-        <v>28.36242831137264</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -1076,40 +1076,40 @@
         <v>0</v>
       </c>
       <c r="E13" t="n">
-        <v>0</v>
+        <v>0.6026822017936269</v>
       </c>
       <c r="F13" t="n">
-        <v>0.6655932215822935</v>
+        <v>1.739817895006764</v>
       </c>
       <c r="G13" t="n">
-        <v>2.188230067011284</v>
+        <v>3.885355926378902</v>
       </c>
       <c r="H13" t="n">
-        <v>5.6714731167924</v>
+        <v>7.933538980994713</v>
       </c>
       <c r="I13" t="n">
-        <v>13.63987489313986</v>
+        <v>15.5716166118993</v>
       </c>
       <c r="J13" t="n">
-        <v>31.86869957228115</v>
+        <v>29.98307703961009</v>
       </c>
       <c r="K13" t="n">
-        <v>90.08422938294635</v>
+        <v>57.17449897791743</v>
       </c>
       <c r="L13" t="n">
-        <v>345.9022345848699</v>
+        <v>70.06569857895894</v>
       </c>
       <c r="M13" t="n">
-        <v>1409.850336946786</v>
+        <v>41.95092191276472</v>
       </c>
       <c r="N13" t="n">
-        <v>1244.134849117668</v>
+        <v>25.11756658427699</v>
       </c>
       <c r="O13" t="n">
-        <v>1079.014836201758</v>
+        <v>15.03881493778619</v>
       </c>
       <c r="P13" t="n">
-        <v>670.7316184561707</v>
+        <v>9.004294025622512</v>
       </c>
     </row>
     <row r="14">
@@ -1128,40 +1128,40 @@
         <v>0</v>
       </c>
       <c r="E14" t="n">
-        <v>0</v>
+        <v>2.051916826055484</v>
       </c>
       <c r="F14" t="n">
-        <v>4.750747948541507</v>
+        <v>6.127450715195469</v>
       </c>
       <c r="G14" t="n">
-        <v>15.61874304710807</v>
+        <v>13.81713366990761</v>
       </c>
       <c r="H14" t="n">
-        <v>40.48078976939898</v>
+        <v>28.57477634019261</v>
       </c>
       <c r="I14" t="n">
-        <v>97.35617125562214</v>
+        <v>57.19898843904972</v>
       </c>
       <c r="J14" t="n">
-        <v>227.4664978645389</v>
+        <v>111.2069103103838</v>
       </c>
       <c r="K14" t="n">
-        <v>600.6415214046094</v>
+        <v>210.3331808491975</v>
       </c>
       <c r="L14" t="n">
-        <v>2468.916867036962</v>
+        <v>559.6583565322301</v>
       </c>
       <c r="M14" t="n">
-        <v>7331.185585050899</v>
+        <v>582.6463016396496</v>
       </c>
       <c r="N14" t="n">
-        <v>7302.302341673685</v>
+        <v>571.8429409542847</v>
       </c>
       <c r="O14" t="n">
-        <v>8856.74026756913</v>
+        <v>374.098091810139</v>
       </c>
       <c r="P14" t="n">
-        <v>11720.4193324589</v>
+        <v>323.9071815611306</v>
       </c>
     </row>
   </sheetData>
@@ -1251,40 +1251,40 @@
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>0.01105838902373627</v>
       </c>
       <c r="F2" t="n">
-        <v>0.01221271966206043</v>
+        <v>0.02086487510482822</v>
       </c>
       <c r="G2" t="n">
-        <v>0.02793829074181634</v>
+        <v>0.03936767030040619</v>
       </c>
       <c r="H2" t="n">
-        <v>0.07299564044173805</v>
+        <v>0.07427858815808831</v>
       </c>
       <c r="I2" t="n">
-        <v>0.1493390026355257</v>
+        <v>0.1512066024348298</v>
       </c>
       <c r="J2" t="n">
-        <v>0.3624121380655098</v>
+        <v>0.2852953416683288</v>
       </c>
       <c r="K2" t="n">
-        <v>0.7651553339992647</v>
+        <v>0.5382928434803577</v>
       </c>
       <c r="L2" t="n">
-        <v>2.609631260159083</v>
+        <v>1.255229658142431</v>
       </c>
       <c r="M2" t="n">
-        <v>11.83836889971621</v>
+        <v>0.04761811688909753</v>
       </c>
       <c r="N2" t="n">
-        <v>4.508948014096386</v>
+        <v>0.07105245497644007</v>
       </c>
       <c r="O2" t="n">
-        <v>20.31661902508299</v>
+        <v>0.7419664696302101</v>
       </c>
       <c r="P2" t="n">
-        <v>0</v>
+        <v>0.04254172941796646</v>
       </c>
     </row>
     <row r="3">
@@ -1306,37 +1306,37 @@
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>0.1721993472350521</v>
+        <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>0.3939298994596104</v>
+        <v>0</v>
       </c>
       <c r="H3" t="n">
-        <v>1.074765643243593</v>
+        <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>2.83597572641606</v>
+        <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>7.052636410902473</v>
+        <v>0</v>
       </c>
       <c r="K3" t="n">
-        <v>15.53384718589288</v>
+        <v>0</v>
       </c>
       <c r="L3" t="n">
-        <v>33.451909647902</v>
+        <v>0</v>
       </c>
       <c r="M3" t="n">
-        <v>0.6996345421782534</v>
+        <v>0</v>
       </c>
       <c r="N3" t="n">
-        <v>6.891155581888235</v>
+        <v>0</v>
       </c>
       <c r="O3" t="n">
-        <v>16.26503916370504</v>
+        <v>0</v>
       </c>
       <c r="P3" t="n">
-        <v>1.780231347316784</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -1358,37 +1358,37 @@
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>0.01831907949309065</v>
+        <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>0.04190743611272452</v>
+        <v>0</v>
       </c>
       <c r="H4" t="n">
-        <v>0.09586907476461796</v>
+        <v>0</v>
       </c>
       <c r="I4" t="n">
-        <v>0.2376328898512777</v>
+        <v>0</v>
       </c>
       <c r="J4" t="n">
-        <v>0.5017107709855403</v>
+        <v>0</v>
       </c>
       <c r="K4" t="n">
-        <v>1.189640437111622</v>
+        <v>0</v>
       </c>
       <c r="L4" t="n">
-        <v>3.914446890238624</v>
+        <v>0</v>
       </c>
       <c r="M4" t="n">
-        <v>17.55122070036548</v>
+        <v>0</v>
       </c>
       <c r="N4" t="n">
-        <v>0.1984786235894613</v>
+        <v>0</v>
       </c>
       <c r="O4" t="n">
-        <v>4.863700378645546</v>
+        <v>0</v>
       </c>
       <c r="P4" t="n">
-        <v>23.7371243386055</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -1407,40 +1407,40 @@
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>0.02875181146171431</v>
       </c>
       <c r="F5" t="n">
-        <v>0.03175307112135712</v>
+        <v>0.05424867527255337</v>
       </c>
       <c r="G5" t="n">
-        <v>0.0726395559287225</v>
+        <v>0.1023559427810561</v>
       </c>
       <c r="H5" t="n">
-        <v>0.1661730629253378</v>
+        <v>0.1931243292110295</v>
       </c>
       <c r="I5" t="n">
-        <v>0.4118970090755474</v>
+        <v>0.3931371663305572</v>
       </c>
       <c r="J5" t="n">
-        <v>0.8696320030416056</v>
+        <v>0.7417678883376546</v>
       </c>
       <c r="K5" t="n">
-        <v>2.293380223885199</v>
+        <v>1.39956139304893</v>
       </c>
       <c r="L5" t="n">
-        <v>6.66937287663442</v>
+        <v>3.26359711117032</v>
       </c>
       <c r="M5" t="n">
-        <v>30.39758782738582</v>
+        <v>0.1052423468070983</v>
       </c>
       <c r="N5" t="n">
-        <v>15.58187280702504</v>
+        <v>0.1570353385780007</v>
       </c>
       <c r="O5" t="n">
-        <v>63.67714295444553</v>
+        <v>1.964263216657359</v>
       </c>
       <c r="P5" t="n">
-        <v>65.47723918074817</v>
+        <v>0.09402285797245463</v>
       </c>
     </row>
     <row r="6">
@@ -1459,40 +1459,40 @@
         <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>0.04976275060681323</v>
       </c>
       <c r="F6" t="n">
-        <v>0.05495723847927195</v>
+        <v>0.09389193797172701</v>
       </c>
       <c r="G6" t="n">
-        <v>0.1257223083381735</v>
+        <v>0.1771545163518279</v>
       </c>
       <c r="H6" t="n">
-        <v>0.2876072242938538</v>
+        <v>0.3342536467113974</v>
       </c>
       <c r="I6" t="n">
-        <v>0.6579414310745613</v>
+        <v>0.6804297109567335</v>
       </c>
       <c r="J6" t="n">
-        <v>1.78127885454015</v>
+        <v>1.28382903750748</v>
       </c>
       <c r="K6" t="n">
-        <v>4.931264277021096</v>
+        <v>2.422317795661608</v>
       </c>
       <c r="L6" t="n">
-        <v>12.00522899516665</v>
+        <v>5.633072717490311</v>
       </c>
       <c r="M6" t="n">
-        <v>52.62859067795183</v>
+        <v>8.58706054710906</v>
       </c>
       <c r="N6" t="n">
-        <v>42.23473540765932</v>
+        <v>5.53603348448003</v>
       </c>
       <c r="O6" t="n">
-        <v>174.9238041916434</v>
+        <v>1.076878691517947</v>
       </c>
       <c r="P6" t="n">
-        <v>352.0909387914712</v>
+        <v>5.126847002201915</v>
       </c>
     </row>
     <row r="7">
@@ -1514,37 +1514,37 @@
         <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>0.04152324685100547</v>
+        <v>0.03759852268070332</v>
       </c>
       <c r="G7" t="n">
-        <v>0.136513435373181</v>
+        <v>0.07094057535641596</v>
       </c>
       <c r="H7" t="n">
-        <v>0.217303236133134</v>
+        <v>0.1338500790213811</v>
       </c>
       <c r="I7" t="n">
-        <v>0.4971113034785575</v>
+        <v>0.2525471997375001</v>
       </c>
       <c r="J7" t="n">
-        <v>1.137211080900558</v>
+        <v>0.514102448278421</v>
       </c>
       <c r="K7" t="n">
-        <v>3.224035430278696</v>
+        <v>0.9700041616723176</v>
       </c>
       <c r="L7" t="n">
-        <v>8.551882561385447</v>
+        <v>2.190938116753216</v>
       </c>
       <c r="M7" t="n">
-        <v>9.58056967329027</v>
+        <v>0</v>
       </c>
       <c r="N7" t="n">
-        <v>3.153992129356284</v>
+        <v>1.038271059729859</v>
       </c>
       <c r="O7" t="n">
-        <v>16.82040090488971</v>
+        <v>0.03579872946725225</v>
       </c>
       <c r="P7" t="n">
-        <v>72.10864664609537</v>
+        <v>0.3722055585573534</v>
       </c>
     </row>
     <row r="8">
@@ -1563,40 +1563,40 @@
         <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>0.1614524797465496</v>
       </c>
       <c r="F8" t="n">
-        <v>0.1783057070660823</v>
+        <v>0.3046271765304921</v>
       </c>
       <c r="G8" t="n">
-        <v>0.4078990448305188</v>
+        <v>0.5747679863859306</v>
       </c>
       <c r="H8" t="n">
-        <v>1.115898433001736</v>
+        <v>1.084467387108089</v>
       </c>
       <c r="I8" t="n">
-        <v>2.918708458738028</v>
+        <v>2.207616395548515</v>
       </c>
       <c r="J8" t="n">
-        <v>7.219041486699777</v>
+        <v>4.165311988357599</v>
       </c>
       <c r="K8" t="n">
-        <v>15.86854723113428</v>
+        <v>7.859075514813224</v>
       </c>
       <c r="L8" t="n">
-        <v>34.12893382648605</v>
+        <v>17.7431737022993</v>
       </c>
       <c r="M8" t="n">
-        <v>126.5206769203277</v>
+        <v>0.2474047986986314</v>
       </c>
       <c r="N8" t="n">
-        <v>3.790151449531429</v>
+        <v>3.528702400943838</v>
       </c>
       <c r="O8" t="n">
-        <v>19.39402016376695</v>
+        <v>9.98682507616795</v>
       </c>
       <c r="P8" t="n">
-        <v>64.01074413462308</v>
+        <v>0.2978358107747358</v>
       </c>
     </row>
     <row r="9">
@@ -1615,40 +1615,40 @@
         <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>0</v>
+        <v>0.0388214940135581</v>
       </c>
       <c r="F9" t="n">
-        <v>0.04640833471582963</v>
+        <v>0.07644845162506543</v>
       </c>
       <c r="G9" t="n">
-        <v>0.1061655048189021</v>
+        <v>0.1442422934923629</v>
       </c>
       <c r="H9" t="n">
-        <v>0.2428683227370321</v>
+        <v>0.2721551423170391</v>
       </c>
       <c r="I9" t="n">
-        <v>0.6020033209565702</v>
+        <v>0.5523215202283346</v>
       </c>
       <c r="J9" t="n">
-        <v>1.33664832365489</v>
+        <v>1.045315968430635</v>
       </c>
       <c r="K9" t="n">
-        <v>3.710305773988566</v>
+        <v>1.972293349381438</v>
       </c>
       <c r="L9" t="n">
-        <v>9.535499936705849</v>
+        <v>4.460708233363363</v>
       </c>
       <c r="M9" t="n">
-        <v>36.34893588161194</v>
+        <v>0</v>
       </c>
       <c r="N9" t="n">
-        <v>2.178584883555112</v>
+        <v>0.4723196494102408</v>
       </c>
       <c r="O9" t="n">
-        <v>12.45670121987707</v>
+        <v>2.917726550808414</v>
       </c>
       <c r="P9" t="n">
-        <v>54.45504762908634</v>
+        <v>0.02441902216341692</v>
       </c>
     </row>
     <row r="10">
@@ -1670,37 +1670,37 @@
         <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>0.05495723847927195</v>
+        <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>0.1806795468174455</v>
+        <v>0</v>
       </c>
       <c r="H10" t="n">
-        <v>0.2876072242938538</v>
+        <v>0.04976275060681323</v>
       </c>
       <c r="I10" t="n">
-        <v>0.657941431074561</v>
+        <v>0.09389193797172701</v>
       </c>
       <c r="J10" t="n">
-        <v>1.5939529361415</v>
+        <v>0.1771545163518279</v>
       </c>
       <c r="K10" t="n">
-        <v>4.554484944644932</v>
+        <v>0.3342536467113974</v>
       </c>
       <c r="L10" t="n">
-        <v>11.24308772379202</v>
+        <v>0.4887197018039945</v>
       </c>
       <c r="M10" t="n">
-        <v>21.84815325979013</v>
+        <v>0</v>
       </c>
       <c r="N10" t="n">
-        <v>0.09216139966207149</v>
+        <v>0.2284444358209828</v>
       </c>
       <c r="O10" t="n">
-        <v>4.281428311757693</v>
+        <v>0.03842101081093909</v>
       </c>
       <c r="P10" t="n">
-        <v>9.628787818401124</v>
+        <v>0.08189411429438404</v>
       </c>
     </row>
     <row r="11">
@@ -1722,37 +1722,37 @@
         <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>0.1721993472350521</v>
+        <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>0.3939298994596104</v>
+        <v>0</v>
       </c>
       <c r="H11" t="n">
-        <v>1.073368650022461</v>
+        <v>0</v>
       </c>
       <c r="I11" t="n">
-        <v>2.835975726416061</v>
+        <v>0.1559232852346815</v>
       </c>
       <c r="J11" t="n">
-        <v>7.052636410902475</v>
+        <v>0.2941947389780779</v>
       </c>
       <c r="K11" t="n">
-        <v>15.53384718589289</v>
+        <v>0</v>
       </c>
       <c r="L11" t="n">
-        <v>33.45190964790201</v>
+        <v>0</v>
       </c>
       <c r="M11" t="n">
-        <v>87.89722233294604</v>
+        <v>0.0806804875513108</v>
       </c>
       <c r="N11" t="n">
-        <v>4.870595119743252</v>
+        <v>0</v>
       </c>
       <c r="O11" t="n">
-        <v>10.93872552195452</v>
+        <v>0.02892281900020256</v>
       </c>
       <c r="P11" t="n">
-        <v>47.88139868855487</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -1774,37 +1774,37 @@
         <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>0.0341956150537692</v>
+        <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>0.112422829130855</v>
+        <v>0</v>
       </c>
       <c r="H12" t="n">
-        <v>0.1789556062272869</v>
+        <v>0</v>
       </c>
       <c r="I12" t="n">
-        <v>0.5218086084661375</v>
+        <v>0</v>
       </c>
       <c r="J12" t="n">
-        <v>0.9365267725063414</v>
+        <v>0</v>
       </c>
       <c r="K12" t="n">
-        <v>2.49277179418978</v>
+        <v>0</v>
       </c>
       <c r="L12" t="n">
-        <v>7.072697931474744</v>
+        <v>0</v>
       </c>
       <c r="M12" t="n">
         <v>0</v>
       </c>
       <c r="N12" t="n">
-        <v>0.7243620635392501</v>
+        <v>0</v>
       </c>
       <c r="O12" t="n">
-        <v>2.501811823945455</v>
+        <v>0</v>
       </c>
       <c r="P12" t="n">
-        <v>0.2178982493030656</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -1823,40 +1823,40 @@
         <v>0</v>
       </c>
       <c r="E13" t="n">
-        <v>0</v>
+        <v>0.1205364403587254</v>
       </c>
       <c r="F13" t="n">
-        <v>0.1331186443164587</v>
+        <v>0.2274271386426275</v>
       </c>
       <c r="G13" t="n">
-        <v>0.3045273690857981</v>
+        <v>0.4291076062744276</v>
       </c>
       <c r="H13" t="n">
-        <v>0.6966486099562234</v>
+        <v>0.8096366109231623</v>
       </c>
       <c r="I13" t="n">
-        <v>1.874244000424753</v>
+        <v>1.648151966539643</v>
       </c>
       <c r="J13" t="n">
-        <v>5.118250391383079</v>
+        <v>3.109719224184783</v>
       </c>
       <c r="K13" t="n">
-        <v>11.64310596213304</v>
+        <v>5.438284387661469</v>
       </c>
       <c r="L13" t="n">
-        <v>25.58180052019235</v>
+        <v>1.600412105269389</v>
       </c>
       <c r="M13" t="n">
-        <v>107.5533946354113</v>
+        <v>0.6688125948725911</v>
       </c>
       <c r="N13" t="n">
-        <v>3.773574610639929</v>
+        <v>0.997955817856817</v>
       </c>
       <c r="O13" t="n">
-        <v>19.32695760495586</v>
+        <v>0.5059256759218019</v>
       </c>
       <c r="P13" t="n">
-        <v>45.58677285084775</v>
+        <v>0.5975130118787235</v>
       </c>
     </row>
     <row r="14">
@@ -1875,40 +1875,40 @@
         <v>0</v>
       </c>
       <c r="E14" t="n">
-        <v>0</v>
+        <v>0.4103833652110969</v>
       </c>
       <c r="F14" t="n">
-        <v>0.9501495897083014</v>
+        <v>0.815106777827997</v>
       </c>
       <c r="G14" t="n">
-        <v>2.304275120097358</v>
+        <v>1.537936590942427</v>
       </c>
       <c r="H14" t="n">
-        <v>5.510060728040867</v>
+        <v>2.951528534057</v>
       </c>
       <c r="I14" t="n">
-        <v>14.20057890860764</v>
+        <v>6.135225784982522</v>
       </c>
       <c r="J14" t="n">
-        <v>34.9619375797239</v>
+        <v>11.61669115209481</v>
       </c>
       <c r="K14" t="n">
-        <v>81.74038578017225</v>
+        <v>20.93408309243074</v>
       </c>
       <c r="L14" t="n">
-        <v>188.2164018180392</v>
+        <v>36.63585134629233</v>
       </c>
       <c r="M14" t="n">
-        <v>502.864355350975</v>
+        <v>9.73681889192779</v>
       </c>
       <c r="N14" t="n">
-        <v>87.99861209028579</v>
+        <v>12.02981464179621</v>
       </c>
       <c r="O14" t="n">
-        <v>365.7663512646697</v>
+        <v>17.29672823998208</v>
       </c>
       <c r="P14" t="n">
-        <v>736.9748296750535</v>
+        <v>6.637279107260948</v>
       </c>
     </row>
   </sheetData>
@@ -1998,40 +1998,40 @@
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>39.86214284453398</v>
       </c>
       <c r="F2" t="n">
-        <v>37.61517655914613</v>
+        <v>68.29554974478945</v>
       </c>
       <c r="G2" t="n">
-        <v>71.29851797311531</v>
+        <v>114.1792745700474</v>
       </c>
       <c r="H2" t="n">
-        <v>151.2225134557333</v>
+        <v>196.9668497107533</v>
       </c>
       <c r="I2" t="n">
-        <v>266.0671310096367</v>
+        <v>369.6343227191189</v>
       </c>
       <c r="J2" t="n">
-        <v>590.0649088364355</v>
+        <v>661.9607388769967</v>
       </c>
       <c r="K2" t="n">
-        <v>1178.19270633184</v>
+        <v>1278.98379610933</v>
       </c>
       <c r="L2" t="n">
-        <v>3670.253750227101</v>
+        <v>2797.023729318964</v>
       </c>
       <c r="M2" t="n">
-        <v>16141.55000507309</v>
+        <v>100.6217618475533</v>
       </c>
       <c r="N2" t="n">
-        <v>6150.20509122747</v>
+        <v>150.1408218215421</v>
       </c>
       <c r="O2" t="n">
-        <v>26814.46916648508</v>
+        <v>1632.326233186462</v>
       </c>
       <c r="P2" t="n">
-        <v>0</v>
+        <v>88.13221187467148</v>
       </c>
     </row>
     <row r="3">
@@ -2053,37 +2053,37 @@
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>483.7806345077944</v>
+        <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>916.9926986853973</v>
+        <v>0</v>
       </c>
       <c r="H3" t="n">
-        <v>2156.764459266215</v>
+        <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>4894.292309744973</v>
+        <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>10977.57197987261</v>
+        <v>0</v>
       </c>
       <c r="K3" t="n">
-        <v>21654.1921916308</v>
+        <v>0</v>
       </c>
       <c r="L3" t="n">
-        <v>42578.78042451402</v>
+        <v>0</v>
       </c>
       <c r="M3" t="n">
-        <v>853.549705331989</v>
+        <v>0</v>
       </c>
       <c r="N3" t="n">
-        <v>8357.990923653228</v>
+        <v>0</v>
       </c>
       <c r="O3" t="n">
-        <v>19583.72522458909</v>
+        <v>0</v>
       </c>
       <c r="P3" t="n">
-        <v>2018.429039316547</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -2105,37 +2105,37 @@
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>56.86552165719917</v>
+        <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>107.7870101593491</v>
+        <v>0</v>
       </c>
       <c r="H4" t="n">
-        <v>212.5670182648022</v>
+        <v>0</v>
       </c>
       <c r="I4" t="n">
-        <v>453.1295088303089</v>
+        <v>0</v>
       </c>
       <c r="J4" t="n">
-        <v>921.4431037488965</v>
+        <v>0</v>
       </c>
       <c r="K4" t="n">
-        <v>1948.191713505729</v>
+        <v>0</v>
       </c>
       <c r="L4" t="n">
-        <v>5786.33029407983</v>
+        <v>0</v>
       </c>
       <c r="M4" t="n">
-        <v>25208.06384911874</v>
+        <v>0</v>
       </c>
       <c r="N4" t="n">
-        <v>272.8492558394497</v>
+        <v>0</v>
       </c>
       <c r="O4" t="n">
-        <v>6637.792181722465</v>
+        <v>0</v>
       </c>
       <c r="P4" t="n">
-        <v>32423.14360892083</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -2154,40 +2154,40 @@
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>110.9256046750557</v>
       </c>
       <c r="F5" t="n">
-        <v>104.6729028355386</v>
+        <v>190.0481161186478</v>
       </c>
       <c r="G5" t="n">
-        <v>186.8308176095384</v>
+        <v>317.7301612318728</v>
       </c>
       <c r="H5" t="n">
-        <v>384.7325572568179</v>
+        <v>548.105679875714</v>
       </c>
       <c r="I5" t="n">
-        <v>793.1219405710829</v>
+        <v>1028.592740640767</v>
       </c>
       <c r="J5" t="n">
-        <v>1590.24357536621</v>
+        <v>1880.666823139359</v>
       </c>
       <c r="K5" t="n">
-        <v>3780.024370276115</v>
+        <v>3526.35272568641</v>
       </c>
       <c r="L5" t="n">
-        <v>9961.207291042592</v>
+        <v>7799.312831696379</v>
       </c>
       <c r="M5" t="n">
-        <v>43908.55016726482</v>
+        <v>238.0170346810957</v>
       </c>
       <c r="N5" t="n">
-        <v>22723.30443980244</v>
+        <v>355.1525290193985</v>
       </c>
       <c r="O5" t="n">
-        <v>89699.53624409564</v>
+        <v>4625.08991953196</v>
       </c>
       <c r="P5" t="n">
-        <v>92504.33943644563</v>
+        <v>208.4734688116119</v>
       </c>
     </row>
     <row r="6">
@@ -2206,40 +2206,40 @@
         <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>179.3796428004029</v>
       </c>
       <c r="F6" t="n">
-        <v>159.3941824358253</v>
+        <v>307.3299738515526</v>
       </c>
       <c r="G6" t="n">
-        <v>302.1272268479466</v>
+        <v>513.8067355652132</v>
       </c>
       <c r="H6" t="n">
-        <v>595.8258203167265</v>
+        <v>886.3508236983899</v>
       </c>
       <c r="I6" t="n">
-        <v>1232.955480828268</v>
+        <v>1672.719661950729</v>
       </c>
       <c r="J6" t="n">
-        <v>3056.674514390898</v>
+        <v>3093.614056095011</v>
       </c>
       <c r="K6" t="n">
-        <v>7533.577141772175</v>
+        <v>5735.779357100485</v>
       </c>
       <c r="L6" t="n">
-        <v>16707.96300030322</v>
+        <v>12639.98476960104</v>
       </c>
       <c r="M6" t="n">
-        <v>70858.04912785527</v>
+        <v>19237.56615487933</v>
       </c>
       <c r="N6" t="n">
-        <v>57519.64712266632</v>
+        <v>12422.85913917319</v>
       </c>
       <c r="O6" t="n">
-        <v>230396.4732498073</v>
+        <v>2350.467959323159</v>
       </c>
       <c r="P6" t="n">
-        <v>464760.039204742</v>
+        <v>11279.06340484421</v>
       </c>
     </row>
     <row r="7">
@@ -2261,37 +2261,37 @@
         <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>143.621116113729</v>
+        <v>138.2049736570903</v>
       </c>
       <c r="G7" t="n">
-        <v>391.2301729416744</v>
+        <v>231.0566895369785</v>
       </c>
       <c r="H7" t="n">
-        <v>505.5475366362721</v>
+        <v>423.2798143982842</v>
       </c>
       <c r="I7" t="n">
-        <v>994.5987159075153</v>
+        <v>693.2986735065595</v>
       </c>
       <c r="J7" t="n">
-        <v>2063.628371283736</v>
+        <v>1339.564097813024</v>
       </c>
       <c r="K7" t="n">
-        <v>5276.893024540383</v>
+        <v>2437.211157282198</v>
       </c>
       <c r="L7" t="n">
-        <v>12875.80329701574</v>
+        <v>5213.754755200701</v>
       </c>
       <c r="M7" t="n">
-        <v>13825.70166812554</v>
+        <v>0</v>
       </c>
       <c r="N7" t="n">
-        <v>4757.585750636288</v>
+        <v>2463.80722931935</v>
       </c>
       <c r="O7" t="n">
-        <v>24470.08059241344</v>
+        <v>88.44363220694997</v>
       </c>
       <c r="P7" t="n">
-        <v>104838.9903908536</v>
+        <v>865.9217718033158</v>
       </c>
     </row>
     <row r="8">
@@ -2310,40 +2310,40 @@
         <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>688.0690180002125</v>
       </c>
       <c r="F8" t="n">
-        <v>638.8152330332834</v>
+        <v>1178.864167688006</v>
       </c>
       <c r="G8" t="n">
-        <v>1197.554782043976</v>
+        <v>1970.873006897621</v>
       </c>
       <c r="H8" t="n">
-        <v>2902.457403729681</v>
+        <v>3480.18283528256</v>
       </c>
       <c r="I8" t="n">
-        <v>6528.754753459119</v>
+        <v>6649.937750715355</v>
       </c>
       <c r="J8" t="n">
-        <v>14566.08090396187</v>
+        <v>12033.27555999994</v>
       </c>
       <c r="K8" t="n">
-        <v>28676.27555309628</v>
+        <v>22076.81428615932</v>
       </c>
       <c r="L8" t="n">
-        <v>56315.10611948904</v>
+        <v>46944.5066127752</v>
       </c>
       <c r="M8" t="n">
-        <v>203358.3302579241</v>
+        <v>656.3711408079164</v>
       </c>
       <c r="N8" t="n">
-        <v>6064.579007654865</v>
+        <v>9284.75129883386</v>
       </c>
       <c r="O8" t="n">
-        <v>29895.53672674207</v>
+        <v>25975.78195723822</v>
       </c>
       <c r="P8" t="n">
-        <v>99895.35932872517</v>
+        <v>729.4826208725113</v>
       </c>
     </row>
     <row r="9">
@@ -2362,40 +2362,40 @@
         <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>0</v>
+        <v>176.8211217892161</v>
       </c>
       <c r="F9" t="n">
-        <v>180.6091799723164</v>
+        <v>316.1829368252248</v>
       </c>
       <c r="G9" t="n">
-        <v>322.369589912238</v>
+        <v>528.6074787162196</v>
       </c>
       <c r="H9" t="n">
-        <v>635.7458325041764</v>
+        <v>911.8830909404908</v>
       </c>
       <c r="I9" t="n">
-        <v>1401.148254047273</v>
+        <v>1811.714552125527</v>
       </c>
       <c r="J9" t="n">
-        <v>2898.194721108746</v>
+        <v>3240.905900442397</v>
       </c>
       <c r="K9" t="n">
-        <v>7180.317807464191</v>
+        <v>5915.414481050653</v>
       </c>
       <c r="L9" t="n">
-        <v>16786.10339208317</v>
+        <v>12638.04348186237</v>
       </c>
       <c r="M9" t="n">
-        <v>62376.03743158367</v>
+        <v>0</v>
       </c>
       <c r="N9" t="n">
-        <v>3754.758211175871</v>
+        <v>1332.474426182715</v>
       </c>
       <c r="O9" t="n">
-        <v>20619.47944218864</v>
+        <v>8110.73828119956</v>
       </c>
       <c r="P9" t="n">
-        <v>89992.61820877693</v>
+        <v>63.92061096839087</v>
       </c>
     </row>
     <row r="10">
@@ -2417,37 +2417,37 @@
         <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>160.3461627122109</v>
+        <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>436.7899280127891</v>
+        <v>0</v>
       </c>
       <c r="H10" t="n">
-        <v>564.4198413278319</v>
+        <v>132.7455529588759</v>
       </c>
       <c r="I10" t="n">
-        <v>1154.388966329427</v>
+        <v>230.8957526195319</v>
       </c>
       <c r="J10" t="n">
-        <v>2584.044108703627</v>
+        <v>389.3791860268568</v>
       </c>
       <c r="K10" t="n">
-        <v>6574.181178240042</v>
+        <v>708.4388855654279</v>
       </c>
       <c r="L10" t="n">
-        <v>14787.36781797493</v>
+        <v>991.5684790341954</v>
       </c>
       <c r="M10" t="n">
-        <v>27922.88552521476</v>
+        <v>0</v>
       </c>
       <c r="N10" t="n">
-        <v>112.1355281493738</v>
+        <v>457.2810852911591</v>
       </c>
       <c r="O10" t="n">
-        <v>5178.299523371239</v>
+        <v>80.07084652840788</v>
       </c>
       <c r="P10" t="n">
-        <v>12040.05582449102</v>
+        <v>160.7145408437063</v>
       </c>
     </row>
     <row r="11">
@@ -2469,37 +2469,37 @@
         <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>483.7806345077944</v>
+        <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>916.9926986853973</v>
+        <v>0</v>
       </c>
       <c r="H11" t="n">
-        <v>2153.961071059573</v>
+        <v>0</v>
       </c>
       <c r="I11" t="n">
-        <v>4894.009435551223</v>
+        <v>347.6792524852219</v>
       </c>
       <c r="J11" t="n">
-        <v>10977.05594543848</v>
+        <v>622.6424352973517</v>
       </c>
       <c r="K11" t="n">
-        <v>21653.26071637739</v>
+        <v>0</v>
       </c>
       <c r="L11" t="n">
-        <v>42577.05775620909</v>
+        <v>0</v>
       </c>
       <c r="M11" t="n">
-        <v>109229.5148178882</v>
+        <v>155.5086234622787</v>
       </c>
       <c r="N11" t="n">
-        <v>5866.18119557629</v>
+        <v>0</v>
       </c>
       <c r="O11" t="n">
-        <v>13170.64120000307</v>
+        <v>54.65456110231143</v>
       </c>
       <c r="P11" t="n">
-        <v>57538.80101464647</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -2521,37 +2521,37 @@
         <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>99.77094568759786</v>
+        <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>271.7803996524021</v>
+        <v>0</v>
       </c>
       <c r="H12" t="n">
-        <v>372.9502836907025</v>
+        <v>0</v>
       </c>
       <c r="I12" t="n">
-        <v>892.6178565534756</v>
+        <v>0</v>
       </c>
       <c r="J12" t="n">
-        <v>1519.298984869117</v>
+        <v>0</v>
       </c>
       <c r="K12" t="n">
-        <v>3636.521801093777</v>
+        <v>0</v>
       </c>
       <c r="L12" t="n">
-        <v>9354.466963991417</v>
+        <v>0</v>
       </c>
       <c r="M12" t="n">
         <v>0</v>
       </c>
       <c r="N12" t="n">
-        <v>890.1364654783389</v>
+        <v>0</v>
       </c>
       <c r="O12" t="n">
-        <v>3128.322545970982</v>
+        <v>0</v>
       </c>
       <c r="P12" t="n">
-        <v>256.5709444869675</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -2570,40 +2570,40 @@
         <v>0</v>
       </c>
       <c r="E13" t="n">
-        <v>0</v>
+        <v>533.7417673137425</v>
       </c>
       <c r="F13" t="n">
-        <v>477.5512649582656</v>
+        <v>914.4562940987495</v>
       </c>
       <c r="G13" t="n">
-        <v>898.9755888345475</v>
+        <v>1623.532473143449</v>
       </c>
       <c r="H13" t="n">
-        <v>1866.927203553883</v>
+        <v>2793.567253699799</v>
       </c>
       <c r="I13" t="n">
-        <v>4356.034509426168</v>
+        <v>5117.232912502095</v>
       </c>
       <c r="J13" t="n">
-        <v>10706.13334152594</v>
+        <v>9028.771118248318</v>
       </c>
       <c r="K13" t="n">
-        <v>21801.83866385588</v>
+        <v>15013.67173823803</v>
       </c>
       <c r="L13" t="n">
-        <v>43729.58530084234</v>
+        <v>4274.372535385646</v>
       </c>
       <c r="M13" t="n">
-        <v>177987.6497242149</v>
+        <v>1736.073843799446</v>
       </c>
       <c r="N13" t="n">
-        <v>6165.058458890851</v>
+        <v>2590.449112249075</v>
       </c>
       <c r="O13" t="n">
-        <v>30529.00900254263</v>
+        <v>1367.267377102996</v>
       </c>
       <c r="P13" t="n">
-        <v>73919.12723085738</v>
+        <v>1520.585855608614</v>
       </c>
     </row>
     <row r="14">
@@ -2622,40 +2622,40 @@
         <v>0</v>
       </c>
       <c r="E14" t="n">
-        <v>0</v>
+        <v>1728.799297423164</v>
       </c>
       <c r="F14" t="n">
-        <v>3026.822954980701</v>
+        <v>3113.38201198406</v>
       </c>
       <c r="G14" t="n">
-        <v>6020.72943135837</v>
+        <v>5299.785819661402</v>
       </c>
       <c r="H14" t="n">
-        <v>12503.12154106242</v>
+        <v>9373.081900564866</v>
       </c>
       <c r="I14" t="n">
-        <v>27861.11886225847</v>
+        <v>17921.7056192649</v>
       </c>
       <c r="J14" t="n">
-        <v>62450.43445910655</v>
+        <v>32290.77991593925</v>
       </c>
       <c r="K14" t="n">
-        <v>130893.4668681846</v>
+        <v>56692.66642719185</v>
       </c>
       <c r="L14" t="n">
-        <v>275130.0254077725</v>
+        <v>93298.56719487447</v>
       </c>
       <c r="M14" t="n">
-        <v>751669.8822795951</v>
+        <v>22124.15855947763</v>
       </c>
       <c r="N14" t="n">
-        <v>122634.4314507508</v>
+        <v>29056.91564189029</v>
       </c>
       <c r="O14" t="n">
-        <v>500123.3650999317</v>
+        <v>44284.84076742003</v>
       </c>
       <c r="P14" t="n">
-        <v>1030187.474232263</v>
+        <v>14916.29448562704</v>
       </c>
     </row>
   </sheetData>
@@ -2727,40 +2727,40 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>0.05031567005800005</v>
       </c>
       <c r="C2" t="n">
-        <v>0.05556787446237497</v>
+        <v>0.1452508517849684</v>
       </c>
       <c r="D2" t="n">
-        <v>0.1826870973376393</v>
+        <v>0.3243737516518166</v>
       </c>
       <c r="E2" t="n">
-        <v>0.4734899574569804</v>
+        <v>0.6623413277711184</v>
       </c>
       <c r="F2" t="n">
-        <v>1.138741848876815</v>
+        <v>1.300015698791594</v>
       </c>
       <c r="G2" t="n">
-        <v>2.66059785419962</v>
+        <v>2.503174321655522</v>
       </c>
       <c r="H2" t="n">
-        <v>6.142054623896274</v>
+        <v>4.773283859624301</v>
       </c>
       <c r="I2" t="n">
-        <v>28.87807646534237</v>
+        <v>15.51391115206189</v>
       </c>
       <c r="J2" t="n">
-        <v>135.1565274756085</v>
+        <v>14.30514719062254</v>
       </c>
       <c r="K2" t="n">
-        <v>173.7902084262982</v>
+        <v>12.35679933717087</v>
       </c>
       <c r="L2" t="n">
-        <v>332.9573045511622</v>
+        <v>7.398472213920517</v>
       </c>
       <c r="M2" t="n">
-        <v>225.9126600565324</v>
+        <v>4.429738608402963</v>
       </c>
     </row>
     <row r="3">
@@ -2773,37 +2773,37 @@
         <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>0.783507029919487</v>
+        <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>2.575888072460714</v>
+        <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>6.676208400143423</v>
+        <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>16.05626006916308</v>
+        <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>37.51442974421462</v>
+        <v>0</v>
       </c>
       <c r="H3" t="n">
-        <v>86.60297019693743</v>
+        <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>407.1808781613272</v>
+        <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>343.0695261122184</v>
+        <v>0</v>
       </c>
       <c r="K3" t="n">
-        <v>343.0219748242209</v>
+        <v>0</v>
       </c>
       <c r="L3" t="n">
-        <v>214.9670163903187</v>
+        <v>0</v>
       </c>
       <c r="M3" t="n">
-        <v>128.7086934307459</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -2816,37 +2816,37 @@
         <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>0.08335181169356246</v>
+        <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>0.274030646006459</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>0.7102349361854707</v>
+        <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>1.708112773315222</v>
+        <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>3.99089678129943</v>
+        <v>0</v>
       </c>
       <c r="H4" t="n">
-        <v>9.213081935844412</v>
+        <v>0</v>
       </c>
       <c r="I4" t="n">
-        <v>43.31711469801356</v>
+        <v>0</v>
       </c>
       <c r="J4" t="n">
-        <v>202.7347912134128</v>
+        <v>0</v>
       </c>
       <c r="K4" t="n">
-        <v>185.4908921280137</v>
+        <v>0</v>
       </c>
       <c r="L4" t="n">
-        <v>161.5086820695238</v>
+        <v>0</v>
       </c>
       <c r="M4" t="n">
-        <v>260.2675049269845</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -2856,40 +2856,40 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
+        <v>0.1308207421508001</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1444764736021749</v>
+        <v>0.377652214640918</v>
       </c>
       <c r="D5" t="n">
-        <v>0.4749864530778622</v>
+        <v>0.8433717542947233</v>
       </c>
       <c r="E5" t="n">
-        <v>1.231073889388149</v>
+        <v>1.722087452204907</v>
       </c>
       <c r="F5" t="n">
-        <v>2.960728807079715</v>
+        <v>3.380040816858143</v>
       </c>
       <c r="G5" t="n">
-        <v>6.917554420919014</v>
+        <v>6.508253236304355</v>
       </c>
       <c r="H5" t="n">
-        <v>15.96934202213031</v>
+        <v>12.41053803502318</v>
       </c>
       <c r="I5" t="n">
-        <v>75.08299880989017</v>
+        <v>40.33616899536089</v>
       </c>
       <c r="J5" t="n">
-        <v>351.4069714365821</v>
+        <v>37.66464050266554</v>
       </c>
       <c r="K5" t="n">
-        <v>475.0836331615369</v>
+        <v>32.24089844397629</v>
       </c>
       <c r="L5" t="n">
-        <v>947.8899193362264</v>
+        <v>19.30381685264177</v>
       </c>
       <c r="M5" t="n">
-        <v>1314.524690026809</v>
+        <v>18.7304032791313</v>
       </c>
     </row>
     <row r="6">
@@ -2899,40 +2899,40 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0</v>
+        <v>0.2264205152610002</v>
       </c>
       <c r="C6" t="n">
-        <v>0.2500554350806873</v>
+        <v>0.6536288330323581</v>
       </c>
       <c r="D6" t="n">
-        <v>0.822091938019377</v>
+        <v>1.459681882433175</v>
       </c>
       <c r="E6" t="n">
-        <v>2.130704808556412</v>
+        <v>2.980535974970033</v>
       </c>
       <c r="F6" t="n">
-        <v>5.124338319945665</v>
+        <v>5.850070644562171</v>
       </c>
       <c r="G6" t="n">
-        <v>11.97269034389829</v>
+        <v>11.26428444744985</v>
       </c>
       <c r="H6" t="n">
-        <v>27.63924580753323</v>
+        <v>21.47977736830935</v>
       </c>
       <c r="I6" t="n">
-        <v>129.9513440940406</v>
+        <v>69.81260018427847</v>
       </c>
       <c r="J6" t="n">
-        <v>608.2043736402384</v>
+        <v>143.8767053993182</v>
       </c>
       <c r="K6" t="n">
-        <v>960.5394987891337</v>
+        <v>184.9255694299553</v>
       </c>
       <c r="L6" t="n">
-        <v>2349.003870778007</v>
+        <v>136.1092443018842</v>
       </c>
       <c r="M6" t="n">
-        <v>5170.045027193077</v>
+        <v>106.831808521619</v>
       </c>
     </row>
     <row r="7">
@@ -2945,37 +2945,37 @@
         <v>0</v>
       </c>
       <c r="C7" t="n">
-        <v>0.1889307731720749</v>
+        <v>0.1710732781972001</v>
       </c>
       <c r="D7" t="n">
-        <v>0.6211361309479737</v>
+        <v>0.4938528960688927</v>
       </c>
       <c r="E7" t="n">
-        <v>1.609865855353733</v>
+        <v>1.102870755616177</v>
       </c>
       <c r="F7" t="n">
-        <v>3.87172228618117</v>
+        <v>2.251960514421802</v>
       </c>
       <c r="G7" t="n">
-        <v>9.046032704278707</v>
+        <v>4.420053375891418</v>
       </c>
       <c r="H7" t="n">
-        <v>20.88298572124733</v>
+        <v>8.510792693628771</v>
       </c>
       <c r="I7" t="n">
-        <v>98.18545998216403</v>
+        <v>27.87378467668022</v>
       </c>
       <c r="J7" t="n">
-        <v>172.9370915840438</v>
+        <v>16.68906452230515</v>
       </c>
       <c r="K7" t="n">
-        <v>129.9538740104225</v>
+        <v>9.992359410836801</v>
       </c>
       <c r="L7" t="n">
-        <v>182.4423258086679</v>
+        <v>5.982794689414238</v>
       </c>
       <c r="M7" t="n">
-        <v>830.4628804789384</v>
+        <v>3.582120180431509</v>
       </c>
     </row>
     <row r="8">
@@ -2985,40 +2985,40 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0</v>
+        <v>0.7346087828468006</v>
       </c>
       <c r="C8" t="n">
-        <v>0.8112909671506745</v>
+        <v>2.12066243606054</v>
       </c>
       <c r="D8" t="n">
-        <v>2.667231621129534</v>
+        <v>4.735856774116524</v>
       </c>
       <c r="E8" t="n">
-        <v>6.912953378871914</v>
+        <v>9.67018338545833</v>
       </c>
       <c r="F8" t="n">
-        <v>16.62563099360149</v>
+        <v>18.98022920235727</v>
       </c>
       <c r="G8" t="n">
-        <v>38.84472867131445</v>
+        <v>36.5463450961706</v>
       </c>
       <c r="H8" t="n">
-        <v>89.67399750888558</v>
+        <v>69.68994435051479</v>
       </c>
       <c r="I8" t="n">
-        <v>421.6199163939985</v>
+        <v>226.5031028201035</v>
       </c>
       <c r="J8" t="n">
-        <v>1562.272152047658</v>
+        <v>219.1520205754426</v>
       </c>
       <c r="K8" t="n">
-        <v>1449.790005894805</v>
+        <v>206.1444281485774</v>
       </c>
       <c r="L8" t="n">
-        <v>1297.323702977862</v>
+        <v>125.2426837098748</v>
       </c>
       <c r="M8" t="n">
-        <v>788.8781398027977</v>
+        <v>121.1749002825676</v>
       </c>
     </row>
     <row r="9">
@@ -3028,40 +3028,40 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0</v>
+        <v>0.1766377977616894</v>
       </c>
       <c r="C9" t="n">
-        <v>0.2111579229570248</v>
+        <v>0.524478252655737</v>
       </c>
       <c r="D9" t="n">
-        <v>0.6942109698830293</v>
+        <v>1.180780688045989</v>
       </c>
       <c r="E9" t="n">
-        <v>1.799261838336525</v>
+        <v>2.419086585588516</v>
       </c>
       <c r="F9" t="n">
-        <v>4.327219025731894</v>
+        <v>4.755511704865749</v>
       </c>
       <c r="G9" t="n">
-        <v>10.11027184595855</v>
+        <v>9.16385890633109</v>
       </c>
       <c r="H9" t="n">
-        <v>23.33980757080584</v>
+        <v>17.48149121062638</v>
       </c>
       <c r="I9" t="n">
-        <v>109.7366905683009</v>
+        <v>56.83563023669046</v>
       </c>
       <c r="J9" t="n">
-        <v>439.7212388489661</v>
+        <v>55.16367563797809</v>
       </c>
       <c r="K9" t="n">
-        <v>421.737099431551</v>
+        <v>48.75765547434567</v>
       </c>
       <c r="L9" t="n">
-        <v>439.4449541887523</v>
+        <v>30.84942042198976</v>
       </c>
       <c r="M9" t="n">
-        <v>628.7220369659185</v>
+        <v>30.70049707438785</v>
       </c>
     </row>
     <row r="10">
@@ -3074,37 +3074,37 @@
         <v>0</v>
       </c>
       <c r="C10" t="n">
-        <v>0.2500554350806873</v>
+        <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>0.8220919380193769</v>
+        <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>2.130704808556412</v>
+        <v>0.2264205152610002</v>
       </c>
       <c r="F10" t="n">
-        <v>5.124338319945664</v>
+        <v>0.6536288330323581</v>
       </c>
       <c r="G10" t="n">
-        <v>11.97269034389829</v>
+        <v>1.459681882433175</v>
       </c>
       <c r="H10" t="n">
-        <v>27.63924580753323</v>
+        <v>2.980535974970033</v>
       </c>
       <c r="I10" t="n">
-        <v>129.9513440940406</v>
+        <v>7.427885261386383</v>
       </c>
       <c r="J10" t="n">
-        <v>326.8975916340127</v>
+        <v>4.447349286416349</v>
       </c>
       <c r="K10" t="n">
-        <v>195.7256634593462</v>
+        <v>2.662792299472913</v>
       </c>
       <c r="L10" t="n">
-        <v>197.598932375977</v>
+        <v>1.594312111213937</v>
       </c>
       <c r="M10" t="n">
-        <v>126.5829667844452</v>
+        <v>0.9545735536589105</v>
       </c>
     </row>
     <row r="11">
@@ -3117,37 +3117,37 @@
         <v>0</v>
       </c>
       <c r="C11" t="n">
-        <v>0.783507029919487</v>
+        <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>2.575888072460714</v>
+        <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>6.676208400143423</v>
+        <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>16.05626006916308</v>
+        <v>0.7094509478178006</v>
       </c>
       <c r="G11" t="n">
-        <v>37.51442974421462</v>
+        <v>2.048037010168055</v>
       </c>
       <c r="H11" t="n">
-        <v>86.60297019693743</v>
+        <v>2.048037010168055</v>
       </c>
       <c r="I11" t="n">
-        <v>407.1808781613273</v>
+        <v>1.226235410914942</v>
       </c>
       <c r="J11" t="n">
-        <v>1170.311148942019</v>
+        <v>0.7341924367169282</v>
       </c>
       <c r="K11" t="n">
-        <v>1132.472988722702</v>
+        <v>0.4395881323718608</v>
       </c>
       <c r="L11" t="n">
-        <v>927.4547366649122</v>
+        <v>0.2631976529018433</v>
       </c>
       <c r="M11" t="n">
-        <v>555.3014103128862</v>
+        <v>0.1575861571131749</v>
       </c>
     </row>
     <row r="12">
@@ -3160,37 +3160,37 @@
         <v>0</v>
       </c>
       <c r="C12" t="n">
-        <v>0.1555900484946499</v>
+        <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>0.5115238725453901</v>
+        <v>0</v>
       </c>
       <c r="E12" t="n">
-        <v>1.325771880879545</v>
+        <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>3.188477176855081</v>
+        <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>7.449673991758935</v>
+        <v>0</v>
       </c>
       <c r="H12" t="n">
-        <v>17.19775294690957</v>
+        <v>0</v>
       </c>
       <c r="I12" t="n">
-        <v>80.8586141029586</v>
+        <v>0</v>
       </c>
       <c r="J12" t="n">
-        <v>75.70366283998368</v>
+        <v>0</v>
       </c>
       <c r="K12" t="n">
-        <v>45.32657937794603</v>
+        <v>0</v>
       </c>
       <c r="L12" t="n">
-        <v>27.13869740289682</v>
+        <v>0</v>
       </c>
       <c r="M12" t="n">
-        <v>25.8098097633491</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -3200,40 +3200,40 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0</v>
+        <v>0.5484408036322005</v>
       </c>
       <c r="C13" t="n">
-        <v>0.6056898316398871</v>
+        <v>1.583234284456156</v>
       </c>
       <c r="D13" t="n">
-        <v>1.991289360980268</v>
+        <v>3.535673893004802</v>
       </c>
       <c r="E13" t="n">
-        <v>5.161040536281085</v>
+        <v>7.21952047270519</v>
       </c>
       <c r="F13" t="n">
-        <v>12.41228615275728</v>
+        <v>14.17017111682837</v>
       </c>
       <c r="G13" t="n">
-        <v>29.00051661077585</v>
+        <v>27.28460010604518</v>
       </c>
       <c r="H13" t="n">
-        <v>66.94839540046935</v>
+        <v>52.02879406990486</v>
       </c>
       <c r="I13" t="n">
-        <v>314.7710334722316</v>
+        <v>63.75978570685265</v>
       </c>
       <c r="J13" t="n">
-        <v>1282.963806621576</v>
+        <v>38.17533894061589</v>
       </c>
       <c r="K13" t="n">
-        <v>1132.162712697078</v>
+        <v>22.85698559169206</v>
       </c>
       <c r="L13" t="n">
-        <v>981.9035009436002</v>
+        <v>13.68532159338543</v>
       </c>
       <c r="M13" t="n">
-        <v>610.3657727951156</v>
+        <v>8.193907563316486</v>
       </c>
     </row>
     <row r="14">
@@ -3243,40 +3243,40 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0</v>
+        <v>1.867244311710491</v>
       </c>
       <c r="C14" t="n">
-        <v>4.323180633172772</v>
+        <v>5.575980150827878</v>
       </c>
       <c r="D14" t="n">
-        <v>14.21305617286834</v>
+        <v>12.57359163961592</v>
       </c>
       <c r="E14" t="n">
-        <v>36.83751869015308</v>
+        <v>26.00304646957527</v>
       </c>
       <c r="F14" t="n">
-        <v>88.59411584261618</v>
+        <v>52.05107947953525</v>
       </c>
       <c r="G14" t="n">
-        <v>206.9945130567304</v>
+        <v>101.1982883824492</v>
       </c>
       <c r="H14" t="n">
-        <v>477.85184973913</v>
+        <v>191.4031945727697</v>
       </c>
       <c r="I14" t="n">
-        <v>2246.714349003636</v>
+        <v>509.2891044443294</v>
       </c>
       <c r="J14" t="n">
-        <v>6671.378882396319</v>
+        <v>530.2081344920812</v>
       </c>
       <c r="K14" t="n">
-        <v>6645.095130923055</v>
+        <v>520.377076268399</v>
       </c>
       <c r="L14" t="n">
-        <v>8059.633643487907</v>
+        <v>340.4292635472265</v>
       </c>
       <c r="M14" t="n">
-        <v>10665.5815925376</v>
+        <v>294.7555352206288</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add default ssp runner
</commit_message>
<xml_diff>
--- a/tutorial/dac_scenarios/SSPs/get_report_output.xlsx
+++ b/tutorial/dac_scenarios/SSPs/get_report_output.xlsx
@@ -504,40 +504,40 @@
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>0.05529194511868137</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0.1596163206428224</v>
+        <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>0.3564546721448534</v>
+        <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>0.727847612935295</v>
+        <v>0</v>
       </c>
       <c r="I2" t="n">
-        <v>1.428588679990762</v>
+        <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>2.750741012808266</v>
+        <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>5.245366878708023</v>
+        <v>0</v>
       </c>
       <c r="L2" t="n">
-        <v>17.04825401325482</v>
+        <v>0</v>
       </c>
       <c r="M2" t="n">
-        <v>55.08467582527396</v>
+        <v>0.1443401756517689</v>
       </c>
       <c r="N2" t="n">
-        <v>177.6622594088009</v>
+        <v>0.609496178833564</v>
       </c>
       <c r="O2" t="n">
-        <v>352.5889261723968</v>
+        <v>0.4651560031817951</v>
       </c>
       <c r="P2" t="n">
-        <v>534.3927044336097</v>
+        <v>0.2785060816134256</v>
       </c>
     </row>
     <row r="3">
@@ -611,37 +611,37 @@
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>0.08293791767802204</v>
+        <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>0.2394244809642337</v>
+        <v>0</v>
       </c>
       <c r="H4" t="n">
-        <v>0.5346820082172803</v>
+        <v>0</v>
       </c>
       <c r="I4" t="n">
-        <v>1.091771419402942</v>
+        <v>0</v>
       </c>
       <c r="J4" t="n">
-        <v>1.00883350172492</v>
+        <v>0</v>
       </c>
       <c r="K4" t="n">
-        <v>0.7806161327461169</v>
+        <v>0</v>
       </c>
       <c r="L4" t="n">
-        <v>0.4673837140405101</v>
+        <v>0</v>
       </c>
       <c r="M4" t="n">
-        <v>0.2798398943944808</v>
+        <v>0.123328842472441</v>
       </c>
       <c r="N4" t="n">
-        <v>0.1675504818465426</v>
+        <v>0.123328842472441</v>
       </c>
       <c r="O4" t="n">
-        <v>0.1003186626687145</v>
+        <v>0.123328842472441</v>
       </c>
       <c r="P4" t="n">
-        <v>0.06006448903475355</v>
+        <v>0.07384153366176154</v>
       </c>
     </row>
     <row r="5">
@@ -660,40 +660,40 @@
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>0.1437590573085715</v>
+        <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>0.4150024336713384</v>
+        <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>0.926782147576619</v>
+        <v>0</v>
       </c>
       <c r="H5" t="n">
-        <v>1.892403793631766</v>
+        <v>0</v>
       </c>
       <c r="I5" t="n">
-        <v>3.71433056797598</v>
+        <v>0.08160003499428663</v>
       </c>
       <c r="J5" t="n">
-        <v>7.151926633301487</v>
+        <v>0.2977213148354964</v>
       </c>
       <c r="K5" t="n">
-        <v>13.63795388464086</v>
+        <v>0.7054971221165923</v>
       </c>
       <c r="L5" t="n">
-        <v>44.32546043446252</v>
+        <v>2.648845647112834</v>
       </c>
       <c r="M5" t="n">
-        <v>28.95828515658352</v>
+        <v>8.911552676494299</v>
       </c>
       <c r="N5" t="n">
-        <v>21.41196108276629</v>
+        <v>29.09398461362708</v>
       </c>
       <c r="O5" t="n">
-        <v>17.338395020245</v>
+        <v>33.60329123522269</v>
       </c>
       <c r="P5" t="n">
-        <v>52.49709297743644</v>
+        <v>72.26226733660984</v>
       </c>
     </row>
     <row r="6">
@@ -712,40 +712,40 @@
         <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>0.2488137530340661</v>
+        <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>0.7182734428927011</v>
+        <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>1.60404602465184</v>
+        <v>0.007689137962905424</v>
       </c>
       <c r="H6" t="n">
-        <v>3.275314258208827</v>
+        <v>0.2633215536653745</v>
       </c>
       <c r="I6" t="n">
-        <v>6.428649059958429</v>
+        <v>0.7456466387142859</v>
       </c>
       <c r="J6" t="n">
-        <v>12.37833455763719</v>
+        <v>1.655693539566667</v>
       </c>
       <c r="K6" t="n">
-        <v>23.6041509541861</v>
+        <v>3.372762353574215</v>
       </c>
       <c r="L6" t="n">
-        <v>76.71714305964667</v>
+        <v>11.51871983628528</v>
       </c>
       <c r="M6" t="n">
-        <v>147.7156347642708</v>
+        <v>37.77018452819678</v>
       </c>
       <c r="N6" t="n">
-        <v>207.9405716000085</v>
+        <v>122.3691282292045</v>
       </c>
       <c r="O6" t="n">
-        <v>235.2969991286237</v>
+        <v>130.6177595407937</v>
       </c>
       <c r="P6" t="n">
-        <v>258.9188392855017</v>
+        <v>197.1508646876741</v>
       </c>
     </row>
     <row r="7">
@@ -764,40 +764,40 @@
         <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>0.1879926134035166</v>
+        <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>0.5426954901855964</v>
+        <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>1.211945885292502</v>
+        <v>0</v>
       </c>
       <c r="H7" t="n">
-        <v>2.474681883980002</v>
+        <v>0</v>
       </c>
       <c r="I7" t="n">
-        <v>4.857201511968591</v>
+        <v>0</v>
       </c>
       <c r="J7" t="n">
-        <v>9.352519443548099</v>
+        <v>0</v>
       </c>
       <c r="K7" t="n">
-        <v>17.83424738760727</v>
+        <v>0</v>
       </c>
       <c r="L7" t="n">
-        <v>57.96406364506638</v>
+        <v>0</v>
       </c>
       <c r="M7" t="n">
-        <v>55.98778054650798</v>
+        <v>0</v>
       </c>
       <c r="N7" t="n">
-        <v>70.15166009003735</v>
+        <v>0</v>
       </c>
       <c r="O7" t="n">
-        <v>113.9323336862493</v>
+        <v>0</v>
       </c>
       <c r="P7" t="n">
-        <v>133.3057504840596</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -816,40 +816,40 @@
         <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>0.8072623987327479</v>
+        <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>2.330398281385208</v>
+        <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>5.204238213314861</v>
+        <v>0</v>
       </c>
       <c r="H8" t="n">
-        <v>10.62657514885531</v>
+        <v>0</v>
       </c>
       <c r="I8" t="n">
-        <v>20.85739472786513</v>
+        <v>0.7243974030836892</v>
       </c>
       <c r="J8" t="n">
-        <v>40.16081878700066</v>
+        <v>2.174049306767965</v>
       </c>
       <c r="K8" t="n">
-        <v>76.58235642913714</v>
+        <v>4.90924028720152</v>
       </c>
       <c r="L8" t="n">
-        <v>248.9045085935203</v>
+        <v>17.92806638244432</v>
       </c>
       <c r="M8" t="n">
-        <v>308.7817861713759</v>
+        <v>59.8830181845816</v>
       </c>
       <c r="N8" t="n">
-        <v>344.3864149612558</v>
+        <v>195.0886018403048</v>
       </c>
       <c r="O8" t="n">
-        <v>314.2588935590917</v>
+        <v>274.6042503599529</v>
       </c>
       <c r="P8" t="n">
-        <v>336.4154646274392</v>
+        <v>344.8637851316872</v>
       </c>
     </row>
     <row r="9">
@@ -868,40 +868,40 @@
         <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>0.2101093914509891</v>
+        <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>0.6065420184427253</v>
+        <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>1.354527754150443</v>
+        <v>0</v>
       </c>
       <c r="H9" t="n">
-        <v>2.76582092915412</v>
+        <v>0</v>
       </c>
       <c r="I9" t="n">
-        <v>5.428636983964894</v>
+        <v>0.1346204224996666</v>
       </c>
       <c r="J9" t="n">
-        <v>10.4528158486714</v>
+        <v>0.4641100687635453</v>
       </c>
       <c r="K9" t="n">
-        <v>19.93239413909048</v>
+        <v>1.085788353265342</v>
       </c>
       <c r="L9" t="n">
-        <v>59.57723083307092</v>
+        <v>4.0475944832092</v>
       </c>
       <c r="M9" t="n">
-        <v>57.26342999625638</v>
+        <v>13.59242076170723</v>
       </c>
       <c r="N9" t="n">
-        <v>63.61884222289123</v>
+        <v>44.35193191459739</v>
       </c>
       <c r="O9" t="n">
-        <v>60.95899113761698</v>
+        <v>52.05223871328284</v>
       </c>
       <c r="P9" t="n">
-        <v>61.06477125841224</v>
+        <v>66.91712191984693</v>
       </c>
     </row>
     <row r="10">
@@ -920,40 +920,40 @@
         <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>0.2488137530340661</v>
+        <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>0.7182734428927011</v>
+        <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>1.60404602465184</v>
+        <v>0</v>
       </c>
       <c r="H10" t="n">
-        <v>3.275314258208827</v>
+        <v>0</v>
       </c>
       <c r="I10" t="n">
-        <v>6.428649059958429</v>
+        <v>0</v>
       </c>
       <c r="J10" t="n">
-        <v>12.37833455763719</v>
+        <v>0</v>
       </c>
       <c r="K10" t="n">
-        <v>23.6041509541861</v>
+        <v>0</v>
       </c>
       <c r="L10" t="n">
-        <v>76.71714305964667</v>
+        <v>0</v>
       </c>
       <c r="M10" t="n">
-        <v>167.3564811048098</v>
+        <v>0</v>
       </c>
       <c r="N10" t="n">
-        <v>152.9369108196454</v>
+        <v>0</v>
       </c>
       <c r="O10" t="n">
-        <v>98.98620702956441</v>
+        <v>0</v>
       </c>
       <c r="P10" t="n">
-        <v>82.22020079458756</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -972,40 +972,40 @@
         <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>0.7796164261734072</v>
+        <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>2.250590121063797</v>
+        <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>5.026010877242434</v>
+        <v>0</v>
       </c>
       <c r="H11" t="n">
-        <v>10.26265134238766</v>
+        <v>0</v>
       </c>
       <c r="I11" t="n">
-        <v>20.14310038786975</v>
+        <v>0</v>
       </c>
       <c r="J11" t="n">
-        <v>38.78544828059653</v>
+        <v>0</v>
       </c>
       <c r="K11" t="n">
-        <v>40.4971259167386</v>
+        <v>0</v>
       </c>
       <c r="L11" t="n">
-        <v>24.2471252193393</v>
+        <v>0.3129708696330907</v>
       </c>
       <c r="M11" t="n">
-        <v>14.51764953915692</v>
+        <v>3.043788008281825</v>
       </c>
       <c r="N11" t="n">
-        <v>8.692253050010272</v>
+        <v>3.759663850826343</v>
       </c>
       <c r="O11" t="n">
-        <v>5.204372986248615</v>
+        <v>2.251049626608942</v>
       </c>
       <c r="P11" t="n">
-        <v>3.116050352441396</v>
+        <v>1.347786563509534</v>
       </c>
     </row>
     <row r="12">
@@ -1027,37 +1027,37 @@
         <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>0.00860380813163082</v>
+        <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>0.1710510389204377</v>
+        <v>0</v>
       </c>
       <c r="H12" t="n">
-        <v>0.4775551033242489</v>
+        <v>0</v>
       </c>
       <c r="I12" t="n">
-        <v>1.055864385913317</v>
+        <v>0</v>
       </c>
       <c r="J12" t="n">
-        <v>2.147013460817798</v>
+        <v>0</v>
       </c>
       <c r="K12" t="n">
-        <v>4.205784328777256</v>
+        <v>0</v>
       </c>
       <c r="L12" t="n">
-        <v>13.9578690491505</v>
+        <v>0</v>
       </c>
       <c r="M12" t="n">
-        <v>45.38529894339614</v>
+        <v>0</v>
       </c>
       <c r="N12" t="n">
-        <v>27.17385497578784</v>
+        <v>0</v>
       </c>
       <c r="O12" t="n">
-        <v>16.2699907555108</v>
+        <v>0</v>
       </c>
       <c r="P12" t="n">
-        <v>9.741444466391256</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -1076,40 +1076,40 @@
         <v>0</v>
       </c>
       <c r="E13" t="n">
-        <v>0.6026822017936269</v>
+        <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>1.739817895006764</v>
+        <v>0</v>
       </c>
       <c r="G13" t="n">
-        <v>3.885355926378902</v>
+        <v>0</v>
       </c>
       <c r="H13" t="n">
-        <v>7.933538980994713</v>
+        <v>0</v>
       </c>
       <c r="I13" t="n">
-        <v>15.5716166118993</v>
+        <v>0</v>
       </c>
       <c r="J13" t="n">
-        <v>29.98307703961008</v>
+        <v>0.2804855394687544</v>
       </c>
       <c r="K13" t="n">
-        <v>57.17449897791742</v>
+        <v>1.131899951066534</v>
       </c>
       <c r="L13" t="n">
-        <v>120.9225153030742</v>
+        <v>5.221010675546056</v>
       </c>
       <c r="M13" t="n">
-        <v>123.7269220271792</v>
+        <v>18.39873054860206</v>
       </c>
       <c r="N13" t="n">
-        <v>74.07987859593879</v>
+        <v>60.86573933199426</v>
       </c>
       <c r="O13" t="n">
-        <v>44.35435976968309</v>
+        <v>56.35092140171584</v>
       </c>
       <c r="P13" t="n">
-        <v>26.55659361037794</v>
+        <v>43.17320152865984</v>
       </c>
     </row>
     <row r="14">
@@ -1128,40 +1128,40 @@
         <v>0</v>
       </c>
       <c r="E14" t="n">
-        <v>3.284341540049673</v>
+        <v>0</v>
       </c>
       <c r="F14" t="n">
-        <v>9.572751171993309</v>
+        <v>0</v>
       </c>
       <c r="G14" t="n">
-        <v>21.58388304528897</v>
+        <v>0.007689137962905424</v>
       </c>
       <c r="H14" t="n">
-        <v>44.24638531989805</v>
+        <v>0.2633215536653745</v>
       </c>
       <c r="I14" t="n">
-        <v>87.00580339676752</v>
+        <v>1.686264499291928</v>
       </c>
       <c r="J14" t="n">
-        <v>166.5498631233536</v>
+        <v>4.872059769402428</v>
       </c>
       <c r="K14" t="n">
-        <v>283.0986459837354</v>
+        <v>11.2051880672242</v>
       </c>
       <c r="L14" t="n">
-        <v>740.8486969242728</v>
+        <v>41.67720789423078</v>
       </c>
       <c r="M14" t="n">
-        <v>1005.057783969205</v>
+        <v>141.867363725988</v>
       </c>
       <c r="N14" t="n">
-        <v>1148.222157288989</v>
+        <v>456.2618748018605</v>
       </c>
       <c r="O14" t="n">
-        <v>1259.289787907899</v>
+        <v>550.0679957232312</v>
       </c>
       <c r="P14" t="n">
-        <v>1498.288976779292</v>
+        <v>726.0673747832627</v>
       </c>
     </row>
   </sheetData>
@@ -1251,40 +1251,40 @@
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>0.01105838902373627</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0.02086487510482822</v>
+        <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>0.03936767030040619</v>
+        <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>0.07427858815808831</v>
+        <v>0</v>
       </c>
       <c r="I2" t="n">
-        <v>0.1512066024348298</v>
+        <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>0.2852953416683288</v>
+        <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>0.5382928434803577</v>
+        <v>0</v>
       </c>
       <c r="L2" t="n">
-        <v>1.255229658142431</v>
+        <v>0</v>
       </c>
       <c r="M2" t="n">
-        <v>3.984091502644787</v>
+        <v>0.01443401756517689</v>
       </c>
       <c r="N2" t="n">
-        <v>12.39233156922279</v>
+        <v>0.04651560031817951</v>
       </c>
       <c r="O2" t="n">
-        <v>18.99051121978045</v>
+        <v>0</v>
       </c>
       <c r="P2" t="n">
-        <v>22.05642765435773</v>
+        <v>0.02785060816134256</v>
       </c>
     </row>
     <row r="3">
@@ -1358,16 +1358,16 @@
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>0.01658758353560441</v>
+        <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>0.03129731265724234</v>
+        <v>0</v>
       </c>
       <c r="H4" t="n">
-        <v>0.0590515054506093</v>
+        <v>0</v>
       </c>
       <c r="I4" t="n">
-        <v>0.1114178822371324</v>
+        <v>0</v>
       </c>
       <c r="J4" t="n">
         <v>0</v>
@@ -1376,19 +1376,19 @@
         <v>0</v>
       </c>
       <c r="L4" t="n">
-        <v>0.0188839008447679</v>
+        <v>0</v>
       </c>
       <c r="M4" t="n">
-        <v>0.009100088594680181</v>
+        <v>0.0123328842472441</v>
       </c>
       <c r="N4" t="n">
-        <v>0.007654959589974079</v>
+        <v>0</v>
       </c>
       <c r="O4" t="n">
-        <v>0.002376906676897371</v>
+        <v>0</v>
       </c>
       <c r="P4" t="n">
-        <v>0.003629542226577984</v>
+        <v>0.007384153366176154</v>
       </c>
     </row>
     <row r="5">
@@ -1407,40 +1407,40 @@
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>0.02875181146171431</v>
+        <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>0.05424867527255337</v>
+        <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>0.1023559427810561</v>
+        <v>0</v>
       </c>
       <c r="H5" t="n">
-        <v>0.1931243292110295</v>
+        <v>0</v>
       </c>
       <c r="I5" t="n">
-        <v>0.3931371663305571</v>
+        <v>0.01632000699885733</v>
       </c>
       <c r="J5" t="n">
-        <v>0.7417678883376548</v>
+        <v>0.04322425596824195</v>
       </c>
       <c r="K5" t="n">
-        <v>1.39956139304893</v>
+        <v>0.0815551614562192</v>
       </c>
       <c r="L5" t="n">
-        <v>3.077144211800086</v>
+        <v>0.197928381028819</v>
       </c>
       <c r="M5" t="n">
-        <v>0</v>
+        <v>0.6509743285976712</v>
       </c>
       <c r="N5" t="n">
-        <v>1.126010196373993</v>
+        <v>2.040106961372163</v>
       </c>
       <c r="O5" t="n">
-        <v>0.6078293056505065</v>
+        <v>0.6835800259622815</v>
       </c>
       <c r="P5" t="n">
-        <v>4.641879992093138</v>
+        <v>4.502926889005515</v>
       </c>
     </row>
     <row r="6">
@@ -1459,40 +1459,40 @@
         <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>0.04976275060681323</v>
+        <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>0.09389193797172701</v>
+        <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>0.1771545163518279</v>
+        <v>0.001537827592581085</v>
       </c>
       <c r="H6" t="n">
-        <v>0.3342536467113974</v>
+        <v>0.05112648314049382</v>
       </c>
       <c r="I6" t="n">
-        <v>0.6804297109567335</v>
+        <v>0.0964650170097823</v>
       </c>
       <c r="J6" t="n">
-        <v>1.28382903750748</v>
+        <v>0.1820093801704763</v>
       </c>
       <c r="K6" t="n">
-        <v>2.422317795661608</v>
+        <v>0.3449515903940907</v>
       </c>
       <c r="L6" t="n">
-        <v>5.633072717490311</v>
+        <v>0.8642752440937992</v>
       </c>
       <c r="M6" t="n">
-        <v>7.547997056578105</v>
+        <v>2.740267413528834</v>
       </c>
       <c r="N6" t="n">
-        <v>7.047662988862908</v>
+        <v>8.546132267699297</v>
       </c>
       <c r="O6" t="n">
-        <v>9.176952777134526</v>
+        <v>1.844303434706212</v>
       </c>
       <c r="P6" t="n">
-        <v>9.667268162552734</v>
+        <v>9.324650766361902</v>
       </c>
     </row>
     <row r="7">
@@ -1511,40 +1511,40 @@
         <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>0.03759852268070332</v>
+        <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>0.07094057535641596</v>
+        <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>0.1338500790213811</v>
+        <v>0</v>
       </c>
       <c r="H7" t="n">
-        <v>0.2525471997375001</v>
+        <v>0</v>
       </c>
       <c r="I7" t="n">
-        <v>0.514102448278421</v>
+        <v>0</v>
       </c>
       <c r="J7" t="n">
-        <v>0.9700041616723177</v>
+        <v>0</v>
       </c>
       <c r="K7" t="n">
-        <v>1.830195667833216</v>
+        <v>0</v>
       </c>
       <c r="L7" t="n">
-        <v>4.267780837684266</v>
+        <v>0</v>
       </c>
       <c r="M7" t="n">
-        <v>0.2393342154919741</v>
+        <v>0</v>
       </c>
       <c r="N7" t="n">
-        <v>2.106055095396093</v>
+        <v>0</v>
       </c>
       <c r="O7" t="n">
-        <v>9.287178273228839</v>
+        <v>0</v>
       </c>
       <c r="P7" t="n">
-        <v>2.013024951371854</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -1563,40 +1563,40 @@
         <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>0.1614524797465496</v>
+        <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>0.3046271765304921</v>
+        <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>0.5747679863859306</v>
+        <v>0</v>
       </c>
       <c r="H8" t="n">
-        <v>1.084467387108089</v>
+        <v>0</v>
       </c>
       <c r="I8" t="n">
-        <v>2.207616395548514</v>
+        <v>0.1448794806167378</v>
       </c>
       <c r="J8" t="n">
-        <v>4.1653119883576</v>
+        <v>0.2899303807368551</v>
       </c>
       <c r="K8" t="n">
-        <v>7.859075514813224</v>
+        <v>0.5470381960867109</v>
       </c>
       <c r="L8" t="n">
-        <v>17.76176944095573</v>
+        <v>1.338102479678464</v>
       </c>
       <c r="M8" t="n">
-        <v>7.005752314848334</v>
+        <v>4.231715050367913</v>
       </c>
       <c r="N8" t="n">
-        <v>8.555762518438682</v>
+        <v>13.8094355831997</v>
       </c>
       <c r="O8" t="n">
-        <v>15.86437452262215</v>
+        <v>9.438090551313886</v>
       </c>
       <c r="P8" t="n">
-        <v>9.729983557241182</v>
+        <v>11.23885237865513</v>
       </c>
     </row>
     <row r="9">
@@ -1615,40 +1615,40 @@
         <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>0.04202187829019783</v>
+        <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>0.07928652539834721</v>
+        <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>0.1495971471415436</v>
+        <v>0</v>
       </c>
       <c r="H9" t="n">
-        <v>0.2822586350007354</v>
+        <v>0</v>
       </c>
       <c r="I9" t="n">
-        <v>0.5745850892523529</v>
+        <v>0.02692408449993333</v>
       </c>
       <c r="J9" t="n">
-        <v>1.084122298339649</v>
+        <v>0.06589792925277575</v>
       </c>
       <c r="K9" t="n">
-        <v>1.895915658083815</v>
+        <v>0.1243356569003593</v>
       </c>
       <c r="L9" t="n">
-        <v>4.143012273683798</v>
+        <v>0.2961806129943859</v>
       </c>
       <c r="M9" t="n">
-        <v>0.01804421847412493</v>
+        <v>0.9612136489747862</v>
       </c>
       <c r="N9" t="n">
-        <v>1.783910287477092</v>
+        <v>3.146715015265477</v>
       </c>
       <c r="O9" t="n">
-        <v>4.311988826284607</v>
+        <v>1.099231683612823</v>
       </c>
       <c r="P9" t="n">
-        <v>0.03750234475953916</v>
+        <v>2.447532208810903</v>
       </c>
     </row>
     <row r="10">
@@ -1667,40 +1667,40 @@
         <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>0.04976275060681323</v>
+        <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>0.09389193797172701</v>
+        <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>0.1771545163518279</v>
+        <v>0</v>
       </c>
       <c r="H10" t="n">
-        <v>0.3342536467113974</v>
+        <v>0</v>
       </c>
       <c r="I10" t="n">
-        <v>0.6804297109567337</v>
+        <v>0</v>
       </c>
       <c r="J10" t="n">
-        <v>1.28382903750748</v>
+        <v>0</v>
       </c>
       <c r="K10" t="n">
-        <v>2.422317795661609</v>
+        <v>0</v>
       </c>
       <c r="L10" t="n">
-        <v>5.572764856703947</v>
+        <v>0</v>
       </c>
       <c r="M10" t="n">
-        <v>9.234041232255496</v>
+        <v>0</v>
       </c>
       <c r="N10" t="n">
         <v>0</v>
       </c>
       <c r="O10" t="n">
-        <v>0.8924876922691458</v>
+        <v>0</v>
       </c>
       <c r="P10" t="n">
-        <v>7.32953238718961</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -1719,40 +1719,40 @@
         <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>0.1559232852346815</v>
+        <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>0.2941947389780779</v>
+        <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>0.5550841512357274</v>
+        <v>0</v>
       </c>
       <c r="H11" t="n">
-        <v>1.047328093029045</v>
+        <v>0</v>
       </c>
       <c r="I11" t="n">
-        <v>2.132013094331099</v>
+        <v>0</v>
       </c>
       <c r="J11" t="n">
-        <v>4.022664317523435</v>
+        <v>0</v>
       </c>
       <c r="K11" t="n">
-        <v>0.8267607263444243</v>
+        <v>0</v>
       </c>
       <c r="L11" t="n">
-        <v>0</v>
+        <v>0.03129708696330907</v>
       </c>
       <c r="M11" t="n">
-        <v>1.221094713258628</v>
+        <v>0.2730817138648735</v>
       </c>
       <c r="N11" t="n">
-        <v>0.01131493925742846</v>
+        <v>0.0715875842544518</v>
       </c>
       <c r="O11" t="n">
-        <v>0.509122359367433</v>
+        <v>0.106818033542946</v>
       </c>
       <c r="P11" t="n">
-        <v>0</v>
+        <v>0.02796062280800733</v>
       </c>
     </row>
     <row r="12">
@@ -1774,37 +1774,37 @@
         <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>0.001720761626326164</v>
+        <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>0.03248944615776139</v>
+        <v>0</v>
       </c>
       <c r="H12" t="n">
-        <v>0.06130081288076224</v>
+        <v>0</v>
       </c>
       <c r="I12" t="n">
-        <v>0.1156618565178136</v>
+        <v>0</v>
       </c>
       <c r="J12" t="n">
-        <v>0.2199505766072225</v>
+        <v>0</v>
       </c>
       <c r="K12" t="n">
-        <v>0.4442436197496527</v>
+        <v>0</v>
       </c>
       <c r="L12" t="n">
-        <v>1.034774342607159</v>
+        <v>0</v>
       </c>
       <c r="M12" t="n">
-        <v>3.174079433797561</v>
+        <v>0</v>
       </c>
       <c r="N12" t="n">
         <v>0</v>
       </c>
       <c r="O12" t="n">
-        <v>1.431689604165426</v>
+        <v>0</v>
       </c>
       <c r="P12" t="n">
-        <v>0.1169389951017126</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -1823,40 +1823,40 @@
         <v>0</v>
       </c>
       <c r="E13" t="n">
-        <v>0.1205364403587254</v>
+        <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>0.2274271386426275</v>
+        <v>0</v>
       </c>
       <c r="G13" t="n">
-        <v>0.4291076062744276</v>
+        <v>0</v>
       </c>
       <c r="H13" t="n">
-        <v>0.8096366109231623</v>
+        <v>0</v>
       </c>
       <c r="I13" t="n">
-        <v>1.648151966539643</v>
+        <v>0</v>
       </c>
       <c r="J13" t="n">
-        <v>3.109719224184783</v>
+        <v>0.05609710789375089</v>
       </c>
       <c r="K13" t="n">
-        <v>5.867391993935896</v>
+        <v>0.1702828823195559</v>
       </c>
       <c r="L13" t="n">
-        <v>6.545301019565625</v>
+        <v>0.4089110724479523</v>
       </c>
       <c r="M13" t="n">
-        <v>0.993983175026622</v>
+        <v>1.3177719873056</v>
       </c>
       <c r="N13" t="n">
-        <v>0.3295078860364108</v>
+        <v>4.317320152865984</v>
       </c>
       <c r="O13" t="n">
-        <v>3.147682860978144</v>
+        <v>0</v>
       </c>
       <c r="P13" t="n">
-        <v>0.03192805781851881</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -1875,40 +1875,40 @@
         <v>0</v>
       </c>
       <c r="E14" t="n">
-        <v>0.6568683080099346</v>
+        <v>0</v>
       </c>
       <c r="F14" t="n">
-        <v>1.257681926388727</v>
+        <v>0</v>
       </c>
       <c r="G14" t="n">
-        <v>2.402226374659132</v>
+        <v>0.001537827592581085</v>
       </c>
       <c r="H14" t="n">
-        <v>4.532500454921816</v>
+        <v>0.05112648314049382</v>
       </c>
       <c r="I14" t="n">
-        <v>9.208751923383829</v>
+        <v>0.2845885891253108</v>
       </c>
       <c r="J14" t="n">
-        <v>17.16649387170595</v>
+        <v>0.6371590540220999</v>
       </c>
       <c r="K14" t="n">
-        <v>25.50607300861273</v>
+        <v>1.268163487156936</v>
       </c>
       <c r="L14" t="n">
-        <v>49.30973325947812</v>
+        <v>3.13669487720673</v>
       </c>
       <c r="M14" t="n">
-        <v>33.42751795097031</v>
+        <v>10.2017910444521</v>
       </c>
       <c r="N14" t="n">
-        <v>33.36021044065537</v>
+        <v>31.97781316497526</v>
       </c>
       <c r="O14" t="n">
-        <v>64.22219434815813</v>
+        <v>13.17202372913815</v>
       </c>
       <c r="P14" t="n">
-        <v>55.62811564471259</v>
+        <v>27.57715762716898</v>
       </c>
     </row>
   </sheetData>
@@ -1998,40 +1998,40 @@
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>39.86214284453398</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>68.29554974478945</v>
+        <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>114.1792745700474</v>
+        <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>196.9668497107533</v>
+        <v>0</v>
       </c>
       <c r="I2" t="n">
-        <v>369.6343227191189</v>
+        <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>661.9607388769967</v>
+        <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>1278.98379610933</v>
+        <v>0</v>
       </c>
       <c r="L2" t="n">
-        <v>2816.735352871615</v>
+        <v>0</v>
       </c>
       <c r="M2" t="n">
-        <v>8926.158493084002</v>
+        <v>30.50049797914543</v>
       </c>
       <c r="N2" t="n">
-        <v>27808.39204133594</v>
+        <v>98.29203595582459</v>
       </c>
       <c r="O2" t="n">
-        <v>41770.82287955059</v>
+        <v>0</v>
       </c>
       <c r="P2" t="n">
-        <v>48524.14083958699</v>
+        <v>57.69713015656774</v>
       </c>
     </row>
     <row r="3">
@@ -2105,16 +2105,16 @@
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>58.11089369581832</v>
+        <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>97.15215283572552</v>
+        <v>0</v>
       </c>
       <c r="H4" t="n">
-        <v>167.5939311992296</v>
+        <v>0</v>
       </c>
       <c r="I4" t="n">
-        <v>291.5105328665908</v>
+        <v>0</v>
       </c>
       <c r="J4" t="n">
         <v>0</v>
@@ -2123,19 +2123,19 @@
         <v>0</v>
       </c>
       <c r="L4" t="n">
-        <v>42.70799938091401</v>
+        <v>0</v>
       </c>
       <c r="M4" t="n">
-        <v>20.58084191728558</v>
+        <v>29.62001838119535</v>
       </c>
       <c r="N4" t="n">
-        <v>17.31252520954195</v>
+        <v>0</v>
       </c>
       <c r="O4" t="n">
-        <v>5.270228864128407</v>
+        <v>0</v>
       </c>
       <c r="P4" t="n">
-        <v>8.047652182564043</v>
+        <v>17.38686190758963</v>
       </c>
     </row>
     <row r="5">
@@ -2154,40 +2154,40 @@
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>110.9256046750557</v>
+        <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>190.0481161186478</v>
+        <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>317.7301612318728</v>
+        <v>0</v>
       </c>
       <c r="H5" t="n">
-        <v>582.0595973415445</v>
+        <v>0</v>
       </c>
       <c r="I5" t="n">
-        <v>1086.870099290752</v>
+        <v>44.85632075145539</v>
       </c>
       <c r="J5" t="n">
-        <v>1842.058404071628</v>
+        <v>107.3403219765687</v>
       </c>
       <c r="K5" t="n">
-        <v>3351.452388204759</v>
+        <v>207.3937688662524</v>
       </c>
       <c r="L5" t="n">
-        <v>7101.526098580091</v>
+        <v>475.366683632332</v>
       </c>
       <c r="M5" t="n">
-        <v>0</v>
+        <v>1561.517718714874</v>
       </c>
       <c r="N5" t="n">
-        <v>2546.594750997509</v>
+        <v>4899.784083423991</v>
       </c>
       <c r="O5" t="n">
-        <v>1431.205945578045</v>
+        <v>1608.426199563224</v>
       </c>
       <c r="P5" t="n">
-        <v>10837.25291112675</v>
+        <v>10602.67360612177</v>
       </c>
     </row>
     <row r="6">
@@ -2206,40 +2206,40 @@
         <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>179.3796428004029</v>
+        <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>307.3299738515526</v>
+        <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>513.8067355652132</v>
+        <v>4.46020903941829</v>
       </c>
       <c r="H6" t="n">
-        <v>886.3508236983899</v>
+        <v>135.5736904899215</v>
       </c>
       <c r="I6" t="n">
-        <v>1672.719661950729</v>
+        <v>235.8149753670133</v>
       </c>
       <c r="J6" t="n">
-        <v>3093.614056095011</v>
+        <v>422.3099580793742</v>
       </c>
       <c r="K6" t="n">
-        <v>5735.779357100485</v>
+        <v>819.6049787763594</v>
       </c>
       <c r="L6" t="n">
-        <v>12639.98476960104</v>
+        <v>1939.433647746485</v>
       </c>
       <c r="M6" t="n">
-        <v>16905.90768212787</v>
+        <v>6140.137393295712</v>
       </c>
       <c r="N6" t="n">
-        <v>15814.95574700837</v>
+        <v>19177.52080871723</v>
       </c>
       <c r="O6" t="n">
-        <v>20170.63094767963</v>
+        <v>4052.171268705275</v>
       </c>
       <c r="P6" t="n">
-        <v>21267.98995761601</v>
+        <v>20514.23168599618</v>
       </c>
     </row>
     <row r="7">
@@ -2258,40 +2258,40 @@
         <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>152.2004140274286</v>
+        <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>260.763978191733</v>
+        <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>435.9558122775533</v>
+        <v>0</v>
       </c>
       <c r="H7" t="n">
-        <v>752.0527983799967</v>
+        <v>0</v>
       </c>
       <c r="I7" t="n">
-        <v>1411.326460195864</v>
+        <v>0</v>
       </c>
       <c r="J7" t="n">
-        <v>2602.412190965603</v>
+        <v>0</v>
       </c>
       <c r="K7" t="n">
-        <v>4848.789777285068</v>
+        <v>0</v>
       </c>
       <c r="L7" t="n">
-        <v>10754.77273223261</v>
+        <v>0</v>
       </c>
       <c r="M7" t="n">
-        <v>567.9377892956239</v>
+        <v>0</v>
       </c>
       <c r="N7" t="n">
-        <v>5296.116029945139</v>
+        <v>0</v>
       </c>
       <c r="O7" t="n">
-        <v>22928.44348731563</v>
+        <v>0</v>
       </c>
       <c r="P7" t="n">
-        <v>4973.339586965267</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -2310,40 +2310,40 @@
         <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>688.0690180002125</v>
+        <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>1178.864167688006</v>
+        <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>1970.873006897621</v>
+        <v>0</v>
       </c>
       <c r="H8" t="n">
-        <v>3476.581565299844</v>
+        <v>0</v>
       </c>
       <c r="I8" t="n">
-        <v>6643.260204222104</v>
+        <v>418.7231021283728</v>
       </c>
       <c r="J8" t="n">
-        <v>12042.76468146569</v>
+        <v>844.6036143422796</v>
       </c>
       <c r="K8" t="n">
-        <v>22076.81428615932</v>
+        <v>1536.677009869517</v>
       </c>
       <c r="L8" t="n">
-        <v>46990.96366405996</v>
+        <v>3548.912534500049</v>
       </c>
       <c r="M8" t="n">
-        <v>18586.43673567573</v>
+        <v>11223.93422346451</v>
       </c>
       <c r="N8" t="n">
-        <v>22619.9448586577</v>
+        <v>36636.77921906194</v>
       </c>
       <c r="O8" t="n">
-        <v>41263.31745521283</v>
+        <v>24546.81136670854</v>
       </c>
       <c r="P8" t="n">
-        <v>25261.53460912602</v>
+        <v>29232.31123114388</v>
       </c>
     </row>
     <row r="9">
@@ -2362,40 +2362,40 @@
         <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>191.397983198887</v>
+        <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>327.9209181902871</v>
+        <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>582.1932253521742</v>
+        <v>0</v>
       </c>
       <c r="H9" t="n">
-        <v>945.7358561657422</v>
+        <v>0</v>
       </c>
       <c r="I9" t="n">
-        <v>1884.743088052191</v>
+        <v>90.12233118512209</v>
       </c>
       <c r="J9" t="n">
-        <v>3350.460358837973</v>
+        <v>205.166094187093</v>
       </c>
       <c r="K9" t="n">
-        <v>5691.917139329014</v>
+        <v>373.2804534438844</v>
       </c>
       <c r="L9" t="n">
-        <v>11737.70325082774</v>
+        <v>839.7936756626733</v>
       </c>
       <c r="M9" t="n">
-        <v>48.17823624657514</v>
+        <v>2725.512543465065</v>
       </c>
       <c r="N9" t="n">
-        <v>5053.664981173389</v>
+        <v>8922.432187615819</v>
       </c>
       <c r="O9" t="n">
-        <v>11986.52863194505</v>
+        <v>3055.660063043169</v>
       </c>
       <c r="P9" t="n">
-        <v>101.6354758230534</v>
+        <v>6803.685278516357</v>
       </c>
     </row>
     <row r="10">
@@ -2414,40 +2414,40 @@
         <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>169.9245418283937</v>
+        <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>291.1306109298373</v>
+        <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>486.7239825335708</v>
+        <v>0</v>
       </c>
       <c r="H10" t="n">
-        <v>839.6312717812476</v>
+        <v>0</v>
       </c>
       <c r="I10" t="n">
-        <v>1619.156017842706</v>
+        <v>0</v>
       </c>
       <c r="J10" t="n">
-        <v>2996.614319629296</v>
+        <v>0</v>
       </c>
       <c r="K10" t="n">
-        <v>5452.05852097383</v>
+        <v>0</v>
       </c>
       <c r="L10" t="n">
-        <v>11831.41246630744</v>
+        <v>0</v>
       </c>
       <c r="M10" t="n">
-        <v>19600.71363203872</v>
+        <v>0</v>
       </c>
       <c r="N10" t="n">
         <v>0</v>
       </c>
       <c r="O10" t="n">
-        <v>1843.389116035006</v>
+        <v>0</v>
       </c>
       <c r="P10" t="n">
-        <v>15002.63384322414</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -2466,40 +2466,40 @@
         <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>512.6795756985475</v>
+        <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>878.3705783659068</v>
+        <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>1480.075564621138</v>
+        <v>0</v>
       </c>
       <c r="H11" t="n">
-        <v>2533.252698687657</v>
+        <v>0</v>
       </c>
       <c r="I11" t="n">
-        <v>4753.983459302242</v>
+        <v>0</v>
       </c>
       <c r="J11" t="n">
-        <v>8523.531807993324</v>
+        <v>0</v>
       </c>
       <c r="K11" t="n">
-        <v>1691.123429564027</v>
+        <v>0</v>
       </c>
       <c r="L11" t="n">
-        <v>0</v>
+        <v>64.06089938831884</v>
       </c>
       <c r="M11" t="n">
-        <v>2353.614408380333</v>
+        <v>531.9307886412913</v>
       </c>
       <c r="N11" t="n">
-        <v>23.16014861718061</v>
+        <v>137.9823923017286</v>
       </c>
       <c r="O11" t="n">
-        <v>962.0728566743599</v>
+        <v>201.8507511685085</v>
       </c>
       <c r="P11" t="n">
-        <v>0</v>
+        <v>56.10942060751254</v>
       </c>
     </row>
     <row r="12">
@@ -2521,37 +2521,37 @@
         <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>5.335563354628049</v>
+        <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>89.26327677026497</v>
+        <v>0</v>
       </c>
       <c r="H12" t="n">
-        <v>153.9850948125607</v>
+        <v>0</v>
       </c>
       <c r="I12" t="n">
-        <v>267.8395137647349</v>
+        <v>0</v>
       </c>
       <c r="J12" t="n">
-        <v>513.3916029439264</v>
+        <v>0</v>
       </c>
       <c r="K12" t="n">
-        <v>998.6147705529783</v>
+        <v>0</v>
       </c>
       <c r="L12" t="n">
-        <v>2071.325277493956</v>
+        <v>0</v>
       </c>
       <c r="M12" t="n">
-        <v>6380.586571781668</v>
+        <v>0</v>
       </c>
       <c r="N12" t="n">
         <v>0</v>
       </c>
       <c r="O12" t="n">
-        <v>2809.644372451964</v>
+        <v>0</v>
       </c>
       <c r="P12" t="n">
-        <v>243.7053094737829</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -2570,40 +2570,40 @@
         <v>0</v>
       </c>
       <c r="E13" t="n">
-        <v>533.7417673137425</v>
+        <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>914.4562940987495</v>
+        <v>0</v>
       </c>
       <c r="G13" t="n">
-        <v>1528.825182261238</v>
+        <v>0</v>
       </c>
       <c r="H13" t="n">
-        <v>2733.46686165604</v>
+        <v>0</v>
       </c>
       <c r="I13" t="n">
-        <v>5252.982151110983</v>
+        <v>0</v>
       </c>
       <c r="J13" t="n">
-        <v>9412.520438229902</v>
+        <v>169.7951282768746</v>
       </c>
       <c r="K13" t="n">
-        <v>17082.09982598452</v>
+        <v>497.0058256213703</v>
       </c>
       <c r="L13" t="n">
-        <v>18034.49522697131</v>
+        <v>1127.186486127884</v>
       </c>
       <c r="M13" t="n">
-        <v>2734.224104705941</v>
+        <v>3632.512974022785</v>
       </c>
       <c r="N13" t="n">
-        <v>899.732279016672</v>
+        <v>11900.93705084869</v>
       </c>
       <c r="O13" t="n">
-        <v>8506.633076963746</v>
+        <v>0</v>
       </c>
       <c r="P13" t="n">
-        <v>81.25237802477804</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -2622,40 +2622,40 @@
         <v>0</v>
       </c>
       <c r="E14" t="n">
-        <v>2578.180690387204</v>
+        <v>0</v>
       </c>
       <c r="F14" t="n">
-        <v>4480.626644229957</v>
+        <v>0</v>
       </c>
       <c r="G14" t="n">
-        <v>7616.778374916419</v>
+        <v>4.46020903941829</v>
       </c>
       <c r="H14" t="n">
-        <v>13267.67734873301</v>
+        <v>135.5736904899215</v>
       </c>
       <c r="I14" t="n">
-        <v>25254.02551131802</v>
+        <v>789.5167294319637</v>
       </c>
       <c r="J14" t="n">
-        <v>45039.32859910934</v>
+        <v>1749.21511686219</v>
       </c>
       <c r="K14" t="n">
-        <v>68207.63329126334</v>
+        <v>3433.962036577383</v>
       </c>
       <c r="L14" t="n">
-        <v>124021.6268383267</v>
+        <v>7994.753927057742</v>
       </c>
       <c r="M14" t="n">
-        <v>76124.33849525375</v>
+        <v>25875.66615796458</v>
       </c>
       <c r="N14" t="n">
-        <v>80079.87336196144</v>
+        <v>81773.72777792522</v>
       </c>
       <c r="O14" t="n">
-        <v>153677.958998271</v>
+        <v>33464.91964918872</v>
       </c>
       <c r="P14" t="n">
-        <v>126301.5325631493</v>
+        <v>67284.09521444986</v>
       </c>
     </row>
   </sheetData>
@@ -2727,40 +2727,40 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.05031567005800005</v>
+        <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>0.1452508517849684</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>0.3243737516518166</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>0.6623413277711184</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>1.300015698791594</v>
+        <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>2.503174321655522</v>
+        <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>4.773283859624301</v>
+        <v>0</v>
       </c>
       <c r="I2" t="n">
-        <v>15.51391115206189</v>
+        <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>50.12705500099931</v>
+        <v>0.1313495598431097</v>
       </c>
       <c r="K2" t="n">
-        <v>161.6726560620089</v>
+        <v>0.5546415227385433</v>
       </c>
       <c r="L2" t="n">
-        <v>320.855922816881</v>
+        <v>0.4232919628954335</v>
       </c>
       <c r="M2" t="n">
-        <v>486.2973610345848</v>
+        <v>0.2534405342682173</v>
       </c>
     </row>
     <row r="3">
@@ -2816,37 +2816,37 @@
         <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>0.07547350508700007</v>
+        <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>0.2178762776774527</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>0.486560627477725</v>
+        <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>0.9935119916566777</v>
+        <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>0.9180384865696777</v>
+        <v>0</v>
       </c>
       <c r="H4" t="n">
-        <v>0.7103606807989664</v>
+        <v>0</v>
       </c>
       <c r="I4" t="n">
-        <v>0.4253191797768642</v>
+        <v>0</v>
       </c>
       <c r="J4" t="n">
-        <v>0.2546543038989775</v>
+        <v>0.1122292466499213</v>
       </c>
       <c r="K4" t="n">
-        <v>0.1524709384803538</v>
+        <v>0.1122292466499213</v>
       </c>
       <c r="L4" t="n">
-        <v>0.0912899830285302</v>
+        <v>0.1122292466499213</v>
       </c>
       <c r="M4" t="n">
-        <v>0.05465868502162573</v>
+        <v>0.067195795632203</v>
       </c>
     </row>
     <row r="5">
@@ -2856,40 +2856,40 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.1308207421508001</v>
+        <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>0.377652214640918</v>
+        <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>0.8433717542947233</v>
+        <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>1.722087452204907</v>
+        <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>3.380040816858143</v>
+        <v>0.07425603184480084</v>
       </c>
       <c r="G5" t="n">
-        <v>6.508253236304354</v>
+        <v>0.2709263965003017</v>
       </c>
       <c r="H5" t="n">
-        <v>12.41053803502318</v>
+        <v>0.6420023811260991</v>
       </c>
       <c r="I5" t="n">
-        <v>40.33616899536089</v>
+        <v>2.410449538872679</v>
       </c>
       <c r="J5" t="n">
-        <v>26.35203949249101</v>
+        <v>8.109512935609814</v>
       </c>
       <c r="K5" t="n">
-        <v>19.48488458531732</v>
+        <v>26.47552599840065</v>
       </c>
       <c r="L5" t="n">
-        <v>15.77793946842295</v>
+        <v>30.57899502405265</v>
       </c>
       <c r="M5" t="n">
-        <v>47.77235460946716</v>
+        <v>65.75866327631495</v>
       </c>
     </row>
     <row r="6">
@@ -2899,40 +2899,40 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.2264205152610002</v>
+        <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>0.6536288330323581</v>
+        <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>1.459681882433175</v>
+        <v>0.006997115546243937</v>
       </c>
       <c r="E6" t="n">
-        <v>2.980535974970033</v>
+        <v>0.2396226138354908</v>
       </c>
       <c r="F6" t="n">
-        <v>5.850070644562171</v>
+        <v>0.6785384412300003</v>
       </c>
       <c r="G6" t="n">
-        <v>11.26428444744985</v>
+        <v>1.506681121005668</v>
       </c>
       <c r="H6" t="n">
-        <v>21.47977736830935</v>
+        <v>3.069213741752536</v>
       </c>
       <c r="I6" t="n">
-        <v>69.81260018427847</v>
+        <v>10.48203505101961</v>
       </c>
       <c r="J6" t="n">
-        <v>134.4212276354864</v>
+        <v>34.37086792065908</v>
       </c>
       <c r="K6" t="n">
-        <v>189.2259201560078</v>
+        <v>111.3559066885761</v>
       </c>
       <c r="L6" t="n">
-        <v>214.1202692070476</v>
+        <v>118.8621611821222</v>
       </c>
       <c r="M6" t="n">
-        <v>235.6161437498065</v>
+        <v>179.4072868657834</v>
       </c>
     </row>
     <row r="7">
@@ -2942,40 +2942,40 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.1710732781972001</v>
+        <v>0</v>
       </c>
       <c r="C7" t="n">
-        <v>0.4938528960688927</v>
+        <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>1.102870755616177</v>
+        <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>2.251960514421802</v>
+        <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>4.420053375891418</v>
+        <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>8.510792693628771</v>
+        <v>0</v>
       </c>
       <c r="H7" t="n">
-        <v>16.22916512272262</v>
+        <v>0</v>
       </c>
       <c r="I7" t="n">
-        <v>52.74729791701039</v>
+        <v>0</v>
       </c>
       <c r="J7" t="n">
-        <v>50.94888029732227</v>
+        <v>0</v>
       </c>
       <c r="K7" t="n">
-        <v>63.83801068193399</v>
+        <v>0</v>
       </c>
       <c r="L7" t="n">
-        <v>103.6784236544869</v>
+        <v>0</v>
       </c>
       <c r="M7" t="n">
-        <v>121.3082329404943</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -2985,40 +2985,40 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.7346087828468006</v>
+        <v>0</v>
       </c>
       <c r="C8" t="n">
-        <v>2.12066243606054</v>
+        <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>4.735856774116524</v>
+        <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>9.67018338545833</v>
+        <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>18.98022920235726</v>
+        <v>0.6592016368061573</v>
       </c>
       <c r="G8" t="n">
-        <v>36.54634509617061</v>
+        <v>1.978384869158848</v>
       </c>
       <c r="H8" t="n">
-        <v>69.68994435051479</v>
+        <v>4.467408661353383</v>
       </c>
       <c r="I8" t="n">
-        <v>226.5031028201035</v>
+        <v>16.31454040802433</v>
       </c>
       <c r="J8" t="n">
-        <v>280.9914254159521</v>
+        <v>54.49354654796927</v>
       </c>
       <c r="K8" t="n">
-        <v>313.3916376147428</v>
+        <v>177.5306276746774</v>
       </c>
       <c r="L8" t="n">
-        <v>285.9755931387734</v>
+        <v>249.8898678275572</v>
       </c>
       <c r="M8" t="n">
-        <v>306.1380728109697</v>
+        <v>313.8260444698353</v>
       </c>
     </row>
     <row r="9">
@@ -3028,40 +3028,40 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.1911995462204001</v>
+        <v>0</v>
       </c>
       <c r="C9" t="n">
-        <v>0.55195323678288</v>
+        <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>1.232620256276903</v>
+        <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>2.51689704553025</v>
+        <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>4.940059655408055</v>
+        <v>0.1225045844746966</v>
       </c>
       <c r="G9" t="n">
-        <v>9.512062422290978</v>
+        <v>0.4223401625748263</v>
       </c>
       <c r="H9" t="n">
-        <v>18.13847866657234</v>
+        <v>0.988067401471461</v>
       </c>
       <c r="I9" t="n">
-        <v>54.21528005809454</v>
+        <v>3.683310979720372</v>
       </c>
       <c r="J9" t="n">
-        <v>52.10972129659331</v>
+        <v>12.36910289315358</v>
       </c>
       <c r="K9" t="n">
-        <v>57.89314642283102</v>
+        <v>40.36025804228363</v>
       </c>
       <c r="L9" t="n">
-        <v>55.47268193523147</v>
+        <v>47.36753722908739</v>
       </c>
       <c r="M9" t="n">
-        <v>55.56894184515514</v>
+        <v>60.89458094706072</v>
       </c>
     </row>
     <row r="10">
@@ -3071,40 +3071,40 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.2264205152610002</v>
+        <v>0</v>
       </c>
       <c r="C10" t="n">
-        <v>0.6536288330323581</v>
+        <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>1.459681882433175</v>
+        <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>2.980535974970033</v>
+        <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>5.850070644562171</v>
+        <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>11.26428444744985</v>
+        <v>0</v>
       </c>
       <c r="H10" t="n">
-        <v>21.47977736830935</v>
+        <v>0</v>
       </c>
       <c r="I10" t="n">
-        <v>69.81260018427848</v>
+        <v>0</v>
       </c>
       <c r="J10" t="n">
-        <v>152.2943978053769</v>
+        <v>0</v>
       </c>
       <c r="K10" t="n">
-        <v>139.1725888458773</v>
+        <v>0</v>
       </c>
       <c r="L10" t="n">
-        <v>90.07744839690362</v>
+        <v>0</v>
       </c>
       <c r="M10" t="n">
-        <v>74.82038272307469</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -3114,40 +3114,40 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.7094509478178006</v>
+        <v>0</v>
       </c>
       <c r="C11" t="n">
-        <v>2.048037010168055</v>
+        <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>4.573669898290615</v>
+        <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>9.339012721572768</v>
+        <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>18.33022135296147</v>
+        <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>35.29475793534284</v>
+        <v>0</v>
       </c>
       <c r="H11" t="n">
-        <v>36.85238458423212</v>
+        <v>0</v>
       </c>
       <c r="I11" t="n">
-        <v>22.06488394959876</v>
+        <v>0.2848034913661126</v>
       </c>
       <c r="J11" t="n">
-        <v>13.21106108063279</v>
+        <v>2.769847087536461</v>
       </c>
       <c r="K11" t="n">
-        <v>7.909950275509349</v>
+        <v>3.421294104251972</v>
       </c>
       <c r="L11" t="n">
-        <v>4.73597941748624</v>
+        <v>2.048455160214137</v>
       </c>
       <c r="M11" t="n">
-        <v>2.835605820721672</v>
+        <v>1.226485772793676</v>
       </c>
     </row>
     <row r="12">
@@ -3160,37 +3160,37 @@
         <v>0</v>
       </c>
       <c r="C12" t="n">
-        <v>0.007829465399784047</v>
+        <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>0.1556564454175983</v>
+        <v>0</v>
       </c>
       <c r="E12" t="n">
-        <v>0.4345751440250665</v>
+        <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>0.9608365911811185</v>
+        <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>1.953782249344197</v>
+        <v>0</v>
       </c>
       <c r="H12" t="n">
-        <v>3.827263739187302</v>
+        <v>0</v>
       </c>
       <c r="I12" t="n">
-        <v>12.70166083472695</v>
+        <v>0</v>
       </c>
       <c r="J12" t="n">
-        <v>41.30062203849049</v>
+        <v>0</v>
       </c>
       <c r="K12" t="n">
-        <v>24.72820802796693</v>
+        <v>0</v>
       </c>
       <c r="L12" t="n">
-        <v>14.80569158751483</v>
+        <v>0</v>
       </c>
       <c r="M12" t="n">
-        <v>8.864714464416044</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -3200,40 +3200,40 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.5484408036322005</v>
+        <v>0</v>
       </c>
       <c r="C13" t="n">
-        <v>1.583234284456156</v>
+        <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>3.535673893004802</v>
+        <v>0</v>
       </c>
       <c r="E13" t="n">
-        <v>7.21952047270519</v>
+        <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>14.17017111682837</v>
+        <v>0</v>
       </c>
       <c r="G13" t="n">
-        <v>27.28460010604518</v>
+        <v>0.2552418409165665</v>
       </c>
       <c r="H13" t="n">
-        <v>52.02879406990486</v>
+        <v>1.030028955470546</v>
       </c>
       <c r="I13" t="n">
-        <v>110.0394889257975</v>
+        <v>4.751119714746912</v>
       </c>
       <c r="J13" t="n">
-        <v>112.591499044733</v>
+        <v>16.74284479922787</v>
       </c>
       <c r="K13" t="n">
-        <v>67.41268952230432</v>
+        <v>55.38782279211477</v>
       </c>
       <c r="L13" t="n">
-        <v>40.36246739041162</v>
+        <v>51.27933847556141</v>
       </c>
       <c r="M13" t="n">
-        <v>24.16650018544393</v>
+        <v>39.28761339108045</v>
       </c>
     </row>
     <row r="14">
@@ -3243,40 +3243,40 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>2.988750801445203</v>
+        <v>0</v>
       </c>
       <c r="C14" t="n">
-        <v>8.711203566513909</v>
+        <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>19.64133357121296</v>
+        <v>0.006997115546243937</v>
       </c>
       <c r="E14" t="n">
-        <v>40.26421064110723</v>
+        <v>0.2396226138354908</v>
       </c>
       <c r="F14" t="n">
-        <v>79.17528109105847</v>
+        <v>1.534500694355655</v>
       </c>
       <c r="G14" t="n">
-        <v>151.5603754422518</v>
+        <v>4.43357439015621</v>
       </c>
       <c r="H14" t="n">
-        <v>257.6197678451992</v>
+        <v>10.19672114117402</v>
       </c>
       <c r="I14" t="n">
-        <v>674.1723142010882</v>
+        <v>37.92625918375001</v>
       </c>
       <c r="J14" t="n">
-        <v>914.6025834119766</v>
+        <v>129.0993009906491</v>
       </c>
       <c r="K14" t="n">
-        <v>1044.88216313298</v>
+        <v>415.198306069693</v>
       </c>
       <c r="L14" t="n">
-        <v>1145.953706996188</v>
+        <v>500.5618761081403</v>
       </c>
       <c r="M14" t="n">
-        <v>1363.442968869156</v>
+        <v>660.721311052769</v>
       </c>
     </row>
   </sheetData>

</xml_diff>